<commit_message>
changed Ndio to Yes
</commit_message>
<xml_diff>
--- a/CS335/GitHub Info sans duplicates.xlsx
+++ b/CS335/GitHub Info sans duplicates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="25600" windowHeight="14340" tabRatio="500"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="28740" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3220" uniqueCount="873">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3220" uniqueCount="874">
   <si>
     <t>Timestamp</t>
   </si>
@@ -2640,6 +2640,9 @@
   </si>
   <si>
     <t>https://github.com/kasambala2021</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -3406,7 +3409,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K54" sqref="K54"/>
+      <selection pane="bottomLeft" activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -4761,7 +4764,7 @@
         <v>262</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>16</v>
+        <v>873</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>263</v>

</xml_diff>

<commit_message>
Add students without git repo access
</commit_message>
<xml_diff>
--- a/CS335/GitHub Info sans duplicates.xlsx
+++ b/CS335/GitHub Info sans duplicates.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\staffcard\CS335\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="25600" windowHeight="14340" tabRatio="500"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="25605" windowHeight="14340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3220" uniqueCount="873">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3228" uniqueCount="877">
   <si>
     <t>Timestamp</t>
   </si>
@@ -2640,16 +2645,28 @@
   </si>
   <si>
     <t>https://github.com/kasambala2021</t>
+  </si>
+  <si>
+    <t>angela-lugano</t>
+  </si>
+  <si>
+    <t>ndengu8</t>
+  </si>
+  <si>
+    <t>Ishabakaki</t>
+  </si>
+  <si>
+    <t>STILL WITHOUT ACCESS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2696,8 +2713,15 @@
       <color theme="11"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2713,6 +2737,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2942,7 +2972,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -2971,6 +3001,8 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="205">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -3198,6 +3230,14 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -3399,22 +3439,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:R122"/>
+  <dimension ref="A1:R131"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K54" sqref="K54"/>
+      <pane ySplit="1" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I124" sqref="I124"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="18" width="21.5" customWidth="1"/>
+    <col min="1" max="18" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3452,7 +3492,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>44517.792739571756</v>
       </c>
@@ -3490,7 +3530,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1">
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>44517.829278495366</v>
       </c>
@@ -3528,7 +3568,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1">
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>44517.829803020832</v>
       </c>
@@ -3566,7 +3606,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>44517.832974606485</v>
       </c>
@@ -3604,7 +3644,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.75" customHeight="1">
+    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>44517.833342615741</v>
       </c>
@@ -3642,7 +3682,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1">
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>44517.834096585648</v>
       </c>
@@ -3680,7 +3720,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>44517.834304884258</v>
       </c>
@@ -3718,7 +3758,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" customHeight="1">
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>44517.834315162036</v>
       </c>
@@ -3756,7 +3796,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1">
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>44517.834467222223</v>
       </c>
@@ -3794,7 +3834,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.75" customHeight="1">
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>44517.836256620372</v>
       </c>
@@ -3832,7 +3872,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1">
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>44517.840131203702</v>
       </c>
@@ -3870,7 +3910,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.75" customHeight="1">
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>44517.840687337964</v>
       </c>
@@ -3908,7 +3948,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1">
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>44517.840723900459</v>
       </c>
@@ -3946,7 +3986,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1">
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>44517.848194363425</v>
       </c>
@@ -3984,7 +4024,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15.75" customHeight="1">
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>44517.849799363423</v>
       </c>
@@ -4022,7 +4062,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15.75" customHeight="1">
+    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>44517.851121805557</v>
       </c>
@@ -4060,7 +4100,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15.75" customHeight="1">
+    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>44517.853374618055</v>
       </c>
@@ -4098,7 +4138,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15.75" customHeight="1">
+    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>44517.855156886573</v>
       </c>
@@ -4136,7 +4176,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15.75" customHeight="1">
+    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>44517.858557291664</v>
       </c>
@@ -4174,7 +4214,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15.75" customHeight="1">
+    <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>44517.859119421293</v>
       </c>
@@ -4212,7 +4252,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15.75" customHeight="1">
+    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>44517.860663136569</v>
       </c>
@@ -4250,7 +4290,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15.75" customHeight="1">
+    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>44517.863773090277</v>
       </c>
@@ -4288,7 +4328,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="15.75" customHeight="1">
+    <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>44517.867895196759</v>
       </c>
@@ -4326,7 +4366,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="15.75" customHeight="1">
+    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>44517.86830321759</v>
       </c>
@@ -4364,7 +4404,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="15.75" customHeight="1">
+    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>44517.869191446764</v>
       </c>
@@ -4402,7 +4442,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="15.75" customHeight="1">
+    <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>44517.874595833331</v>
       </c>
@@ -4440,7 +4480,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="15.75" customHeight="1">
+    <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>44517.877297905092</v>
       </c>
@@ -4478,7 +4518,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="15.75" customHeight="1">
+    <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>44517.877863587964</v>
       </c>
@@ -4516,7 +4556,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="15.75" customHeight="1">
+    <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>44517.886029872687</v>
       </c>
@@ -4554,7 +4594,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="15.75" customHeight="1">
+    <row r="31" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>44517.888174652777</v>
       </c>
@@ -4592,7 +4632,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="15.75" customHeight="1">
+    <row r="32" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>44517.89089574074</v>
       </c>
@@ -4630,7 +4670,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="15.75" customHeight="1">
+    <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>44517.898055138889</v>
       </c>
@@ -4668,7 +4708,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="15.75" customHeight="1">
+    <row r="34" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>44517.903385925922</v>
       </c>
@@ -4706,7 +4746,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="15.75" customHeight="1">
+    <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>44517.916796608799</v>
       </c>
@@ -4744,7 +4784,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="15.75" customHeight="1">
+    <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>44517.919944965281</v>
       </c>
@@ -4782,7 +4822,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="15.75" customHeight="1">
+    <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>44517.920174733794</v>
       </c>
@@ -4820,7 +4860,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="15.75" customHeight="1">
+    <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>44517.920207002317</v>
       </c>
@@ -4858,7 +4898,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="15.75" customHeight="1">
+    <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>44517.925676087965</v>
       </c>
@@ -4896,7 +4936,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="15.75" customHeight="1">
+    <row r="40" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>44517.942313136577</v>
       </c>
@@ -4934,7 +4974,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="15.75" customHeight="1">
+    <row r="41" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>44517.967181493055</v>
       </c>
@@ -4972,7 +5012,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="15.75" customHeight="1">
+    <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>44517.970856388885</v>
       </c>
@@ -5010,7 +5050,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="15.75" customHeight="1">
+    <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>44517.974103865738</v>
       </c>
@@ -5048,7 +5088,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="15.75" customHeight="1">
+    <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>44517.995788912041</v>
       </c>
@@ -5086,7 +5126,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="15.75" customHeight="1">
+    <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>44518.053331921299</v>
       </c>
@@ -5124,7 +5164,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="15.75" customHeight="1">
+    <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>44518.141680740737</v>
       </c>
@@ -5162,7 +5202,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="15.75" customHeight="1">
+    <row r="47" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>44518.338707534727</v>
       </c>
@@ -5200,7 +5240,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="15.75" customHeight="1">
+    <row r="48" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>44518.348475844905</v>
       </c>
@@ -5238,7 +5278,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="15.75" customHeight="1">
+    <row r="49" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>44518.368981018517</v>
       </c>
@@ -5276,7 +5316,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="15.75" customHeight="1">
+    <row r="50" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>44518.376564247686</v>
       </c>
@@ -5314,7 +5354,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="15.75" customHeight="1">
+    <row r="51" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>44518.395640312505</v>
       </c>
@@ -5352,7 +5392,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="15.75" customHeight="1">
+    <row r="52" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>44518.396610844909</v>
       </c>
@@ -5390,7 +5430,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="15.75" customHeight="1">
+    <row r="53" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>44518.416108634265</v>
       </c>
@@ -5428,7 +5468,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="15.75" customHeight="1">
+    <row r="54" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>44518.419745173611</v>
       </c>
@@ -5466,7 +5506,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="15.75" customHeight="1">
+    <row r="55" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>44518.433273449074</v>
       </c>
@@ -5504,7 +5544,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="15.75" customHeight="1">
+    <row r="56" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>44518.43360689815</v>
       </c>
@@ -5542,7 +5582,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="15.75" customHeight="1">
+    <row r="57" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>44518.462937638891</v>
       </c>
@@ -5580,7 +5620,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="15.75" customHeight="1">
+    <row r="58" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>44518.479146377314</v>
       </c>
@@ -5618,7 +5658,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="15.75" customHeight="1">
+    <row r="59" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>44518.500450555555</v>
       </c>
@@ -5656,7 +5696,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="15.75" customHeight="1">
+    <row r="60" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>44518.545351886569</v>
       </c>
@@ -5694,7 +5734,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="15.75" customHeight="1">
+    <row r="61" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>44518.57691783565</v>
       </c>
@@ -5732,7 +5772,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="15.75" customHeight="1">
+    <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>44518.580951863427</v>
       </c>
@@ -5770,7 +5810,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="15.75" customHeight="1">
+    <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>44518.584114340279</v>
       </c>
@@ -5808,7 +5848,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="15.75" customHeight="1">
+    <row r="64" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>44518.599512685185</v>
       </c>
@@ -5846,7 +5886,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="15.75" customHeight="1">
+    <row r="65" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>44518.611133506944</v>
       </c>
@@ -5884,7 +5924,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="15.75" customHeight="1">
+    <row r="66" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>44518.639018194444</v>
       </c>
@@ -5922,7 +5962,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="15.75" customHeight="1">
+    <row r="67" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>44518.65679601852</v>
       </c>
@@ -5960,7 +6000,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="15.75" customHeight="1">
+    <row r="68" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>44518.669622650465</v>
       </c>
@@ -5998,7 +6038,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="15.75" customHeight="1">
+    <row r="69" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>44518.675713946759</v>
       </c>
@@ -6036,7 +6076,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="15.75" customHeight="1">
+    <row r="70" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>44518.678410173612</v>
       </c>
@@ -6074,7 +6114,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="15.75" customHeight="1">
+    <row r="71" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>44518.67904717593</v>
       </c>
@@ -6112,7 +6152,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="15.75" customHeight="1">
+    <row r="72" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>44518.681073298612</v>
       </c>
@@ -6150,7 +6190,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="15.75" customHeight="1">
+    <row r="73" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>44518.681981574075</v>
       </c>
@@ -6188,7 +6228,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="15.75" customHeight="1">
+    <row r="74" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>44518.682995844909</v>
       </c>
@@ -6226,7 +6266,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="15.75" customHeight="1">
+    <row r="75" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>44518.68484347222</v>
       </c>
@@ -6264,7 +6304,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="15.75" customHeight="1">
+    <row r="76" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>44518.690567743055</v>
       </c>
@@ -6302,7 +6342,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="15.75" customHeight="1">
+    <row r="77" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>44518.704118368056</v>
       </c>
@@ -6340,7 +6380,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="15.75" customHeight="1">
+    <row r="78" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>44518.717275173607</v>
       </c>
@@ -6378,7 +6418,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="15.75" customHeight="1">
+    <row r="79" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>44518.718211203704</v>
       </c>
@@ -6416,7 +6456,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="80" spans="1:12" ht="15.75" customHeight="1">
+    <row r="80" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>44518.721890682871</v>
       </c>
@@ -6454,7 +6494,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="81" spans="1:12" ht="15.75" customHeight="1">
+    <row r="81" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>44518.845550972226</v>
       </c>
@@ -6492,7 +6532,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="82" spans="1:12" ht="15.75" customHeight="1">
+    <row r="82" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>44518.845807673613</v>
       </c>
@@ -6530,7 +6570,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="83" spans="1:12" ht="15.75" customHeight="1">
+    <row r="83" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>44518.847130671296</v>
       </c>
@@ -6568,7 +6608,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="84" spans="1:12" ht="15.75" customHeight="1">
+    <row r="84" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>44518.848048738422</v>
       </c>
@@ -6606,7 +6646,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="85" spans="1:12" ht="15.75" customHeight="1">
+    <row r="85" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>44518.848206620372</v>
       </c>
@@ -6644,7 +6684,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="86" spans="1:12" ht="15.75" customHeight="1">
+    <row r="86" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>44518.851609803241</v>
       </c>
@@ -6682,7 +6722,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="87" spans="1:12" ht="15.75" customHeight="1">
+    <row r="87" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>44518.853343229166</v>
       </c>
@@ -6720,7 +6760,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="88" spans="1:12" ht="15.75" customHeight="1">
+    <row r="88" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>44518.854456469911</v>
       </c>
@@ -6758,7 +6798,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="89" spans="1:12" ht="15.75" customHeight="1">
+    <row r="89" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>44518.857002847217</v>
       </c>
@@ -6796,7 +6836,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="90" spans="1:12" ht="15.75" customHeight="1">
+    <row r="90" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>44518.857458969913</v>
       </c>
@@ -6834,7 +6874,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="91" spans="1:12" ht="15.75" customHeight="1">
+    <row r="91" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>44518.864664201392</v>
       </c>
@@ -6872,7 +6912,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="92" spans="1:12" ht="15.75" customHeight="1">
+    <row r="92" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>44518.865544432869</v>
       </c>
@@ -6910,7 +6950,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="93" spans="1:12" ht="15.75" customHeight="1">
+    <row r="93" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>44518.873488796293</v>
       </c>
@@ -6948,7 +6988,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="94" spans="1:12" ht="15.75" customHeight="1">
+    <row r="94" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>44518.880978576388</v>
       </c>
@@ -6986,7 +7026,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="95" spans="1:12" ht="15.75" customHeight="1">
+    <row r="95" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>44518.890144791665</v>
       </c>
@@ -7024,7 +7064,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="96" spans="1:12" ht="15.75" customHeight="1">
+    <row r="96" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>44518.892673622686</v>
       </c>
@@ -7062,7 +7102,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="97" spans="1:12" ht="15.75" customHeight="1">
+    <row r="97" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>44518.893882627315</v>
       </c>
@@ -7100,7 +7140,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="98" spans="1:12" ht="15.75" customHeight="1">
+    <row r="98" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>44518.895629976847</v>
       </c>
@@ -7138,7 +7178,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="99" spans="1:12" ht="15.75" customHeight="1">
+    <row r="99" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <v>44518.897268032408</v>
       </c>
@@ -7176,7 +7216,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="100" spans="1:12" ht="15.75" customHeight="1">
+    <row r="100" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>44518.901678900467</v>
       </c>
@@ -7214,7 +7254,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="101" spans="1:12" ht="15.75" customHeight="1">
+    <row r="101" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
         <v>44518.905369791668</v>
       </c>
@@ -7252,7 +7292,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="102" spans="1:12" ht="15.75" customHeight="1">
+    <row r="102" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>44518.914951886574</v>
       </c>
@@ -7290,7 +7330,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="103" spans="1:12" ht="15.75" customHeight="1">
+    <row r="103" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>44518.926460324074</v>
       </c>
@@ -7325,7 +7365,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="104" spans="1:12" ht="15.75" customHeight="1">
+    <row r="104" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>44518.943910335649</v>
       </c>
@@ -7360,7 +7400,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="105" spans="1:12" ht="15.75" customHeight="1">
+    <row r="105" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
         <v>44518.94905171296</v>
       </c>
@@ -7398,7 +7438,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="106" spans="1:12" ht="15.75" customHeight="1">
+    <row r="106" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
         <v>44518.949835740743</v>
       </c>
@@ -7436,7 +7476,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="107" spans="1:12" ht="15.75" customHeight="1">
+    <row r="107" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
         <v>44518.954430393518</v>
       </c>
@@ -7474,7 +7514,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="108" spans="1:12" ht="15.75" customHeight="1">
+    <row r="108" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <v>44518.964523217597</v>
       </c>
@@ -7512,7 +7552,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="109" spans="1:12" ht="15.75" customHeight="1">
+    <row r="109" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
         <v>44518.971188981479</v>
       </c>
@@ -7550,7 +7590,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="110" spans="1:12" ht="15.75" customHeight="1">
+    <row r="110" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
         <v>44518.972234583329</v>
       </c>
@@ -7588,7 +7628,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="111" spans="1:12" ht="15.75" customHeight="1">
+    <row r="111" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
         <v>44518.972730138892</v>
       </c>
@@ -7626,7 +7666,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="112" spans="1:12" ht="15.75" customHeight="1">
+    <row r="112" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
         <v>44518.977785532406</v>
       </c>
@@ -7664,7 +7704,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="113" spans="1:18" ht="15.75" customHeight="1">
+    <row r="113" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="6">
         <v>44519.003693425926</v>
       </c>
@@ -7706,7 +7746,7 @@
       <c r="Q113" s="9"/>
       <c r="R113" s="9"/>
     </row>
-    <row r="114" spans="1:18" ht="15.75" customHeight="1">
+    <row r="114" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
         <v>44521.695289421295</v>
       </c>
@@ -7744,7 +7784,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="115" spans="1:18" ht="15.75" customHeight="1">
+    <row r="115" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
         <v>44521.703645162037</v>
       </c>
@@ -7782,7 +7822,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="116" spans="1:18" ht="15.75" customHeight="1">
+    <row r="116" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
         <v>44521.798439618055</v>
       </c>
@@ -7820,7 +7860,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="117" spans="1:18" ht="15.75" customHeight="1">
+    <row r="117" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
         <v>44521.806830486108</v>
       </c>
@@ -7858,7 +7898,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="118" spans="1:18" ht="15.75" customHeight="1">
+    <row r="118" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
         <v>44521.997838750001</v>
       </c>
@@ -7896,7 +7936,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="119" spans="1:18" ht="15.75" customHeight="1">
+    <row r="119" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
         <v>44522.038008958334</v>
       </c>
@@ -7934,7 +7974,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="120" spans="1:18" ht="15.75" customHeight="1">
+    <row r="120" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
         <v>44522.396687349537</v>
       </c>
@@ -7972,7 +8012,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="121" spans="1:18" ht="15.75" customHeight="1">
+    <row r="121" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
         <v>44522.424870671297</v>
       </c>
@@ -8010,7 +8050,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="122" spans="1:18" ht="15.75" customHeight="1">
+    <row r="122" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
         <v>44522.601772291666</v>
       </c>
@@ -8046,6 +8086,47 @@
       </c>
       <c r="L122" s="5" t="s">
         <v>849</v>
+      </c>
+    </row>
+    <row r="123" spans="1:18" s="18" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="124" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K124" s="19" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="125" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K125" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="126" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K126" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="127" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K127" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="128" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K128" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="129" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K129" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="130" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K130" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="131" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K131" t="s">
+        <v>875</v>
       </c>
     </row>
   </sheetData>
@@ -8173,7 +8254,7 @@
     <hyperlink ref="L122" r:id="rId121"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId122"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -8184,7 +8265,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -8195,22 +8276,22 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="25.5" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="33.1640625" customWidth="1"/>
-    <col min="8" max="8" width="9.5" customWidth="1"/>
-    <col min="9" max="9" width="17.5" customWidth="1"/>
-    <col min="10" max="10" width="33.1640625" customWidth="1"/>
-    <col min="11" max="16" width="21.5" customWidth="1"/>
+    <col min="7" max="7" width="33.140625" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="10" max="10" width="33.140625" customWidth="1"/>
+    <col min="11" max="16" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="39.75" customHeight="1">
+    <row r="1" spans="1:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>850</v>
       </c>
@@ -8248,7 +8329,7 @@
       <c r="O1" s="12"/>
       <c r="P1" s="12"/>
     </row>
-    <row r="2" spans="1:16" ht="12">
+    <row r="2" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -8280,7 +8361,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="12">
+    <row r="3" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -8312,7 +8393,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="12">
+    <row r="4" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -8344,7 +8425,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="12">
+    <row r="5" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -8376,7 +8457,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="12">
+    <row r="6" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -8408,7 +8489,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="12">
+    <row r="7" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -8440,7 +8521,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="12">
+    <row r="8" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -8472,7 +8553,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="12">
+    <row r="9" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -8504,7 +8585,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="12">
+    <row r="10" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -8536,7 +8617,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="12">
+    <row r="11" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -8568,7 +8649,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="12">
+    <row r="12" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -8600,7 +8681,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="12">
+    <row r="13" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -8632,7 +8713,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="12">
+    <row r="14" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -8664,7 +8745,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="12">
+    <row r="15" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -8696,7 +8777,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="12">
+    <row r="16" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -8728,7 +8809,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="12">
+    <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -8760,7 +8841,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="12">
+    <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -8792,7 +8873,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="36">
+    <row r="19" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -8824,7 +8905,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="12">
+    <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -8856,7 +8937,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="12">
+    <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -8888,7 +8969,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="12">
+    <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -8920,7 +9001,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="12">
+    <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -8952,7 +9033,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="12">
+    <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -8984,7 +9065,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="12">
+    <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -9016,7 +9097,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="12">
+    <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -9048,7 +9129,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="12">
+    <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -9080,7 +9161,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="12">
+    <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -9112,7 +9193,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="12">
+    <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -9144,7 +9225,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="12">
+    <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -9176,7 +9257,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="12">
+    <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -9208,7 +9289,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="12">
+    <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -9240,7 +9321,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="12">
+    <row r="33" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -9272,7 +9353,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="12">
+    <row r="34" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -9304,7 +9385,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="12">
+    <row r="35" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -9336,7 +9417,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="12">
+    <row r="36" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -9368,7 +9449,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="12">
+    <row r="37" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -9400,7 +9481,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="12">
+    <row r="38" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -9432,7 +9513,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="12">
+    <row r="39" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -9464,7 +9545,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="12">
+    <row r="40" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -9496,7 +9577,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="12">
+    <row r="41" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -9528,7 +9609,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="12">
+    <row r="42" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -9560,7 +9641,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="12">
+    <row r="43" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -9592,7 +9673,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="12">
+    <row r="44" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -9624,7 +9705,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="12">
+    <row r="45" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -9656,7 +9737,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="12">
+    <row r="46" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -9688,7 +9769,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="12">
+    <row r="47" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -9720,7 +9801,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="12">
+    <row r="48" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -9752,7 +9833,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="12">
+    <row r="49" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -9784,7 +9865,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="12">
+    <row r="50" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -9816,7 +9897,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="12">
+    <row r="51" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -9848,7 +9929,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="12">
+    <row r="52" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -9880,7 +9961,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="12">
+    <row r="53" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -9912,7 +9993,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="12">
+    <row r="54" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -9944,7 +10025,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="12">
+    <row r="55" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -9976,7 +10057,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="12">
+    <row r="56" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -10008,7 +10089,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="12">
+    <row r="57" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -10040,7 +10121,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="12">
+    <row r="58" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -10072,7 +10153,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="12">
+    <row r="59" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -10104,7 +10185,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="12">
+    <row r="60" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -10136,7 +10217,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="12">
+    <row r="61" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -10168,7 +10249,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="12">
+    <row r="62" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -10200,7 +10281,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="12">
+    <row r="63" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -10232,7 +10313,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="12">
+    <row r="64" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -10264,7 +10345,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="12">
+    <row r="65" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -10296,7 +10377,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="12">
+    <row r="66" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -10328,7 +10409,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="12">
+    <row r="67" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -10360,7 +10441,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="12">
+    <row r="68" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -10392,7 +10473,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="12">
+    <row r="69" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -10424,7 +10505,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="12">
+    <row r="70" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -10456,7 +10537,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="12">
+    <row r="71" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -10488,7 +10569,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="12">
+    <row r="72" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -10520,7 +10601,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="12">
+    <row r="73" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -10552,7 +10633,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="24">
+    <row r="74" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -10584,7 +10665,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="12">
+    <row r="75" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -10616,7 +10697,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="12">
+    <row r="76" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -10648,7 +10729,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="12">
+    <row r="77" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -10680,7 +10761,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="12">
+    <row r="78" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -10712,7 +10793,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="12">
+    <row r="79" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -10744,7 +10825,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="12">
+    <row r="80" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -10776,7 +10857,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="12">
+    <row r="81" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -10808,7 +10889,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="12">
+    <row r="82" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -10840,7 +10921,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="12">
+    <row r="83" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -10872,7 +10953,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="12">
+    <row r="84" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="3">
         <v>83</v>
       </c>
@@ -10904,7 +10985,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="12">
+    <row r="85" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
         <v>84</v>
       </c>
@@ -10936,7 +11017,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="12">
+    <row r="86" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A86" s="3">
         <v>85</v>
       </c>
@@ -10968,7 +11049,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="12">
+    <row r="87" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>86</v>
       </c>
@@ -11000,7 +11081,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="12">
+    <row r="88" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="3">
         <v>87</v>
       </c>
@@ -11032,7 +11113,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="12">
+    <row r="89" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
         <v>88</v>
       </c>
@@ -11064,7 +11145,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="12">
+    <row r="90" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="3">
         <v>89</v>
       </c>
@@ -11096,7 +11177,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="12">
+    <row r="91" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="3">
         <v>90</v>
       </c>
@@ -11128,7 +11209,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="12">
+    <row r="92" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="3">
         <v>91</v>
       </c>
@@ -11160,7 +11241,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="12">
+    <row r="93" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="3">
         <v>92</v>
       </c>
@@ -11192,7 +11273,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="12">
+    <row r="94" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="3">
         <v>93</v>
       </c>
@@ -11224,7 +11305,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="95" spans="1:10" ht="12">
+    <row r="95" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="3">
         <v>94</v>
       </c>
@@ -11256,7 +11337,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="96" spans="1:10" ht="12">
+    <row r="96" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="3">
         <v>95</v>
       </c>
@@ -11288,7 +11369,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="12">
+    <row r="97" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="3">
         <v>96</v>
       </c>
@@ -11320,7 +11401,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="12">
+    <row r="98" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" s="3">
         <v>97</v>
       </c>
@@ -11352,7 +11433,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="99" spans="1:10" ht="12">
+    <row r="99" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="3">
         <v>98</v>
       </c>
@@ -11384,7 +11465,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="12">
+    <row r="100" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A100" s="3">
         <v>99</v>
       </c>
@@ -11416,7 +11497,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="12">
+    <row r="101" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A101" s="3">
         <v>100</v>
       </c>
@@ -11448,7 +11529,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="12">
+    <row r="102" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" s="3">
         <v>101</v>
       </c>
@@ -11477,7 +11558,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="103" spans="1:10" ht="12">
+    <row r="103" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A103" s="3">
         <v>102</v>
       </c>
@@ -11506,7 +11587,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="104" spans="1:10" ht="12">
+    <row r="104" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A104" s="3">
         <v>103</v>
       </c>
@@ -11538,7 +11619,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="105" spans="1:10" ht="12">
+    <row r="105" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A105" s="3">
         <v>104</v>
       </c>
@@ -11570,7 +11651,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="106" spans="1:10" ht="12">
+    <row r="106" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A106" s="3">
         <v>105</v>
       </c>
@@ -11602,7 +11683,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="12">
+    <row r="107" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A107" s="3">
         <v>106</v>
       </c>
@@ -11634,7 +11715,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="108" spans="1:10" ht="12">
+    <row r="108" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A108" s="3">
         <v>107</v>
       </c>
@@ -11666,7 +11747,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="109" spans="1:10" ht="12">
+    <row r="109" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A109" s="3">
         <v>108</v>
       </c>
@@ -11698,7 +11779,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="110" spans="1:10" ht="12">
+    <row r="110" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A110" s="3">
         <v>109</v>
       </c>
@@ -11730,7 +11811,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="111" spans="1:10" ht="12">
+    <row r="111" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A111" s="3">
         <v>110</v>
       </c>
@@ -11762,7 +11843,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="12">
+    <row r="112" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A112" s="3">
         <v>111</v>
       </c>
@@ -11791,7 +11872,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="113" spans="1:10" ht="12">
+    <row r="113" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A113" s="3">
         <v>112</v>
       </c>
@@ -11823,7 +11904,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="114" spans="1:10" ht="12">
+    <row r="114" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A114" s="3">
         <v>113</v>
       </c>
@@ -11855,298 +11936,298 @@
         <v>872</v>
       </c>
     </row>
-    <row r="115" spans="1:10" ht="12">
+    <row r="115" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J115" s="15"/>
     </row>
-    <row r="116" spans="1:10" ht="12">
+    <row r="116" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J116" s="15"/>
     </row>
-    <row r="117" spans="1:10" ht="12">
+    <row r="117" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J117" s="15"/>
     </row>
-    <row r="118" spans="1:10" ht="12">
+    <row r="118" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J118" s="15"/>
     </row>
-    <row r="119" spans="1:10" ht="12">
+    <row r="119" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J119" s="15"/>
     </row>
-    <row r="120" spans="1:10" ht="12">
+    <row r="120" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J120" s="15"/>
     </row>
-    <row r="121" spans="1:10" ht="12">
+    <row r="121" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J121" s="15"/>
     </row>
-    <row r="122" spans="1:10" ht="12">
+    <row r="122" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J122" s="15"/>
     </row>
-    <row r="123" spans="1:10" ht="12">
+    <row r="123" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J123" s="15"/>
     </row>
-    <row r="124" spans="1:10" ht="12">
+    <row r="124" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J124" s="15"/>
     </row>
-    <row r="125" spans="1:10" ht="12">
+    <row r="125" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J125" s="15"/>
     </row>
-    <row r="126" spans="1:10" ht="12">
+    <row r="126" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J126" s="15"/>
     </row>
-    <row r="127" spans="1:10" ht="12">
+    <row r="127" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J127" s="15"/>
     </row>
-    <row r="128" spans="1:10" ht="12">
+    <row r="128" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J128" s="15"/>
     </row>
-    <row r="129" spans="10:10" ht="12">
+    <row r="129" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J129" s="15"/>
     </row>
-    <row r="130" spans="10:10" ht="12">
+    <row r="130" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J130" s="15"/>
     </row>
-    <row r="131" spans="10:10" ht="12">
+    <row r="131" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J131" s="15"/>
     </row>
-    <row r="132" spans="10:10" ht="12">
+    <row r="132" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J132" s="15"/>
     </row>
-    <row r="133" spans="10:10" ht="12">
+    <row r="133" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J133" s="15"/>
     </row>
-    <row r="134" spans="10:10" ht="12">
+    <row r="134" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J134" s="15"/>
     </row>
-    <row r="135" spans="10:10" ht="12">
+    <row r="135" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J135" s="15"/>
     </row>
-    <row r="136" spans="10:10" ht="12">
+    <row r="136" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J136" s="15"/>
     </row>
-    <row r="137" spans="10:10" ht="12">
+    <row r="137" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J137" s="15"/>
     </row>
-    <row r="138" spans="10:10" ht="12">
+    <row r="138" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J138" s="15"/>
     </row>
-    <row r="139" spans="10:10" ht="12">
+    <row r="139" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J139" s="15"/>
     </row>
-    <row r="140" spans="10:10" ht="12">
+    <row r="140" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J140" s="15"/>
     </row>
-    <row r="141" spans="10:10" ht="12">
+    <row r="141" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J141" s="15"/>
     </row>
-    <row r="142" spans="10:10" ht="12">
+    <row r="142" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J142" s="15"/>
     </row>
-    <row r="143" spans="10:10" ht="12">
+    <row r="143" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J143" s="15"/>
     </row>
-    <row r="144" spans="10:10" ht="12">
+    <row r="144" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J144" s="15"/>
     </row>
-    <row r="145" spans="10:10" ht="12">
+    <row r="145" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J145" s="15"/>
     </row>
-    <row r="146" spans="10:10" ht="12">
+    <row r="146" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J146" s="15"/>
     </row>
-    <row r="147" spans="10:10" ht="12">
+    <row r="147" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J147" s="15"/>
     </row>
-    <row r="148" spans="10:10" ht="12">
+    <row r="148" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J148" s="15"/>
     </row>
-    <row r="149" spans="10:10" ht="12">
+    <row r="149" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J149" s="15"/>
     </row>
-    <row r="150" spans="10:10" ht="12">
+    <row r="150" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J150" s="15"/>
     </row>
-    <row r="151" spans="10:10" ht="12">
+    <row r="151" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J151" s="15"/>
     </row>
-    <row r="152" spans="10:10" ht="12">
+    <row r="152" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J152" s="15"/>
     </row>
-    <row r="153" spans="10:10" ht="12">
+    <row r="153" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J153" s="15"/>
     </row>
-    <row r="154" spans="10:10" ht="12">
+    <row r="154" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J154" s="15"/>
     </row>
-    <row r="155" spans="10:10" ht="12">
+    <row r="155" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J155" s="15"/>
     </row>
-    <row r="156" spans="10:10" ht="12">
+    <row r="156" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J156" s="15"/>
     </row>
-    <row r="157" spans="10:10" ht="12">
+    <row r="157" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J157" s="15"/>
     </row>
-    <row r="158" spans="10:10" ht="12">
+    <row r="158" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J158" s="15"/>
     </row>
-    <row r="159" spans="10:10" ht="12">
+    <row r="159" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J159" s="15"/>
     </row>
-    <row r="160" spans="10:10" ht="12">
+    <row r="160" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J160" s="15"/>
     </row>
-    <row r="161" spans="10:10" ht="12">
+    <row r="161" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J161" s="15"/>
     </row>
-    <row r="162" spans="10:10" ht="12">
+    <row r="162" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J162" s="15"/>
     </row>
-    <row r="163" spans="10:10" ht="12">
+    <row r="163" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J163" s="15"/>
     </row>
-    <row r="164" spans="10:10" ht="12">
+    <row r="164" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J164" s="15"/>
     </row>
-    <row r="165" spans="10:10" ht="12">
+    <row r="165" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J165" s="15"/>
     </row>
-    <row r="166" spans="10:10" ht="12">
+    <row r="166" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J166" s="15"/>
     </row>
-    <row r="167" spans="10:10" ht="12">
+    <row r="167" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J167" s="15"/>
     </row>
-    <row r="168" spans="10:10" ht="12">
+    <row r="168" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J168" s="15"/>
     </row>
-    <row r="169" spans="10:10" ht="12">
+    <row r="169" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J169" s="15"/>
     </row>
-    <row r="170" spans="10:10" ht="12">
+    <row r="170" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J170" s="15"/>
     </row>
-    <row r="171" spans="10:10" ht="12">
+    <row r="171" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J171" s="15"/>
     </row>
-    <row r="172" spans="10:10" ht="12">
+    <row r="172" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J172" s="15"/>
     </row>
-    <row r="173" spans="10:10" ht="12">
+    <row r="173" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J173" s="15"/>
     </row>
-    <row r="174" spans="10:10" ht="12">
+    <row r="174" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J174" s="15"/>
     </row>
-    <row r="175" spans="10:10" ht="12">
+    <row r="175" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J175" s="15"/>
     </row>
-    <row r="176" spans="10:10" ht="12">
+    <row r="176" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J176" s="15"/>
     </row>
-    <row r="177" spans="10:10" ht="12">
+    <row r="177" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J177" s="15"/>
     </row>
-    <row r="178" spans="10:10" ht="12">
+    <row r="178" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J178" s="15"/>
     </row>
-    <row r="179" spans="10:10" ht="12">
+    <row r="179" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J179" s="15"/>
     </row>
-    <row r="180" spans="10:10" ht="12">
+    <row r="180" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J180" s="15"/>
     </row>
-    <row r="181" spans="10:10" ht="12">
+    <row r="181" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J181" s="15"/>
     </row>
-    <row r="182" spans="10:10" ht="12">
+    <row r="182" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J182" s="15"/>
     </row>
-    <row r="183" spans="10:10" ht="12">
+    <row r="183" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J183" s="15"/>
     </row>
-    <row r="184" spans="10:10" ht="12">
+    <row r="184" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J184" s="15"/>
     </row>
-    <row r="185" spans="10:10" ht="12">
+    <row r="185" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J185" s="15"/>
     </row>
-    <row r="186" spans="10:10" ht="12">
+    <row r="186" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J186" s="15"/>
     </row>
-    <row r="187" spans="10:10" ht="12">
+    <row r="187" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J187" s="15"/>
     </row>
-    <row r="188" spans="10:10" ht="12">
+    <row r="188" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J188" s="15"/>
     </row>
-    <row r="189" spans="10:10" ht="12">
+    <row r="189" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J189" s="15"/>
     </row>
-    <row r="190" spans="10:10" ht="12">
+    <row r="190" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J190" s="15"/>
     </row>
-    <row r="191" spans="10:10" ht="12">
+    <row r="191" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J191" s="15"/>
     </row>
-    <row r="192" spans="10:10" ht="12">
+    <row r="192" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J192" s="15"/>
     </row>
-    <row r="193" spans="10:10" ht="12">
+    <row r="193" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J193" s="15"/>
     </row>
-    <row r="194" spans="10:10" ht="12">
+    <row r="194" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J194" s="15"/>
     </row>
-    <row r="195" spans="10:10" ht="12">
+    <row r="195" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J195" s="15"/>
     </row>
-    <row r="196" spans="10:10" ht="12">
+    <row r="196" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J196" s="15"/>
     </row>
-    <row r="197" spans="10:10" ht="12">
+    <row r="197" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J197" s="15"/>
     </row>
-    <row r="198" spans="10:10" ht="12">
+    <row r="198" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J198" s="15"/>
     </row>
-    <row r="199" spans="10:10" ht="12">
+    <row r="199" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J199" s="15"/>
     </row>
-    <row r="200" spans="10:10" ht="12">
+    <row r="200" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J200" s="15"/>
     </row>
-    <row r="201" spans="10:10" ht="12">
+    <row r="201" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J201" s="15"/>
     </row>
-    <row r="202" spans="10:10" ht="12">
+    <row r="202" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J202" s="15"/>
     </row>
-    <row r="203" spans="10:10" ht="12">
+    <row r="203" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J203" s="15"/>
     </row>
-    <row r="204" spans="10:10" ht="12">
+    <row r="204" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J204" s="15"/>
     </row>
-    <row r="205" spans="10:10" ht="12">
+    <row r="205" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J205" s="15"/>
     </row>
-    <row r="206" spans="10:10" ht="12">
+    <row r="206" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J206" s="15"/>
     </row>
-    <row r="207" spans="10:10" ht="12">
+    <row r="207" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J207" s="15"/>
     </row>
-    <row r="208" spans="10:10" ht="12">
+    <row r="208" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J208" s="15"/>
     </row>
-    <row r="209" spans="10:10" ht="12">
+    <row r="209" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J209" s="15"/>
     </row>
-    <row r="210" spans="10:10" ht="12">
+    <row r="210" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J210" s="15"/>
     </row>
-    <row r="211" spans="10:10" ht="12">
+    <row r="211" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J211" s="15"/>
     </row>
-    <row r="212" spans="10:10" ht="12">
+    <row r="212" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J212" s="15"/>
     </row>
   </sheetData>
@@ -12283,7 +12364,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -12294,22 +12375,22 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="25.5" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="33.1640625" customWidth="1"/>
-    <col min="8" max="8" width="9.5" customWidth="1"/>
-    <col min="9" max="9" width="17.5" customWidth="1"/>
-    <col min="10" max="10" width="33.1640625" customWidth="1"/>
-    <col min="11" max="16" width="21.5" customWidth="1"/>
+    <col min="7" max="7" width="33.140625" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="10" max="10" width="33.140625" customWidth="1"/>
+    <col min="11" max="16" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="39.75" customHeight="1">
+    <row r="1" spans="1:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>850</v>
       </c>
@@ -12347,7 +12428,7 @@
       <c r="O1" s="12"/>
       <c r="P1" s="12"/>
     </row>
-    <row r="2" spans="1:16" ht="12">
+    <row r="2" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -12379,7 +12460,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="12">
+    <row r="3" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -12411,7 +12492,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="12">
+    <row r="4" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -12443,7 +12524,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="12">
+    <row r="5" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -12475,7 +12556,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="12">
+    <row r="6" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -12507,7 +12588,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="12">
+    <row r="7" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -12539,7 +12620,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="12">
+    <row r="8" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -12571,7 +12652,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="12">
+    <row r="9" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -12603,7 +12684,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="12">
+    <row r="10" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -12635,7 +12716,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="12">
+    <row r="11" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -12667,7 +12748,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="12">
+    <row r="12" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -12699,7 +12780,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="12">
+    <row r="13" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -12731,7 +12812,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="12">
+    <row r="14" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -12763,7 +12844,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="12">
+    <row r="15" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -12795,7 +12876,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="12">
+    <row r="16" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -12827,7 +12908,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="12">
+    <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -12859,7 +12940,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="36">
+    <row r="18" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -12891,7 +12972,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="12">
+    <row r="19" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -12923,7 +13004,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="12">
+    <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -12955,7 +13036,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="12">
+    <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -12987,7 +13068,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="12">
+    <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -13019,7 +13100,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="12">
+    <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -13051,7 +13132,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="12">
+    <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -13083,7 +13164,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="12">
+    <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -13115,7 +13196,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="12">
+    <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -13147,7 +13228,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="12">
+    <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -13179,7 +13260,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="12">
+    <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -13211,7 +13292,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="12">
+    <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -13243,7 +13324,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="12">
+    <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -13275,7 +13356,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="12">
+    <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -13307,7 +13388,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="12">
+    <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -13339,7 +13420,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="12">
+    <row r="33" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -13371,7 +13452,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="12">
+    <row r="34" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -13403,7 +13484,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="12">
+    <row r="35" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -13435,7 +13516,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="12">
+    <row r="36" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -13467,7 +13548,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="12">
+    <row r="37" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -13499,7 +13580,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="12">
+    <row r="38" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -13531,7 +13612,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="12">
+    <row r="39" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -13563,7 +13644,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="12">
+    <row r="40" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -13595,7 +13676,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="12">
+    <row r="41" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -13627,7 +13708,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="12">
+    <row r="42" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -13659,7 +13740,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="12">
+    <row r="43" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -13691,7 +13772,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="12">
+    <row r="44" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -13723,7 +13804,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="12">
+    <row r="45" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -13755,7 +13836,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="12">
+    <row r="46" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -13787,7 +13868,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="12">
+    <row r="47" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -13819,7 +13900,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="12">
+    <row r="48" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -13851,7 +13932,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="12">
+    <row r="49" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -13883,7 +13964,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="12">
+    <row r="50" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -13915,7 +13996,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="12">
+    <row r="51" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -13947,7 +14028,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="12">
+    <row r="52" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -13979,7 +14060,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="12">
+    <row r="53" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -14011,7 +14092,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="12">
+    <row r="54" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -14043,7 +14124,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="12">
+    <row r="55" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -14075,7 +14156,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="12">
+    <row r="56" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -14107,7 +14188,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="12">
+    <row r="57" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -14139,7 +14220,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="12">
+    <row r="58" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -14171,7 +14252,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="12">
+    <row r="59" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -14203,7 +14284,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="12">
+    <row r="60" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -14235,7 +14316,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="12">
+    <row r="61" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -14267,7 +14348,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="12">
+    <row r="62" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -14299,7 +14380,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="12">
+    <row r="63" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -14331,7 +14412,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="24">
+    <row r="64" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -14363,7 +14444,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="12">
+    <row r="65" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -14395,7 +14476,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="12">
+    <row r="66" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -14427,7 +14508,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="12">
+    <row r="67" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -14459,7 +14540,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="12">
+    <row r="68" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -14491,7 +14572,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="12">
+    <row r="69" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -14523,7 +14604,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="12">
+    <row r="70" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -14555,7 +14636,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="12">
+    <row r="71" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -14587,7 +14668,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="12">
+    <row r="72" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -14619,7 +14700,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="12">
+    <row r="73" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -14651,7 +14732,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="12">
+    <row r="74" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -14683,7 +14764,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="12">
+    <row r="75" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -14715,7 +14796,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="12">
+    <row r="76" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -14747,7 +14828,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="12">
+    <row r="77" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -14779,7 +14860,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="12">
+    <row r="78" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -14811,7 +14892,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="12">
+    <row r="79" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -14843,7 +14924,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="12">
+    <row r="80" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -14875,7 +14956,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="12">
+    <row r="81" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -14907,7 +14988,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="12">
+    <row r="82" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -14939,7 +15020,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="12">
+    <row r="83" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -14971,7 +15052,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="12">
+    <row r="84" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="3">
         <v>83</v>
       </c>
@@ -15003,7 +15084,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="12">
+    <row r="85" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
         <v>84</v>
       </c>
@@ -15035,7 +15116,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="12">
+    <row r="86" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="3">
         <v>85</v>
       </c>
@@ -15067,7 +15148,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="12">
+    <row r="87" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>86</v>
       </c>
@@ -15099,7 +15180,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="12">
+    <row r="88" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="3">
         <v>87</v>
       </c>
@@ -15128,7 +15209,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="12">
+    <row r="89" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
         <v>88</v>
       </c>
@@ -15157,7 +15238,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="12">
+    <row r="90" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="3">
         <v>89</v>
       </c>
@@ -15189,7 +15270,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="12">
+    <row r="91" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="3">
         <v>90</v>
       </c>
@@ -15221,7 +15302,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="12">
+    <row r="92" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="3">
         <v>91</v>
       </c>
@@ -15253,7 +15334,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="12">
+    <row r="93" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="3">
         <v>92</v>
       </c>
@@ -15285,7 +15366,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="12">
+    <row r="94" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="3">
         <v>93</v>
       </c>
@@ -15317,7 +15398,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="95" spans="1:10" ht="12">
+    <row r="95" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="3">
         <v>94</v>
       </c>
@@ -15349,7 +15430,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="96" spans="1:10" ht="12">
+    <row r="96" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="3">
         <v>95</v>
       </c>
@@ -15381,7 +15462,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="12">
+    <row r="97" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="3">
         <v>96</v>
       </c>
@@ -15413,7 +15494,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="12">
+    <row r="98" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" s="3">
         <v>97</v>
       </c>
@@ -15442,7 +15523,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="99" spans="1:10" ht="12">
+    <row r="99" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="3">
         <v>98</v>
       </c>
@@ -15474,7 +15555,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="12">
+    <row r="100" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A100" s="3">
         <v>99</v>
       </c>
@@ -15506,7 +15587,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="12">
+    <row r="101" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A101" s="3">
         <v>100</v>
       </c>
@@ -15538,7 +15619,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="12">
+    <row r="102" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" s="3">
         <v>101</v>
       </c>
@@ -15570,7 +15651,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="103" spans="1:10" ht="12">
+    <row r="103" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A103" s="3">
         <v>102</v>
       </c>
@@ -15602,7 +15683,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="104" spans="1:10" ht="12">
+    <row r="104" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A104" s="3">
         <v>103</v>
       </c>
@@ -15634,7 +15715,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="105" spans="1:10" ht="12">
+    <row r="105" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A105" s="3">
         <v>104</v>
       </c>
@@ -15666,7 +15747,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="106" spans="1:10" ht="12">
+    <row r="106" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A106" s="3">
         <v>105</v>
       </c>
@@ -15698,7 +15779,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="12">
+    <row r="107" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A107" s="3">
         <v>106</v>
       </c>
@@ -15730,7 +15811,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="108" spans="1:10" ht="12">
+    <row r="108" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A108" s="3">
         <v>107</v>
       </c>
@@ -15762,7 +15843,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="109" spans="1:10" ht="12">
+    <row r="109" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A109" s="3">
         <v>108</v>
       </c>
@@ -15794,271 +15875,271 @@
         <v>849</v>
       </c>
     </row>
-    <row r="110" spans="1:10" ht="12">
+    <row r="110" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J110" s="15"/>
     </row>
-    <row r="111" spans="1:10" ht="12">
+    <row r="111" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J111" s="15"/>
     </row>
-    <row r="112" spans="1:10" ht="12">
+    <row r="112" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J112" s="15"/>
     </row>
-    <row r="113" spans="10:10" ht="12">
+    <row r="113" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J113" s="15"/>
     </row>
-    <row r="114" spans="10:10" ht="12">
+    <row r="114" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J114" s="15"/>
     </row>
-    <row r="115" spans="10:10" ht="12">
+    <row r="115" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J115" s="15"/>
     </row>
-    <row r="116" spans="10:10" ht="12">
+    <row r="116" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J116" s="15"/>
     </row>
-    <row r="117" spans="10:10" ht="12">
+    <row r="117" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J117" s="15"/>
     </row>
-    <row r="118" spans="10:10" ht="12">
+    <row r="118" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J118" s="15"/>
     </row>
-    <row r="119" spans="10:10" ht="12">
+    <row r="119" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J119" s="15"/>
     </row>
-    <row r="120" spans="10:10" ht="12">
+    <row r="120" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J120" s="15"/>
     </row>
-    <row r="121" spans="10:10" ht="12">
+    <row r="121" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J121" s="15"/>
     </row>
-    <row r="122" spans="10:10" ht="12">
+    <row r="122" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J122" s="15"/>
     </row>
-    <row r="123" spans="10:10" ht="12">
+    <row r="123" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J123" s="15"/>
     </row>
-    <row r="124" spans="10:10" ht="12">
+    <row r="124" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J124" s="15"/>
     </row>
-    <row r="125" spans="10:10" ht="12">
+    <row r="125" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J125" s="15"/>
     </row>
-    <row r="126" spans="10:10" ht="12">
+    <row r="126" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J126" s="15"/>
     </row>
-    <row r="127" spans="10:10" ht="12">
+    <row r="127" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J127" s="15"/>
     </row>
-    <row r="128" spans="10:10" ht="12">
+    <row r="128" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J128" s="15"/>
     </row>
-    <row r="129" spans="10:10" ht="12">
+    <row r="129" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J129" s="15"/>
     </row>
-    <row r="130" spans="10:10" ht="12">
+    <row r="130" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J130" s="15"/>
     </row>
-    <row r="131" spans="10:10" ht="12">
+    <row r="131" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J131" s="15"/>
     </row>
-    <row r="132" spans="10:10" ht="12">
+    <row r="132" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J132" s="15"/>
     </row>
-    <row r="133" spans="10:10" ht="12">
+    <row r="133" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J133" s="15"/>
     </row>
-    <row r="134" spans="10:10" ht="12">
+    <row r="134" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J134" s="15"/>
     </row>
-    <row r="135" spans="10:10" ht="12">
+    <row r="135" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J135" s="15"/>
     </row>
-    <row r="136" spans="10:10" ht="12">
+    <row r="136" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J136" s="15"/>
     </row>
-    <row r="137" spans="10:10" ht="12">
+    <row r="137" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J137" s="15"/>
     </row>
-    <row r="138" spans="10:10" ht="12">
+    <row r="138" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J138" s="15"/>
     </row>
-    <row r="139" spans="10:10" ht="12">
+    <row r="139" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J139" s="15"/>
     </row>
-    <row r="140" spans="10:10" ht="12">
+    <row r="140" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J140" s="15"/>
     </row>
-    <row r="141" spans="10:10" ht="12">
+    <row r="141" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J141" s="15"/>
     </row>
-    <row r="142" spans="10:10" ht="12">
+    <row r="142" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J142" s="15"/>
     </row>
-    <row r="143" spans="10:10" ht="12">
+    <row r="143" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J143" s="15"/>
     </row>
-    <row r="144" spans="10:10" ht="12">
+    <row r="144" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J144" s="15"/>
     </row>
-    <row r="145" spans="10:10" ht="12">
+    <row r="145" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J145" s="15"/>
     </row>
-    <row r="146" spans="10:10" ht="12">
+    <row r="146" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J146" s="15"/>
     </row>
-    <row r="147" spans="10:10" ht="12">
+    <row r="147" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J147" s="15"/>
     </row>
-    <row r="148" spans="10:10" ht="12">
+    <row r="148" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J148" s="15"/>
     </row>
-    <row r="149" spans="10:10" ht="12">
+    <row r="149" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J149" s="15"/>
     </row>
-    <row r="150" spans="10:10" ht="12">
+    <row r="150" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J150" s="15"/>
     </row>
-    <row r="151" spans="10:10" ht="12">
+    <row r="151" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J151" s="15"/>
     </row>
-    <row r="152" spans="10:10" ht="12">
+    <row r="152" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J152" s="15"/>
     </row>
-    <row r="153" spans="10:10" ht="12">
+    <row r="153" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J153" s="15"/>
     </row>
-    <row r="154" spans="10:10" ht="12">
+    <row r="154" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J154" s="15"/>
     </row>
-    <row r="155" spans="10:10" ht="12">
+    <row r="155" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J155" s="15"/>
     </row>
-    <row r="156" spans="10:10" ht="12">
+    <row r="156" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J156" s="15"/>
     </row>
-    <row r="157" spans="10:10" ht="12">
+    <row r="157" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J157" s="15"/>
     </row>
-    <row r="158" spans="10:10" ht="12">
+    <row r="158" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J158" s="15"/>
     </row>
-    <row r="159" spans="10:10" ht="12">
+    <row r="159" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J159" s="15"/>
     </row>
-    <row r="160" spans="10:10" ht="12">
+    <row r="160" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J160" s="15"/>
     </row>
-    <row r="161" spans="10:10" ht="12">
+    <row r="161" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J161" s="15"/>
     </row>
-    <row r="162" spans="10:10" ht="12">
+    <row r="162" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J162" s="15"/>
     </row>
-    <row r="163" spans="10:10" ht="12">
+    <row r="163" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J163" s="15"/>
     </row>
-    <row r="164" spans="10:10" ht="12">
+    <row r="164" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J164" s="15"/>
     </row>
-    <row r="165" spans="10:10" ht="12">
+    <row r="165" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J165" s="15"/>
     </row>
-    <row r="166" spans="10:10" ht="12">
+    <row r="166" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J166" s="15"/>
     </row>
-    <row r="167" spans="10:10" ht="12">
+    <row r="167" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J167" s="15"/>
     </row>
-    <row r="168" spans="10:10" ht="12">
+    <row r="168" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J168" s="15"/>
     </row>
-    <row r="169" spans="10:10" ht="12">
+    <row r="169" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J169" s="15"/>
     </row>
-    <row r="170" spans="10:10" ht="12">
+    <row r="170" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J170" s="15"/>
     </row>
-    <row r="171" spans="10:10" ht="12">
+    <row r="171" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J171" s="15"/>
     </row>
-    <row r="172" spans="10:10" ht="12">
+    <row r="172" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J172" s="15"/>
     </row>
-    <row r="173" spans="10:10" ht="12">
+    <row r="173" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J173" s="15"/>
     </row>
-    <row r="174" spans="10:10" ht="12">
+    <row r="174" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J174" s="15"/>
     </row>
-    <row r="175" spans="10:10" ht="12">
+    <row r="175" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J175" s="15"/>
     </row>
-    <row r="176" spans="10:10" ht="12">
+    <row r="176" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J176" s="15"/>
     </row>
-    <row r="177" spans="10:10" ht="12">
+    <row r="177" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J177" s="15"/>
     </row>
-    <row r="178" spans="10:10" ht="12">
+    <row r="178" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J178" s="15"/>
     </row>
-    <row r="179" spans="10:10" ht="12">
+    <row r="179" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J179" s="15"/>
     </row>
-    <row r="180" spans="10:10" ht="12">
+    <row r="180" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J180" s="15"/>
     </row>
-    <row r="181" spans="10:10" ht="12">
+    <row r="181" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J181" s="15"/>
     </row>
-    <row r="182" spans="10:10" ht="12">
+    <row r="182" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J182" s="15"/>
     </row>
-    <row r="183" spans="10:10" ht="12">
+    <row r="183" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J183" s="15"/>
     </row>
-    <row r="184" spans="10:10" ht="12">
+    <row r="184" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J184" s="15"/>
     </row>
-    <row r="185" spans="10:10" ht="12">
+    <row r="185" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J185" s="15"/>
     </row>
-    <row r="186" spans="10:10" ht="12">
+    <row r="186" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J186" s="15"/>
     </row>
-    <row r="187" spans="10:10" ht="12">
+    <row r="187" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J187" s="15"/>
     </row>
-    <row r="188" spans="10:10" ht="12">
+    <row r="188" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J188" s="15"/>
     </row>
-    <row r="189" spans="10:10" ht="12">
+    <row r="189" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J189" s="15"/>
     </row>
-    <row r="190" spans="10:10" ht="12">
+    <row r="190" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J190" s="15"/>
     </row>
-    <row r="191" spans="10:10" ht="12">
+    <row r="191" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J191" s="15"/>
     </row>
-    <row r="192" spans="10:10" ht="12">
+    <row r="192" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J192" s="15"/>
     </row>
-    <row r="193" spans="10:10" ht="12">
+    <row r="193" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J193" s="15"/>
     </row>
-    <row r="194" spans="10:10" ht="12">
+    <row r="194" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J194" s="15"/>
     </row>
-    <row r="195" spans="10:10" ht="12">
+    <row r="195" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J195" s="15"/>
     </row>
-    <row r="196" spans="10:10" ht="12">
+    <row r="196" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J196" s="15"/>
     </row>
-    <row r="197" spans="10:10" ht="12">
+    <row r="197" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J197" s="15"/>
     </row>
-    <row r="198" spans="10:10" ht="12">
+    <row r="198" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J198" s="15"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding my name to the Excel file
</commit_message>
<xml_diff>
--- a/CS335/GitHub Info sans duplicates.xlsx
+++ b/CS335/GitHub Info sans duplicates.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="25605" windowHeight="14340" tabRatio="500"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="25605" windowHeight="14340" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3228" uniqueCount="877">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3237" uniqueCount="884">
   <si>
     <t>Timestamp</t>
   </si>
@@ -2657,6 +2657,27 @@
   </si>
   <si>
     <t>STILL WITHOUT ACCESS</t>
+  </si>
+  <si>
+    <t>2019-04-03618</t>
+  </si>
+  <si>
+    <t>noelikapungu3@gmail.com</t>
+  </si>
+  <si>
+    <t>DePosta20</t>
+  </si>
+  <si>
+    <t>https://github.com/DePosta20</t>
+  </si>
+  <si>
+    <t>KAPUNGU</t>
+  </si>
+  <si>
+    <t>NOEL K</t>
+  </si>
+  <si>
+    <t>0718327770</t>
   </si>
 </sst>
 </file>
@@ -2666,7 +2687,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2720,6 +2741,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -2765,7 +2792,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="205">
+  <cellStyleXfs count="206">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2971,8 +2998,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -3003,8 +3031,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="205" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="205" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="205">
+  <cellStyles count="206">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -3209,6 +3241,7 @@
     <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="203" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -3444,9 +3477,9 @@
   </sheetPr>
   <dimension ref="A1:R131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I124" sqref="I124"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C126" sqref="C126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8008,7 +8041,7 @@
       <c r="K120" s="3" t="s">
         <v>834</v>
       </c>
-      <c r="L120" s="5" t="s">
+      <c r="L120" s="20" t="s">
         <v>835</v>
       </c>
     </row>
@@ -8052,7 +8085,7 @@
     </row>
     <row r="122" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
-        <v>44522.601772291666</v>
+        <v>44522.601770833331</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>843</v>
@@ -8271,9 +8304,9 @@
   </sheetPr>
   <dimension ref="A1:P212"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I117" sqref="I117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11868,7 +11901,7 @@
       <c r="I112" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="J112" s="13" t="s">
+      <c r="J112" s="21" t="s">
         <v>250</v>
       </c>
     </row>
@@ -11937,7 +11970,36 @@
       </c>
     </row>
     <row r="115" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="J115" s="15"/>
+      <c r="A115" s="3">
+        <v>114</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>877</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>881</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>882</v>
+      </c>
+      <c r="E115" s="4" t="s">
+        <v>883</v>
+      </c>
+      <c r="F115" s="3" t="s">
+        <v>857</v>
+      </c>
+      <c r="G115" s="20" t="s">
+        <v>878</v>
+      </c>
+      <c r="H115" s="3" t="s">
+        <v>858</v>
+      </c>
+      <c r="I115" s="3" t="s">
+        <v>879</v>
+      </c>
+      <c r="J115" s="21" t="s">
+        <v>880</v>
+      </c>
     </row>
     <row r="116" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J116" s="15"/>
@@ -12231,7 +12293,7 @@
       <c r="J212" s="15"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B113">
+  <conditionalFormatting sqref="B2:B113 B115">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>COUNTIF($A$2:$A$14,A2)&gt;1</formula>
     </cfRule>
@@ -12350,6 +12412,8 @@
     <hyperlink ref="J112" r:id="rId111"/>
     <hyperlink ref="J113" r:id="rId112"/>
     <hyperlink ref="J114" r:id="rId113"/>
+    <hyperlink ref="G115" r:id="rId114"/>
+    <hyperlink ref="J115" r:id="rId115"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
add my details to the excel sheet
</commit_message>
<xml_diff>
--- a/CS335/GitHub Info sans duplicates.xlsx
+++ b/CS335/GitHub Info sans duplicates.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\lungo\staffcard\CS335\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC6735F-34BB-43A5-83B8-966AB6DF94B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="25600" windowHeight="14340" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -21,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3220" uniqueCount="873">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3229" uniqueCount="879">
   <si>
     <t>Timestamp</t>
   </si>
@@ -2640,16 +2646,34 @@
   </si>
   <si>
     <t>https://github.com/kasambala2021</t>
+  </si>
+  <si>
+    <t>2019-04-12003</t>
+  </si>
+  <si>
+    <t>Sikato</t>
+  </si>
+  <si>
+    <t>Amon L</t>
+  </si>
+  <si>
+    <t>Amonsikato21@gmail.com</t>
+  </si>
+  <si>
+    <t>Sikato-41</t>
+  </si>
+  <si>
+    <t>https://github.com/Sikato-41</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2696,6 +2720,12 @@
       <color theme="11"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -2735,7 +2765,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="205">
+  <cellStyleXfs count="206">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2941,8 +2971,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -2971,8 +3002,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="205" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="205">
+  <cellStyles count="206">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -3177,6 +3209,7 @@
     <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="203" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -3198,6 +3231,14 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -3398,23 +3439,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:R122"/>
+  <dimension ref="A1:R123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K54" sqref="K54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U123" sqref="U123"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="18" width="21.5" customWidth="1"/>
+    <col min="1" max="18" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3452,7 +3493,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>44517.792739571756</v>
       </c>
@@ -3490,7 +3531,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1">
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>44517.829278495366</v>
       </c>
@@ -3528,7 +3569,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1">
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>44517.829803020832</v>
       </c>
@@ -3566,7 +3607,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>44517.832974606485</v>
       </c>
@@ -3604,7 +3645,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.75" customHeight="1">
+    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>44517.833342615741</v>
       </c>
@@ -3642,7 +3683,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1">
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>44517.834096585648</v>
       </c>
@@ -3680,7 +3721,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>44517.834304884258</v>
       </c>
@@ -3718,7 +3759,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" customHeight="1">
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>44517.834315162036</v>
       </c>
@@ -3756,7 +3797,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1">
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>44517.834467222223</v>
       </c>
@@ -3794,7 +3835,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.75" customHeight="1">
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>44517.836256620372</v>
       </c>
@@ -3832,7 +3873,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1">
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>44517.840131203702</v>
       </c>
@@ -3870,7 +3911,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.75" customHeight="1">
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>44517.840687337964</v>
       </c>
@@ -3908,7 +3949,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1">
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>44517.840723900459</v>
       </c>
@@ -3946,7 +3987,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1">
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>44517.848194363425</v>
       </c>
@@ -3984,7 +4025,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15.75" customHeight="1">
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>44517.849799363423</v>
       </c>
@@ -4022,7 +4063,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15.75" customHeight="1">
+    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>44517.851121805557</v>
       </c>
@@ -4060,7 +4101,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15.75" customHeight="1">
+    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>44517.853374618055</v>
       </c>
@@ -4098,7 +4139,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15.75" customHeight="1">
+    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>44517.855156886573</v>
       </c>
@@ -4136,7 +4177,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15.75" customHeight="1">
+    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>44517.858557291664</v>
       </c>
@@ -4174,7 +4215,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15.75" customHeight="1">
+    <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>44517.859119421293</v>
       </c>
@@ -4212,7 +4253,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15.75" customHeight="1">
+    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>44517.860663136569</v>
       </c>
@@ -4250,7 +4291,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15.75" customHeight="1">
+    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>44517.863773090277</v>
       </c>
@@ -4288,7 +4329,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="15.75" customHeight="1">
+    <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>44517.867895196759</v>
       </c>
@@ -4326,7 +4367,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="15.75" customHeight="1">
+    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>44517.86830321759</v>
       </c>
@@ -4364,7 +4405,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="15.75" customHeight="1">
+    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>44517.869191446764</v>
       </c>
@@ -4402,7 +4443,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="15.75" customHeight="1">
+    <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>44517.874595833331</v>
       </c>
@@ -4440,7 +4481,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="15.75" customHeight="1">
+    <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>44517.877297905092</v>
       </c>
@@ -4478,7 +4519,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="15.75" customHeight="1">
+    <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>44517.877863587964</v>
       </c>
@@ -4516,7 +4557,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="15.75" customHeight="1">
+    <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>44517.886029872687</v>
       </c>
@@ -4554,7 +4595,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="15.75" customHeight="1">
+    <row r="31" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>44517.888174652777</v>
       </c>
@@ -4592,7 +4633,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="15.75" customHeight="1">
+    <row r="32" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>44517.89089574074</v>
       </c>
@@ -4630,7 +4671,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="15.75" customHeight="1">
+    <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>44517.898055138889</v>
       </c>
@@ -4668,7 +4709,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="15.75" customHeight="1">
+    <row r="34" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>44517.903385925922</v>
       </c>
@@ -4706,7 +4747,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="15.75" customHeight="1">
+    <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>44517.916796608799</v>
       </c>
@@ -4744,7 +4785,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="15.75" customHeight="1">
+    <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>44517.919944965281</v>
       </c>
@@ -4782,7 +4823,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="15.75" customHeight="1">
+    <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>44517.920174733794</v>
       </c>
@@ -4820,7 +4861,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="15.75" customHeight="1">
+    <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>44517.920207002317</v>
       </c>
@@ -4858,7 +4899,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="15.75" customHeight="1">
+    <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>44517.925676087965</v>
       </c>
@@ -4896,7 +4937,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="15.75" customHeight="1">
+    <row r="40" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>44517.942313136577</v>
       </c>
@@ -4934,7 +4975,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="15.75" customHeight="1">
+    <row r="41" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>44517.967181493055</v>
       </c>
@@ -4972,7 +5013,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="15.75" customHeight="1">
+    <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>44517.970856388885</v>
       </c>
@@ -5010,7 +5051,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="15.75" customHeight="1">
+    <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>44517.974103865738</v>
       </c>
@@ -5048,7 +5089,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="15.75" customHeight="1">
+    <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>44517.995788912041</v>
       </c>
@@ -5086,7 +5127,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="15.75" customHeight="1">
+    <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>44518.053331921299</v>
       </c>
@@ -5124,7 +5165,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="15.75" customHeight="1">
+    <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>44518.141680740737</v>
       </c>
@@ -5162,7 +5203,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="15.75" customHeight="1">
+    <row r="47" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>44518.338707534727</v>
       </c>
@@ -5200,7 +5241,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="15.75" customHeight="1">
+    <row r="48" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>44518.348475844905</v>
       </c>
@@ -5238,7 +5279,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="15.75" customHeight="1">
+    <row r="49" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>44518.368981018517</v>
       </c>
@@ -5276,7 +5317,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="15.75" customHeight="1">
+    <row r="50" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>44518.376564247686</v>
       </c>
@@ -5314,7 +5355,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="15.75" customHeight="1">
+    <row r="51" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>44518.395640312505</v>
       </c>
@@ -5352,7 +5393,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="15.75" customHeight="1">
+    <row r="52" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>44518.396610844909</v>
       </c>
@@ -5390,7 +5431,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="15.75" customHeight="1">
+    <row r="53" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>44518.416108634265</v>
       </c>
@@ -5428,7 +5469,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="15.75" customHeight="1">
+    <row r="54" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>44518.419745173611</v>
       </c>
@@ -5466,7 +5507,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="15.75" customHeight="1">
+    <row r="55" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>44518.433273449074</v>
       </c>
@@ -5504,7 +5545,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="15.75" customHeight="1">
+    <row r="56" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>44518.43360689815</v>
       </c>
@@ -5542,7 +5583,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="15.75" customHeight="1">
+    <row r="57" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>44518.462937638891</v>
       </c>
@@ -5580,7 +5621,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="15.75" customHeight="1">
+    <row r="58" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>44518.479146377314</v>
       </c>
@@ -5618,7 +5659,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="15.75" customHeight="1">
+    <row r="59" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>44518.500450555555</v>
       </c>
@@ -5656,7 +5697,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="15.75" customHeight="1">
+    <row r="60" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>44518.545351886569</v>
       </c>
@@ -5694,7 +5735,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="15.75" customHeight="1">
+    <row r="61" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>44518.57691783565</v>
       </c>
@@ -5732,7 +5773,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="15.75" customHeight="1">
+    <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>44518.580951863427</v>
       </c>
@@ -5770,7 +5811,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="15.75" customHeight="1">
+    <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>44518.584114340279</v>
       </c>
@@ -5808,7 +5849,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="15.75" customHeight="1">
+    <row r="64" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>44518.599512685185</v>
       </c>
@@ -5846,7 +5887,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="15.75" customHeight="1">
+    <row r="65" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>44518.611133506944</v>
       </c>
@@ -5884,7 +5925,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="15.75" customHeight="1">
+    <row r="66" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>44518.639018194444</v>
       </c>
@@ -5922,7 +5963,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="15.75" customHeight="1">
+    <row r="67" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>44518.65679601852</v>
       </c>
@@ -5960,7 +6001,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="15.75" customHeight="1">
+    <row r="68" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>44518.669622650465</v>
       </c>
@@ -5998,7 +6039,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="15.75" customHeight="1">
+    <row r="69" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>44518.675713946759</v>
       </c>
@@ -6036,7 +6077,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="15.75" customHeight="1">
+    <row r="70" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>44518.678410173612</v>
       </c>
@@ -6074,7 +6115,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="15.75" customHeight="1">
+    <row r="71" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>44518.67904717593</v>
       </c>
@@ -6112,7 +6153,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="15.75" customHeight="1">
+    <row r="72" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>44518.681073298612</v>
       </c>
@@ -6150,7 +6191,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="15.75" customHeight="1">
+    <row r="73" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>44518.681981574075</v>
       </c>
@@ -6188,7 +6229,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="15.75" customHeight="1">
+    <row r="74" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>44518.682995844909</v>
       </c>
@@ -6226,7 +6267,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="15.75" customHeight="1">
+    <row r="75" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>44518.68484347222</v>
       </c>
@@ -6264,7 +6305,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="15.75" customHeight="1">
+    <row r="76" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>44518.690567743055</v>
       </c>
@@ -6302,7 +6343,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="15.75" customHeight="1">
+    <row r="77" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>44518.704118368056</v>
       </c>
@@ -6340,7 +6381,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="15.75" customHeight="1">
+    <row r="78" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>44518.717275173607</v>
       </c>
@@ -6378,7 +6419,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="15.75" customHeight="1">
+    <row r="79" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>44518.718211203704</v>
       </c>
@@ -6416,7 +6457,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="80" spans="1:12" ht="15.75" customHeight="1">
+    <row r="80" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>44518.721890682871</v>
       </c>
@@ -6454,7 +6495,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="81" spans="1:12" ht="15.75" customHeight="1">
+    <row r="81" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>44518.845550972226</v>
       </c>
@@ -6492,7 +6533,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="82" spans="1:12" ht="15.75" customHeight="1">
+    <row r="82" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>44518.845807673613</v>
       </c>
@@ -6530,7 +6571,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="83" spans="1:12" ht="15.75" customHeight="1">
+    <row r="83" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>44518.847130671296</v>
       </c>
@@ -6568,7 +6609,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="84" spans="1:12" ht="15.75" customHeight="1">
+    <row r="84" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>44518.848048738422</v>
       </c>
@@ -6606,7 +6647,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="85" spans="1:12" ht="15.75" customHeight="1">
+    <row r="85" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>44518.848206620372</v>
       </c>
@@ -6644,7 +6685,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="86" spans="1:12" ht="15.75" customHeight="1">
+    <row r="86" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>44518.851609803241</v>
       </c>
@@ -6682,7 +6723,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="87" spans="1:12" ht="15.75" customHeight="1">
+    <row r="87" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>44518.853343229166</v>
       </c>
@@ -6720,7 +6761,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="88" spans="1:12" ht="15.75" customHeight="1">
+    <row r="88" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>44518.854456469911</v>
       </c>
@@ -6758,7 +6799,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="89" spans="1:12" ht="15.75" customHeight="1">
+    <row r="89" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>44518.857002847217</v>
       </c>
@@ -6796,7 +6837,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="90" spans="1:12" ht="15.75" customHeight="1">
+    <row r="90" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>44518.857458969913</v>
       </c>
@@ -6834,7 +6875,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="91" spans="1:12" ht="15.75" customHeight="1">
+    <row r="91" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>44518.864664201392</v>
       </c>
@@ -6872,7 +6913,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="92" spans="1:12" ht="15.75" customHeight="1">
+    <row r="92" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>44518.865544432869</v>
       </c>
@@ -6910,7 +6951,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="93" spans="1:12" ht="15.75" customHeight="1">
+    <row r="93" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>44518.873488796293</v>
       </c>
@@ -6948,7 +6989,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="94" spans="1:12" ht="15.75" customHeight="1">
+    <row r="94" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>44518.880978576388</v>
       </c>
@@ -6986,7 +7027,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="95" spans="1:12" ht="15.75" customHeight="1">
+    <row r="95" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>44518.890144791665</v>
       </c>
@@ -7024,7 +7065,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="96" spans="1:12" ht="15.75" customHeight="1">
+    <row r="96" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>44518.892673622686</v>
       </c>
@@ -7062,7 +7103,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="97" spans="1:12" ht="15.75" customHeight="1">
+    <row r="97" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>44518.893882627315</v>
       </c>
@@ -7100,7 +7141,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="98" spans="1:12" ht="15.75" customHeight="1">
+    <row r="98" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>44518.895629976847</v>
       </c>
@@ -7138,7 +7179,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="99" spans="1:12" ht="15.75" customHeight="1">
+    <row r="99" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <v>44518.897268032408</v>
       </c>
@@ -7176,7 +7217,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="100" spans="1:12" ht="15.75" customHeight="1">
+    <row r="100" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>44518.901678900467</v>
       </c>
@@ -7214,7 +7255,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="101" spans="1:12" ht="15.75" customHeight="1">
+    <row r="101" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
         <v>44518.905369791668</v>
       </c>
@@ -7252,7 +7293,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="102" spans="1:12" ht="15.75" customHeight="1">
+    <row r="102" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>44518.914951886574</v>
       </c>
@@ -7290,7 +7331,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="103" spans="1:12" ht="15.75" customHeight="1">
+    <row r="103" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>44518.926460324074</v>
       </c>
@@ -7325,7 +7366,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="104" spans="1:12" ht="15.75" customHeight="1">
+    <row r="104" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>44518.943910335649</v>
       </c>
@@ -7360,7 +7401,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="105" spans="1:12" ht="15.75" customHeight="1">
+    <row r="105" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
         <v>44518.94905171296</v>
       </c>
@@ -7398,7 +7439,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="106" spans="1:12" ht="15.75" customHeight="1">
+    <row r="106" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
         <v>44518.949835740743</v>
       </c>
@@ -7436,7 +7477,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="107" spans="1:12" ht="15.75" customHeight="1">
+    <row r="107" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
         <v>44518.954430393518</v>
       </c>
@@ -7474,7 +7515,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="108" spans="1:12" ht="15.75" customHeight="1">
+    <row r="108" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <v>44518.964523217597</v>
       </c>
@@ -7512,7 +7553,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="109" spans="1:12" ht="15.75" customHeight="1">
+    <row r="109" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
         <v>44518.971188981479</v>
       </c>
@@ -7550,7 +7591,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="110" spans="1:12" ht="15.75" customHeight="1">
+    <row r="110" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
         <v>44518.972234583329</v>
       </c>
@@ -7588,7 +7629,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="111" spans="1:12" ht="15.75" customHeight="1">
+    <row r="111" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
         <v>44518.972730138892</v>
       </c>
@@ -7626,7 +7667,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="112" spans="1:12" ht="15.75" customHeight="1">
+    <row r="112" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
         <v>44518.977785532406</v>
       </c>
@@ -7664,7 +7705,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="113" spans="1:18" ht="15.75" customHeight="1">
+    <row r="113" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="6">
         <v>44519.003693425926</v>
       </c>
@@ -7706,7 +7747,7 @@
       <c r="Q113" s="9"/>
       <c r="R113" s="9"/>
     </row>
-    <row r="114" spans="1:18" ht="15.75" customHeight="1">
+    <row r="114" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
         <v>44521.695289421295</v>
       </c>
@@ -7744,7 +7785,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="115" spans="1:18" ht="15.75" customHeight="1">
+    <row r="115" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
         <v>44521.703645162037</v>
       </c>
@@ -7782,7 +7823,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="116" spans="1:18" ht="15.75" customHeight="1">
+    <row r="116" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
         <v>44521.798439618055</v>
       </c>
@@ -7820,7 +7861,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="117" spans="1:18" ht="15.75" customHeight="1">
+    <row r="117" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
         <v>44521.806830486108</v>
       </c>
@@ -7858,7 +7899,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="118" spans="1:18" ht="15.75" customHeight="1">
+    <row r="118" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
         <v>44521.997838750001</v>
       </c>
@@ -7896,7 +7937,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="119" spans="1:18" ht="15.75" customHeight="1">
+    <row r="119" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
         <v>44522.038008958334</v>
       </c>
@@ -7934,7 +7975,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="120" spans="1:18" ht="15.75" customHeight="1">
+    <row r="120" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
         <v>44522.396687349537</v>
       </c>
@@ -7972,7 +8013,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="121" spans="1:18" ht="15.75" customHeight="1">
+    <row r="121" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
         <v>44522.424870671297</v>
       </c>
@@ -8010,7 +8051,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="122" spans="1:18" ht="15.75" customHeight="1">
+    <row r="122" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
         <v>44522.601772291666</v>
       </c>
@@ -8048,129 +8089,166 @@
         <v>849</v>
       </c>
     </row>
+    <row r="123" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B123" s="3" t="s">
+        <v>873</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>874</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>875</v>
+      </c>
+      <c r="E123">
+        <v>629642063</v>
+      </c>
+      <c r="F123" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G123" s="18" t="s">
+        <v>876</v>
+      </c>
+      <c r="H123" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I123" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J123" s="3">
+        <v>3</v>
+      </c>
+      <c r="K123" s="3" t="s">
+        <v>877</v>
+      </c>
+      <c r="L123" s="18" t="s">
+        <v>878</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1"/>
-    <hyperlink ref="L3" r:id="rId2"/>
-    <hyperlink ref="L4" r:id="rId3"/>
-    <hyperlink ref="L5" r:id="rId4"/>
-    <hyperlink ref="L6" r:id="rId5"/>
-    <hyperlink ref="L7" r:id="rId6"/>
-    <hyperlink ref="L8" r:id="rId7"/>
-    <hyperlink ref="L9" r:id="rId8"/>
-    <hyperlink ref="L10" r:id="rId9"/>
-    <hyperlink ref="L11" r:id="rId10"/>
-    <hyperlink ref="L12" r:id="rId11"/>
-    <hyperlink ref="L13" r:id="rId12"/>
-    <hyperlink ref="L14" r:id="rId13"/>
-    <hyperlink ref="L15" r:id="rId14"/>
-    <hyperlink ref="L16" r:id="rId15"/>
-    <hyperlink ref="L17" r:id="rId16"/>
-    <hyperlink ref="L18" r:id="rId17"/>
-    <hyperlink ref="L19" r:id="rId18"/>
-    <hyperlink ref="L20" r:id="rId19"/>
-    <hyperlink ref="L21" r:id="rId20"/>
-    <hyperlink ref="L22" r:id="rId21"/>
-    <hyperlink ref="L23" r:id="rId22"/>
-    <hyperlink ref="L24" r:id="rId23"/>
-    <hyperlink ref="L25" r:id="rId24"/>
-    <hyperlink ref="L26" r:id="rId25"/>
-    <hyperlink ref="L27" r:id="rId26"/>
-    <hyperlink ref="L28" r:id="rId27"/>
-    <hyperlink ref="L29" r:id="rId28"/>
-    <hyperlink ref="L30" r:id="rId29"/>
-    <hyperlink ref="L31" r:id="rId30"/>
-    <hyperlink ref="L32" r:id="rId31"/>
-    <hyperlink ref="L33" r:id="rId32"/>
-    <hyperlink ref="L34" r:id="rId33"/>
-    <hyperlink ref="L35" r:id="rId34"/>
-    <hyperlink ref="L36" r:id="rId35"/>
-    <hyperlink ref="L37" r:id="rId36"/>
-    <hyperlink ref="L38" r:id="rId37"/>
-    <hyperlink ref="L39" r:id="rId38"/>
-    <hyperlink ref="L40" r:id="rId39"/>
-    <hyperlink ref="L41" r:id="rId40"/>
-    <hyperlink ref="L42" r:id="rId41"/>
-    <hyperlink ref="L43" r:id="rId42"/>
-    <hyperlink ref="L44" r:id="rId43"/>
-    <hyperlink ref="L45" r:id="rId44"/>
-    <hyperlink ref="L46" r:id="rId45"/>
-    <hyperlink ref="L47" r:id="rId46"/>
-    <hyperlink ref="L48" r:id="rId47"/>
-    <hyperlink ref="L49" r:id="rId48"/>
-    <hyperlink ref="L50" r:id="rId49"/>
-    <hyperlink ref="L51" r:id="rId50"/>
-    <hyperlink ref="L52" r:id="rId51"/>
-    <hyperlink ref="L53" r:id="rId52"/>
-    <hyperlink ref="L54" r:id="rId53"/>
-    <hyperlink ref="L55" r:id="rId54"/>
-    <hyperlink ref="L56" r:id="rId55"/>
-    <hyperlink ref="L57" r:id="rId56"/>
-    <hyperlink ref="L58" r:id="rId57"/>
-    <hyperlink ref="L59" r:id="rId58"/>
-    <hyperlink ref="L60" r:id="rId59"/>
-    <hyperlink ref="L61" r:id="rId60"/>
-    <hyperlink ref="L62" r:id="rId61"/>
-    <hyperlink ref="L63" r:id="rId62"/>
-    <hyperlink ref="L64" r:id="rId63"/>
-    <hyperlink ref="L65" r:id="rId64"/>
-    <hyperlink ref="L66" r:id="rId65"/>
-    <hyperlink ref="L67" r:id="rId66"/>
-    <hyperlink ref="L68" r:id="rId67"/>
-    <hyperlink ref="L69" r:id="rId68"/>
-    <hyperlink ref="L70" r:id="rId69"/>
-    <hyperlink ref="L71" r:id="rId70"/>
-    <hyperlink ref="L72" r:id="rId71"/>
-    <hyperlink ref="L73" r:id="rId72"/>
-    <hyperlink ref="L74" r:id="rId73"/>
-    <hyperlink ref="L75" r:id="rId74"/>
-    <hyperlink ref="L76" r:id="rId75"/>
-    <hyperlink ref="L77" r:id="rId76"/>
-    <hyperlink ref="L78" r:id="rId77"/>
-    <hyperlink ref="L79" r:id="rId78"/>
-    <hyperlink ref="L80" r:id="rId79"/>
-    <hyperlink ref="L81" r:id="rId80"/>
-    <hyperlink ref="L82" r:id="rId81"/>
-    <hyperlink ref="L83" r:id="rId82"/>
-    <hyperlink ref="L84" r:id="rId83"/>
-    <hyperlink ref="L85" r:id="rId84"/>
-    <hyperlink ref="L86" r:id="rId85"/>
-    <hyperlink ref="L87" r:id="rId86"/>
-    <hyperlink ref="L88" r:id="rId87"/>
-    <hyperlink ref="L89" r:id="rId88"/>
-    <hyperlink ref="L90" r:id="rId89"/>
-    <hyperlink ref="L91" r:id="rId90"/>
-    <hyperlink ref="L92" r:id="rId91"/>
-    <hyperlink ref="L93" r:id="rId92"/>
-    <hyperlink ref="L94" r:id="rId93"/>
-    <hyperlink ref="L95" r:id="rId94"/>
-    <hyperlink ref="L96" r:id="rId95"/>
-    <hyperlink ref="L97" r:id="rId96"/>
-    <hyperlink ref="L98" r:id="rId97"/>
-    <hyperlink ref="L99" r:id="rId98"/>
-    <hyperlink ref="L100" r:id="rId99"/>
-    <hyperlink ref="L101" r:id="rId100"/>
-    <hyperlink ref="L102" r:id="rId101"/>
-    <hyperlink ref="L103" r:id="rId102"/>
-    <hyperlink ref="L104" r:id="rId103"/>
-    <hyperlink ref="L105" r:id="rId104"/>
-    <hyperlink ref="L106" r:id="rId105"/>
-    <hyperlink ref="L107" r:id="rId106"/>
-    <hyperlink ref="L108" r:id="rId107"/>
-    <hyperlink ref="L109" r:id="rId108"/>
-    <hyperlink ref="L110" r:id="rId109"/>
-    <hyperlink ref="L111" r:id="rId110"/>
-    <hyperlink ref="L112" r:id="rId111"/>
-    <hyperlink ref="L113" r:id="rId112"/>
-    <hyperlink ref="L114" r:id="rId113"/>
-    <hyperlink ref="L115" r:id="rId114"/>
-    <hyperlink ref="L116" r:id="rId115"/>
-    <hyperlink ref="L117" r:id="rId116"/>
-    <hyperlink ref="L118" r:id="rId117"/>
-    <hyperlink ref="L119" r:id="rId118"/>
-    <hyperlink ref="L120" r:id="rId119"/>
-    <hyperlink ref="L121" r:id="rId120"/>
-    <hyperlink ref="L122" r:id="rId121"/>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="L3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="L4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="L5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="L6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="L7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="L8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="L9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="L10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="L11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="L12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="L13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="L14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="L15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="L16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="L17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="L18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="L19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="L20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="L21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="L22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="L23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="L24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="L25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="L26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="L27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="L28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="L29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="L30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="L31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="L32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="L33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="L34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="L35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="L36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="L37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="L38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="L39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="L40" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="L41" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="L42" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="L43" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="L44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="L45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="L46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="L47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="L48" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="L49" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="L50" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="L51" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="L52" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="L53" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="L54" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="L55" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="L56" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="L57" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="L58" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="L59" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="L60" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="L61" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="L62" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="L63" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="L64" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="L65" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="L66" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="L67" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="L68" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="L69" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="L70" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="L71" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="L72" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="L73" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="L74" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="L75" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="L76" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="L77" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="L78" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="L79" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="L80" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="L81" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="L82" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="L83" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="L84" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="L85" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="L86" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="L87" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="L88" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="L89" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="L90" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="L91" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="L92" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="L93" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="L94" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="L95" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="L96" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="L97" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="L98" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="L99" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="L100" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="L101" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="L102" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="L103" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="L104" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="L105" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="L106" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="L107" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="L108" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="L109" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="L110" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="L111" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="L112" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="L113" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="L114" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="L115" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="L116" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="L117" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="L118" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="L119" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="L120" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="L121" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="L122" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="G123" r:id="rId122" xr:uid="{A3315EC1-3128-49A2-B40B-124CA4151A1B}"/>
+    <hyperlink ref="L123" r:id="rId123" xr:uid="{A3B29158-AFE6-4259-8040-F3DAC172B55B}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -8183,8 +8261,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -8195,22 +8273,22 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="25.5" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="33.1640625" customWidth="1"/>
-    <col min="8" max="8" width="9.5" customWidth="1"/>
-    <col min="9" max="9" width="17.5" customWidth="1"/>
-    <col min="10" max="10" width="33.1640625" customWidth="1"/>
-    <col min="11" max="16" width="21.5" customWidth="1"/>
+    <col min="7" max="7" width="33.140625" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="10" max="10" width="33.140625" customWidth="1"/>
+    <col min="11" max="16" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="39.75" customHeight="1">
+    <row r="1" spans="1:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>850</v>
       </c>
@@ -8248,7 +8326,7 @@
       <c r="O1" s="12"/>
       <c r="P1" s="12"/>
     </row>
-    <row r="2" spans="1:16" ht="12">
+    <row r="2" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -8280,7 +8358,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="12">
+    <row r="3" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -8312,7 +8390,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="12">
+    <row r="4" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -8344,7 +8422,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="12">
+    <row r="5" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -8376,7 +8454,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="12">
+    <row r="6" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -8408,7 +8486,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="12">
+    <row r="7" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -8440,7 +8518,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="12">
+    <row r="8" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -8472,7 +8550,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="12">
+    <row r="9" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -8504,7 +8582,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="12">
+    <row r="10" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -8536,7 +8614,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="12">
+    <row r="11" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -8568,7 +8646,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="12">
+    <row r="12" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -8600,7 +8678,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="12">
+    <row r="13" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -8632,7 +8710,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="12">
+    <row r="14" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -8664,7 +8742,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="12">
+    <row r="15" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -8696,7 +8774,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="12">
+    <row r="16" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -8728,7 +8806,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="12">
+    <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -8760,7 +8838,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="12">
+    <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -8792,7 +8870,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="36">
+    <row r="19" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -8824,7 +8902,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="12">
+    <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -8856,7 +8934,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="12">
+    <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -8888,7 +8966,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="12">
+    <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -8920,7 +8998,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="12">
+    <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -8952,7 +9030,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="12">
+    <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -8984,7 +9062,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="12">
+    <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -9016,7 +9094,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="12">
+    <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -9048,7 +9126,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="12">
+    <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -9080,7 +9158,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="12">
+    <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -9112,7 +9190,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="12">
+    <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -9144,7 +9222,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="12">
+    <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -9176,7 +9254,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="12">
+    <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -9208,7 +9286,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="12">
+    <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -9240,7 +9318,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="12">
+    <row r="33" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -9272,7 +9350,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="12">
+    <row r="34" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -9304,7 +9382,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="12">
+    <row r="35" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -9336,7 +9414,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="12">
+    <row r="36" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -9368,7 +9446,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="12">
+    <row r="37" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -9400,7 +9478,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="12">
+    <row r="38" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -9432,7 +9510,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="12">
+    <row r="39" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -9464,7 +9542,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="12">
+    <row r="40" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -9496,7 +9574,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="12">
+    <row r="41" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -9528,7 +9606,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="12">
+    <row r="42" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -9560,7 +9638,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="12">
+    <row r="43" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -9592,7 +9670,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="12">
+    <row r="44" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -9624,7 +9702,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="12">
+    <row r="45" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -9656,7 +9734,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="12">
+    <row r="46" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -9688,7 +9766,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="12">
+    <row r="47" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -9720,7 +9798,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="12">
+    <row r="48" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -9752,7 +9830,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="12">
+    <row r="49" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -9784,7 +9862,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="12">
+    <row r="50" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -9816,7 +9894,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="12">
+    <row r="51" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -9848,7 +9926,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="12">
+    <row r="52" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -9880,7 +9958,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="12">
+    <row r="53" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -9912,7 +9990,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="12">
+    <row r="54" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -9944,7 +10022,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="12">
+    <row r="55" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -9976,7 +10054,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="12">
+    <row r="56" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -10008,7 +10086,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="12">
+    <row r="57" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -10040,7 +10118,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="12">
+    <row r="58" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -10072,7 +10150,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="12">
+    <row r="59" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -10104,7 +10182,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="12">
+    <row r="60" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -10136,7 +10214,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="12">
+    <row r="61" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -10168,7 +10246,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="12">
+    <row r="62" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -10200,7 +10278,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="12">
+    <row r="63" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -10232,7 +10310,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="12">
+    <row r="64" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -10264,7 +10342,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="12">
+    <row r="65" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -10296,7 +10374,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="12">
+    <row r="66" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -10328,7 +10406,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="12">
+    <row r="67" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -10360,7 +10438,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="12">
+    <row r="68" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -10392,7 +10470,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="12">
+    <row r="69" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -10424,7 +10502,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="12">
+    <row r="70" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -10456,7 +10534,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="12">
+    <row r="71" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -10488,7 +10566,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="12">
+    <row r="72" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -10520,7 +10598,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="12">
+    <row r="73" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -10552,7 +10630,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="24">
+    <row r="74" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -10584,7 +10662,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="12">
+    <row r="75" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -10616,7 +10694,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="12">
+    <row r="76" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -10648,7 +10726,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="12">
+    <row r="77" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -10680,7 +10758,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="12">
+    <row r="78" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -10712,7 +10790,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="12">
+    <row r="79" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -10744,7 +10822,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="12">
+    <row r="80" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -10776,7 +10854,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="12">
+    <row r="81" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -10808,7 +10886,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="12">
+    <row r="82" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -10840,7 +10918,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="12">
+    <row r="83" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -10872,7 +10950,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="12">
+    <row r="84" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="3">
         <v>83</v>
       </c>
@@ -10904,7 +10982,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="12">
+    <row r="85" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
         <v>84</v>
       </c>
@@ -10936,7 +11014,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="12">
+    <row r="86" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A86" s="3">
         <v>85</v>
       </c>
@@ -10968,7 +11046,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="12">
+    <row r="87" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>86</v>
       </c>
@@ -11000,7 +11078,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="12">
+    <row r="88" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="3">
         <v>87</v>
       </c>
@@ -11032,7 +11110,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="12">
+    <row r="89" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
         <v>88</v>
       </c>
@@ -11064,7 +11142,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="12">
+    <row r="90" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="3">
         <v>89</v>
       </c>
@@ -11096,7 +11174,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="12">
+    <row r="91" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="3">
         <v>90</v>
       </c>
@@ -11128,7 +11206,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="12">
+    <row r="92" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="3">
         <v>91</v>
       </c>
@@ -11160,7 +11238,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="12">
+    <row r="93" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="3">
         <v>92</v>
       </c>
@@ -11192,7 +11270,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="12">
+    <row r="94" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="3">
         <v>93</v>
       </c>
@@ -11224,7 +11302,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="95" spans="1:10" ht="12">
+    <row r="95" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="3">
         <v>94</v>
       </c>
@@ -11256,7 +11334,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="96" spans="1:10" ht="12">
+    <row r="96" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="3">
         <v>95</v>
       </c>
@@ -11288,7 +11366,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="12">
+    <row r="97" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="3">
         <v>96</v>
       </c>
@@ -11320,7 +11398,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="12">
+    <row r="98" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" s="3">
         <v>97</v>
       </c>
@@ -11352,7 +11430,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="99" spans="1:10" ht="12">
+    <row r="99" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="3">
         <v>98</v>
       </c>
@@ -11384,7 +11462,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="12">
+    <row r="100" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A100" s="3">
         <v>99</v>
       </c>
@@ -11416,7 +11494,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="12">
+    <row r="101" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A101" s="3">
         <v>100</v>
       </c>
@@ -11448,7 +11526,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="12">
+    <row r="102" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" s="3">
         <v>101</v>
       </c>
@@ -11477,7 +11555,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="103" spans="1:10" ht="12">
+    <row r="103" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A103" s="3">
         <v>102</v>
       </c>
@@ -11506,7 +11584,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="104" spans="1:10" ht="12">
+    <row r="104" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A104" s="3">
         <v>103</v>
       </c>
@@ -11538,7 +11616,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="105" spans="1:10" ht="12">
+    <row r="105" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A105" s="3">
         <v>104</v>
       </c>
@@ -11570,7 +11648,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="106" spans="1:10" ht="12">
+    <row r="106" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A106" s="3">
         <v>105</v>
       </c>
@@ -11602,7 +11680,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="12">
+    <row r="107" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A107" s="3">
         <v>106</v>
       </c>
@@ -11634,7 +11712,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="108" spans="1:10" ht="12">
+    <row r="108" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A108" s="3">
         <v>107</v>
       </c>
@@ -11666,7 +11744,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="109" spans="1:10" ht="12">
+    <row r="109" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A109" s="3">
         <v>108</v>
       </c>
@@ -11698,7 +11776,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="110" spans="1:10" ht="12">
+    <row r="110" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A110" s="3">
         <v>109</v>
       </c>
@@ -11730,7 +11808,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="111" spans="1:10" ht="12">
+    <row r="111" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A111" s="3">
         <v>110</v>
       </c>
@@ -11762,7 +11840,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="12">
+    <row r="112" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A112" s="3">
         <v>111</v>
       </c>
@@ -11791,7 +11869,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="113" spans="1:10" ht="12">
+    <row r="113" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A113" s="3">
         <v>112</v>
       </c>
@@ -11823,7 +11901,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="114" spans="1:10" ht="12">
+    <row r="114" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A114" s="3">
         <v>113</v>
       </c>
@@ -11855,298 +11933,298 @@
         <v>872</v>
       </c>
     </row>
-    <row r="115" spans="1:10" ht="12">
+    <row r="115" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J115" s="15"/>
     </row>
-    <row r="116" spans="1:10" ht="12">
+    <row r="116" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J116" s="15"/>
     </row>
-    <row r="117" spans="1:10" ht="12">
+    <row r="117" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J117" s="15"/>
     </row>
-    <row r="118" spans="1:10" ht="12">
+    <row r="118" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J118" s="15"/>
     </row>
-    <row r="119" spans="1:10" ht="12">
+    <row r="119" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J119" s="15"/>
     </row>
-    <row r="120" spans="1:10" ht="12">
+    <row r="120" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J120" s="15"/>
     </row>
-    <row r="121" spans="1:10" ht="12">
+    <row r="121" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J121" s="15"/>
     </row>
-    <row r="122" spans="1:10" ht="12">
+    <row r="122" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J122" s="15"/>
     </row>
-    <row r="123" spans="1:10" ht="12">
+    <row r="123" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J123" s="15"/>
     </row>
-    <row r="124" spans="1:10" ht="12">
+    <row r="124" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J124" s="15"/>
     </row>
-    <row r="125" spans="1:10" ht="12">
+    <row r="125" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J125" s="15"/>
     </row>
-    <row r="126" spans="1:10" ht="12">
+    <row r="126" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J126" s="15"/>
     </row>
-    <row r="127" spans="1:10" ht="12">
+    <row r="127" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J127" s="15"/>
     </row>
-    <row r="128" spans="1:10" ht="12">
+    <row r="128" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J128" s="15"/>
     </row>
-    <row r="129" spans="10:10" ht="12">
+    <row r="129" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J129" s="15"/>
     </row>
-    <row r="130" spans="10:10" ht="12">
+    <row r="130" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J130" s="15"/>
     </row>
-    <row r="131" spans="10:10" ht="12">
+    <row r="131" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J131" s="15"/>
     </row>
-    <row r="132" spans="10:10" ht="12">
+    <row r="132" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J132" s="15"/>
     </row>
-    <row r="133" spans="10:10" ht="12">
+    <row r="133" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J133" s="15"/>
     </row>
-    <row r="134" spans="10:10" ht="12">
+    <row r="134" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J134" s="15"/>
     </row>
-    <row r="135" spans="10:10" ht="12">
+    <row r="135" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J135" s="15"/>
     </row>
-    <row r="136" spans="10:10" ht="12">
+    <row r="136" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J136" s="15"/>
     </row>
-    <row r="137" spans="10:10" ht="12">
+    <row r="137" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J137" s="15"/>
     </row>
-    <row r="138" spans="10:10" ht="12">
+    <row r="138" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J138" s="15"/>
     </row>
-    <row r="139" spans="10:10" ht="12">
+    <row r="139" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J139" s="15"/>
     </row>
-    <row r="140" spans="10:10" ht="12">
+    <row r="140" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J140" s="15"/>
     </row>
-    <row r="141" spans="10:10" ht="12">
+    <row r="141" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J141" s="15"/>
     </row>
-    <row r="142" spans="10:10" ht="12">
+    <row r="142" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J142" s="15"/>
     </row>
-    <row r="143" spans="10:10" ht="12">
+    <row r="143" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J143" s="15"/>
     </row>
-    <row r="144" spans="10:10" ht="12">
+    <row r="144" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J144" s="15"/>
     </row>
-    <row r="145" spans="10:10" ht="12">
+    <row r="145" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J145" s="15"/>
     </row>
-    <row r="146" spans="10:10" ht="12">
+    <row r="146" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J146" s="15"/>
     </row>
-    <row r="147" spans="10:10" ht="12">
+    <row r="147" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J147" s="15"/>
     </row>
-    <row r="148" spans="10:10" ht="12">
+    <row r="148" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J148" s="15"/>
     </row>
-    <row r="149" spans="10:10" ht="12">
+    <row r="149" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J149" s="15"/>
     </row>
-    <row r="150" spans="10:10" ht="12">
+    <row r="150" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J150" s="15"/>
     </row>
-    <row r="151" spans="10:10" ht="12">
+    <row r="151" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J151" s="15"/>
     </row>
-    <row r="152" spans="10:10" ht="12">
+    <row r="152" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J152" s="15"/>
     </row>
-    <row r="153" spans="10:10" ht="12">
+    <row r="153" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J153" s="15"/>
     </row>
-    <row r="154" spans="10:10" ht="12">
+    <row r="154" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J154" s="15"/>
     </row>
-    <row r="155" spans="10:10" ht="12">
+    <row r="155" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J155" s="15"/>
     </row>
-    <row r="156" spans="10:10" ht="12">
+    <row r="156" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J156" s="15"/>
     </row>
-    <row r="157" spans="10:10" ht="12">
+    <row r="157" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J157" s="15"/>
     </row>
-    <row r="158" spans="10:10" ht="12">
+    <row r="158" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J158" s="15"/>
     </row>
-    <row r="159" spans="10:10" ht="12">
+    <row r="159" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J159" s="15"/>
     </row>
-    <row r="160" spans="10:10" ht="12">
+    <row r="160" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J160" s="15"/>
     </row>
-    <row r="161" spans="10:10" ht="12">
+    <row r="161" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J161" s="15"/>
     </row>
-    <row r="162" spans="10:10" ht="12">
+    <row r="162" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J162" s="15"/>
     </row>
-    <row r="163" spans="10:10" ht="12">
+    <row r="163" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J163" s="15"/>
     </row>
-    <row r="164" spans="10:10" ht="12">
+    <row r="164" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J164" s="15"/>
     </row>
-    <row r="165" spans="10:10" ht="12">
+    <row r="165" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J165" s="15"/>
     </row>
-    <row r="166" spans="10:10" ht="12">
+    <row r="166" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J166" s="15"/>
     </row>
-    <row r="167" spans="10:10" ht="12">
+    <row r="167" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J167" s="15"/>
     </row>
-    <row r="168" spans="10:10" ht="12">
+    <row r="168" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J168" s="15"/>
     </row>
-    <row r="169" spans="10:10" ht="12">
+    <row r="169" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J169" s="15"/>
     </row>
-    <row r="170" spans="10:10" ht="12">
+    <row r="170" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J170" s="15"/>
     </row>
-    <row r="171" spans="10:10" ht="12">
+    <row r="171" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J171" s="15"/>
     </row>
-    <row r="172" spans="10:10" ht="12">
+    <row r="172" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J172" s="15"/>
     </row>
-    <row r="173" spans="10:10" ht="12">
+    <row r="173" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J173" s="15"/>
     </row>
-    <row r="174" spans="10:10" ht="12">
+    <row r="174" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J174" s="15"/>
     </row>
-    <row r="175" spans="10:10" ht="12">
+    <row r="175" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J175" s="15"/>
     </row>
-    <row r="176" spans="10:10" ht="12">
+    <row r="176" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J176" s="15"/>
     </row>
-    <row r="177" spans="10:10" ht="12">
+    <row r="177" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J177" s="15"/>
     </row>
-    <row r="178" spans="10:10" ht="12">
+    <row r="178" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J178" s="15"/>
     </row>
-    <row r="179" spans="10:10" ht="12">
+    <row r="179" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J179" s="15"/>
     </row>
-    <row r="180" spans="10:10" ht="12">
+    <row r="180" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J180" s="15"/>
     </row>
-    <row r="181" spans="10:10" ht="12">
+    <row r="181" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J181" s="15"/>
     </row>
-    <row r="182" spans="10:10" ht="12">
+    <row r="182" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J182" s="15"/>
     </row>
-    <row r="183" spans="10:10" ht="12">
+    <row r="183" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J183" s="15"/>
     </row>
-    <row r="184" spans="10:10" ht="12">
+    <row r="184" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J184" s="15"/>
     </row>
-    <row r="185" spans="10:10" ht="12">
+    <row r="185" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J185" s="15"/>
     </row>
-    <row r="186" spans="10:10" ht="12">
+    <row r="186" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J186" s="15"/>
     </row>
-    <row r="187" spans="10:10" ht="12">
+    <row r="187" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J187" s="15"/>
     </row>
-    <row r="188" spans="10:10" ht="12">
+    <row r="188" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J188" s="15"/>
     </row>
-    <row r="189" spans="10:10" ht="12">
+    <row r="189" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J189" s="15"/>
     </row>
-    <row r="190" spans="10:10" ht="12">
+    <row r="190" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J190" s="15"/>
     </row>
-    <row r="191" spans="10:10" ht="12">
+    <row r="191" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J191" s="15"/>
     </row>
-    <row r="192" spans="10:10" ht="12">
+    <row r="192" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J192" s="15"/>
     </row>
-    <row r="193" spans="10:10" ht="12">
+    <row r="193" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J193" s="15"/>
     </row>
-    <row r="194" spans="10:10" ht="12">
+    <row r="194" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J194" s="15"/>
     </row>
-    <row r="195" spans="10:10" ht="12">
+    <row r="195" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J195" s="15"/>
     </row>
-    <row r="196" spans="10:10" ht="12">
+    <row r="196" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J196" s="15"/>
     </row>
-    <row r="197" spans="10:10" ht="12">
+    <row r="197" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J197" s="15"/>
     </row>
-    <row r="198" spans="10:10" ht="12">
+    <row r="198" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J198" s="15"/>
     </row>
-    <row r="199" spans="10:10" ht="12">
+    <row r="199" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J199" s="15"/>
     </row>
-    <row r="200" spans="10:10" ht="12">
+    <row r="200" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J200" s="15"/>
     </row>
-    <row r="201" spans="10:10" ht="12">
+    <row r="201" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J201" s="15"/>
     </row>
-    <row r="202" spans="10:10" ht="12">
+    <row r="202" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J202" s="15"/>
     </row>
-    <row r="203" spans="10:10" ht="12">
+    <row r="203" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J203" s="15"/>
     </row>
-    <row r="204" spans="10:10" ht="12">
+    <row r="204" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J204" s="15"/>
     </row>
-    <row r="205" spans="10:10" ht="12">
+    <row r="205" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J205" s="15"/>
     </row>
-    <row r="206" spans="10:10" ht="12">
+    <row r="206" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J206" s="15"/>
     </row>
-    <row r="207" spans="10:10" ht="12">
+    <row r="207" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J207" s="15"/>
     </row>
-    <row r="208" spans="10:10" ht="12">
+    <row r="208" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J208" s="15"/>
     </row>
-    <row r="209" spans="10:10" ht="12">
+    <row r="209" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J209" s="15"/>
     </row>
-    <row r="210" spans="10:10" ht="12">
+    <row r="210" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J210" s="15"/>
     </row>
-    <row r="211" spans="10:10" ht="12">
+    <row r="211" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J211" s="15"/>
     </row>
-    <row r="212" spans="10:10" ht="12">
+    <row r="212" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J212" s="15"/>
     </row>
   </sheetData>
@@ -12156,119 +12234,119 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1"/>
-    <hyperlink ref="J3" r:id="rId2"/>
-    <hyperlink ref="J4" r:id="rId3"/>
-    <hyperlink ref="J5" r:id="rId4"/>
-    <hyperlink ref="J6" r:id="rId5"/>
-    <hyperlink ref="J7" r:id="rId6"/>
-    <hyperlink ref="J8" r:id="rId7"/>
-    <hyperlink ref="J9" r:id="rId8"/>
-    <hyperlink ref="J10" r:id="rId9"/>
-    <hyperlink ref="J11" r:id="rId10"/>
-    <hyperlink ref="J12" r:id="rId11"/>
-    <hyperlink ref="J13" r:id="rId12"/>
-    <hyperlink ref="J14" r:id="rId13"/>
-    <hyperlink ref="J15" r:id="rId14"/>
-    <hyperlink ref="J16" r:id="rId15"/>
-    <hyperlink ref="J17" r:id="rId16"/>
-    <hyperlink ref="J18" r:id="rId17"/>
-    <hyperlink ref="J19" r:id="rId18"/>
-    <hyperlink ref="J20" r:id="rId19"/>
-    <hyperlink ref="J21" r:id="rId20"/>
-    <hyperlink ref="J22" r:id="rId21"/>
-    <hyperlink ref="J23" r:id="rId22"/>
-    <hyperlink ref="J24" r:id="rId23"/>
-    <hyperlink ref="J25" r:id="rId24"/>
-    <hyperlink ref="J26" r:id="rId25"/>
-    <hyperlink ref="J27" r:id="rId26"/>
-    <hyperlink ref="J28" r:id="rId27"/>
-    <hyperlink ref="J29" r:id="rId28"/>
-    <hyperlink ref="J30" r:id="rId29"/>
-    <hyperlink ref="J31" r:id="rId30"/>
-    <hyperlink ref="J32" r:id="rId31"/>
-    <hyperlink ref="J33" r:id="rId32"/>
-    <hyperlink ref="J34" r:id="rId33"/>
-    <hyperlink ref="J35" r:id="rId34"/>
-    <hyperlink ref="J36" r:id="rId35"/>
-    <hyperlink ref="J37" r:id="rId36"/>
-    <hyperlink ref="J38" r:id="rId37"/>
-    <hyperlink ref="J39" r:id="rId38"/>
-    <hyperlink ref="J40" r:id="rId39"/>
-    <hyperlink ref="J41" r:id="rId40"/>
-    <hyperlink ref="J42" r:id="rId41"/>
-    <hyperlink ref="J43" r:id="rId42"/>
-    <hyperlink ref="J44" r:id="rId43"/>
-    <hyperlink ref="J45" r:id="rId44"/>
-    <hyperlink ref="J46" r:id="rId45"/>
-    <hyperlink ref="J47" r:id="rId46"/>
-    <hyperlink ref="J48" r:id="rId47"/>
-    <hyperlink ref="J49" r:id="rId48"/>
-    <hyperlink ref="J50" r:id="rId49"/>
-    <hyperlink ref="J51" r:id="rId50"/>
-    <hyperlink ref="J52" r:id="rId51"/>
-    <hyperlink ref="J53" r:id="rId52"/>
-    <hyperlink ref="J54" r:id="rId53"/>
-    <hyperlink ref="J55" r:id="rId54"/>
-    <hyperlink ref="J56" r:id="rId55"/>
-    <hyperlink ref="J57" r:id="rId56"/>
-    <hyperlink ref="J58" r:id="rId57"/>
-    <hyperlink ref="J59" r:id="rId58"/>
-    <hyperlink ref="J60" r:id="rId59"/>
-    <hyperlink ref="J61" r:id="rId60"/>
-    <hyperlink ref="J62" r:id="rId61"/>
-    <hyperlink ref="J63" r:id="rId62"/>
-    <hyperlink ref="J64" r:id="rId63"/>
-    <hyperlink ref="J65" r:id="rId64"/>
-    <hyperlink ref="J66" r:id="rId65"/>
-    <hyperlink ref="J67" r:id="rId66"/>
-    <hyperlink ref="J68" r:id="rId67"/>
-    <hyperlink ref="J69" r:id="rId68"/>
-    <hyperlink ref="J70" r:id="rId69"/>
-    <hyperlink ref="J71" r:id="rId70"/>
-    <hyperlink ref="J72" r:id="rId71"/>
-    <hyperlink ref="J73" r:id="rId72"/>
-    <hyperlink ref="J74" r:id="rId73"/>
-    <hyperlink ref="J75" r:id="rId74"/>
-    <hyperlink ref="J76" r:id="rId75"/>
-    <hyperlink ref="J77" r:id="rId76"/>
-    <hyperlink ref="J78" r:id="rId77"/>
-    <hyperlink ref="J79" r:id="rId78"/>
-    <hyperlink ref="J80" r:id="rId79"/>
-    <hyperlink ref="J81" r:id="rId80"/>
-    <hyperlink ref="J82" r:id="rId81"/>
-    <hyperlink ref="J83" r:id="rId82"/>
-    <hyperlink ref="J84" r:id="rId83"/>
-    <hyperlink ref="J85" r:id="rId84"/>
-    <hyperlink ref="J86" r:id="rId85"/>
-    <hyperlink ref="J87" r:id="rId86"/>
-    <hyperlink ref="J88" r:id="rId87"/>
-    <hyperlink ref="J89" r:id="rId88"/>
-    <hyperlink ref="J90" r:id="rId89"/>
-    <hyperlink ref="J91" r:id="rId90"/>
-    <hyperlink ref="J92" r:id="rId91"/>
-    <hyperlink ref="J93" r:id="rId92"/>
-    <hyperlink ref="J94" r:id="rId93"/>
-    <hyperlink ref="J95" r:id="rId94"/>
-    <hyperlink ref="J96" r:id="rId95"/>
-    <hyperlink ref="J97" r:id="rId96"/>
-    <hyperlink ref="J98" r:id="rId97"/>
-    <hyperlink ref="J99" r:id="rId98"/>
-    <hyperlink ref="J100" r:id="rId99"/>
-    <hyperlink ref="J101" r:id="rId100"/>
-    <hyperlink ref="J102" r:id="rId101"/>
-    <hyperlink ref="J103" r:id="rId102"/>
-    <hyperlink ref="J104" r:id="rId103"/>
-    <hyperlink ref="J105" r:id="rId104"/>
-    <hyperlink ref="J106" r:id="rId105"/>
-    <hyperlink ref="J107" r:id="rId106"/>
-    <hyperlink ref="J108" r:id="rId107"/>
-    <hyperlink ref="J109" r:id="rId108"/>
-    <hyperlink ref="J110" r:id="rId109"/>
-    <hyperlink ref="J111" r:id="rId110"/>
-    <hyperlink ref="J112" r:id="rId111"/>
-    <hyperlink ref="J113" r:id="rId112"/>
-    <hyperlink ref="J114" r:id="rId113"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="J3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="J4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="J5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="J6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="J7" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="J8" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="J9" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="J10" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="J11" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="J12" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="J13" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="J14" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="J15" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="J16" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="J17" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="J18" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="J19" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="J20" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="J21" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="J22" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="J23" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
+    <hyperlink ref="J24" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink ref="J25" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
+    <hyperlink ref="J26" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink ref="J27" r:id="rId26" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
+    <hyperlink ref="J28" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
+    <hyperlink ref="J29" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
+    <hyperlink ref="J30" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="J31" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
+    <hyperlink ref="J32" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="J33" r:id="rId32" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
+    <hyperlink ref="J34" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink ref="J35" r:id="rId34" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
+    <hyperlink ref="J36" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink ref="J37" r:id="rId36" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
+    <hyperlink ref="J38" r:id="rId37" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
+    <hyperlink ref="J39" r:id="rId38" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
+    <hyperlink ref="J40" r:id="rId39" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
+    <hyperlink ref="J41" r:id="rId40" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
+    <hyperlink ref="J42" r:id="rId41" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
+    <hyperlink ref="J43" r:id="rId42" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
+    <hyperlink ref="J44" r:id="rId43" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
+    <hyperlink ref="J45" r:id="rId44" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
+    <hyperlink ref="J46" r:id="rId45" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
+    <hyperlink ref="J47" r:id="rId46" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
+    <hyperlink ref="J48" r:id="rId47" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
+    <hyperlink ref="J49" r:id="rId48" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
+    <hyperlink ref="J50" r:id="rId49" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
+    <hyperlink ref="J51" r:id="rId50" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
+    <hyperlink ref="J52" r:id="rId51" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
+    <hyperlink ref="J53" r:id="rId52" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
+    <hyperlink ref="J54" r:id="rId53" xr:uid="{00000000-0004-0000-0100-000034000000}"/>
+    <hyperlink ref="J55" r:id="rId54" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
+    <hyperlink ref="J56" r:id="rId55" xr:uid="{00000000-0004-0000-0100-000036000000}"/>
+    <hyperlink ref="J57" r:id="rId56" xr:uid="{00000000-0004-0000-0100-000037000000}"/>
+    <hyperlink ref="J58" r:id="rId57" xr:uid="{00000000-0004-0000-0100-000038000000}"/>
+    <hyperlink ref="J59" r:id="rId58" xr:uid="{00000000-0004-0000-0100-000039000000}"/>
+    <hyperlink ref="J60" r:id="rId59" xr:uid="{00000000-0004-0000-0100-00003A000000}"/>
+    <hyperlink ref="J61" r:id="rId60" xr:uid="{00000000-0004-0000-0100-00003B000000}"/>
+    <hyperlink ref="J62" r:id="rId61" xr:uid="{00000000-0004-0000-0100-00003C000000}"/>
+    <hyperlink ref="J63" r:id="rId62" xr:uid="{00000000-0004-0000-0100-00003D000000}"/>
+    <hyperlink ref="J64" r:id="rId63" xr:uid="{00000000-0004-0000-0100-00003E000000}"/>
+    <hyperlink ref="J65" r:id="rId64" xr:uid="{00000000-0004-0000-0100-00003F000000}"/>
+    <hyperlink ref="J66" r:id="rId65" xr:uid="{00000000-0004-0000-0100-000040000000}"/>
+    <hyperlink ref="J67" r:id="rId66" xr:uid="{00000000-0004-0000-0100-000041000000}"/>
+    <hyperlink ref="J68" r:id="rId67" xr:uid="{00000000-0004-0000-0100-000042000000}"/>
+    <hyperlink ref="J69" r:id="rId68" xr:uid="{00000000-0004-0000-0100-000043000000}"/>
+    <hyperlink ref="J70" r:id="rId69" xr:uid="{00000000-0004-0000-0100-000044000000}"/>
+    <hyperlink ref="J71" r:id="rId70" xr:uid="{00000000-0004-0000-0100-000045000000}"/>
+    <hyperlink ref="J72" r:id="rId71" xr:uid="{00000000-0004-0000-0100-000046000000}"/>
+    <hyperlink ref="J73" r:id="rId72" xr:uid="{00000000-0004-0000-0100-000047000000}"/>
+    <hyperlink ref="J74" r:id="rId73" xr:uid="{00000000-0004-0000-0100-000048000000}"/>
+    <hyperlink ref="J75" r:id="rId74" xr:uid="{00000000-0004-0000-0100-000049000000}"/>
+    <hyperlink ref="J76" r:id="rId75" xr:uid="{00000000-0004-0000-0100-00004A000000}"/>
+    <hyperlink ref="J77" r:id="rId76" xr:uid="{00000000-0004-0000-0100-00004B000000}"/>
+    <hyperlink ref="J78" r:id="rId77" xr:uid="{00000000-0004-0000-0100-00004C000000}"/>
+    <hyperlink ref="J79" r:id="rId78" xr:uid="{00000000-0004-0000-0100-00004D000000}"/>
+    <hyperlink ref="J80" r:id="rId79" xr:uid="{00000000-0004-0000-0100-00004E000000}"/>
+    <hyperlink ref="J81" r:id="rId80" xr:uid="{00000000-0004-0000-0100-00004F000000}"/>
+    <hyperlink ref="J82" r:id="rId81" xr:uid="{00000000-0004-0000-0100-000050000000}"/>
+    <hyperlink ref="J83" r:id="rId82" xr:uid="{00000000-0004-0000-0100-000051000000}"/>
+    <hyperlink ref="J84" r:id="rId83" xr:uid="{00000000-0004-0000-0100-000052000000}"/>
+    <hyperlink ref="J85" r:id="rId84" xr:uid="{00000000-0004-0000-0100-000053000000}"/>
+    <hyperlink ref="J86" r:id="rId85" xr:uid="{00000000-0004-0000-0100-000054000000}"/>
+    <hyperlink ref="J87" r:id="rId86" xr:uid="{00000000-0004-0000-0100-000055000000}"/>
+    <hyperlink ref="J88" r:id="rId87" xr:uid="{00000000-0004-0000-0100-000056000000}"/>
+    <hyperlink ref="J89" r:id="rId88" xr:uid="{00000000-0004-0000-0100-000057000000}"/>
+    <hyperlink ref="J90" r:id="rId89" xr:uid="{00000000-0004-0000-0100-000058000000}"/>
+    <hyperlink ref="J91" r:id="rId90" xr:uid="{00000000-0004-0000-0100-000059000000}"/>
+    <hyperlink ref="J92" r:id="rId91" xr:uid="{00000000-0004-0000-0100-00005A000000}"/>
+    <hyperlink ref="J93" r:id="rId92" xr:uid="{00000000-0004-0000-0100-00005B000000}"/>
+    <hyperlink ref="J94" r:id="rId93" xr:uid="{00000000-0004-0000-0100-00005C000000}"/>
+    <hyperlink ref="J95" r:id="rId94" xr:uid="{00000000-0004-0000-0100-00005D000000}"/>
+    <hyperlink ref="J96" r:id="rId95" xr:uid="{00000000-0004-0000-0100-00005E000000}"/>
+    <hyperlink ref="J97" r:id="rId96" xr:uid="{00000000-0004-0000-0100-00005F000000}"/>
+    <hyperlink ref="J98" r:id="rId97" xr:uid="{00000000-0004-0000-0100-000060000000}"/>
+    <hyperlink ref="J99" r:id="rId98" xr:uid="{00000000-0004-0000-0100-000061000000}"/>
+    <hyperlink ref="J100" r:id="rId99" xr:uid="{00000000-0004-0000-0100-000062000000}"/>
+    <hyperlink ref="J101" r:id="rId100" xr:uid="{00000000-0004-0000-0100-000063000000}"/>
+    <hyperlink ref="J102" r:id="rId101" xr:uid="{00000000-0004-0000-0100-000064000000}"/>
+    <hyperlink ref="J103" r:id="rId102" xr:uid="{00000000-0004-0000-0100-000065000000}"/>
+    <hyperlink ref="J104" r:id="rId103" xr:uid="{00000000-0004-0000-0100-000066000000}"/>
+    <hyperlink ref="J105" r:id="rId104" xr:uid="{00000000-0004-0000-0100-000067000000}"/>
+    <hyperlink ref="J106" r:id="rId105" xr:uid="{00000000-0004-0000-0100-000068000000}"/>
+    <hyperlink ref="J107" r:id="rId106" xr:uid="{00000000-0004-0000-0100-000069000000}"/>
+    <hyperlink ref="J108" r:id="rId107" xr:uid="{00000000-0004-0000-0100-00006A000000}"/>
+    <hyperlink ref="J109" r:id="rId108" xr:uid="{00000000-0004-0000-0100-00006B000000}"/>
+    <hyperlink ref="J110" r:id="rId109" xr:uid="{00000000-0004-0000-0100-00006C000000}"/>
+    <hyperlink ref="J111" r:id="rId110" xr:uid="{00000000-0004-0000-0100-00006D000000}"/>
+    <hyperlink ref="J112" r:id="rId111" xr:uid="{00000000-0004-0000-0100-00006E000000}"/>
+    <hyperlink ref="J113" r:id="rId112" xr:uid="{00000000-0004-0000-0100-00006F000000}"/>
+    <hyperlink ref="J114" r:id="rId113" xr:uid="{00000000-0004-0000-0100-000070000000}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -12282,8 +12360,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -12294,22 +12372,22 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="25.5" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="33.1640625" customWidth="1"/>
-    <col min="8" max="8" width="9.5" customWidth="1"/>
-    <col min="9" max="9" width="17.5" customWidth="1"/>
-    <col min="10" max="10" width="33.1640625" customWidth="1"/>
-    <col min="11" max="16" width="21.5" customWidth="1"/>
+    <col min="7" max="7" width="33.140625" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="10" max="10" width="33.140625" customWidth="1"/>
+    <col min="11" max="16" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="39.75" customHeight="1">
+    <row r="1" spans="1:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>850</v>
       </c>
@@ -12347,7 +12425,7 @@
       <c r="O1" s="12"/>
       <c r="P1" s="12"/>
     </row>
-    <row r="2" spans="1:16" ht="12">
+    <row r="2" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -12379,7 +12457,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="12">
+    <row r="3" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -12411,7 +12489,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="12">
+    <row r="4" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -12443,7 +12521,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="12">
+    <row r="5" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -12475,7 +12553,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="12">
+    <row r="6" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -12507,7 +12585,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="12">
+    <row r="7" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -12539,7 +12617,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="12">
+    <row r="8" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -12571,7 +12649,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="12">
+    <row r="9" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -12603,7 +12681,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="12">
+    <row r="10" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -12635,7 +12713,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="12">
+    <row r="11" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -12667,7 +12745,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="12">
+    <row r="12" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -12699,7 +12777,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="12">
+    <row r="13" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -12731,7 +12809,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="12">
+    <row r="14" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -12763,7 +12841,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="12">
+    <row r="15" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -12795,7 +12873,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="12">
+    <row r="16" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -12827,7 +12905,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="12">
+    <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -12859,7 +12937,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="36">
+    <row r="18" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -12891,7 +12969,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="12">
+    <row r="19" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -12923,7 +13001,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="12">
+    <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -12955,7 +13033,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="12">
+    <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -12987,7 +13065,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="12">
+    <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -13019,7 +13097,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="12">
+    <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -13051,7 +13129,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="12">
+    <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -13083,7 +13161,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="12">
+    <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -13115,7 +13193,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="12">
+    <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -13147,7 +13225,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="12">
+    <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -13179,7 +13257,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="12">
+    <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -13211,7 +13289,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="12">
+    <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -13243,7 +13321,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="12">
+    <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -13275,7 +13353,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="12">
+    <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -13307,7 +13385,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="12">
+    <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -13339,7 +13417,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="12">
+    <row r="33" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -13371,7 +13449,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="12">
+    <row r="34" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -13403,7 +13481,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="12">
+    <row r="35" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -13435,7 +13513,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="12">
+    <row r="36" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -13467,7 +13545,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="12">
+    <row r="37" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -13499,7 +13577,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="12">
+    <row r="38" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -13531,7 +13609,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="12">
+    <row r="39" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -13563,7 +13641,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="12">
+    <row r="40" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -13595,7 +13673,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="12">
+    <row r="41" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -13627,7 +13705,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="12">
+    <row r="42" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -13659,7 +13737,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="12">
+    <row r="43" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -13691,7 +13769,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="12">
+    <row r="44" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -13723,7 +13801,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="12">
+    <row r="45" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -13755,7 +13833,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="12">
+    <row r="46" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -13787,7 +13865,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="12">
+    <row r="47" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -13819,7 +13897,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="12">
+    <row r="48" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -13851,7 +13929,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="12">
+    <row r="49" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -13883,7 +13961,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="12">
+    <row r="50" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -13915,7 +13993,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="12">
+    <row r="51" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -13947,7 +14025,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="12">
+    <row r="52" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -13979,7 +14057,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="12">
+    <row r="53" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -14011,7 +14089,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="12">
+    <row r="54" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -14043,7 +14121,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="12">
+    <row r="55" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -14075,7 +14153,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="12">
+    <row r="56" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -14107,7 +14185,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="12">
+    <row r="57" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -14139,7 +14217,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="12">
+    <row r="58" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -14171,7 +14249,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="12">
+    <row r="59" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -14203,7 +14281,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="12">
+    <row r="60" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -14235,7 +14313,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="12">
+    <row r="61" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -14267,7 +14345,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="12">
+    <row r="62" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -14299,7 +14377,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="12">
+    <row r="63" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -14331,7 +14409,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="24">
+    <row r="64" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -14363,7 +14441,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="12">
+    <row r="65" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -14395,7 +14473,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="12">
+    <row r="66" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -14427,7 +14505,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="12">
+    <row r="67" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -14459,7 +14537,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="12">
+    <row r="68" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -14491,7 +14569,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="12">
+    <row r="69" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -14523,7 +14601,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="12">
+    <row r="70" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -14555,7 +14633,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="12">
+    <row r="71" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -14587,7 +14665,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="12">
+    <row r="72" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -14619,7 +14697,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="12">
+    <row r="73" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -14651,7 +14729,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="12">
+    <row r="74" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -14683,7 +14761,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="12">
+    <row r="75" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -14715,7 +14793,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="12">
+    <row r="76" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -14747,7 +14825,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="12">
+    <row r="77" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -14779,7 +14857,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="12">
+    <row r="78" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -14811,7 +14889,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="12">
+    <row r="79" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -14843,7 +14921,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="12">
+    <row r="80" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -14875,7 +14953,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="12">
+    <row r="81" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -14907,7 +14985,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="12">
+    <row r="82" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -14939,7 +15017,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="12">
+    <row r="83" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -14971,7 +15049,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="12">
+    <row r="84" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="3">
         <v>83</v>
       </c>
@@ -15003,7 +15081,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="12">
+    <row r="85" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
         <v>84</v>
       </c>
@@ -15035,7 +15113,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="12">
+    <row r="86" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="3">
         <v>85</v>
       </c>
@@ -15067,7 +15145,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="12">
+    <row r="87" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>86</v>
       </c>
@@ -15099,7 +15177,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="12">
+    <row r="88" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="3">
         <v>87</v>
       </c>
@@ -15128,7 +15206,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="12">
+    <row r="89" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
         <v>88</v>
       </c>
@@ -15157,7 +15235,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="12">
+    <row r="90" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="3">
         <v>89</v>
       </c>
@@ -15189,7 +15267,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="12">
+    <row r="91" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="3">
         <v>90</v>
       </c>
@@ -15221,7 +15299,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="12">
+    <row r="92" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="3">
         <v>91</v>
       </c>
@@ -15253,7 +15331,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="12">
+    <row r="93" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="3">
         <v>92</v>
       </c>
@@ -15285,7 +15363,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="12">
+    <row r="94" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="3">
         <v>93</v>
       </c>
@@ -15317,7 +15395,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="95" spans="1:10" ht="12">
+    <row r="95" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="3">
         <v>94</v>
       </c>
@@ -15349,7 +15427,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="96" spans="1:10" ht="12">
+    <row r="96" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="3">
         <v>95</v>
       </c>
@@ -15381,7 +15459,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="12">
+    <row r="97" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="3">
         <v>96</v>
       </c>
@@ -15413,7 +15491,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="12">
+    <row r="98" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" s="3">
         <v>97</v>
       </c>
@@ -15442,7 +15520,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="99" spans="1:10" ht="12">
+    <row r="99" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="3">
         <v>98</v>
       </c>
@@ -15474,7 +15552,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="12">
+    <row r="100" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A100" s="3">
         <v>99</v>
       </c>
@@ -15506,7 +15584,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="12">
+    <row r="101" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A101" s="3">
         <v>100</v>
       </c>
@@ -15538,7 +15616,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="12">
+    <row r="102" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" s="3">
         <v>101</v>
       </c>
@@ -15570,7 +15648,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="103" spans="1:10" ht="12">
+    <row r="103" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A103" s="3">
         <v>102</v>
       </c>
@@ -15602,7 +15680,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="104" spans="1:10" ht="12">
+    <row r="104" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A104" s="3">
         <v>103</v>
       </c>
@@ -15634,7 +15712,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="105" spans="1:10" ht="12">
+    <row r="105" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A105" s="3">
         <v>104</v>
       </c>
@@ -15666,7 +15744,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="106" spans="1:10" ht="12">
+    <row r="106" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A106" s="3">
         <v>105</v>
       </c>
@@ -15698,7 +15776,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="12">
+    <row r="107" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A107" s="3">
         <v>106</v>
       </c>
@@ -15730,7 +15808,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="108" spans="1:10" ht="12">
+    <row r="108" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A108" s="3">
         <v>107</v>
       </c>
@@ -15762,7 +15840,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="109" spans="1:10" ht="12">
+    <row r="109" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A109" s="3">
         <v>108</v>
       </c>
@@ -15794,271 +15872,271 @@
         <v>849</v>
       </c>
     </row>
-    <row r="110" spans="1:10" ht="12">
+    <row r="110" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J110" s="15"/>
     </row>
-    <row r="111" spans="1:10" ht="12">
+    <row r="111" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J111" s="15"/>
     </row>
-    <row r="112" spans="1:10" ht="12">
+    <row r="112" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J112" s="15"/>
     </row>
-    <row r="113" spans="10:10" ht="12">
+    <row r="113" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J113" s="15"/>
     </row>
-    <row r="114" spans="10:10" ht="12">
+    <row r="114" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J114" s="15"/>
     </row>
-    <row r="115" spans="10:10" ht="12">
+    <row r="115" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J115" s="15"/>
     </row>
-    <row r="116" spans="10:10" ht="12">
+    <row r="116" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J116" s="15"/>
     </row>
-    <row r="117" spans="10:10" ht="12">
+    <row r="117" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J117" s="15"/>
     </row>
-    <row r="118" spans="10:10" ht="12">
+    <row r="118" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J118" s="15"/>
     </row>
-    <row r="119" spans="10:10" ht="12">
+    <row r="119" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J119" s="15"/>
     </row>
-    <row r="120" spans="10:10" ht="12">
+    <row r="120" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J120" s="15"/>
     </row>
-    <row r="121" spans="10:10" ht="12">
+    <row r="121" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J121" s="15"/>
     </row>
-    <row r="122" spans="10:10" ht="12">
+    <row r="122" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J122" s="15"/>
     </row>
-    <row r="123" spans="10:10" ht="12">
+    <row r="123" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J123" s="15"/>
     </row>
-    <row r="124" spans="10:10" ht="12">
+    <row r="124" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J124" s="15"/>
     </row>
-    <row r="125" spans="10:10" ht="12">
+    <row r="125" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J125" s="15"/>
     </row>
-    <row r="126" spans="10:10" ht="12">
+    <row r="126" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J126" s="15"/>
     </row>
-    <row r="127" spans="10:10" ht="12">
+    <row r="127" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J127" s="15"/>
     </row>
-    <row r="128" spans="10:10" ht="12">
+    <row r="128" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J128" s="15"/>
     </row>
-    <row r="129" spans="10:10" ht="12">
+    <row r="129" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J129" s="15"/>
     </row>
-    <row r="130" spans="10:10" ht="12">
+    <row r="130" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J130" s="15"/>
     </row>
-    <row r="131" spans="10:10" ht="12">
+    <row r="131" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J131" s="15"/>
     </row>
-    <row r="132" spans="10:10" ht="12">
+    <row r="132" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J132" s="15"/>
     </row>
-    <row r="133" spans="10:10" ht="12">
+    <row r="133" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J133" s="15"/>
     </row>
-    <row r="134" spans="10:10" ht="12">
+    <row r="134" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J134" s="15"/>
     </row>
-    <row r="135" spans="10:10" ht="12">
+    <row r="135" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J135" s="15"/>
     </row>
-    <row r="136" spans="10:10" ht="12">
+    <row r="136" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J136" s="15"/>
     </row>
-    <row r="137" spans="10:10" ht="12">
+    <row r="137" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J137" s="15"/>
     </row>
-    <row r="138" spans="10:10" ht="12">
+    <row r="138" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J138" s="15"/>
     </row>
-    <row r="139" spans="10:10" ht="12">
+    <row r="139" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J139" s="15"/>
     </row>
-    <row r="140" spans="10:10" ht="12">
+    <row r="140" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J140" s="15"/>
     </row>
-    <row r="141" spans="10:10" ht="12">
+    <row r="141" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J141" s="15"/>
     </row>
-    <row r="142" spans="10:10" ht="12">
+    <row r="142" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J142" s="15"/>
     </row>
-    <row r="143" spans="10:10" ht="12">
+    <row r="143" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J143" s="15"/>
     </row>
-    <row r="144" spans="10:10" ht="12">
+    <row r="144" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J144" s="15"/>
     </row>
-    <row r="145" spans="10:10" ht="12">
+    <row r="145" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J145" s="15"/>
     </row>
-    <row r="146" spans="10:10" ht="12">
+    <row r="146" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J146" s="15"/>
     </row>
-    <row r="147" spans="10:10" ht="12">
+    <row r="147" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J147" s="15"/>
     </row>
-    <row r="148" spans="10:10" ht="12">
+    <row r="148" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J148" s="15"/>
     </row>
-    <row r="149" spans="10:10" ht="12">
+    <row r="149" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J149" s="15"/>
     </row>
-    <row r="150" spans="10:10" ht="12">
+    <row r="150" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J150" s="15"/>
     </row>
-    <row r="151" spans="10:10" ht="12">
+    <row r="151" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J151" s="15"/>
     </row>
-    <row r="152" spans="10:10" ht="12">
+    <row r="152" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J152" s="15"/>
     </row>
-    <row r="153" spans="10:10" ht="12">
+    <row r="153" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J153" s="15"/>
     </row>
-    <row r="154" spans="10:10" ht="12">
+    <row r="154" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J154" s="15"/>
     </row>
-    <row r="155" spans="10:10" ht="12">
+    <row r="155" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J155" s="15"/>
     </row>
-    <row r="156" spans="10:10" ht="12">
+    <row r="156" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J156" s="15"/>
     </row>
-    <row r="157" spans="10:10" ht="12">
+    <row r="157" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J157" s="15"/>
     </row>
-    <row r="158" spans="10:10" ht="12">
+    <row r="158" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J158" s="15"/>
     </row>
-    <row r="159" spans="10:10" ht="12">
+    <row r="159" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J159" s="15"/>
     </row>
-    <row r="160" spans="10:10" ht="12">
+    <row r="160" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J160" s="15"/>
     </row>
-    <row r="161" spans="10:10" ht="12">
+    <row r="161" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J161" s="15"/>
     </row>
-    <row r="162" spans="10:10" ht="12">
+    <row r="162" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J162" s="15"/>
     </row>
-    <row r="163" spans="10:10" ht="12">
+    <row r="163" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J163" s="15"/>
     </row>
-    <row r="164" spans="10:10" ht="12">
+    <row r="164" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J164" s="15"/>
     </row>
-    <row r="165" spans="10:10" ht="12">
+    <row r="165" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J165" s="15"/>
     </row>
-    <row r="166" spans="10:10" ht="12">
+    <row r="166" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J166" s="15"/>
     </row>
-    <row r="167" spans="10:10" ht="12">
+    <row r="167" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J167" s="15"/>
     </row>
-    <row r="168" spans="10:10" ht="12">
+    <row r="168" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J168" s="15"/>
     </row>
-    <row r="169" spans="10:10" ht="12">
+    <row r="169" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J169" s="15"/>
     </row>
-    <row r="170" spans="10:10" ht="12">
+    <row r="170" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J170" s="15"/>
     </row>
-    <row r="171" spans="10:10" ht="12">
+    <row r="171" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J171" s="15"/>
     </row>
-    <row r="172" spans="10:10" ht="12">
+    <row r="172" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J172" s="15"/>
     </row>
-    <row r="173" spans="10:10" ht="12">
+    <row r="173" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J173" s="15"/>
     </row>
-    <row r="174" spans="10:10" ht="12">
+    <row r="174" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J174" s="15"/>
     </row>
-    <row r="175" spans="10:10" ht="12">
+    <row r="175" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J175" s="15"/>
     </row>
-    <row r="176" spans="10:10" ht="12">
+    <row r="176" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J176" s="15"/>
     </row>
-    <row r="177" spans="10:10" ht="12">
+    <row r="177" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J177" s="15"/>
     </row>
-    <row r="178" spans="10:10" ht="12">
+    <row r="178" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J178" s="15"/>
     </row>
-    <row r="179" spans="10:10" ht="12">
+    <row r="179" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J179" s="15"/>
     </row>
-    <row r="180" spans="10:10" ht="12">
+    <row r="180" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J180" s="15"/>
     </row>
-    <row r="181" spans="10:10" ht="12">
+    <row r="181" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J181" s="15"/>
     </row>
-    <row r="182" spans="10:10" ht="12">
+    <row r="182" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J182" s="15"/>
     </row>
-    <row r="183" spans="10:10" ht="12">
+    <row r="183" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J183" s="15"/>
     </row>
-    <row r="184" spans="10:10" ht="12">
+    <row r="184" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J184" s="15"/>
     </row>
-    <row r="185" spans="10:10" ht="12">
+    <row r="185" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J185" s="15"/>
     </row>
-    <row r="186" spans="10:10" ht="12">
+    <row r="186" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J186" s="15"/>
     </row>
-    <row r="187" spans="10:10" ht="12">
+    <row r="187" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J187" s="15"/>
     </row>
-    <row r="188" spans="10:10" ht="12">
+    <row r="188" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J188" s="15"/>
     </row>
-    <row r="189" spans="10:10" ht="12">
+    <row r="189" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J189" s="15"/>
     </row>
-    <row r="190" spans="10:10" ht="12">
+    <row r="190" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J190" s="15"/>
     </row>
-    <row r="191" spans="10:10" ht="12">
+    <row r="191" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J191" s="15"/>
     </row>
-    <row r="192" spans="10:10" ht="12">
+    <row r="192" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J192" s="15"/>
     </row>
-    <row r="193" spans="10:10" ht="12">
+    <row r="193" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J193" s="15"/>
     </row>
-    <row r="194" spans="10:10" ht="12">
+    <row r="194" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J194" s="15"/>
     </row>
-    <row r="195" spans="10:10" ht="12">
+    <row r="195" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J195" s="15"/>
     </row>
-    <row r="196" spans="10:10" ht="12">
+    <row r="196" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J196" s="15"/>
     </row>
-    <row r="197" spans="10:10" ht="12">
+    <row r="197" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J197" s="15"/>
     </row>
-    <row r="198" spans="10:10" ht="12">
+    <row r="198" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J198" s="15"/>
     </row>
   </sheetData>
@@ -16068,114 +16146,114 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1"/>
-    <hyperlink ref="J3" r:id="rId2"/>
-    <hyperlink ref="J4" r:id="rId3"/>
-    <hyperlink ref="J5" r:id="rId4"/>
-    <hyperlink ref="J6" r:id="rId5"/>
-    <hyperlink ref="J7" r:id="rId6"/>
-    <hyperlink ref="J8" r:id="rId7"/>
-    <hyperlink ref="J9" r:id="rId8"/>
-    <hyperlink ref="J10" r:id="rId9"/>
-    <hyperlink ref="J11" r:id="rId10"/>
-    <hyperlink ref="J12" r:id="rId11"/>
-    <hyperlink ref="J13" r:id="rId12"/>
-    <hyperlink ref="J14" r:id="rId13"/>
-    <hyperlink ref="J15" r:id="rId14"/>
-    <hyperlink ref="J16" r:id="rId15"/>
-    <hyperlink ref="J17" r:id="rId16"/>
-    <hyperlink ref="J18" r:id="rId17"/>
-    <hyperlink ref="J19" r:id="rId18"/>
-    <hyperlink ref="J20" r:id="rId19"/>
-    <hyperlink ref="J21" r:id="rId20"/>
-    <hyperlink ref="J22" r:id="rId21"/>
-    <hyperlink ref="J23" r:id="rId22"/>
-    <hyperlink ref="J24" r:id="rId23"/>
-    <hyperlink ref="J25" r:id="rId24"/>
-    <hyperlink ref="J26" r:id="rId25"/>
-    <hyperlink ref="J27" r:id="rId26"/>
-    <hyperlink ref="J28" r:id="rId27"/>
-    <hyperlink ref="J29" r:id="rId28"/>
-    <hyperlink ref="J30" r:id="rId29"/>
-    <hyperlink ref="J31" r:id="rId30"/>
-    <hyperlink ref="J32" r:id="rId31"/>
-    <hyperlink ref="J33" r:id="rId32"/>
-    <hyperlink ref="J34" r:id="rId33"/>
-    <hyperlink ref="J35" r:id="rId34"/>
-    <hyperlink ref="J36" r:id="rId35"/>
-    <hyperlink ref="J37" r:id="rId36"/>
-    <hyperlink ref="J38" r:id="rId37"/>
-    <hyperlink ref="J39" r:id="rId38"/>
-    <hyperlink ref="J40" r:id="rId39"/>
-    <hyperlink ref="J41" r:id="rId40"/>
-    <hyperlink ref="J42" r:id="rId41"/>
-    <hyperlink ref="J43" r:id="rId42"/>
-    <hyperlink ref="J44" r:id="rId43"/>
-    <hyperlink ref="J45" r:id="rId44"/>
-    <hyperlink ref="J46" r:id="rId45"/>
-    <hyperlink ref="J47" r:id="rId46"/>
-    <hyperlink ref="J48" r:id="rId47"/>
-    <hyperlink ref="J49" r:id="rId48"/>
-    <hyperlink ref="J50" r:id="rId49"/>
-    <hyperlink ref="J51" r:id="rId50"/>
-    <hyperlink ref="J52" r:id="rId51"/>
-    <hyperlink ref="J53" r:id="rId52"/>
-    <hyperlink ref="J54" r:id="rId53"/>
-    <hyperlink ref="J55" r:id="rId54"/>
-    <hyperlink ref="J56" r:id="rId55"/>
-    <hyperlink ref="J57" r:id="rId56"/>
-    <hyperlink ref="J58" r:id="rId57"/>
-    <hyperlink ref="J59" r:id="rId58"/>
-    <hyperlink ref="J60" r:id="rId59"/>
-    <hyperlink ref="J61" r:id="rId60"/>
-    <hyperlink ref="J62" r:id="rId61"/>
-    <hyperlink ref="J63" r:id="rId62"/>
-    <hyperlink ref="J64" r:id="rId63"/>
-    <hyperlink ref="J65" r:id="rId64"/>
-    <hyperlink ref="J66" r:id="rId65"/>
-    <hyperlink ref="J67" r:id="rId66"/>
-    <hyperlink ref="J68" r:id="rId67"/>
-    <hyperlink ref="J69" r:id="rId68"/>
-    <hyperlink ref="J70" r:id="rId69"/>
-    <hyperlink ref="J71" r:id="rId70"/>
-    <hyperlink ref="J72" r:id="rId71"/>
-    <hyperlink ref="J73" r:id="rId72"/>
-    <hyperlink ref="J74" r:id="rId73"/>
-    <hyperlink ref="J75" r:id="rId74"/>
-    <hyperlink ref="J76" r:id="rId75"/>
-    <hyperlink ref="J77" r:id="rId76"/>
-    <hyperlink ref="J78" r:id="rId77"/>
-    <hyperlink ref="J79" r:id="rId78"/>
-    <hyperlink ref="J80" r:id="rId79"/>
-    <hyperlink ref="J81" r:id="rId80"/>
-    <hyperlink ref="J82" r:id="rId81"/>
-    <hyperlink ref="J83" r:id="rId82"/>
-    <hyperlink ref="J84" r:id="rId83"/>
-    <hyperlink ref="J85" r:id="rId84"/>
-    <hyperlink ref="J86" r:id="rId85"/>
-    <hyperlink ref="J87" r:id="rId86"/>
-    <hyperlink ref="J88" r:id="rId87"/>
-    <hyperlink ref="J89" r:id="rId88"/>
-    <hyperlink ref="J90" r:id="rId89"/>
-    <hyperlink ref="J91" r:id="rId90"/>
-    <hyperlink ref="J92" r:id="rId91"/>
-    <hyperlink ref="J93" r:id="rId92"/>
-    <hyperlink ref="J94" r:id="rId93"/>
-    <hyperlink ref="J95" r:id="rId94"/>
-    <hyperlink ref="J96" r:id="rId95"/>
-    <hyperlink ref="J97" r:id="rId96"/>
-    <hyperlink ref="J98" r:id="rId97"/>
-    <hyperlink ref="J99" r:id="rId98"/>
-    <hyperlink ref="J100" r:id="rId99"/>
-    <hyperlink ref="J101" r:id="rId100"/>
-    <hyperlink ref="J102" r:id="rId101"/>
-    <hyperlink ref="J103" r:id="rId102"/>
-    <hyperlink ref="J104" r:id="rId103"/>
-    <hyperlink ref="J105" r:id="rId104"/>
-    <hyperlink ref="J106" r:id="rId105"/>
-    <hyperlink ref="J107" r:id="rId106"/>
-    <hyperlink ref="J108" r:id="rId107"/>
-    <hyperlink ref="J109" r:id="rId108"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="J3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="J4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="J5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="J6" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="J7" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="J8" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="J9" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="J10" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="J11" r:id="rId10" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="J12" r:id="rId11" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
+    <hyperlink ref="J13" r:id="rId12" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
+    <hyperlink ref="J14" r:id="rId13" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
+    <hyperlink ref="J15" r:id="rId14" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
+    <hyperlink ref="J16" r:id="rId15" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
+    <hyperlink ref="J17" r:id="rId16" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
+    <hyperlink ref="J18" r:id="rId17" xr:uid="{00000000-0004-0000-0200-000010000000}"/>
+    <hyperlink ref="J19" r:id="rId18" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
+    <hyperlink ref="J20" r:id="rId19" xr:uid="{00000000-0004-0000-0200-000012000000}"/>
+    <hyperlink ref="J21" r:id="rId20" xr:uid="{00000000-0004-0000-0200-000013000000}"/>
+    <hyperlink ref="J22" r:id="rId21" xr:uid="{00000000-0004-0000-0200-000014000000}"/>
+    <hyperlink ref="J23" r:id="rId22" xr:uid="{00000000-0004-0000-0200-000015000000}"/>
+    <hyperlink ref="J24" r:id="rId23" xr:uid="{00000000-0004-0000-0200-000016000000}"/>
+    <hyperlink ref="J25" r:id="rId24" xr:uid="{00000000-0004-0000-0200-000017000000}"/>
+    <hyperlink ref="J26" r:id="rId25" xr:uid="{00000000-0004-0000-0200-000018000000}"/>
+    <hyperlink ref="J27" r:id="rId26" xr:uid="{00000000-0004-0000-0200-000019000000}"/>
+    <hyperlink ref="J28" r:id="rId27" xr:uid="{00000000-0004-0000-0200-00001A000000}"/>
+    <hyperlink ref="J29" r:id="rId28" xr:uid="{00000000-0004-0000-0200-00001B000000}"/>
+    <hyperlink ref="J30" r:id="rId29" xr:uid="{00000000-0004-0000-0200-00001C000000}"/>
+    <hyperlink ref="J31" r:id="rId30" xr:uid="{00000000-0004-0000-0200-00001D000000}"/>
+    <hyperlink ref="J32" r:id="rId31" xr:uid="{00000000-0004-0000-0200-00001E000000}"/>
+    <hyperlink ref="J33" r:id="rId32" xr:uid="{00000000-0004-0000-0200-00001F000000}"/>
+    <hyperlink ref="J34" r:id="rId33" xr:uid="{00000000-0004-0000-0200-000020000000}"/>
+    <hyperlink ref="J35" r:id="rId34" xr:uid="{00000000-0004-0000-0200-000021000000}"/>
+    <hyperlink ref="J36" r:id="rId35" xr:uid="{00000000-0004-0000-0200-000022000000}"/>
+    <hyperlink ref="J37" r:id="rId36" xr:uid="{00000000-0004-0000-0200-000023000000}"/>
+    <hyperlink ref="J38" r:id="rId37" xr:uid="{00000000-0004-0000-0200-000024000000}"/>
+    <hyperlink ref="J39" r:id="rId38" xr:uid="{00000000-0004-0000-0200-000025000000}"/>
+    <hyperlink ref="J40" r:id="rId39" xr:uid="{00000000-0004-0000-0200-000026000000}"/>
+    <hyperlink ref="J41" r:id="rId40" xr:uid="{00000000-0004-0000-0200-000027000000}"/>
+    <hyperlink ref="J42" r:id="rId41" xr:uid="{00000000-0004-0000-0200-000028000000}"/>
+    <hyperlink ref="J43" r:id="rId42" xr:uid="{00000000-0004-0000-0200-000029000000}"/>
+    <hyperlink ref="J44" r:id="rId43" xr:uid="{00000000-0004-0000-0200-00002A000000}"/>
+    <hyperlink ref="J45" r:id="rId44" xr:uid="{00000000-0004-0000-0200-00002B000000}"/>
+    <hyperlink ref="J46" r:id="rId45" xr:uid="{00000000-0004-0000-0200-00002C000000}"/>
+    <hyperlink ref="J47" r:id="rId46" xr:uid="{00000000-0004-0000-0200-00002D000000}"/>
+    <hyperlink ref="J48" r:id="rId47" xr:uid="{00000000-0004-0000-0200-00002E000000}"/>
+    <hyperlink ref="J49" r:id="rId48" xr:uid="{00000000-0004-0000-0200-00002F000000}"/>
+    <hyperlink ref="J50" r:id="rId49" xr:uid="{00000000-0004-0000-0200-000030000000}"/>
+    <hyperlink ref="J51" r:id="rId50" xr:uid="{00000000-0004-0000-0200-000031000000}"/>
+    <hyperlink ref="J52" r:id="rId51" xr:uid="{00000000-0004-0000-0200-000032000000}"/>
+    <hyperlink ref="J53" r:id="rId52" xr:uid="{00000000-0004-0000-0200-000033000000}"/>
+    <hyperlink ref="J54" r:id="rId53" xr:uid="{00000000-0004-0000-0200-000034000000}"/>
+    <hyperlink ref="J55" r:id="rId54" xr:uid="{00000000-0004-0000-0200-000035000000}"/>
+    <hyperlink ref="J56" r:id="rId55" xr:uid="{00000000-0004-0000-0200-000036000000}"/>
+    <hyperlink ref="J57" r:id="rId56" xr:uid="{00000000-0004-0000-0200-000037000000}"/>
+    <hyperlink ref="J58" r:id="rId57" xr:uid="{00000000-0004-0000-0200-000038000000}"/>
+    <hyperlink ref="J59" r:id="rId58" xr:uid="{00000000-0004-0000-0200-000039000000}"/>
+    <hyperlink ref="J60" r:id="rId59" xr:uid="{00000000-0004-0000-0200-00003A000000}"/>
+    <hyperlink ref="J61" r:id="rId60" xr:uid="{00000000-0004-0000-0200-00003B000000}"/>
+    <hyperlink ref="J62" r:id="rId61" xr:uid="{00000000-0004-0000-0200-00003C000000}"/>
+    <hyperlink ref="J63" r:id="rId62" xr:uid="{00000000-0004-0000-0200-00003D000000}"/>
+    <hyperlink ref="J64" r:id="rId63" xr:uid="{00000000-0004-0000-0200-00003E000000}"/>
+    <hyperlink ref="J65" r:id="rId64" xr:uid="{00000000-0004-0000-0200-00003F000000}"/>
+    <hyperlink ref="J66" r:id="rId65" xr:uid="{00000000-0004-0000-0200-000040000000}"/>
+    <hyperlink ref="J67" r:id="rId66" xr:uid="{00000000-0004-0000-0200-000041000000}"/>
+    <hyperlink ref="J68" r:id="rId67" xr:uid="{00000000-0004-0000-0200-000042000000}"/>
+    <hyperlink ref="J69" r:id="rId68" xr:uid="{00000000-0004-0000-0200-000043000000}"/>
+    <hyperlink ref="J70" r:id="rId69" xr:uid="{00000000-0004-0000-0200-000044000000}"/>
+    <hyperlink ref="J71" r:id="rId70" xr:uid="{00000000-0004-0000-0200-000045000000}"/>
+    <hyperlink ref="J72" r:id="rId71" xr:uid="{00000000-0004-0000-0200-000046000000}"/>
+    <hyperlink ref="J73" r:id="rId72" xr:uid="{00000000-0004-0000-0200-000047000000}"/>
+    <hyperlink ref="J74" r:id="rId73" xr:uid="{00000000-0004-0000-0200-000048000000}"/>
+    <hyperlink ref="J75" r:id="rId74" xr:uid="{00000000-0004-0000-0200-000049000000}"/>
+    <hyperlink ref="J76" r:id="rId75" xr:uid="{00000000-0004-0000-0200-00004A000000}"/>
+    <hyperlink ref="J77" r:id="rId76" xr:uid="{00000000-0004-0000-0200-00004B000000}"/>
+    <hyperlink ref="J78" r:id="rId77" xr:uid="{00000000-0004-0000-0200-00004C000000}"/>
+    <hyperlink ref="J79" r:id="rId78" xr:uid="{00000000-0004-0000-0200-00004D000000}"/>
+    <hyperlink ref="J80" r:id="rId79" xr:uid="{00000000-0004-0000-0200-00004E000000}"/>
+    <hyperlink ref="J81" r:id="rId80" xr:uid="{00000000-0004-0000-0200-00004F000000}"/>
+    <hyperlink ref="J82" r:id="rId81" xr:uid="{00000000-0004-0000-0200-000050000000}"/>
+    <hyperlink ref="J83" r:id="rId82" xr:uid="{00000000-0004-0000-0200-000051000000}"/>
+    <hyperlink ref="J84" r:id="rId83" xr:uid="{00000000-0004-0000-0200-000052000000}"/>
+    <hyperlink ref="J85" r:id="rId84" xr:uid="{00000000-0004-0000-0200-000053000000}"/>
+    <hyperlink ref="J86" r:id="rId85" xr:uid="{00000000-0004-0000-0200-000054000000}"/>
+    <hyperlink ref="J87" r:id="rId86" xr:uid="{00000000-0004-0000-0200-000055000000}"/>
+    <hyperlink ref="J88" r:id="rId87" xr:uid="{00000000-0004-0000-0200-000056000000}"/>
+    <hyperlink ref="J89" r:id="rId88" xr:uid="{00000000-0004-0000-0200-000057000000}"/>
+    <hyperlink ref="J90" r:id="rId89" xr:uid="{00000000-0004-0000-0200-000058000000}"/>
+    <hyperlink ref="J91" r:id="rId90" xr:uid="{00000000-0004-0000-0200-000059000000}"/>
+    <hyperlink ref="J92" r:id="rId91" xr:uid="{00000000-0004-0000-0200-00005A000000}"/>
+    <hyperlink ref="J93" r:id="rId92" xr:uid="{00000000-0004-0000-0200-00005B000000}"/>
+    <hyperlink ref="J94" r:id="rId93" xr:uid="{00000000-0004-0000-0200-00005C000000}"/>
+    <hyperlink ref="J95" r:id="rId94" xr:uid="{00000000-0004-0000-0200-00005D000000}"/>
+    <hyperlink ref="J96" r:id="rId95" xr:uid="{00000000-0004-0000-0200-00005E000000}"/>
+    <hyperlink ref="J97" r:id="rId96" xr:uid="{00000000-0004-0000-0200-00005F000000}"/>
+    <hyperlink ref="J98" r:id="rId97" xr:uid="{00000000-0004-0000-0200-000060000000}"/>
+    <hyperlink ref="J99" r:id="rId98" xr:uid="{00000000-0004-0000-0200-000061000000}"/>
+    <hyperlink ref="J100" r:id="rId99" xr:uid="{00000000-0004-0000-0200-000062000000}"/>
+    <hyperlink ref="J101" r:id="rId100" xr:uid="{00000000-0004-0000-0200-000063000000}"/>
+    <hyperlink ref="J102" r:id="rId101" xr:uid="{00000000-0004-0000-0200-000064000000}"/>
+    <hyperlink ref="J103" r:id="rId102" xr:uid="{00000000-0004-0000-0200-000065000000}"/>
+    <hyperlink ref="J104" r:id="rId103" xr:uid="{00000000-0004-0000-0200-000066000000}"/>
+    <hyperlink ref="J105" r:id="rId104" xr:uid="{00000000-0004-0000-0200-000067000000}"/>
+    <hyperlink ref="J106" r:id="rId105" xr:uid="{00000000-0004-0000-0200-000068000000}"/>
+    <hyperlink ref="J107" r:id="rId106" xr:uid="{00000000-0004-0000-0200-000069000000}"/>
+    <hyperlink ref="J108" r:id="rId107" xr:uid="{00000000-0004-0000-0200-00006A000000}"/>
+    <hyperlink ref="J109" r:id="rId108" xr:uid="{00000000-0004-0000-0200-00006B000000}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
Added my Juma Reg Number
</commit_message>
<xml_diff>
--- a/CS335/GitHub Info sans duplicates.xlsx
+++ b/CS335/GitHub Info sans duplicates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\lungo\staffcard\CS335\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JUMA KBS2HB\Documents\staffcard\CS335\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC84944-46C7-4A57-8DE2-0B7BC110E1DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA8BE334-FEDC-4892-B706-13BF604D5736}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3229" uniqueCount="879">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3230" uniqueCount="880">
   <si>
     <t>Timestamp</t>
   </si>
@@ -2664,6 +2664,9 @@
   </si>
   <si>
     <t>https://github.com/Sikato-41</t>
+  </si>
+  <si>
+    <t>2019-04-10833</t>
   </si>
 </sst>
 </file>
@@ -3443,11 +3446,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:R123"/>
+  <dimension ref="A1:R124"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U123" sqref="U123"/>
+      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C124" sqref="C124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8122,6 +8125,11 @@
       </c>
       <c r="L123" s="18" t="s">
         <v>878</v>
+      </c>
+    </row>
+    <row r="124" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B124" s="3" t="s">
+        <v>879</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
juma full details added
</commit_message>
<xml_diff>
--- a/CS335/GitHub Info sans duplicates.xlsx
+++ b/CS335/GitHub Info sans duplicates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JUMA KBS2HB\Documents\staffcard\CS335\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00CF72B-7498-4F37-8312-645AEE858859}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2596D40-9386-440B-BBDA-507E4ABC37FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3284" uniqueCount="900">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3292" uniqueCount="906">
   <si>
     <t>Timestamp</t>
   </si>
@@ -2730,6 +2730,24 @@
   </si>
   <si>
     <t>2019-04-10833</t>
+  </si>
+  <si>
+    <t>RAJABU</t>
+  </si>
+  <si>
+    <t>JUMA SHAIBU</t>
+  </si>
+  <si>
+    <t>ndio</t>
+  </si>
+  <si>
+    <t>jumakbs@gmail.com</t>
+  </si>
+  <si>
+    <t>jumakbs</t>
+  </si>
+  <si>
+    <t>https://github.com/jumakbs</t>
   </si>
 </sst>
 </file>
@@ -3242,8 +3260,8 @@
   <dimension ref="A1:R133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B124" sqref="B124"/>
+      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D123" sqref="D123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7930,16 +7948,36 @@
       <c r="B124" s="3" t="s">
         <v>899</v>
       </c>
-      <c r="C124" s="3"/>
-      <c r="D124" s="3"/>
-      <c r="E124" s="3"/>
-      <c r="F124" s="3"/>
-      <c r="G124" s="3"/>
-      <c r="H124" s="3"/>
-      <c r="I124" s="3"/>
-      <c r="J124" s="3"/>
-      <c r="K124" s="3"/>
-      <c r="L124" s="4"/>
+      <c r="C124" s="3" t="s">
+        <v>900</v>
+      </c>
+      <c r="D124" s="3" t="s">
+        <v>901</v>
+      </c>
+      <c r="E124" s="3">
+        <v>716865555</v>
+      </c>
+      <c r="F124" s="3" t="s">
+        <v>902</v>
+      </c>
+      <c r="G124" s="17" t="s">
+        <v>903</v>
+      </c>
+      <c r="H124" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I124" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J124" s="3">
+        <v>3</v>
+      </c>
+      <c r="K124" s="3" t="s">
+        <v>904</v>
+      </c>
+      <c r="L124" s="17" t="s">
+        <v>905</v>
+      </c>
     </row>
     <row r="125" spans="1:18" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="126" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8108,6 +8146,8 @@
     <hyperlink ref="G38" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
     <hyperlink ref="L38" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
     <hyperlink ref="G72" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="G124" r:id="rId125" xr:uid="{5C5B248C-01EA-420E-ABE2-41FC19650C15}"/>
+    <hyperlink ref="L124" r:id="rId126" xr:uid="{B1DE431B-670A-441C-B29E-CF9718E317A8}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
added crecidentials to xlsx
</commit_message>
<xml_diff>
--- a/CS335/GitHub Info sans duplicates.xlsx
+++ b/CS335/GitHub Info sans duplicates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Lungo\staffcard\CS335\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C75FFF6-9C04-4210-B0B6-F58AC4EE8A3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61C003B-D046-4C33-8590-20DF269D9423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3296" uniqueCount="909">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3300" uniqueCount="913">
   <si>
     <t>Timestamp</t>
   </si>
@@ -2757,6 +2757,18 @@
   </si>
   <si>
     <t>https://github.com/Festo99</t>
+  </si>
+  <si>
+    <t>MAPUNDA</t>
+  </si>
+  <si>
+    <t>FESTO SIDON</t>
+  </si>
+  <si>
+    <t>22019-04-05980</t>
+  </si>
+  <si>
+    <t>11/17/2021 19:50:29</t>
   </si>
 </sst>
 </file>
@@ -3272,9 +3284,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3359,10 +3371,18 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="A3" s="2" t="s">
+        <v>912</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>911</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>909</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>910</v>
+      </c>
       <c r="E3" s="26">
         <v>748020893</v>
       </c>

</xml_diff>

<commit_message>
edited my other name: Mialla to Yonas
</commit_message>
<xml_diff>
--- a/CS335/GitHub Info sans duplicates.xlsx
+++ b/CS335/GitHub Info sans duplicates.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\staffcard\CS335\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\devtPgms\xampp\htdocs\staffcard\CS335\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3322" uniqueCount="924">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3322" uniqueCount="925">
   <si>
     <t>Timestamp</t>
   </si>
@@ -2798,12 +2798,15 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>MESHACK YONAS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
@@ -3305,9 +3308,9 @@
   <dimension ref="A1:X135"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="E129" sqref="E129"/>
+      <selection pane="bottomLeft" activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5262,7 +5265,7 @@
         <v>374</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>375</v>
+        <v>924</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>376</v>

</xml_diff>

<commit_message>
updated the students' excel sheet
</commit_message>
<xml_diff>
--- a/CS335/GitHub Info sans duplicates.xlsx
+++ b/CS335/GitHub Info sans duplicates.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\devtPgms\xampp\htdocs\staffcard\CS335\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\lungo\staffcard\CS335\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B3928A-6D71-435A-A1C9-9542474283ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3322" uniqueCount="925">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3331" uniqueCount="931">
   <si>
     <t>Timestamp</t>
   </si>
@@ -2801,12 +2802,30 @@
   </si>
   <si>
     <t>MESHACK YONAS</t>
+  </si>
+  <si>
+    <t>2019-04-12003</t>
+  </si>
+  <si>
+    <t>SIKATO</t>
+  </si>
+  <si>
+    <t>AMON LAURENT</t>
+  </si>
+  <si>
+    <t>amonsikato21@gmail.com</t>
+  </si>
+  <si>
+    <t>Sikato-41</t>
+  </si>
+  <si>
+    <t>https://github.com/Sikato-41</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
@@ -3304,13 +3323,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X135"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:X137"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="E52" sqref="E52"/>
+      <selection pane="bottomLeft" activeCell="E134" sqref="E134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8168,175 +8187,215 @@
       <c r="I128" t="s">
         <v>19</v>
       </c>
-      <c r="K128" s="14" t="s">
+      <c r="K128" s="3"/>
+    </row>
+    <row r="129" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B129" t="s">
+        <v>925</v>
+      </c>
+      <c r="C129" t="s">
+        <v>926</v>
+      </c>
+      <c r="D129" t="s">
+        <v>927</v>
+      </c>
+      <c r="E129">
+        <v>629642063</v>
+      </c>
+      <c r="F129" t="s">
+        <v>16</v>
+      </c>
+      <c r="G129" s="24" t="s">
+        <v>928</v>
+      </c>
+      <c r="H129" t="s">
+        <v>18</v>
+      </c>
+      <c r="I129" t="s">
+        <v>19</v>
+      </c>
+      <c r="J129">
+        <v>3</v>
+      </c>
+      <c r="K129" t="s">
+        <v>929</v>
+      </c>
+      <c r="L129" s="24" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="130" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K130" s="14" t="s">
         <v>880</v>
       </c>
     </row>
-    <row r="129" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K129" t="s">
+    <row r="131" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K131" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="130" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K130" t="s">
+    <row r="132" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K132" t="s">
         <v>881</v>
       </c>
     </row>
-    <row r="131" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K131" t="s">
+    <row r="133" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K133" t="s">
         <v>882</v>
       </c>
     </row>
-    <row r="132" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K132" t="s">
+    <row r="134" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="K134" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="133" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K133" t="s">
+    <row r="135" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="K135" t="s">
         <v>786</v>
       </c>
     </row>
-    <row r="134" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K134" t="s">
+    <row r="136" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="K136" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="135" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K135" t="s">
+    <row r="137" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="K137" t="s">
         <v>883</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="L4" r:id="rId3"/>
-    <hyperlink ref="L5" r:id="rId4"/>
-    <hyperlink ref="L6" r:id="rId5"/>
-    <hyperlink ref="L7" r:id="rId6"/>
-    <hyperlink ref="L8" r:id="rId7"/>
-    <hyperlink ref="L9" r:id="rId8"/>
-    <hyperlink ref="L10" r:id="rId9"/>
-    <hyperlink ref="L11" r:id="rId10"/>
-    <hyperlink ref="L12" r:id="rId11"/>
-    <hyperlink ref="L13" r:id="rId12"/>
-    <hyperlink ref="L14" r:id="rId13"/>
-    <hyperlink ref="L15" r:id="rId14"/>
-    <hyperlink ref="L16" r:id="rId15"/>
-    <hyperlink ref="L17" r:id="rId16"/>
-    <hyperlink ref="L18" r:id="rId17"/>
-    <hyperlink ref="L19" r:id="rId18"/>
-    <hyperlink ref="L20" r:id="rId19"/>
-    <hyperlink ref="L21" r:id="rId20"/>
-    <hyperlink ref="L22" r:id="rId21"/>
-    <hyperlink ref="L23" r:id="rId22"/>
-    <hyperlink ref="L24" r:id="rId23"/>
-    <hyperlink ref="L25" r:id="rId24"/>
-    <hyperlink ref="L26" r:id="rId25"/>
-    <hyperlink ref="L27" r:id="rId26"/>
-    <hyperlink ref="L28" r:id="rId27"/>
-    <hyperlink ref="L29" r:id="rId28"/>
-    <hyperlink ref="L30" r:id="rId29"/>
-    <hyperlink ref="L31" r:id="rId30"/>
-    <hyperlink ref="L32" r:id="rId31"/>
-    <hyperlink ref="L33" r:id="rId32"/>
-    <hyperlink ref="L34" r:id="rId33"/>
-    <hyperlink ref="L35" r:id="rId34"/>
-    <hyperlink ref="L36" r:id="rId35"/>
-    <hyperlink ref="L37" r:id="rId36"/>
-    <hyperlink ref="L38" r:id="rId37"/>
-    <hyperlink ref="G39" r:id="rId38"/>
-    <hyperlink ref="L39" r:id="rId39"/>
-    <hyperlink ref="L40" r:id="rId40"/>
-    <hyperlink ref="L41" r:id="rId41"/>
-    <hyperlink ref="L42" r:id="rId42"/>
-    <hyperlink ref="L43" r:id="rId43"/>
-    <hyperlink ref="L44" r:id="rId44"/>
-    <hyperlink ref="L45" r:id="rId45"/>
-    <hyperlink ref="L46" r:id="rId46"/>
-    <hyperlink ref="L47" r:id="rId47"/>
-    <hyperlink ref="L48" r:id="rId48"/>
-    <hyperlink ref="L49" r:id="rId49"/>
-    <hyperlink ref="L50" r:id="rId50"/>
-    <hyperlink ref="L51" r:id="rId51"/>
-    <hyperlink ref="L52" r:id="rId52"/>
-    <hyperlink ref="L53" r:id="rId53"/>
-    <hyperlink ref="L54" r:id="rId54"/>
-    <hyperlink ref="L55" r:id="rId55"/>
-    <hyperlink ref="L56" r:id="rId56"/>
-    <hyperlink ref="L57" r:id="rId57"/>
-    <hyperlink ref="L58" r:id="rId58"/>
-    <hyperlink ref="L59" r:id="rId59"/>
-    <hyperlink ref="L60" r:id="rId60"/>
-    <hyperlink ref="L61" r:id="rId61"/>
-    <hyperlink ref="L62" r:id="rId62"/>
-    <hyperlink ref="L63" r:id="rId63"/>
-    <hyperlink ref="L64" r:id="rId64"/>
-    <hyperlink ref="L65" r:id="rId65"/>
-    <hyperlink ref="L66" r:id="rId66"/>
-    <hyperlink ref="L67" r:id="rId67"/>
-    <hyperlink ref="L68" r:id="rId68"/>
-    <hyperlink ref="L69" r:id="rId69"/>
-    <hyperlink ref="L70" r:id="rId70"/>
-    <hyperlink ref="L71" r:id="rId71"/>
-    <hyperlink ref="L72" r:id="rId72"/>
-    <hyperlink ref="L73" r:id="rId73"/>
-    <hyperlink ref="L74" r:id="rId74"/>
-    <hyperlink ref="L75" r:id="rId75"/>
-    <hyperlink ref="L76" r:id="rId76"/>
-    <hyperlink ref="L77" r:id="rId77"/>
-    <hyperlink ref="L78" r:id="rId78"/>
-    <hyperlink ref="L79" r:id="rId79"/>
-    <hyperlink ref="L80" r:id="rId80"/>
-    <hyperlink ref="L81" r:id="rId81"/>
-    <hyperlink ref="L82" r:id="rId82"/>
-    <hyperlink ref="L83" r:id="rId83"/>
-    <hyperlink ref="L84" r:id="rId84"/>
-    <hyperlink ref="L85" r:id="rId85"/>
-    <hyperlink ref="L86" r:id="rId86"/>
-    <hyperlink ref="L87" r:id="rId87"/>
-    <hyperlink ref="L88" r:id="rId88"/>
-    <hyperlink ref="L89" r:id="rId89"/>
-    <hyperlink ref="L90" r:id="rId90"/>
-    <hyperlink ref="L91" r:id="rId91"/>
-    <hyperlink ref="L92" r:id="rId92"/>
-    <hyperlink ref="L93" r:id="rId93"/>
-    <hyperlink ref="L94" r:id="rId94"/>
-    <hyperlink ref="L95" r:id="rId95"/>
-    <hyperlink ref="L96" r:id="rId96"/>
-    <hyperlink ref="L97" r:id="rId97"/>
-    <hyperlink ref="L98" r:id="rId98"/>
-    <hyperlink ref="L99" r:id="rId99"/>
-    <hyperlink ref="L100" r:id="rId100"/>
-    <hyperlink ref="L101" r:id="rId101"/>
-    <hyperlink ref="L102" r:id="rId102"/>
-    <hyperlink ref="L103" r:id="rId103"/>
-    <hyperlink ref="L104" r:id="rId104"/>
-    <hyperlink ref="L105" r:id="rId105"/>
-    <hyperlink ref="L106" r:id="rId106"/>
-    <hyperlink ref="L107" r:id="rId107"/>
-    <hyperlink ref="L108" r:id="rId108"/>
-    <hyperlink ref="L109" r:id="rId109"/>
-    <hyperlink ref="L110" r:id="rId110"/>
-    <hyperlink ref="L111" r:id="rId111"/>
-    <hyperlink ref="L112" r:id="rId112"/>
-    <hyperlink ref="L113" r:id="rId113"/>
-    <hyperlink ref="L114" r:id="rId114"/>
-    <hyperlink ref="L115" r:id="rId115"/>
-    <hyperlink ref="L116" r:id="rId116"/>
-    <hyperlink ref="L117" r:id="rId117"/>
-    <hyperlink ref="L118" r:id="rId118"/>
-    <hyperlink ref="L119" r:id="rId119"/>
-    <hyperlink ref="L120" r:id="rId120"/>
-    <hyperlink ref="L121" r:id="rId121"/>
-    <hyperlink ref="L122" r:id="rId122"/>
-    <hyperlink ref="L123" r:id="rId123"/>
-    <hyperlink ref="L124" r:id="rId124"/>
-    <hyperlink ref="G125" r:id="rId125"/>
-    <hyperlink ref="G126" r:id="rId126"/>
-    <hyperlink ref="L126" r:id="rId127"/>
-    <hyperlink ref="G128" r:id="rId128"/>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="L4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="L5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="L6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="L7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="L8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="L9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="L10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="L11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="L12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="L13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="L14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="L15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="L16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="L17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="L18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="L19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="L20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="L21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="L22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="L23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="L24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="L25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="L26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="L27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="L28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="L29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="L30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="L31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="L32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="L33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="L34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="L35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="L36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="L37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="L38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="G39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="L39" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="L40" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="L41" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="L42" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="L43" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="L44" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="L45" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="L46" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="L47" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="L48" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="L49" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="L50" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="L51" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="L52" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="L53" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="L54" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="L55" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="L56" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="L57" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="L58" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="L59" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="L60" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="L61" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="L62" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="L63" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="L64" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="L65" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="L66" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="L67" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="L68" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="L69" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="L70" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="L71" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="L72" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="L73" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="L74" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="L75" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="L76" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="L77" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="L78" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="L79" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="L80" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="L81" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="L82" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="L83" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="L84" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="L85" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="L86" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="L87" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="L88" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="L89" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="L90" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="L91" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="L92" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="L93" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="L94" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="L95" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="L96" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="L97" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="L98" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="L99" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="L100" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="L101" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="L102" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="L103" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="L104" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="L105" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="L106" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="L107" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="L108" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="L109" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="L110" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="L111" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="L112" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="L113" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="L114" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="L115" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="L116" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="L117" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="L118" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="L119" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="L120" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="L121" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="L122" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="L123" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="L124" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="G125" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="G126" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="L126" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="G128" r:id="rId128" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="G129" r:id="rId129" xr:uid="{5FCEE3BB-9F0C-4948-9926-6195AB90C69F}"/>
+    <hyperlink ref="L129" r:id="rId130" xr:uid="{76AF10C0-C35F-4891-8355-A7FFE4F4EDD9}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -8344,7 +8403,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -12403,124 +12462,124 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1"/>
-    <hyperlink ref="J3" r:id="rId2"/>
-    <hyperlink ref="J4" r:id="rId3"/>
-    <hyperlink ref="J5" r:id="rId4"/>
-    <hyperlink ref="J6" r:id="rId5"/>
-    <hyperlink ref="J7" r:id="rId6"/>
-    <hyperlink ref="J8" r:id="rId7"/>
-    <hyperlink ref="J9" r:id="rId8"/>
-    <hyperlink ref="J10" r:id="rId9"/>
-    <hyperlink ref="J11" r:id="rId10"/>
-    <hyperlink ref="J12" r:id="rId11"/>
-    <hyperlink ref="J13" r:id="rId12"/>
-    <hyperlink ref="J14" r:id="rId13"/>
-    <hyperlink ref="J15" r:id="rId14"/>
-    <hyperlink ref="J16" r:id="rId15"/>
-    <hyperlink ref="J17" r:id="rId16"/>
-    <hyperlink ref="J18" r:id="rId17"/>
-    <hyperlink ref="J19" r:id="rId18"/>
-    <hyperlink ref="J20" r:id="rId19"/>
-    <hyperlink ref="J21" r:id="rId20"/>
-    <hyperlink ref="J22" r:id="rId21"/>
-    <hyperlink ref="J23" r:id="rId22"/>
-    <hyperlink ref="J24" r:id="rId23"/>
-    <hyperlink ref="J25" r:id="rId24"/>
-    <hyperlink ref="J26" r:id="rId25"/>
-    <hyperlink ref="J27" r:id="rId26"/>
-    <hyperlink ref="J28" r:id="rId27"/>
-    <hyperlink ref="J29" r:id="rId28"/>
-    <hyperlink ref="J30" r:id="rId29"/>
-    <hyperlink ref="J31" r:id="rId30"/>
-    <hyperlink ref="J32" r:id="rId31"/>
-    <hyperlink ref="J33" r:id="rId32"/>
-    <hyperlink ref="J34" r:id="rId33"/>
-    <hyperlink ref="J35" r:id="rId34"/>
-    <hyperlink ref="J36" r:id="rId35"/>
-    <hyperlink ref="J37" r:id="rId36"/>
-    <hyperlink ref="J38" r:id="rId37"/>
-    <hyperlink ref="J39" r:id="rId38"/>
-    <hyperlink ref="J40" r:id="rId39"/>
-    <hyperlink ref="J41" r:id="rId40"/>
-    <hyperlink ref="J42" r:id="rId41"/>
-    <hyperlink ref="J43" r:id="rId42"/>
-    <hyperlink ref="J44" r:id="rId43"/>
-    <hyperlink ref="J45" r:id="rId44"/>
-    <hyperlink ref="J46" r:id="rId45"/>
-    <hyperlink ref="J47" r:id="rId46"/>
-    <hyperlink ref="J48" r:id="rId47"/>
-    <hyperlink ref="J49" r:id="rId48"/>
-    <hyperlink ref="J50" r:id="rId49"/>
-    <hyperlink ref="J51" r:id="rId50"/>
-    <hyperlink ref="J52" r:id="rId51"/>
-    <hyperlink ref="J53" r:id="rId52"/>
-    <hyperlink ref="J54" r:id="rId53"/>
-    <hyperlink ref="J55" r:id="rId54"/>
-    <hyperlink ref="J56" r:id="rId55"/>
-    <hyperlink ref="J57" r:id="rId56"/>
-    <hyperlink ref="J58" r:id="rId57"/>
-    <hyperlink ref="J59" r:id="rId58"/>
-    <hyperlink ref="J60" r:id="rId59"/>
-    <hyperlink ref="J61" r:id="rId60"/>
-    <hyperlink ref="J62" r:id="rId61"/>
-    <hyperlink ref="J63" r:id="rId62"/>
-    <hyperlink ref="J64" r:id="rId63"/>
-    <hyperlink ref="J65" r:id="rId64"/>
-    <hyperlink ref="J66" r:id="rId65"/>
-    <hyperlink ref="J67" r:id="rId66"/>
-    <hyperlink ref="J68" r:id="rId67"/>
-    <hyperlink ref="J69" r:id="rId68"/>
-    <hyperlink ref="J70" r:id="rId69"/>
-    <hyperlink ref="J71" r:id="rId70"/>
-    <hyperlink ref="J72" r:id="rId71"/>
-    <hyperlink ref="J73" r:id="rId72"/>
-    <hyperlink ref="J74" r:id="rId73"/>
-    <hyperlink ref="J75" r:id="rId74"/>
-    <hyperlink ref="J76" r:id="rId75"/>
-    <hyperlink ref="J77" r:id="rId76"/>
-    <hyperlink ref="J78" r:id="rId77"/>
-    <hyperlink ref="J79" r:id="rId78"/>
-    <hyperlink ref="J80" r:id="rId79"/>
-    <hyperlink ref="J81" r:id="rId80"/>
-    <hyperlink ref="J82" r:id="rId81"/>
-    <hyperlink ref="J83" r:id="rId82"/>
-    <hyperlink ref="J84" r:id="rId83"/>
-    <hyperlink ref="J85" r:id="rId84"/>
-    <hyperlink ref="J86" r:id="rId85"/>
-    <hyperlink ref="J87" r:id="rId86"/>
-    <hyperlink ref="J88" r:id="rId87"/>
-    <hyperlink ref="J89" r:id="rId88"/>
-    <hyperlink ref="J90" r:id="rId89"/>
-    <hyperlink ref="J91" r:id="rId90"/>
-    <hyperlink ref="J92" r:id="rId91"/>
-    <hyperlink ref="J93" r:id="rId92"/>
-    <hyperlink ref="J94" r:id="rId93"/>
-    <hyperlink ref="J95" r:id="rId94"/>
-    <hyperlink ref="J96" r:id="rId95"/>
-    <hyperlink ref="J97" r:id="rId96"/>
-    <hyperlink ref="J98" r:id="rId97"/>
-    <hyperlink ref="J99" r:id="rId98"/>
-    <hyperlink ref="J100" r:id="rId99"/>
-    <hyperlink ref="J101" r:id="rId100"/>
-    <hyperlink ref="J102" r:id="rId101"/>
-    <hyperlink ref="J103" r:id="rId102"/>
-    <hyperlink ref="J104" r:id="rId103"/>
-    <hyperlink ref="J105" r:id="rId104"/>
-    <hyperlink ref="J106" r:id="rId105"/>
-    <hyperlink ref="J107" r:id="rId106"/>
-    <hyperlink ref="J108" r:id="rId107"/>
-    <hyperlink ref="J109" r:id="rId108"/>
-    <hyperlink ref="J110" r:id="rId109"/>
-    <hyperlink ref="J111" r:id="rId110"/>
-    <hyperlink ref="J112" r:id="rId111"/>
-    <hyperlink ref="J113" r:id="rId112"/>
-    <hyperlink ref="J114" r:id="rId113"/>
-    <hyperlink ref="G115" r:id="rId114"/>
-    <hyperlink ref="J115" r:id="rId115"/>
-    <hyperlink ref="J116" r:id="rId116"/>
-    <hyperlink ref="G117" r:id="rId117"/>
-    <hyperlink ref="J117" r:id="rId118"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="J3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="J4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="J5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="J6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="J7" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="J8" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="J9" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="J10" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="J11" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="J12" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="J13" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="J14" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="J15" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="J16" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="J17" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="J18" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="J19" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="J20" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="J21" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="J22" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="J23" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
+    <hyperlink ref="J24" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink ref="J25" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
+    <hyperlink ref="J26" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink ref="J27" r:id="rId26" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
+    <hyperlink ref="J28" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
+    <hyperlink ref="J29" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
+    <hyperlink ref="J30" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="J31" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
+    <hyperlink ref="J32" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="J33" r:id="rId32" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
+    <hyperlink ref="J34" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink ref="J35" r:id="rId34" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
+    <hyperlink ref="J36" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink ref="J37" r:id="rId36" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
+    <hyperlink ref="J38" r:id="rId37" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
+    <hyperlink ref="J39" r:id="rId38" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
+    <hyperlink ref="J40" r:id="rId39" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
+    <hyperlink ref="J41" r:id="rId40" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
+    <hyperlink ref="J42" r:id="rId41" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
+    <hyperlink ref="J43" r:id="rId42" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
+    <hyperlink ref="J44" r:id="rId43" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
+    <hyperlink ref="J45" r:id="rId44" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
+    <hyperlink ref="J46" r:id="rId45" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
+    <hyperlink ref="J47" r:id="rId46" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
+    <hyperlink ref="J48" r:id="rId47" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
+    <hyperlink ref="J49" r:id="rId48" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
+    <hyperlink ref="J50" r:id="rId49" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
+    <hyperlink ref="J51" r:id="rId50" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
+    <hyperlink ref="J52" r:id="rId51" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
+    <hyperlink ref="J53" r:id="rId52" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
+    <hyperlink ref="J54" r:id="rId53" xr:uid="{00000000-0004-0000-0100-000034000000}"/>
+    <hyperlink ref="J55" r:id="rId54" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
+    <hyperlink ref="J56" r:id="rId55" xr:uid="{00000000-0004-0000-0100-000036000000}"/>
+    <hyperlink ref="J57" r:id="rId56" xr:uid="{00000000-0004-0000-0100-000037000000}"/>
+    <hyperlink ref="J58" r:id="rId57" xr:uid="{00000000-0004-0000-0100-000038000000}"/>
+    <hyperlink ref="J59" r:id="rId58" xr:uid="{00000000-0004-0000-0100-000039000000}"/>
+    <hyperlink ref="J60" r:id="rId59" xr:uid="{00000000-0004-0000-0100-00003A000000}"/>
+    <hyperlink ref="J61" r:id="rId60" xr:uid="{00000000-0004-0000-0100-00003B000000}"/>
+    <hyperlink ref="J62" r:id="rId61" xr:uid="{00000000-0004-0000-0100-00003C000000}"/>
+    <hyperlink ref="J63" r:id="rId62" xr:uid="{00000000-0004-0000-0100-00003D000000}"/>
+    <hyperlink ref="J64" r:id="rId63" xr:uid="{00000000-0004-0000-0100-00003E000000}"/>
+    <hyperlink ref="J65" r:id="rId64" xr:uid="{00000000-0004-0000-0100-00003F000000}"/>
+    <hyperlink ref="J66" r:id="rId65" xr:uid="{00000000-0004-0000-0100-000040000000}"/>
+    <hyperlink ref="J67" r:id="rId66" xr:uid="{00000000-0004-0000-0100-000041000000}"/>
+    <hyperlink ref="J68" r:id="rId67" xr:uid="{00000000-0004-0000-0100-000042000000}"/>
+    <hyperlink ref="J69" r:id="rId68" xr:uid="{00000000-0004-0000-0100-000043000000}"/>
+    <hyperlink ref="J70" r:id="rId69" xr:uid="{00000000-0004-0000-0100-000044000000}"/>
+    <hyperlink ref="J71" r:id="rId70" xr:uid="{00000000-0004-0000-0100-000045000000}"/>
+    <hyperlink ref="J72" r:id="rId71" xr:uid="{00000000-0004-0000-0100-000046000000}"/>
+    <hyperlink ref="J73" r:id="rId72" xr:uid="{00000000-0004-0000-0100-000047000000}"/>
+    <hyperlink ref="J74" r:id="rId73" xr:uid="{00000000-0004-0000-0100-000048000000}"/>
+    <hyperlink ref="J75" r:id="rId74" xr:uid="{00000000-0004-0000-0100-000049000000}"/>
+    <hyperlink ref="J76" r:id="rId75" xr:uid="{00000000-0004-0000-0100-00004A000000}"/>
+    <hyperlink ref="J77" r:id="rId76" xr:uid="{00000000-0004-0000-0100-00004B000000}"/>
+    <hyperlink ref="J78" r:id="rId77" xr:uid="{00000000-0004-0000-0100-00004C000000}"/>
+    <hyperlink ref="J79" r:id="rId78" xr:uid="{00000000-0004-0000-0100-00004D000000}"/>
+    <hyperlink ref="J80" r:id="rId79" xr:uid="{00000000-0004-0000-0100-00004E000000}"/>
+    <hyperlink ref="J81" r:id="rId80" xr:uid="{00000000-0004-0000-0100-00004F000000}"/>
+    <hyperlink ref="J82" r:id="rId81" xr:uid="{00000000-0004-0000-0100-000050000000}"/>
+    <hyperlink ref="J83" r:id="rId82" xr:uid="{00000000-0004-0000-0100-000051000000}"/>
+    <hyperlink ref="J84" r:id="rId83" xr:uid="{00000000-0004-0000-0100-000052000000}"/>
+    <hyperlink ref="J85" r:id="rId84" xr:uid="{00000000-0004-0000-0100-000053000000}"/>
+    <hyperlink ref="J86" r:id="rId85" xr:uid="{00000000-0004-0000-0100-000054000000}"/>
+    <hyperlink ref="J87" r:id="rId86" xr:uid="{00000000-0004-0000-0100-000055000000}"/>
+    <hyperlink ref="J88" r:id="rId87" xr:uid="{00000000-0004-0000-0100-000056000000}"/>
+    <hyperlink ref="J89" r:id="rId88" xr:uid="{00000000-0004-0000-0100-000057000000}"/>
+    <hyperlink ref="J90" r:id="rId89" xr:uid="{00000000-0004-0000-0100-000058000000}"/>
+    <hyperlink ref="J91" r:id="rId90" xr:uid="{00000000-0004-0000-0100-000059000000}"/>
+    <hyperlink ref="J92" r:id="rId91" xr:uid="{00000000-0004-0000-0100-00005A000000}"/>
+    <hyperlink ref="J93" r:id="rId92" xr:uid="{00000000-0004-0000-0100-00005B000000}"/>
+    <hyperlink ref="J94" r:id="rId93" xr:uid="{00000000-0004-0000-0100-00005C000000}"/>
+    <hyperlink ref="J95" r:id="rId94" xr:uid="{00000000-0004-0000-0100-00005D000000}"/>
+    <hyperlink ref="J96" r:id="rId95" xr:uid="{00000000-0004-0000-0100-00005E000000}"/>
+    <hyperlink ref="J97" r:id="rId96" xr:uid="{00000000-0004-0000-0100-00005F000000}"/>
+    <hyperlink ref="J98" r:id="rId97" xr:uid="{00000000-0004-0000-0100-000060000000}"/>
+    <hyperlink ref="J99" r:id="rId98" xr:uid="{00000000-0004-0000-0100-000061000000}"/>
+    <hyperlink ref="J100" r:id="rId99" xr:uid="{00000000-0004-0000-0100-000062000000}"/>
+    <hyperlink ref="J101" r:id="rId100" xr:uid="{00000000-0004-0000-0100-000063000000}"/>
+    <hyperlink ref="J102" r:id="rId101" xr:uid="{00000000-0004-0000-0100-000064000000}"/>
+    <hyperlink ref="J103" r:id="rId102" xr:uid="{00000000-0004-0000-0100-000065000000}"/>
+    <hyperlink ref="J104" r:id="rId103" xr:uid="{00000000-0004-0000-0100-000066000000}"/>
+    <hyperlink ref="J105" r:id="rId104" xr:uid="{00000000-0004-0000-0100-000067000000}"/>
+    <hyperlink ref="J106" r:id="rId105" xr:uid="{00000000-0004-0000-0100-000068000000}"/>
+    <hyperlink ref="J107" r:id="rId106" xr:uid="{00000000-0004-0000-0100-000069000000}"/>
+    <hyperlink ref="J108" r:id="rId107" xr:uid="{00000000-0004-0000-0100-00006A000000}"/>
+    <hyperlink ref="J109" r:id="rId108" xr:uid="{00000000-0004-0000-0100-00006B000000}"/>
+    <hyperlink ref="J110" r:id="rId109" xr:uid="{00000000-0004-0000-0100-00006C000000}"/>
+    <hyperlink ref="J111" r:id="rId110" xr:uid="{00000000-0004-0000-0100-00006D000000}"/>
+    <hyperlink ref="J112" r:id="rId111" xr:uid="{00000000-0004-0000-0100-00006E000000}"/>
+    <hyperlink ref="J113" r:id="rId112" xr:uid="{00000000-0004-0000-0100-00006F000000}"/>
+    <hyperlink ref="J114" r:id="rId113" xr:uid="{00000000-0004-0000-0100-000070000000}"/>
+    <hyperlink ref="G115" r:id="rId114" xr:uid="{00000000-0004-0000-0100-000071000000}"/>
+    <hyperlink ref="J115" r:id="rId115" xr:uid="{00000000-0004-0000-0100-000072000000}"/>
+    <hyperlink ref="J116" r:id="rId116" xr:uid="{00000000-0004-0000-0100-000073000000}"/>
+    <hyperlink ref="G117" r:id="rId117" xr:uid="{00000000-0004-0000-0100-000074000000}"/>
+    <hyperlink ref="J117" r:id="rId118" xr:uid="{00000000-0004-0000-0100-000075000000}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -12529,7 +12588,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -16372,117 +16431,117 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1"/>
-    <hyperlink ref="J3" r:id="rId2"/>
-    <hyperlink ref="J4" r:id="rId3"/>
-    <hyperlink ref="J5" r:id="rId4"/>
-    <hyperlink ref="J6" r:id="rId5"/>
-    <hyperlink ref="J7" r:id="rId6"/>
-    <hyperlink ref="J8" r:id="rId7"/>
-    <hyperlink ref="J9" r:id="rId8"/>
-    <hyperlink ref="J10" r:id="rId9"/>
-    <hyperlink ref="J11" r:id="rId10"/>
-    <hyperlink ref="J12" r:id="rId11"/>
-    <hyperlink ref="J13" r:id="rId12"/>
-    <hyperlink ref="J14" r:id="rId13"/>
-    <hyperlink ref="J15" r:id="rId14"/>
-    <hyperlink ref="J16" r:id="rId15"/>
-    <hyperlink ref="J17" r:id="rId16"/>
-    <hyperlink ref="J18" r:id="rId17"/>
-    <hyperlink ref="J19" r:id="rId18"/>
-    <hyperlink ref="J20" r:id="rId19"/>
-    <hyperlink ref="J21" r:id="rId20"/>
-    <hyperlink ref="J22" r:id="rId21"/>
-    <hyperlink ref="J23" r:id="rId22"/>
-    <hyperlink ref="J24" r:id="rId23"/>
-    <hyperlink ref="J25" r:id="rId24"/>
-    <hyperlink ref="J26" r:id="rId25"/>
-    <hyperlink ref="J27" r:id="rId26"/>
-    <hyperlink ref="J28" r:id="rId27"/>
-    <hyperlink ref="J29" r:id="rId28"/>
-    <hyperlink ref="J30" r:id="rId29"/>
-    <hyperlink ref="J31" r:id="rId30"/>
-    <hyperlink ref="J32" r:id="rId31"/>
-    <hyperlink ref="J33" r:id="rId32"/>
-    <hyperlink ref="J34" r:id="rId33"/>
-    <hyperlink ref="J35" r:id="rId34"/>
-    <hyperlink ref="J36" r:id="rId35"/>
-    <hyperlink ref="J37" r:id="rId36"/>
-    <hyperlink ref="J38" r:id="rId37"/>
-    <hyperlink ref="J39" r:id="rId38"/>
-    <hyperlink ref="J40" r:id="rId39"/>
-    <hyperlink ref="J41" r:id="rId40"/>
-    <hyperlink ref="J42" r:id="rId41"/>
-    <hyperlink ref="J43" r:id="rId42"/>
-    <hyperlink ref="J44" r:id="rId43"/>
-    <hyperlink ref="J45" r:id="rId44"/>
-    <hyperlink ref="J46" r:id="rId45"/>
-    <hyperlink ref="J47" r:id="rId46"/>
-    <hyperlink ref="J48" r:id="rId47"/>
-    <hyperlink ref="J49" r:id="rId48"/>
-    <hyperlink ref="J50" r:id="rId49"/>
-    <hyperlink ref="J51" r:id="rId50"/>
-    <hyperlink ref="J52" r:id="rId51"/>
-    <hyperlink ref="J53" r:id="rId52"/>
-    <hyperlink ref="J54" r:id="rId53"/>
-    <hyperlink ref="J55" r:id="rId54"/>
-    <hyperlink ref="J56" r:id="rId55"/>
-    <hyperlink ref="J57" r:id="rId56"/>
-    <hyperlink ref="J58" r:id="rId57"/>
-    <hyperlink ref="J59" r:id="rId58"/>
-    <hyperlink ref="J60" r:id="rId59"/>
-    <hyperlink ref="J61" r:id="rId60"/>
-    <hyperlink ref="J62" r:id="rId61"/>
-    <hyperlink ref="J63" r:id="rId62"/>
-    <hyperlink ref="J64" r:id="rId63"/>
-    <hyperlink ref="J65" r:id="rId64"/>
-    <hyperlink ref="J66" r:id="rId65"/>
-    <hyperlink ref="J67" r:id="rId66"/>
-    <hyperlink ref="J68" r:id="rId67"/>
-    <hyperlink ref="J69" r:id="rId68"/>
-    <hyperlink ref="J70" r:id="rId69"/>
-    <hyperlink ref="J71" r:id="rId70"/>
-    <hyperlink ref="J72" r:id="rId71"/>
-    <hyperlink ref="J73" r:id="rId72"/>
-    <hyperlink ref="J74" r:id="rId73"/>
-    <hyperlink ref="J75" r:id="rId74"/>
-    <hyperlink ref="J76" r:id="rId75"/>
-    <hyperlink ref="J77" r:id="rId76"/>
-    <hyperlink ref="J78" r:id="rId77"/>
-    <hyperlink ref="J79" r:id="rId78"/>
-    <hyperlink ref="J80" r:id="rId79"/>
-    <hyperlink ref="J81" r:id="rId80"/>
-    <hyperlink ref="J82" r:id="rId81"/>
-    <hyperlink ref="J83" r:id="rId82"/>
-    <hyperlink ref="J84" r:id="rId83"/>
-    <hyperlink ref="J85" r:id="rId84"/>
-    <hyperlink ref="J86" r:id="rId85"/>
-    <hyperlink ref="J87" r:id="rId86"/>
-    <hyperlink ref="J88" r:id="rId87"/>
-    <hyperlink ref="J89" r:id="rId88"/>
-    <hyperlink ref="J90" r:id="rId89"/>
-    <hyperlink ref="J91" r:id="rId90"/>
-    <hyperlink ref="J92" r:id="rId91"/>
-    <hyperlink ref="J93" r:id="rId92"/>
-    <hyperlink ref="J94" r:id="rId93"/>
-    <hyperlink ref="J95" r:id="rId94"/>
-    <hyperlink ref="J96" r:id="rId95"/>
-    <hyperlink ref="J97" r:id="rId96"/>
-    <hyperlink ref="J98" r:id="rId97"/>
-    <hyperlink ref="J99" r:id="rId98"/>
-    <hyperlink ref="J100" r:id="rId99"/>
-    <hyperlink ref="J101" r:id="rId100"/>
-    <hyperlink ref="J102" r:id="rId101"/>
-    <hyperlink ref="J103" r:id="rId102"/>
-    <hyperlink ref="J104" r:id="rId103"/>
-    <hyperlink ref="J105" r:id="rId104"/>
-    <hyperlink ref="J106" r:id="rId105"/>
-    <hyperlink ref="J107" r:id="rId106"/>
-    <hyperlink ref="J108" r:id="rId107"/>
-    <hyperlink ref="J109" r:id="rId108"/>
-    <hyperlink ref="J110" r:id="rId109"/>
-    <hyperlink ref="G111" r:id="rId110"/>
-    <hyperlink ref="J111" r:id="rId111"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="J3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="J4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="J5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="J6" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="J7" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="J8" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="J9" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="J10" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="J11" r:id="rId10" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="J12" r:id="rId11" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
+    <hyperlink ref="J13" r:id="rId12" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
+    <hyperlink ref="J14" r:id="rId13" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
+    <hyperlink ref="J15" r:id="rId14" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
+    <hyperlink ref="J16" r:id="rId15" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
+    <hyperlink ref="J17" r:id="rId16" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
+    <hyperlink ref="J18" r:id="rId17" xr:uid="{00000000-0004-0000-0200-000010000000}"/>
+    <hyperlink ref="J19" r:id="rId18" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
+    <hyperlink ref="J20" r:id="rId19" xr:uid="{00000000-0004-0000-0200-000012000000}"/>
+    <hyperlink ref="J21" r:id="rId20" xr:uid="{00000000-0004-0000-0200-000013000000}"/>
+    <hyperlink ref="J22" r:id="rId21" xr:uid="{00000000-0004-0000-0200-000014000000}"/>
+    <hyperlink ref="J23" r:id="rId22" xr:uid="{00000000-0004-0000-0200-000015000000}"/>
+    <hyperlink ref="J24" r:id="rId23" xr:uid="{00000000-0004-0000-0200-000016000000}"/>
+    <hyperlink ref="J25" r:id="rId24" xr:uid="{00000000-0004-0000-0200-000017000000}"/>
+    <hyperlink ref="J26" r:id="rId25" xr:uid="{00000000-0004-0000-0200-000018000000}"/>
+    <hyperlink ref="J27" r:id="rId26" xr:uid="{00000000-0004-0000-0200-000019000000}"/>
+    <hyperlink ref="J28" r:id="rId27" xr:uid="{00000000-0004-0000-0200-00001A000000}"/>
+    <hyperlink ref="J29" r:id="rId28" xr:uid="{00000000-0004-0000-0200-00001B000000}"/>
+    <hyperlink ref="J30" r:id="rId29" xr:uid="{00000000-0004-0000-0200-00001C000000}"/>
+    <hyperlink ref="J31" r:id="rId30" xr:uid="{00000000-0004-0000-0200-00001D000000}"/>
+    <hyperlink ref="J32" r:id="rId31" xr:uid="{00000000-0004-0000-0200-00001E000000}"/>
+    <hyperlink ref="J33" r:id="rId32" xr:uid="{00000000-0004-0000-0200-00001F000000}"/>
+    <hyperlink ref="J34" r:id="rId33" xr:uid="{00000000-0004-0000-0200-000020000000}"/>
+    <hyperlink ref="J35" r:id="rId34" xr:uid="{00000000-0004-0000-0200-000021000000}"/>
+    <hyperlink ref="J36" r:id="rId35" xr:uid="{00000000-0004-0000-0200-000022000000}"/>
+    <hyperlink ref="J37" r:id="rId36" xr:uid="{00000000-0004-0000-0200-000023000000}"/>
+    <hyperlink ref="J38" r:id="rId37" xr:uid="{00000000-0004-0000-0200-000024000000}"/>
+    <hyperlink ref="J39" r:id="rId38" xr:uid="{00000000-0004-0000-0200-000025000000}"/>
+    <hyperlink ref="J40" r:id="rId39" xr:uid="{00000000-0004-0000-0200-000026000000}"/>
+    <hyperlink ref="J41" r:id="rId40" xr:uid="{00000000-0004-0000-0200-000027000000}"/>
+    <hyperlink ref="J42" r:id="rId41" xr:uid="{00000000-0004-0000-0200-000028000000}"/>
+    <hyperlink ref="J43" r:id="rId42" xr:uid="{00000000-0004-0000-0200-000029000000}"/>
+    <hyperlink ref="J44" r:id="rId43" xr:uid="{00000000-0004-0000-0200-00002A000000}"/>
+    <hyperlink ref="J45" r:id="rId44" xr:uid="{00000000-0004-0000-0200-00002B000000}"/>
+    <hyperlink ref="J46" r:id="rId45" xr:uid="{00000000-0004-0000-0200-00002C000000}"/>
+    <hyperlink ref="J47" r:id="rId46" xr:uid="{00000000-0004-0000-0200-00002D000000}"/>
+    <hyperlink ref="J48" r:id="rId47" xr:uid="{00000000-0004-0000-0200-00002E000000}"/>
+    <hyperlink ref="J49" r:id="rId48" xr:uid="{00000000-0004-0000-0200-00002F000000}"/>
+    <hyperlink ref="J50" r:id="rId49" xr:uid="{00000000-0004-0000-0200-000030000000}"/>
+    <hyperlink ref="J51" r:id="rId50" xr:uid="{00000000-0004-0000-0200-000031000000}"/>
+    <hyperlink ref="J52" r:id="rId51" xr:uid="{00000000-0004-0000-0200-000032000000}"/>
+    <hyperlink ref="J53" r:id="rId52" xr:uid="{00000000-0004-0000-0200-000033000000}"/>
+    <hyperlink ref="J54" r:id="rId53" xr:uid="{00000000-0004-0000-0200-000034000000}"/>
+    <hyperlink ref="J55" r:id="rId54" xr:uid="{00000000-0004-0000-0200-000035000000}"/>
+    <hyperlink ref="J56" r:id="rId55" xr:uid="{00000000-0004-0000-0200-000036000000}"/>
+    <hyperlink ref="J57" r:id="rId56" xr:uid="{00000000-0004-0000-0200-000037000000}"/>
+    <hyperlink ref="J58" r:id="rId57" xr:uid="{00000000-0004-0000-0200-000038000000}"/>
+    <hyperlink ref="J59" r:id="rId58" xr:uid="{00000000-0004-0000-0200-000039000000}"/>
+    <hyperlink ref="J60" r:id="rId59" xr:uid="{00000000-0004-0000-0200-00003A000000}"/>
+    <hyperlink ref="J61" r:id="rId60" xr:uid="{00000000-0004-0000-0200-00003B000000}"/>
+    <hyperlink ref="J62" r:id="rId61" xr:uid="{00000000-0004-0000-0200-00003C000000}"/>
+    <hyperlink ref="J63" r:id="rId62" xr:uid="{00000000-0004-0000-0200-00003D000000}"/>
+    <hyperlink ref="J64" r:id="rId63" xr:uid="{00000000-0004-0000-0200-00003E000000}"/>
+    <hyperlink ref="J65" r:id="rId64" xr:uid="{00000000-0004-0000-0200-00003F000000}"/>
+    <hyperlink ref="J66" r:id="rId65" xr:uid="{00000000-0004-0000-0200-000040000000}"/>
+    <hyperlink ref="J67" r:id="rId66" xr:uid="{00000000-0004-0000-0200-000041000000}"/>
+    <hyperlink ref="J68" r:id="rId67" xr:uid="{00000000-0004-0000-0200-000042000000}"/>
+    <hyperlink ref="J69" r:id="rId68" xr:uid="{00000000-0004-0000-0200-000043000000}"/>
+    <hyperlink ref="J70" r:id="rId69" xr:uid="{00000000-0004-0000-0200-000044000000}"/>
+    <hyperlink ref="J71" r:id="rId70" xr:uid="{00000000-0004-0000-0200-000045000000}"/>
+    <hyperlink ref="J72" r:id="rId71" xr:uid="{00000000-0004-0000-0200-000046000000}"/>
+    <hyperlink ref="J73" r:id="rId72" xr:uid="{00000000-0004-0000-0200-000047000000}"/>
+    <hyperlink ref="J74" r:id="rId73" xr:uid="{00000000-0004-0000-0200-000048000000}"/>
+    <hyperlink ref="J75" r:id="rId74" xr:uid="{00000000-0004-0000-0200-000049000000}"/>
+    <hyperlink ref="J76" r:id="rId75" xr:uid="{00000000-0004-0000-0200-00004A000000}"/>
+    <hyperlink ref="J77" r:id="rId76" xr:uid="{00000000-0004-0000-0200-00004B000000}"/>
+    <hyperlink ref="J78" r:id="rId77" xr:uid="{00000000-0004-0000-0200-00004C000000}"/>
+    <hyperlink ref="J79" r:id="rId78" xr:uid="{00000000-0004-0000-0200-00004D000000}"/>
+    <hyperlink ref="J80" r:id="rId79" xr:uid="{00000000-0004-0000-0200-00004E000000}"/>
+    <hyperlink ref="J81" r:id="rId80" xr:uid="{00000000-0004-0000-0200-00004F000000}"/>
+    <hyperlink ref="J82" r:id="rId81" xr:uid="{00000000-0004-0000-0200-000050000000}"/>
+    <hyperlink ref="J83" r:id="rId82" xr:uid="{00000000-0004-0000-0200-000051000000}"/>
+    <hyperlink ref="J84" r:id="rId83" xr:uid="{00000000-0004-0000-0200-000052000000}"/>
+    <hyperlink ref="J85" r:id="rId84" xr:uid="{00000000-0004-0000-0200-000053000000}"/>
+    <hyperlink ref="J86" r:id="rId85" xr:uid="{00000000-0004-0000-0200-000054000000}"/>
+    <hyperlink ref="J87" r:id="rId86" xr:uid="{00000000-0004-0000-0200-000055000000}"/>
+    <hyperlink ref="J88" r:id="rId87" xr:uid="{00000000-0004-0000-0200-000056000000}"/>
+    <hyperlink ref="J89" r:id="rId88" xr:uid="{00000000-0004-0000-0200-000057000000}"/>
+    <hyperlink ref="J90" r:id="rId89" xr:uid="{00000000-0004-0000-0200-000058000000}"/>
+    <hyperlink ref="J91" r:id="rId90" xr:uid="{00000000-0004-0000-0200-000059000000}"/>
+    <hyperlink ref="J92" r:id="rId91" xr:uid="{00000000-0004-0000-0200-00005A000000}"/>
+    <hyperlink ref="J93" r:id="rId92" xr:uid="{00000000-0004-0000-0200-00005B000000}"/>
+    <hyperlink ref="J94" r:id="rId93" xr:uid="{00000000-0004-0000-0200-00005C000000}"/>
+    <hyperlink ref="J95" r:id="rId94" xr:uid="{00000000-0004-0000-0200-00005D000000}"/>
+    <hyperlink ref="J96" r:id="rId95" xr:uid="{00000000-0004-0000-0200-00005E000000}"/>
+    <hyperlink ref="J97" r:id="rId96" xr:uid="{00000000-0004-0000-0200-00005F000000}"/>
+    <hyperlink ref="J98" r:id="rId97" xr:uid="{00000000-0004-0000-0200-000060000000}"/>
+    <hyperlink ref="J99" r:id="rId98" xr:uid="{00000000-0004-0000-0200-000061000000}"/>
+    <hyperlink ref="J100" r:id="rId99" xr:uid="{00000000-0004-0000-0200-000062000000}"/>
+    <hyperlink ref="J101" r:id="rId100" xr:uid="{00000000-0004-0000-0200-000063000000}"/>
+    <hyperlink ref="J102" r:id="rId101" xr:uid="{00000000-0004-0000-0200-000064000000}"/>
+    <hyperlink ref="J103" r:id="rId102" xr:uid="{00000000-0004-0000-0200-000065000000}"/>
+    <hyperlink ref="J104" r:id="rId103" xr:uid="{00000000-0004-0000-0200-000066000000}"/>
+    <hyperlink ref="J105" r:id="rId104" xr:uid="{00000000-0004-0000-0200-000067000000}"/>
+    <hyperlink ref="J106" r:id="rId105" xr:uid="{00000000-0004-0000-0200-000068000000}"/>
+    <hyperlink ref="J107" r:id="rId106" xr:uid="{00000000-0004-0000-0200-000069000000}"/>
+    <hyperlink ref="J108" r:id="rId107" xr:uid="{00000000-0004-0000-0200-00006A000000}"/>
+    <hyperlink ref="J109" r:id="rId108" xr:uid="{00000000-0004-0000-0200-00006B000000}"/>
+    <hyperlink ref="J110" r:id="rId109" xr:uid="{00000000-0004-0000-0200-00006C000000}"/>
+    <hyperlink ref="G111" r:id="rId110" xr:uid="{00000000-0004-0000-0200-00006D000000}"/>
+    <hyperlink ref="J111" r:id="rId111" xr:uid="{00000000-0004-0000-0200-00006E000000}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
finally updated my details
</commit_message>
<xml_diff>
--- a/CS335/GitHub Info sans duplicates.xlsx
+++ b/CS335/GitHub Info sans duplicates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\staffcard\CS335\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Applications\Xampp\htdocs\staffcard\CS335\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6BDB9B-8C56-4329-B76B-09A0D91E9E6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09EAB587-9458-4C91-BC9B-E3FC24BFE22F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3336" uniqueCount="915">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3344" uniqueCount="922">
   <si>
     <t>Timestamp</t>
   </si>
@@ -2772,6 +2772,27 @@
   </si>
   <si>
     <t>https://github.com/Sikato-41</t>
+  </si>
+  <si>
+    <t>2019-04-12687</t>
+  </si>
+  <si>
+    <t>TWEVE</t>
+  </si>
+  <si>
+    <t>YUSTER B</t>
+  </si>
+  <si>
+    <t>yusterbenny@gmail.com</t>
+  </si>
+  <si>
+    <t>Bsc in comouter science</t>
+  </si>
+  <si>
+    <t>YusterBenjamin</t>
+  </si>
+  <si>
+    <t>https://github.com/YusterBenjamin</t>
   </si>
 </sst>
 </file>
@@ -3280,20 +3301,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R132"/>
+  <dimension ref="A1:R133"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C125" sqref="C125"/>
+      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L134" sqref="L134"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="21.44140625" customWidth="1"/>
-    <col min="5" max="5" width="26.44140625" customWidth="1"/>
-    <col min="6" max="7" width="21.44140625" customWidth="1"/>
-    <col min="8" max="8" width="22.109375" customWidth="1"/>
-    <col min="9" max="18" width="21.44140625" customWidth="1"/>
+    <col min="1" max="4" width="21.453125" customWidth="1"/>
+    <col min="5" max="5" width="26.453125" customWidth="1"/>
+    <col min="6" max="7" width="21.453125" customWidth="1"/>
+    <col min="8" max="8" width="22.08984375" customWidth="1"/>
+    <col min="9" max="18" width="21.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8251,6 +8272,41 @@
       </c>
       <c r="L132" s="18" t="s">
         <v>899</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B133" t="s">
+        <v>915</v>
+      </c>
+      <c r="C133" t="s">
+        <v>916</v>
+      </c>
+      <c r="D133" t="s">
+        <v>917</v>
+      </c>
+      <c r="E133">
+        <v>747343174</v>
+      </c>
+      <c r="F133">
+        <v>734303746</v>
+      </c>
+      <c r="G133" s="18" t="s">
+        <v>918</v>
+      </c>
+      <c r="H133" t="s">
+        <v>919</v>
+      </c>
+      <c r="I133" t="s">
+        <v>19</v>
+      </c>
+      <c r="J133">
+        <v>3</v>
+      </c>
+      <c r="K133" t="s">
+        <v>920</v>
+      </c>
+      <c r="L133" t="s">
+        <v>921</v>
       </c>
     </row>
   </sheetData>
@@ -8394,6 +8450,7 @@
     <hyperlink ref="L131" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
     <hyperlink ref="G132" r:id="rId138" xr:uid="{4E7E53EA-D1B0-449F-A3FF-DFFCE2E5069E}"/>
     <hyperlink ref="L132" r:id="rId139" xr:uid="{B85D0C13-9EB5-4A5A-9E9C-2174882A171D}"/>
+    <hyperlink ref="G133" r:id="rId140" xr:uid="{5073CA39-C587-466D-AE72-0F712E05490D}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -8413,19 +8470,19 @@
       <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" customWidth="1"/>
-    <col min="4" max="4" width="25.44140625" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" customWidth="1"/>
+    <col min="1" max="1" width="4.453125" customWidth="1"/>
+    <col min="2" max="2" width="16.90625" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" customWidth="1"/>
+    <col min="4" max="4" width="25.453125" customWidth="1"/>
+    <col min="5" max="5" width="16.90625" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="33.109375" customWidth="1"/>
-    <col min="8" max="8" width="9.44140625" customWidth="1"/>
-    <col min="9" max="9" width="17.44140625" customWidth="1"/>
-    <col min="10" max="10" width="33.109375" customWidth="1"/>
-    <col min="11" max="16" width="21.44140625" customWidth="1"/>
+    <col min="7" max="7" width="33.08984375" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" customWidth="1"/>
+    <col min="9" max="9" width="17.453125" customWidth="1"/>
+    <col min="10" max="10" width="33.08984375" customWidth="1"/>
+    <col min="11" max="16" width="21.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9010,7 +9067,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -10770,7 +10827,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" ht="25" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -10962,7 +11019,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" ht="25" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -12589,23 +12646,23 @@
   <dimension ref="A1:P198"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E96" sqref="E96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" customWidth="1"/>
-    <col min="4" max="4" width="25.44140625" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" customWidth="1"/>
+    <col min="1" max="1" width="4.453125" customWidth="1"/>
+    <col min="2" max="2" width="16.90625" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" customWidth="1"/>
+    <col min="4" max="4" width="25.453125" customWidth="1"/>
+    <col min="5" max="5" width="16.90625" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="33.109375" customWidth="1"/>
-    <col min="8" max="8" width="9.44140625" customWidth="1"/>
-    <col min="9" max="9" width="17.44140625" customWidth="1"/>
-    <col min="10" max="10" width="33.109375" customWidth="1"/>
-    <col min="11" max="16" width="21.44140625" customWidth="1"/>
+    <col min="7" max="7" width="33.08984375" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" customWidth="1"/>
+    <col min="9" max="9" width="17.453125" customWidth="1"/>
+    <col min="10" max="10" width="33.08984375" customWidth="1"/>
+    <col min="11" max="16" width="21.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13158,7 +13215,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -14630,7 +14687,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" ht="25" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
edited my other name from Mialla to Yonas
</commit_message>
<xml_diff>
--- a/CS335/GitHub Info sans duplicates.xlsx
+++ b/CS335/GitHub Info sans duplicates.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\3RD YEAR\CS335\staffcard\CS335\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\devtPgms\xampp\htdocs\staffcard\CS335\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C890B8-9189-4C1B-AA94-EBB7F960B36C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="435" windowWidth="24315" windowHeight="15555" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3283" uniqueCount="900">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3283" uniqueCount="901">
   <si>
     <t>Timestamp</t>
   </si>
@@ -2732,12 +2733,15 @@
   </si>
   <si>
     <t>YES</t>
+  </si>
+  <si>
+    <t>MESHACK YONAS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
@@ -3240,12 +3244,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R132"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5166,7 +5170,7 @@
         <v>360</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>361</v>
+        <v>900</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>362</v>
@@ -7970,131 +7974,131 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1"/>
-    <hyperlink ref="L3" r:id="rId2"/>
-    <hyperlink ref="L4" r:id="rId3"/>
-    <hyperlink ref="L5" r:id="rId4"/>
-    <hyperlink ref="L6" r:id="rId5"/>
-    <hyperlink ref="L7" r:id="rId6"/>
-    <hyperlink ref="L8" r:id="rId7"/>
-    <hyperlink ref="L9" r:id="rId8"/>
-    <hyperlink ref="L10" r:id="rId9"/>
-    <hyperlink ref="L11" r:id="rId10"/>
-    <hyperlink ref="L12" r:id="rId11"/>
-    <hyperlink ref="L13" r:id="rId12"/>
-    <hyperlink ref="L14" r:id="rId13"/>
-    <hyperlink ref="L15" r:id="rId14"/>
-    <hyperlink ref="L16" r:id="rId15"/>
-    <hyperlink ref="L17" r:id="rId16"/>
-    <hyperlink ref="L18" r:id="rId17"/>
-    <hyperlink ref="L19" r:id="rId18"/>
-    <hyperlink ref="L20" r:id="rId19"/>
-    <hyperlink ref="L21" r:id="rId20"/>
-    <hyperlink ref="L22" r:id="rId21"/>
-    <hyperlink ref="L23" r:id="rId22"/>
-    <hyperlink ref="L24" r:id="rId23"/>
-    <hyperlink ref="L25" r:id="rId24"/>
-    <hyperlink ref="L26" r:id="rId25"/>
-    <hyperlink ref="L27" r:id="rId26"/>
-    <hyperlink ref="L28" r:id="rId27"/>
-    <hyperlink ref="L29" r:id="rId28"/>
-    <hyperlink ref="L30" r:id="rId29"/>
-    <hyperlink ref="L31" r:id="rId30"/>
-    <hyperlink ref="L32" r:id="rId31"/>
-    <hyperlink ref="L33" r:id="rId32"/>
-    <hyperlink ref="L34" r:id="rId33"/>
-    <hyperlink ref="L35" r:id="rId34"/>
-    <hyperlink ref="L36" r:id="rId35"/>
-    <hyperlink ref="L37" r:id="rId36"/>
-    <hyperlink ref="L39" r:id="rId37"/>
-    <hyperlink ref="L40" r:id="rId38"/>
-    <hyperlink ref="L41" r:id="rId39"/>
-    <hyperlink ref="L42" r:id="rId40"/>
-    <hyperlink ref="L43" r:id="rId41"/>
-    <hyperlink ref="L44" r:id="rId42"/>
-    <hyperlink ref="L45" r:id="rId43"/>
-    <hyperlink ref="L46" r:id="rId44"/>
-    <hyperlink ref="L47" r:id="rId45"/>
-    <hyperlink ref="L48" r:id="rId46"/>
-    <hyperlink ref="L49" r:id="rId47"/>
-    <hyperlink ref="L50" r:id="rId48"/>
-    <hyperlink ref="L51" r:id="rId49"/>
-    <hyperlink ref="L52" r:id="rId50"/>
-    <hyperlink ref="L53" r:id="rId51"/>
-    <hyperlink ref="L54" r:id="rId52"/>
-    <hyperlink ref="L55" r:id="rId53"/>
-    <hyperlink ref="L56" r:id="rId54"/>
-    <hyperlink ref="L57" r:id="rId55"/>
-    <hyperlink ref="L58" r:id="rId56"/>
-    <hyperlink ref="L59" r:id="rId57"/>
-    <hyperlink ref="L60" r:id="rId58"/>
-    <hyperlink ref="L61" r:id="rId59"/>
-    <hyperlink ref="L62" r:id="rId60"/>
-    <hyperlink ref="L63" r:id="rId61"/>
-    <hyperlink ref="L64" r:id="rId62"/>
-    <hyperlink ref="L65" r:id="rId63"/>
-    <hyperlink ref="L66" r:id="rId64"/>
-    <hyperlink ref="L67" r:id="rId65"/>
-    <hyperlink ref="L68" r:id="rId66"/>
-    <hyperlink ref="L69" r:id="rId67"/>
-    <hyperlink ref="L70" r:id="rId68"/>
-    <hyperlink ref="L71" r:id="rId69"/>
-    <hyperlink ref="L72" r:id="rId70"/>
-    <hyperlink ref="L73" r:id="rId71"/>
-    <hyperlink ref="L74" r:id="rId72"/>
-    <hyperlink ref="L75" r:id="rId73"/>
-    <hyperlink ref="L76" r:id="rId74"/>
-    <hyperlink ref="L77" r:id="rId75"/>
-    <hyperlink ref="L78" r:id="rId76"/>
-    <hyperlink ref="L79" r:id="rId77"/>
-    <hyperlink ref="L80" r:id="rId78"/>
-    <hyperlink ref="L81" r:id="rId79"/>
-    <hyperlink ref="L82" r:id="rId80"/>
-    <hyperlink ref="L83" r:id="rId81"/>
-    <hyperlink ref="L84" r:id="rId82"/>
-    <hyperlink ref="L85" r:id="rId83"/>
-    <hyperlink ref="L86" r:id="rId84"/>
-    <hyperlink ref="L87" r:id="rId85"/>
-    <hyperlink ref="L88" r:id="rId86"/>
-    <hyperlink ref="L89" r:id="rId87"/>
-    <hyperlink ref="L90" r:id="rId88"/>
-    <hyperlink ref="L91" r:id="rId89"/>
-    <hyperlink ref="L92" r:id="rId90"/>
-    <hyperlink ref="L93" r:id="rId91"/>
-    <hyperlink ref="L94" r:id="rId92"/>
-    <hyperlink ref="L95" r:id="rId93"/>
-    <hyperlink ref="L96" r:id="rId94"/>
-    <hyperlink ref="L97" r:id="rId95"/>
-    <hyperlink ref="L98" r:id="rId96"/>
-    <hyperlink ref="L99" r:id="rId97"/>
-    <hyperlink ref="L100" r:id="rId98"/>
-    <hyperlink ref="L101" r:id="rId99"/>
-    <hyperlink ref="L102" r:id="rId100"/>
-    <hyperlink ref="L103" r:id="rId101"/>
-    <hyperlink ref="L104" r:id="rId102"/>
-    <hyperlink ref="L105" r:id="rId103"/>
-    <hyperlink ref="L106" r:id="rId104"/>
-    <hyperlink ref="L107" r:id="rId105"/>
-    <hyperlink ref="L108" r:id="rId106"/>
-    <hyperlink ref="L109" r:id="rId107"/>
-    <hyperlink ref="L110" r:id="rId108"/>
-    <hyperlink ref="L111" r:id="rId109"/>
-    <hyperlink ref="L112" r:id="rId110"/>
-    <hyperlink ref="L113" r:id="rId111"/>
-    <hyperlink ref="L114" r:id="rId112"/>
-    <hyperlink ref="L115" r:id="rId113"/>
-    <hyperlink ref="L116" r:id="rId114"/>
-    <hyperlink ref="L117" r:id="rId115"/>
-    <hyperlink ref="L118" r:id="rId116"/>
-    <hyperlink ref="L119" r:id="rId117"/>
-    <hyperlink ref="L120" r:id="rId118"/>
-    <hyperlink ref="L121" r:id="rId119"/>
-    <hyperlink ref="L122" r:id="rId120"/>
-    <hyperlink ref="L123" r:id="rId121"/>
-    <hyperlink ref="G38" r:id="rId122"/>
-    <hyperlink ref="L38" r:id="rId123"/>
-    <hyperlink ref="G72" r:id="rId124"/>
-    <hyperlink ref="G119" r:id="rId125"/>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="L3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="L4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="L5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="L6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="L7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="L8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="L9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="L10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="L11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="L12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="L13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="L14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="L15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="L16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="L17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="L18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="L19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="L20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="L21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="L22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="L23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="L24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="L25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="L26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="L27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="L28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="L29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="L30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="L31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="L32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="L33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="L34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="L35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="L36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="L37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="L39" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="L40" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="L41" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="L42" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="L43" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="L44" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="L45" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="L46" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="L47" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="L48" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="L49" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="L50" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="L51" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="L52" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="L53" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="L54" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="L55" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="L56" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="L57" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="L58" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="L59" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="L60" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="L61" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="L62" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="L63" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="L64" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="L65" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="L66" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="L67" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="L68" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="L69" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="L70" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="L71" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="L72" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="L73" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="L74" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="L75" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="L76" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="L77" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="L78" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="L79" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="L80" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="L81" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="L82" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="L83" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="L84" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="L85" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="L86" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="L87" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="L88" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="L89" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="L90" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="L91" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="L92" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="L93" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="L94" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="L95" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="L96" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="L97" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="L98" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="L99" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="L100" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="L101" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="L102" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="L103" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="L104" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="L105" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="L106" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="L107" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="L108" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="L109" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="L110" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="L111" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="L112" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="L113" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="L114" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="L115" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="L116" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="L117" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="L118" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="L119" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="L120" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="L121" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="L122" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="L123" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="G38" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="L38" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="G72" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="G119" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId126"/>
@@ -8102,7 +8106,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -12161,124 +12165,124 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1"/>
-    <hyperlink ref="J3" r:id="rId2"/>
-    <hyperlink ref="J4" r:id="rId3"/>
-    <hyperlink ref="J5" r:id="rId4"/>
-    <hyperlink ref="J6" r:id="rId5"/>
-    <hyperlink ref="J7" r:id="rId6"/>
-    <hyperlink ref="J8" r:id="rId7"/>
-    <hyperlink ref="J9" r:id="rId8"/>
-    <hyperlink ref="J10" r:id="rId9"/>
-    <hyperlink ref="J11" r:id="rId10"/>
-    <hyperlink ref="J12" r:id="rId11"/>
-    <hyperlink ref="J13" r:id="rId12"/>
-    <hyperlink ref="J14" r:id="rId13"/>
-    <hyperlink ref="J15" r:id="rId14"/>
-    <hyperlink ref="J16" r:id="rId15"/>
-    <hyperlink ref="J17" r:id="rId16"/>
-    <hyperlink ref="J18" r:id="rId17"/>
-    <hyperlink ref="J19" r:id="rId18"/>
-    <hyperlink ref="J20" r:id="rId19"/>
-    <hyperlink ref="J21" r:id="rId20"/>
-    <hyperlink ref="J22" r:id="rId21"/>
-    <hyperlink ref="J23" r:id="rId22"/>
-    <hyperlink ref="J24" r:id="rId23"/>
-    <hyperlink ref="J25" r:id="rId24"/>
-    <hyperlink ref="J26" r:id="rId25"/>
-    <hyperlink ref="J27" r:id="rId26"/>
-    <hyperlink ref="J28" r:id="rId27"/>
-    <hyperlink ref="J29" r:id="rId28"/>
-    <hyperlink ref="J30" r:id="rId29"/>
-    <hyperlink ref="J31" r:id="rId30"/>
-    <hyperlink ref="J32" r:id="rId31"/>
-    <hyperlink ref="J33" r:id="rId32"/>
-    <hyperlink ref="J34" r:id="rId33"/>
-    <hyperlink ref="J35" r:id="rId34"/>
-    <hyperlink ref="J36" r:id="rId35"/>
-    <hyperlink ref="J37" r:id="rId36"/>
-    <hyperlink ref="J38" r:id="rId37"/>
-    <hyperlink ref="J39" r:id="rId38"/>
-    <hyperlink ref="J40" r:id="rId39"/>
-    <hyperlink ref="J41" r:id="rId40"/>
-    <hyperlink ref="J42" r:id="rId41"/>
-    <hyperlink ref="J43" r:id="rId42"/>
-    <hyperlink ref="J44" r:id="rId43"/>
-    <hyperlink ref="J45" r:id="rId44"/>
-    <hyperlink ref="J46" r:id="rId45"/>
-    <hyperlink ref="J47" r:id="rId46"/>
-    <hyperlink ref="J48" r:id="rId47"/>
-    <hyperlink ref="J49" r:id="rId48"/>
-    <hyperlink ref="J50" r:id="rId49"/>
-    <hyperlink ref="J51" r:id="rId50"/>
-    <hyperlink ref="J52" r:id="rId51"/>
-    <hyperlink ref="J53" r:id="rId52"/>
-    <hyperlink ref="J54" r:id="rId53"/>
-    <hyperlink ref="J55" r:id="rId54"/>
-    <hyperlink ref="J56" r:id="rId55"/>
-    <hyperlink ref="J57" r:id="rId56"/>
-    <hyperlink ref="J58" r:id="rId57"/>
-    <hyperlink ref="J59" r:id="rId58"/>
-    <hyperlink ref="J60" r:id="rId59"/>
-    <hyperlink ref="J61" r:id="rId60"/>
-    <hyperlink ref="J62" r:id="rId61"/>
-    <hyperlink ref="J63" r:id="rId62"/>
-    <hyperlink ref="J64" r:id="rId63"/>
-    <hyperlink ref="J65" r:id="rId64"/>
-    <hyperlink ref="J66" r:id="rId65"/>
-    <hyperlink ref="J67" r:id="rId66"/>
-    <hyperlink ref="J68" r:id="rId67"/>
-    <hyperlink ref="J69" r:id="rId68"/>
-    <hyperlink ref="J70" r:id="rId69"/>
-    <hyperlink ref="J71" r:id="rId70"/>
-    <hyperlink ref="J72" r:id="rId71"/>
-    <hyperlink ref="J73" r:id="rId72"/>
-    <hyperlink ref="J74" r:id="rId73"/>
-    <hyperlink ref="J75" r:id="rId74"/>
-    <hyperlink ref="J76" r:id="rId75"/>
-    <hyperlink ref="J77" r:id="rId76"/>
-    <hyperlink ref="J78" r:id="rId77"/>
-    <hyperlink ref="J79" r:id="rId78"/>
-    <hyperlink ref="J80" r:id="rId79"/>
-    <hyperlink ref="J81" r:id="rId80"/>
-    <hyperlink ref="J82" r:id="rId81"/>
-    <hyperlink ref="J83" r:id="rId82"/>
-    <hyperlink ref="J84" r:id="rId83"/>
-    <hyperlink ref="J85" r:id="rId84"/>
-    <hyperlink ref="J86" r:id="rId85"/>
-    <hyperlink ref="J87" r:id="rId86"/>
-    <hyperlink ref="J88" r:id="rId87"/>
-    <hyperlink ref="J89" r:id="rId88"/>
-    <hyperlink ref="J90" r:id="rId89"/>
-    <hyperlink ref="J91" r:id="rId90"/>
-    <hyperlink ref="J92" r:id="rId91"/>
-    <hyperlink ref="J93" r:id="rId92"/>
-    <hyperlink ref="J94" r:id="rId93"/>
-    <hyperlink ref="J95" r:id="rId94"/>
-    <hyperlink ref="J96" r:id="rId95"/>
-    <hyperlink ref="J97" r:id="rId96"/>
-    <hyperlink ref="J98" r:id="rId97"/>
-    <hyperlink ref="J99" r:id="rId98"/>
-    <hyperlink ref="J100" r:id="rId99"/>
-    <hyperlink ref="J101" r:id="rId100"/>
-    <hyperlink ref="J102" r:id="rId101"/>
-    <hyperlink ref="J103" r:id="rId102"/>
-    <hyperlink ref="J104" r:id="rId103"/>
-    <hyperlink ref="J105" r:id="rId104"/>
-    <hyperlink ref="J106" r:id="rId105"/>
-    <hyperlink ref="J107" r:id="rId106"/>
-    <hyperlink ref="J108" r:id="rId107"/>
-    <hyperlink ref="J109" r:id="rId108"/>
-    <hyperlink ref="J110" r:id="rId109"/>
-    <hyperlink ref="J111" r:id="rId110"/>
-    <hyperlink ref="J112" r:id="rId111"/>
-    <hyperlink ref="J113" r:id="rId112"/>
-    <hyperlink ref="J114" r:id="rId113"/>
-    <hyperlink ref="G115" r:id="rId114"/>
-    <hyperlink ref="J115" r:id="rId115"/>
-    <hyperlink ref="J116" r:id="rId116"/>
-    <hyperlink ref="G117" r:id="rId117"/>
-    <hyperlink ref="J117" r:id="rId118"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="J3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="J4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="J5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="J6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="J7" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="J8" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="J9" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="J10" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="J11" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="J12" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="J13" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="J14" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="J15" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="J16" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="J17" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="J18" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="J19" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="J20" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="J21" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="J22" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="J23" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
+    <hyperlink ref="J24" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink ref="J25" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
+    <hyperlink ref="J26" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink ref="J27" r:id="rId26" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
+    <hyperlink ref="J28" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
+    <hyperlink ref="J29" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
+    <hyperlink ref="J30" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="J31" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
+    <hyperlink ref="J32" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="J33" r:id="rId32" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
+    <hyperlink ref="J34" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink ref="J35" r:id="rId34" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
+    <hyperlink ref="J36" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink ref="J37" r:id="rId36" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
+    <hyperlink ref="J38" r:id="rId37" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
+    <hyperlink ref="J39" r:id="rId38" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
+    <hyperlink ref="J40" r:id="rId39" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
+    <hyperlink ref="J41" r:id="rId40" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
+    <hyperlink ref="J42" r:id="rId41" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
+    <hyperlink ref="J43" r:id="rId42" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
+    <hyperlink ref="J44" r:id="rId43" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
+    <hyperlink ref="J45" r:id="rId44" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
+    <hyperlink ref="J46" r:id="rId45" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
+    <hyperlink ref="J47" r:id="rId46" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
+    <hyperlink ref="J48" r:id="rId47" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
+    <hyperlink ref="J49" r:id="rId48" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
+    <hyperlink ref="J50" r:id="rId49" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
+    <hyperlink ref="J51" r:id="rId50" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
+    <hyperlink ref="J52" r:id="rId51" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
+    <hyperlink ref="J53" r:id="rId52" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
+    <hyperlink ref="J54" r:id="rId53" xr:uid="{00000000-0004-0000-0100-000034000000}"/>
+    <hyperlink ref="J55" r:id="rId54" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
+    <hyperlink ref="J56" r:id="rId55" xr:uid="{00000000-0004-0000-0100-000036000000}"/>
+    <hyperlink ref="J57" r:id="rId56" xr:uid="{00000000-0004-0000-0100-000037000000}"/>
+    <hyperlink ref="J58" r:id="rId57" xr:uid="{00000000-0004-0000-0100-000038000000}"/>
+    <hyperlink ref="J59" r:id="rId58" xr:uid="{00000000-0004-0000-0100-000039000000}"/>
+    <hyperlink ref="J60" r:id="rId59" xr:uid="{00000000-0004-0000-0100-00003A000000}"/>
+    <hyperlink ref="J61" r:id="rId60" xr:uid="{00000000-0004-0000-0100-00003B000000}"/>
+    <hyperlink ref="J62" r:id="rId61" xr:uid="{00000000-0004-0000-0100-00003C000000}"/>
+    <hyperlink ref="J63" r:id="rId62" xr:uid="{00000000-0004-0000-0100-00003D000000}"/>
+    <hyperlink ref="J64" r:id="rId63" xr:uid="{00000000-0004-0000-0100-00003E000000}"/>
+    <hyperlink ref="J65" r:id="rId64" xr:uid="{00000000-0004-0000-0100-00003F000000}"/>
+    <hyperlink ref="J66" r:id="rId65" xr:uid="{00000000-0004-0000-0100-000040000000}"/>
+    <hyperlink ref="J67" r:id="rId66" xr:uid="{00000000-0004-0000-0100-000041000000}"/>
+    <hyperlink ref="J68" r:id="rId67" xr:uid="{00000000-0004-0000-0100-000042000000}"/>
+    <hyperlink ref="J69" r:id="rId68" xr:uid="{00000000-0004-0000-0100-000043000000}"/>
+    <hyperlink ref="J70" r:id="rId69" xr:uid="{00000000-0004-0000-0100-000044000000}"/>
+    <hyperlink ref="J71" r:id="rId70" xr:uid="{00000000-0004-0000-0100-000045000000}"/>
+    <hyperlink ref="J72" r:id="rId71" xr:uid="{00000000-0004-0000-0100-000046000000}"/>
+    <hyperlink ref="J73" r:id="rId72" xr:uid="{00000000-0004-0000-0100-000047000000}"/>
+    <hyperlink ref="J74" r:id="rId73" xr:uid="{00000000-0004-0000-0100-000048000000}"/>
+    <hyperlink ref="J75" r:id="rId74" xr:uid="{00000000-0004-0000-0100-000049000000}"/>
+    <hyperlink ref="J76" r:id="rId75" xr:uid="{00000000-0004-0000-0100-00004A000000}"/>
+    <hyperlink ref="J77" r:id="rId76" xr:uid="{00000000-0004-0000-0100-00004B000000}"/>
+    <hyperlink ref="J78" r:id="rId77" xr:uid="{00000000-0004-0000-0100-00004C000000}"/>
+    <hyperlink ref="J79" r:id="rId78" xr:uid="{00000000-0004-0000-0100-00004D000000}"/>
+    <hyperlink ref="J80" r:id="rId79" xr:uid="{00000000-0004-0000-0100-00004E000000}"/>
+    <hyperlink ref="J81" r:id="rId80" xr:uid="{00000000-0004-0000-0100-00004F000000}"/>
+    <hyperlink ref="J82" r:id="rId81" xr:uid="{00000000-0004-0000-0100-000050000000}"/>
+    <hyperlink ref="J83" r:id="rId82" xr:uid="{00000000-0004-0000-0100-000051000000}"/>
+    <hyperlink ref="J84" r:id="rId83" xr:uid="{00000000-0004-0000-0100-000052000000}"/>
+    <hyperlink ref="J85" r:id="rId84" xr:uid="{00000000-0004-0000-0100-000053000000}"/>
+    <hyperlink ref="J86" r:id="rId85" xr:uid="{00000000-0004-0000-0100-000054000000}"/>
+    <hyperlink ref="J87" r:id="rId86" xr:uid="{00000000-0004-0000-0100-000055000000}"/>
+    <hyperlink ref="J88" r:id="rId87" xr:uid="{00000000-0004-0000-0100-000056000000}"/>
+    <hyperlink ref="J89" r:id="rId88" xr:uid="{00000000-0004-0000-0100-000057000000}"/>
+    <hyperlink ref="J90" r:id="rId89" xr:uid="{00000000-0004-0000-0100-000058000000}"/>
+    <hyperlink ref="J91" r:id="rId90" xr:uid="{00000000-0004-0000-0100-000059000000}"/>
+    <hyperlink ref="J92" r:id="rId91" xr:uid="{00000000-0004-0000-0100-00005A000000}"/>
+    <hyperlink ref="J93" r:id="rId92" xr:uid="{00000000-0004-0000-0100-00005B000000}"/>
+    <hyperlink ref="J94" r:id="rId93" xr:uid="{00000000-0004-0000-0100-00005C000000}"/>
+    <hyperlink ref="J95" r:id="rId94" xr:uid="{00000000-0004-0000-0100-00005D000000}"/>
+    <hyperlink ref="J96" r:id="rId95" xr:uid="{00000000-0004-0000-0100-00005E000000}"/>
+    <hyperlink ref="J97" r:id="rId96" xr:uid="{00000000-0004-0000-0100-00005F000000}"/>
+    <hyperlink ref="J98" r:id="rId97" xr:uid="{00000000-0004-0000-0100-000060000000}"/>
+    <hyperlink ref="J99" r:id="rId98" xr:uid="{00000000-0004-0000-0100-000061000000}"/>
+    <hyperlink ref="J100" r:id="rId99" xr:uid="{00000000-0004-0000-0100-000062000000}"/>
+    <hyperlink ref="J101" r:id="rId100" xr:uid="{00000000-0004-0000-0100-000063000000}"/>
+    <hyperlink ref="J102" r:id="rId101" xr:uid="{00000000-0004-0000-0100-000064000000}"/>
+    <hyperlink ref="J103" r:id="rId102" xr:uid="{00000000-0004-0000-0100-000065000000}"/>
+    <hyperlink ref="J104" r:id="rId103" xr:uid="{00000000-0004-0000-0100-000066000000}"/>
+    <hyperlink ref="J105" r:id="rId104" xr:uid="{00000000-0004-0000-0100-000067000000}"/>
+    <hyperlink ref="J106" r:id="rId105" xr:uid="{00000000-0004-0000-0100-000068000000}"/>
+    <hyperlink ref="J107" r:id="rId106" xr:uid="{00000000-0004-0000-0100-000069000000}"/>
+    <hyperlink ref="J108" r:id="rId107" xr:uid="{00000000-0004-0000-0100-00006A000000}"/>
+    <hyperlink ref="J109" r:id="rId108" xr:uid="{00000000-0004-0000-0100-00006B000000}"/>
+    <hyperlink ref="J110" r:id="rId109" xr:uid="{00000000-0004-0000-0100-00006C000000}"/>
+    <hyperlink ref="J111" r:id="rId110" xr:uid="{00000000-0004-0000-0100-00006D000000}"/>
+    <hyperlink ref="J112" r:id="rId111" xr:uid="{00000000-0004-0000-0100-00006E000000}"/>
+    <hyperlink ref="J113" r:id="rId112" xr:uid="{00000000-0004-0000-0100-00006F000000}"/>
+    <hyperlink ref="J114" r:id="rId113" xr:uid="{00000000-0004-0000-0100-000070000000}"/>
+    <hyperlink ref="G115" r:id="rId114" xr:uid="{00000000-0004-0000-0100-000071000000}"/>
+    <hyperlink ref="J115" r:id="rId115" xr:uid="{00000000-0004-0000-0100-000072000000}"/>
+    <hyperlink ref="J116" r:id="rId116" xr:uid="{00000000-0004-0000-0100-000073000000}"/>
+    <hyperlink ref="G117" r:id="rId117" xr:uid="{00000000-0004-0000-0100-000074000000}"/>
+    <hyperlink ref="J117" r:id="rId118" xr:uid="{00000000-0004-0000-0100-000075000000}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -12287,7 +12291,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -16130,117 +16134,117 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1"/>
-    <hyperlink ref="J3" r:id="rId2"/>
-    <hyperlink ref="J4" r:id="rId3"/>
-    <hyperlink ref="J5" r:id="rId4"/>
-    <hyperlink ref="J6" r:id="rId5"/>
-    <hyperlink ref="J7" r:id="rId6"/>
-    <hyperlink ref="J8" r:id="rId7"/>
-    <hyperlink ref="J9" r:id="rId8"/>
-    <hyperlink ref="J10" r:id="rId9"/>
-    <hyperlink ref="J11" r:id="rId10"/>
-    <hyperlink ref="J12" r:id="rId11"/>
-    <hyperlink ref="J13" r:id="rId12"/>
-    <hyperlink ref="J14" r:id="rId13"/>
-    <hyperlink ref="J15" r:id="rId14"/>
-    <hyperlink ref="J16" r:id="rId15"/>
-    <hyperlink ref="J17" r:id="rId16"/>
-    <hyperlink ref="J18" r:id="rId17"/>
-    <hyperlink ref="J19" r:id="rId18"/>
-    <hyperlink ref="J20" r:id="rId19"/>
-    <hyperlink ref="J21" r:id="rId20"/>
-    <hyperlink ref="J22" r:id="rId21"/>
-    <hyperlink ref="J23" r:id="rId22"/>
-    <hyperlink ref="J24" r:id="rId23"/>
-    <hyperlink ref="J25" r:id="rId24"/>
-    <hyperlink ref="J26" r:id="rId25"/>
-    <hyperlink ref="J27" r:id="rId26"/>
-    <hyperlink ref="J28" r:id="rId27"/>
-    <hyperlink ref="J29" r:id="rId28"/>
-    <hyperlink ref="J30" r:id="rId29"/>
-    <hyperlink ref="J31" r:id="rId30"/>
-    <hyperlink ref="J32" r:id="rId31"/>
-    <hyperlink ref="J33" r:id="rId32"/>
-    <hyperlink ref="J34" r:id="rId33"/>
-    <hyperlink ref="J35" r:id="rId34"/>
-    <hyperlink ref="J36" r:id="rId35"/>
-    <hyperlink ref="J37" r:id="rId36"/>
-    <hyperlink ref="J38" r:id="rId37"/>
-    <hyperlink ref="J39" r:id="rId38"/>
-    <hyperlink ref="J40" r:id="rId39"/>
-    <hyperlink ref="J41" r:id="rId40"/>
-    <hyperlink ref="J42" r:id="rId41"/>
-    <hyperlink ref="J43" r:id="rId42"/>
-    <hyperlink ref="J44" r:id="rId43"/>
-    <hyperlink ref="J45" r:id="rId44"/>
-    <hyperlink ref="J46" r:id="rId45"/>
-    <hyperlink ref="J47" r:id="rId46"/>
-    <hyperlink ref="J48" r:id="rId47"/>
-    <hyperlink ref="J49" r:id="rId48"/>
-    <hyperlink ref="J50" r:id="rId49"/>
-    <hyperlink ref="J51" r:id="rId50"/>
-    <hyperlink ref="J52" r:id="rId51"/>
-    <hyperlink ref="J53" r:id="rId52"/>
-    <hyperlink ref="J54" r:id="rId53"/>
-    <hyperlink ref="J55" r:id="rId54"/>
-    <hyperlink ref="J56" r:id="rId55"/>
-    <hyperlink ref="J57" r:id="rId56"/>
-    <hyperlink ref="J58" r:id="rId57"/>
-    <hyperlink ref="J59" r:id="rId58"/>
-    <hyperlink ref="J60" r:id="rId59"/>
-    <hyperlink ref="J61" r:id="rId60"/>
-    <hyperlink ref="J62" r:id="rId61"/>
-    <hyperlink ref="J63" r:id="rId62"/>
-    <hyperlink ref="J64" r:id="rId63"/>
-    <hyperlink ref="J65" r:id="rId64"/>
-    <hyperlink ref="J66" r:id="rId65"/>
-    <hyperlink ref="J67" r:id="rId66"/>
-    <hyperlink ref="J68" r:id="rId67"/>
-    <hyperlink ref="J69" r:id="rId68"/>
-    <hyperlink ref="J70" r:id="rId69"/>
-    <hyperlink ref="J71" r:id="rId70"/>
-    <hyperlink ref="J72" r:id="rId71"/>
-    <hyperlink ref="J73" r:id="rId72"/>
-    <hyperlink ref="J74" r:id="rId73"/>
-    <hyperlink ref="J75" r:id="rId74"/>
-    <hyperlink ref="J76" r:id="rId75"/>
-    <hyperlink ref="J77" r:id="rId76"/>
-    <hyperlink ref="J78" r:id="rId77"/>
-    <hyperlink ref="J79" r:id="rId78"/>
-    <hyperlink ref="J80" r:id="rId79"/>
-    <hyperlink ref="J81" r:id="rId80"/>
-    <hyperlink ref="J82" r:id="rId81"/>
-    <hyperlink ref="J83" r:id="rId82"/>
-    <hyperlink ref="J84" r:id="rId83"/>
-    <hyperlink ref="J85" r:id="rId84"/>
-    <hyperlink ref="J86" r:id="rId85"/>
-    <hyperlink ref="J87" r:id="rId86"/>
-    <hyperlink ref="J88" r:id="rId87"/>
-    <hyperlink ref="J89" r:id="rId88"/>
-    <hyperlink ref="J90" r:id="rId89"/>
-    <hyperlink ref="J91" r:id="rId90"/>
-    <hyperlink ref="J92" r:id="rId91"/>
-    <hyperlink ref="J93" r:id="rId92"/>
-    <hyperlink ref="J94" r:id="rId93"/>
-    <hyperlink ref="J95" r:id="rId94"/>
-    <hyperlink ref="J96" r:id="rId95"/>
-    <hyperlink ref="J97" r:id="rId96"/>
-    <hyperlink ref="J98" r:id="rId97"/>
-    <hyperlink ref="J99" r:id="rId98"/>
-    <hyperlink ref="J100" r:id="rId99"/>
-    <hyperlink ref="J101" r:id="rId100"/>
-    <hyperlink ref="J102" r:id="rId101"/>
-    <hyperlink ref="J103" r:id="rId102"/>
-    <hyperlink ref="J104" r:id="rId103"/>
-    <hyperlink ref="J105" r:id="rId104"/>
-    <hyperlink ref="J106" r:id="rId105"/>
-    <hyperlink ref="J107" r:id="rId106"/>
-    <hyperlink ref="J108" r:id="rId107"/>
-    <hyperlink ref="J109" r:id="rId108"/>
-    <hyperlink ref="J110" r:id="rId109"/>
-    <hyperlink ref="G111" r:id="rId110"/>
-    <hyperlink ref="J111" r:id="rId111"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="J3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="J4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="J5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="J6" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="J7" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="J8" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="J9" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="J10" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="J11" r:id="rId10" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="J12" r:id="rId11" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
+    <hyperlink ref="J13" r:id="rId12" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
+    <hyperlink ref="J14" r:id="rId13" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
+    <hyperlink ref="J15" r:id="rId14" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
+    <hyperlink ref="J16" r:id="rId15" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
+    <hyperlink ref="J17" r:id="rId16" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
+    <hyperlink ref="J18" r:id="rId17" xr:uid="{00000000-0004-0000-0200-000010000000}"/>
+    <hyperlink ref="J19" r:id="rId18" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
+    <hyperlink ref="J20" r:id="rId19" xr:uid="{00000000-0004-0000-0200-000012000000}"/>
+    <hyperlink ref="J21" r:id="rId20" xr:uid="{00000000-0004-0000-0200-000013000000}"/>
+    <hyperlink ref="J22" r:id="rId21" xr:uid="{00000000-0004-0000-0200-000014000000}"/>
+    <hyperlink ref="J23" r:id="rId22" xr:uid="{00000000-0004-0000-0200-000015000000}"/>
+    <hyperlink ref="J24" r:id="rId23" xr:uid="{00000000-0004-0000-0200-000016000000}"/>
+    <hyperlink ref="J25" r:id="rId24" xr:uid="{00000000-0004-0000-0200-000017000000}"/>
+    <hyperlink ref="J26" r:id="rId25" xr:uid="{00000000-0004-0000-0200-000018000000}"/>
+    <hyperlink ref="J27" r:id="rId26" xr:uid="{00000000-0004-0000-0200-000019000000}"/>
+    <hyperlink ref="J28" r:id="rId27" xr:uid="{00000000-0004-0000-0200-00001A000000}"/>
+    <hyperlink ref="J29" r:id="rId28" xr:uid="{00000000-0004-0000-0200-00001B000000}"/>
+    <hyperlink ref="J30" r:id="rId29" xr:uid="{00000000-0004-0000-0200-00001C000000}"/>
+    <hyperlink ref="J31" r:id="rId30" xr:uid="{00000000-0004-0000-0200-00001D000000}"/>
+    <hyperlink ref="J32" r:id="rId31" xr:uid="{00000000-0004-0000-0200-00001E000000}"/>
+    <hyperlink ref="J33" r:id="rId32" xr:uid="{00000000-0004-0000-0200-00001F000000}"/>
+    <hyperlink ref="J34" r:id="rId33" xr:uid="{00000000-0004-0000-0200-000020000000}"/>
+    <hyperlink ref="J35" r:id="rId34" xr:uid="{00000000-0004-0000-0200-000021000000}"/>
+    <hyperlink ref="J36" r:id="rId35" xr:uid="{00000000-0004-0000-0200-000022000000}"/>
+    <hyperlink ref="J37" r:id="rId36" xr:uid="{00000000-0004-0000-0200-000023000000}"/>
+    <hyperlink ref="J38" r:id="rId37" xr:uid="{00000000-0004-0000-0200-000024000000}"/>
+    <hyperlink ref="J39" r:id="rId38" xr:uid="{00000000-0004-0000-0200-000025000000}"/>
+    <hyperlink ref="J40" r:id="rId39" xr:uid="{00000000-0004-0000-0200-000026000000}"/>
+    <hyperlink ref="J41" r:id="rId40" xr:uid="{00000000-0004-0000-0200-000027000000}"/>
+    <hyperlink ref="J42" r:id="rId41" xr:uid="{00000000-0004-0000-0200-000028000000}"/>
+    <hyperlink ref="J43" r:id="rId42" xr:uid="{00000000-0004-0000-0200-000029000000}"/>
+    <hyperlink ref="J44" r:id="rId43" xr:uid="{00000000-0004-0000-0200-00002A000000}"/>
+    <hyperlink ref="J45" r:id="rId44" xr:uid="{00000000-0004-0000-0200-00002B000000}"/>
+    <hyperlink ref="J46" r:id="rId45" xr:uid="{00000000-0004-0000-0200-00002C000000}"/>
+    <hyperlink ref="J47" r:id="rId46" xr:uid="{00000000-0004-0000-0200-00002D000000}"/>
+    <hyperlink ref="J48" r:id="rId47" xr:uid="{00000000-0004-0000-0200-00002E000000}"/>
+    <hyperlink ref="J49" r:id="rId48" xr:uid="{00000000-0004-0000-0200-00002F000000}"/>
+    <hyperlink ref="J50" r:id="rId49" xr:uid="{00000000-0004-0000-0200-000030000000}"/>
+    <hyperlink ref="J51" r:id="rId50" xr:uid="{00000000-0004-0000-0200-000031000000}"/>
+    <hyperlink ref="J52" r:id="rId51" xr:uid="{00000000-0004-0000-0200-000032000000}"/>
+    <hyperlink ref="J53" r:id="rId52" xr:uid="{00000000-0004-0000-0200-000033000000}"/>
+    <hyperlink ref="J54" r:id="rId53" xr:uid="{00000000-0004-0000-0200-000034000000}"/>
+    <hyperlink ref="J55" r:id="rId54" xr:uid="{00000000-0004-0000-0200-000035000000}"/>
+    <hyperlink ref="J56" r:id="rId55" xr:uid="{00000000-0004-0000-0200-000036000000}"/>
+    <hyperlink ref="J57" r:id="rId56" xr:uid="{00000000-0004-0000-0200-000037000000}"/>
+    <hyperlink ref="J58" r:id="rId57" xr:uid="{00000000-0004-0000-0200-000038000000}"/>
+    <hyperlink ref="J59" r:id="rId58" xr:uid="{00000000-0004-0000-0200-000039000000}"/>
+    <hyperlink ref="J60" r:id="rId59" xr:uid="{00000000-0004-0000-0200-00003A000000}"/>
+    <hyperlink ref="J61" r:id="rId60" xr:uid="{00000000-0004-0000-0200-00003B000000}"/>
+    <hyperlink ref="J62" r:id="rId61" xr:uid="{00000000-0004-0000-0200-00003C000000}"/>
+    <hyperlink ref="J63" r:id="rId62" xr:uid="{00000000-0004-0000-0200-00003D000000}"/>
+    <hyperlink ref="J64" r:id="rId63" xr:uid="{00000000-0004-0000-0200-00003E000000}"/>
+    <hyperlink ref="J65" r:id="rId64" xr:uid="{00000000-0004-0000-0200-00003F000000}"/>
+    <hyperlink ref="J66" r:id="rId65" xr:uid="{00000000-0004-0000-0200-000040000000}"/>
+    <hyperlink ref="J67" r:id="rId66" xr:uid="{00000000-0004-0000-0200-000041000000}"/>
+    <hyperlink ref="J68" r:id="rId67" xr:uid="{00000000-0004-0000-0200-000042000000}"/>
+    <hyperlink ref="J69" r:id="rId68" xr:uid="{00000000-0004-0000-0200-000043000000}"/>
+    <hyperlink ref="J70" r:id="rId69" xr:uid="{00000000-0004-0000-0200-000044000000}"/>
+    <hyperlink ref="J71" r:id="rId70" xr:uid="{00000000-0004-0000-0200-000045000000}"/>
+    <hyperlink ref="J72" r:id="rId71" xr:uid="{00000000-0004-0000-0200-000046000000}"/>
+    <hyperlink ref="J73" r:id="rId72" xr:uid="{00000000-0004-0000-0200-000047000000}"/>
+    <hyperlink ref="J74" r:id="rId73" xr:uid="{00000000-0004-0000-0200-000048000000}"/>
+    <hyperlink ref="J75" r:id="rId74" xr:uid="{00000000-0004-0000-0200-000049000000}"/>
+    <hyperlink ref="J76" r:id="rId75" xr:uid="{00000000-0004-0000-0200-00004A000000}"/>
+    <hyperlink ref="J77" r:id="rId76" xr:uid="{00000000-0004-0000-0200-00004B000000}"/>
+    <hyperlink ref="J78" r:id="rId77" xr:uid="{00000000-0004-0000-0200-00004C000000}"/>
+    <hyperlink ref="J79" r:id="rId78" xr:uid="{00000000-0004-0000-0200-00004D000000}"/>
+    <hyperlink ref="J80" r:id="rId79" xr:uid="{00000000-0004-0000-0200-00004E000000}"/>
+    <hyperlink ref="J81" r:id="rId80" xr:uid="{00000000-0004-0000-0200-00004F000000}"/>
+    <hyperlink ref="J82" r:id="rId81" xr:uid="{00000000-0004-0000-0200-000050000000}"/>
+    <hyperlink ref="J83" r:id="rId82" xr:uid="{00000000-0004-0000-0200-000051000000}"/>
+    <hyperlink ref="J84" r:id="rId83" xr:uid="{00000000-0004-0000-0200-000052000000}"/>
+    <hyperlink ref="J85" r:id="rId84" xr:uid="{00000000-0004-0000-0200-000053000000}"/>
+    <hyperlink ref="J86" r:id="rId85" xr:uid="{00000000-0004-0000-0200-000054000000}"/>
+    <hyperlink ref="J87" r:id="rId86" xr:uid="{00000000-0004-0000-0200-000055000000}"/>
+    <hyperlink ref="J88" r:id="rId87" xr:uid="{00000000-0004-0000-0200-000056000000}"/>
+    <hyperlink ref="J89" r:id="rId88" xr:uid="{00000000-0004-0000-0200-000057000000}"/>
+    <hyperlink ref="J90" r:id="rId89" xr:uid="{00000000-0004-0000-0200-000058000000}"/>
+    <hyperlink ref="J91" r:id="rId90" xr:uid="{00000000-0004-0000-0200-000059000000}"/>
+    <hyperlink ref="J92" r:id="rId91" xr:uid="{00000000-0004-0000-0200-00005A000000}"/>
+    <hyperlink ref="J93" r:id="rId92" xr:uid="{00000000-0004-0000-0200-00005B000000}"/>
+    <hyperlink ref="J94" r:id="rId93" xr:uid="{00000000-0004-0000-0200-00005C000000}"/>
+    <hyperlink ref="J95" r:id="rId94" xr:uid="{00000000-0004-0000-0200-00005D000000}"/>
+    <hyperlink ref="J96" r:id="rId95" xr:uid="{00000000-0004-0000-0200-00005E000000}"/>
+    <hyperlink ref="J97" r:id="rId96" xr:uid="{00000000-0004-0000-0200-00005F000000}"/>
+    <hyperlink ref="J98" r:id="rId97" xr:uid="{00000000-0004-0000-0200-000060000000}"/>
+    <hyperlink ref="J99" r:id="rId98" xr:uid="{00000000-0004-0000-0200-000061000000}"/>
+    <hyperlink ref="J100" r:id="rId99" xr:uid="{00000000-0004-0000-0200-000062000000}"/>
+    <hyperlink ref="J101" r:id="rId100" xr:uid="{00000000-0004-0000-0200-000063000000}"/>
+    <hyperlink ref="J102" r:id="rId101" xr:uid="{00000000-0004-0000-0200-000064000000}"/>
+    <hyperlink ref="J103" r:id="rId102" xr:uid="{00000000-0004-0000-0200-000065000000}"/>
+    <hyperlink ref="J104" r:id="rId103" xr:uid="{00000000-0004-0000-0200-000066000000}"/>
+    <hyperlink ref="J105" r:id="rId104" xr:uid="{00000000-0004-0000-0200-000067000000}"/>
+    <hyperlink ref="J106" r:id="rId105" xr:uid="{00000000-0004-0000-0200-000068000000}"/>
+    <hyperlink ref="J107" r:id="rId106" xr:uid="{00000000-0004-0000-0200-000069000000}"/>
+    <hyperlink ref="J108" r:id="rId107" xr:uid="{00000000-0004-0000-0200-00006A000000}"/>
+    <hyperlink ref="J109" r:id="rId108" xr:uid="{00000000-0004-0000-0200-00006B000000}"/>
+    <hyperlink ref="J110" r:id="rId109" xr:uid="{00000000-0004-0000-0200-00006C000000}"/>
+    <hyperlink ref="G111" r:id="rId110" xr:uid="{00000000-0004-0000-0200-00006D000000}"/>
+    <hyperlink ref="J111" r:id="rId111" xr:uid="{00000000-0004-0000-0200-00006E000000}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
here are some changes
</commit_message>
<xml_diff>
--- a/CS335/GitHub Info sans duplicates.xlsx
+++ b/CS335/GitHub Info sans duplicates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Applications\Xampp\htdocs\staffcard\CS335\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\staffcard\CS335\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09EAB587-9458-4C91-BC9B-E3FC24BFE22F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B636C021-AED8-48F7-862A-D3686ED0E402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3344" uniqueCount="922">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3344" uniqueCount="923">
   <si>
     <t>Timestamp</t>
   </si>
@@ -2793,6 +2793,9 @@
   </si>
   <si>
     <t>https://github.com/YusterBenjamin</t>
+  </si>
+  <si>
+    <t>SHAMIRA SAID</t>
   </si>
 </sst>
 </file>
@@ -3304,20 +3307,20 @@
   <dimension ref="A1:R133"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L134" sqref="L134"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="21.453125" customWidth="1"/>
-    <col min="5" max="5" width="26.453125" customWidth="1"/>
-    <col min="6" max="7" width="21.453125" customWidth="1"/>
-    <col min="8" max="8" width="22.08984375" customWidth="1"/>
-    <col min="9" max="18" width="21.453125" customWidth="1"/>
+    <col min="1" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" customWidth="1"/>
+    <col min="6" max="7" width="21.42578125" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" customWidth="1"/>
+    <col min="9" max="18" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3355,7 +3358,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>44517.7927395718</v>
       </c>
@@ -3393,7 +3396,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>44517.829278495403</v>
       </c>
@@ -3431,7 +3434,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>44517.829803020803</v>
       </c>
@@ -3469,7 +3472,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>44517.832974606499</v>
       </c>
@@ -3507,7 +3510,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>44517.833342615697</v>
       </c>
@@ -3545,7 +3548,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>44517.834096585699</v>
       </c>
@@ -3583,7 +3586,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>44517.834304884302</v>
       </c>
@@ -3621,7 +3624,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>44517.834315161999</v>
       </c>
@@ -3659,7 +3662,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>44517.834467222201</v>
       </c>
@@ -3670,7 +3673,7 @@
         <v>74</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>75</v>
+        <v>922</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>76</v>
@@ -3697,7 +3700,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>44517.836256620401</v>
       </c>
@@ -3735,7 +3738,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>44517.840131203702</v>
       </c>
@@ -3773,7 +3776,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>44517.840687338001</v>
       </c>
@@ -3811,7 +3814,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>44517.840723900503</v>
       </c>
@@ -3849,7 +3852,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>44517.848194363403</v>
       </c>
@@ -3887,7 +3890,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>44517.849799363401</v>
       </c>
@@ -3925,7 +3928,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>44517.851121805601</v>
       </c>
@@ -3963,7 +3966,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>44517.853374618098</v>
       </c>
@@ -4001,7 +4004,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>44517.855156886602</v>
       </c>
@@ -4039,7 +4042,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>44517.8585572917</v>
       </c>
@@ -4077,7 +4080,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>44517.8591194213</v>
       </c>
@@ -4115,7 +4118,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>44517.860663136598</v>
       </c>
@@ -4153,7 +4156,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>44517.863773090299</v>
       </c>
@@ -4191,7 +4194,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>44517.867895196803</v>
       </c>
@@ -4229,7 +4232,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>44517.868303217598</v>
       </c>
@@ -4267,7 +4270,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>44517.8691914468</v>
       </c>
@@ -4305,7 +4308,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>44517.874595833302</v>
       </c>
@@ -4343,7 +4346,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>44517.877297905099</v>
       </c>
@@ -4381,7 +4384,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>44517.877863588001</v>
       </c>
@@ -4419,7 +4422,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>44517.886029872701</v>
       </c>
@@ -4457,7 +4460,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>44517.888174652799</v>
       </c>
@@ -4495,7 +4498,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>44517.890895740697</v>
       </c>
@@ -4533,7 +4536,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>44517.898055138903</v>
       </c>
@@ -4571,7 +4574,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>44517.9033859259</v>
       </c>
@@ -4609,7 +4612,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>44517.916796608799</v>
       </c>
@@ -4647,7 +4650,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>44517.919944965302</v>
       </c>
@@ -4685,7 +4688,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>44517.920174733801</v>
       </c>
@@ -4723,7 +4726,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>44517.920207002302</v>
       </c>
@@ -4761,7 +4764,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>44517.925676088002</v>
       </c>
@@ -4799,7 +4802,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>44517.942313136598</v>
       </c>
@@ -4837,7 +4840,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>44517.967181493099</v>
       </c>
@@ -4875,7 +4878,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>44517.9708563889</v>
       </c>
@@ -4913,7 +4916,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>44517.974103865701</v>
       </c>
@@ -4951,7 +4954,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>44517.995788911998</v>
       </c>
@@ -4989,7 +4992,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>44518.053331921299</v>
       </c>
@@ -5027,7 +5030,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>44518.1416807407</v>
       </c>
@@ -5065,7 +5068,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>44518.338707534698</v>
       </c>
@@ -5103,7 +5106,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>44518.348475844898</v>
       </c>
@@ -5141,7 +5144,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>44518.368981018502</v>
       </c>
@@ -5179,7 +5182,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>44518.376564247701</v>
       </c>
@@ -5217,7 +5220,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>44518.395640312498</v>
       </c>
@@ -5255,7 +5258,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>44518.396610844902</v>
       </c>
@@ -5293,7 +5296,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>44518.416108634301</v>
       </c>
@@ -5331,7 +5334,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>44518.419745173604</v>
       </c>
@@ -5369,7 +5372,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>44518.433273449104</v>
       </c>
@@ -5407,7 +5410,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>44518.433606898201</v>
       </c>
@@ -5445,7 +5448,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>44518.462937638898</v>
       </c>
@@ -5483,7 +5486,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>44518.4791463773</v>
       </c>
@@ -5521,7 +5524,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>44518.500450555599</v>
       </c>
@@ -5559,7 +5562,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>44518.545351886598</v>
       </c>
@@ -5597,7 +5600,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>44518.5769178357</v>
       </c>
@@ -5635,7 +5638,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>44518.580951863398</v>
       </c>
@@ -5673,7 +5676,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>44518.584114340301</v>
       </c>
@@ -5711,7 +5714,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>44518.599512685199</v>
       </c>
@@ -5749,7 +5752,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>44518.6111335069</v>
       </c>
@@ -5787,7 +5790,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>44518.639018194401</v>
       </c>
@@ -5825,7 +5828,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>44518.656796018498</v>
       </c>
@@ -5863,7 +5866,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>44518.669622650501</v>
       </c>
@@ -5901,7 +5904,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>44518.675713946803</v>
       </c>
@@ -5939,7 +5942,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>44518.678410173598</v>
       </c>
@@ -5977,7 +5980,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>44518.679047175901</v>
       </c>
@@ -6015,7 +6018,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>44518.681073298598</v>
       </c>
@@ -6053,7 +6056,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>44518.681981574096</v>
       </c>
@@ -6091,7 +6094,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>44518.682995844902</v>
       </c>
@@ -6129,7 +6132,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>44518.684843472198</v>
       </c>
@@ -6167,7 +6170,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>44518.690567743099</v>
       </c>
@@ -6205,7 +6208,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>44518.704118368099</v>
       </c>
@@ -6243,7 +6246,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>44518.7172751736</v>
       </c>
@@ -6281,7 +6284,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>44518.718211203697</v>
       </c>
@@ -6319,7 +6322,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="80" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>44518.7218906829</v>
       </c>
@@ -6357,7 +6360,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="81" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>44518.845550972197</v>
       </c>
@@ -6395,7 +6398,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="82" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>44518.845807673599</v>
       </c>
@@ -6433,7 +6436,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="83" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>44518.847130671304</v>
       </c>
@@ -6471,7 +6474,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="84" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>44518.8480487384</v>
       </c>
@@ -6509,7 +6512,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="85" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>44518.848206620401</v>
       </c>
@@ -6547,7 +6550,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="86" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>44518.851609803198</v>
       </c>
@@ -6585,7 +6588,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="87" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>44518.853343229202</v>
       </c>
@@ -6623,7 +6626,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="88" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>44518.854456469897</v>
       </c>
@@ -6661,7 +6664,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="89" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>44518.857002847202</v>
       </c>
@@ -6699,7 +6702,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="90" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>44518.857458969898</v>
       </c>
@@ -6737,7 +6740,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="91" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>44518.864664201399</v>
       </c>
@@ -6775,7 +6778,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="92" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>44518.865544432898</v>
       </c>
@@ -6813,7 +6816,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="93" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>44518.8734887963</v>
       </c>
@@ -6851,7 +6854,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="94" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>44518.880978576402</v>
       </c>
@@ -6889,7 +6892,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="95" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>44518.890144791701</v>
       </c>
@@ -6927,7 +6930,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="96" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>44518.8926736227</v>
       </c>
@@ -6965,7 +6968,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="97" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>44518.893882627301</v>
       </c>
@@ -7003,7 +7006,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="98" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>44518.895629976803</v>
       </c>
@@ -7041,7 +7044,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="99" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <v>44518.8972680324</v>
       </c>
@@ -7079,7 +7082,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="100" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>44518.901678900504</v>
       </c>
@@ -7117,7 +7120,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="101" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
         <v>44518.905369791697</v>
       </c>
@@ -7155,7 +7158,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="102" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>44518.914951886603</v>
       </c>
@@ -7193,7 +7196,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="103" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>44518.926460324103</v>
       </c>
@@ -7228,7 +7231,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="104" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>44518.9439103357</v>
       </c>
@@ -7263,7 +7266,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="105" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
         <v>44518.949051713003</v>
       </c>
@@ -7301,7 +7304,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="106" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
         <v>44518.949835740699</v>
       </c>
@@ -7339,7 +7342,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="107" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
         <v>44518.954430393504</v>
       </c>
@@ -7377,7 +7380,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="108" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <v>44518.964523217597</v>
       </c>
@@ -7415,7 +7418,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="109" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
         <v>44518.971188981501</v>
       </c>
@@ -7453,7 +7456,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="110" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
         <v>44518.9722345833</v>
       </c>
@@ -7491,7 +7494,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="111" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
         <v>44518.972730138899</v>
       </c>
@@ -7529,7 +7532,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="112" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
         <v>44518.977785532399</v>
       </c>
@@ -7567,7 +7570,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="113" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="7">
         <v>44519.003693425897</v>
       </c>
@@ -7609,7 +7612,7 @@
       <c r="Q113" s="9"/>
       <c r="R113" s="9"/>
     </row>
-    <row r="114" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
         <v>44521.695289421303</v>
       </c>
@@ -7647,7 +7650,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="115" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
         <v>44521.703645162001</v>
       </c>
@@ -7685,7 +7688,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="116" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
         <v>44521.798439618098</v>
       </c>
@@ -7723,7 +7726,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="117" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
         <v>44521.806830486101</v>
       </c>
@@ -7761,7 +7764,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="118" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
         <v>44521.997838750001</v>
       </c>
@@ -7799,7 +7802,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="119" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
         <v>44522.038008958298</v>
       </c>
@@ -7837,7 +7840,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="120" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
         <v>44522.396687349501</v>
       </c>
@@ -7875,7 +7878,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="121" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
         <v>44522.424870671297</v>
       </c>
@@ -7913,7 +7916,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="122" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
         <v>44522.601772291702</v>
       </c>
@@ -7951,7 +7954,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="123" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="11">
         <v>44532</v>
       </c>
@@ -7986,7 +7989,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="124" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B124" s="3" t="s">
         <v>423</v>
       </c>
@@ -8021,7 +8024,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="125" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B125" s="3" t="s">
         <v>564</v>
       </c>
@@ -8047,7 +8050,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="126" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B126" s="3" t="s">
         <v>458</v>
       </c>
@@ -8070,7 +8073,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="127" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B127" s="3" t="s">
         <v>855</v>
       </c>
@@ -8105,7 +8108,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="128" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B128" s="3" t="s">
         <v>387</v>
       </c>
@@ -8140,7 +8143,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="129" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E129">
         <v>763501830</v>
       </c>
@@ -8166,7 +8169,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="130" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B130" s="3" t="s">
         <v>745</v>
       </c>
@@ -8201,7 +8204,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="131" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B131" t="s">
         <v>869</v>
       </c>
@@ -8236,7 +8239,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>902</v>
       </c>
@@ -8274,7 +8277,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B133" t="s">
         <v>915</v>
       </c>
@@ -8470,22 +8473,22 @@
       <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.453125" customWidth="1"/>
-    <col min="2" max="2" width="16.90625" customWidth="1"/>
-    <col min="3" max="3" width="15.54296875" customWidth="1"/>
-    <col min="4" max="4" width="25.453125" customWidth="1"/>
-    <col min="5" max="5" width="16.90625" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="33.08984375" customWidth="1"/>
-    <col min="8" max="8" width="9.453125" customWidth="1"/>
-    <col min="9" max="9" width="17.453125" customWidth="1"/>
-    <col min="10" max="10" width="33.08984375" customWidth="1"/>
-    <col min="11" max="16" width="21.453125" customWidth="1"/>
+    <col min="7" max="7" width="33.140625" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="10" max="10" width="33.140625" customWidth="1"/>
+    <col min="11" max="16" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>875</v>
       </c>
@@ -8523,7 +8526,7 @@
       <c r="O1" s="13"/>
       <c r="P1" s="13"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -8555,7 +8558,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -8587,7 +8590,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -8619,7 +8622,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -8651,7 +8654,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -8683,7 +8686,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -8715,7 +8718,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -8747,7 +8750,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -8779,7 +8782,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -8811,7 +8814,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -8843,7 +8846,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -8875,7 +8878,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -8907,7 +8910,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -8939,7 +8942,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -8971,7 +8974,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -9003,7 +9006,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -9035,7 +9038,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -9067,7 +9070,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -9099,7 +9102,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -9131,7 +9134,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -9163,7 +9166,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -9195,7 +9198,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -9227,7 +9230,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -9259,7 +9262,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -9291,7 +9294,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -9323,7 +9326,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -9355,7 +9358,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -9387,7 +9390,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -9419,7 +9422,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -9451,7 +9454,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -9483,7 +9486,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -9515,7 +9518,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -9547,7 +9550,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -9579,7 +9582,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -9611,7 +9614,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -9643,7 +9646,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -9675,7 +9678,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -9707,7 +9710,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -9739,7 +9742,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -9771,7 +9774,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -9803,7 +9806,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -9835,7 +9838,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -9867,7 +9870,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -9899,7 +9902,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -9931,7 +9934,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -9963,7 +9966,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -9995,7 +9998,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -10027,7 +10030,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -10059,7 +10062,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -10091,7 +10094,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -10123,7 +10126,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -10155,7 +10158,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -10187,7 +10190,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -10219,7 +10222,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -10251,7 +10254,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -10283,7 +10286,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -10315,7 +10318,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -10347,7 +10350,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -10379,7 +10382,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -10411,7 +10414,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -10443,7 +10446,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -10475,7 +10478,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -10507,7 +10510,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -10539,7 +10542,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -10571,7 +10574,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -10603,7 +10606,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -10635,7 +10638,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -10667,7 +10670,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -10699,7 +10702,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -10731,7 +10734,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -10763,7 +10766,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -10795,7 +10798,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -10827,7 +10830,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="25" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -10859,7 +10862,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -10891,7 +10894,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -10923,7 +10926,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -10955,7 +10958,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -10987,7 +10990,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -11019,7 +11022,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="25" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -11051,7 +11054,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -11083,7 +11086,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -11115,7 +11118,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -11147,7 +11150,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" s="3">
         <v>83</v>
       </c>
@@ -11179,7 +11182,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
         <v>84</v>
       </c>
@@ -11211,7 +11214,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A86" s="3">
         <v>85</v>
       </c>
@@ -11243,7 +11246,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>86</v>
       </c>
@@ -11275,7 +11278,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" s="3">
         <v>87</v>
       </c>
@@ -11307,7 +11310,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
         <v>88</v>
       </c>
@@ -11339,7 +11342,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" s="3">
         <v>89</v>
       </c>
@@ -11371,7 +11374,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" s="3">
         <v>90</v>
       </c>
@@ -11403,7 +11406,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" s="3">
         <v>91</v>
       </c>
@@ -11435,7 +11438,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" s="3">
         <v>92</v>
       </c>
@@ -11467,7 +11470,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94" s="3">
         <v>93</v>
       </c>
@@ -11499,7 +11502,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" s="3">
         <v>94</v>
       </c>
@@ -11531,7 +11534,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" s="3">
         <v>95</v>
       </c>
@@ -11563,7 +11566,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" s="3">
         <v>96</v>
       </c>
@@ -11595,7 +11598,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" s="3">
         <v>97</v>
       </c>
@@ -11627,7 +11630,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" s="3">
         <v>98</v>
       </c>
@@ -11659,7 +11662,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" s="3">
         <v>99</v>
       </c>
@@ -11691,7 +11694,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" s="3">
         <v>100</v>
       </c>
@@ -11723,7 +11726,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" s="3">
         <v>101</v>
       </c>
@@ -11752,7 +11755,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" s="3">
         <v>102</v>
       </c>
@@ -11781,7 +11784,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" s="3">
         <v>103</v>
       </c>
@@ -11813,7 +11816,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" s="3">
         <v>104</v>
       </c>
@@ -11845,7 +11848,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" s="3">
         <v>105</v>
       </c>
@@ -11877,7 +11880,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" s="3">
         <v>106</v>
       </c>
@@ -11909,7 +11912,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" s="3">
         <v>107</v>
       </c>
@@ -11941,7 +11944,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" s="3">
         <v>108</v>
       </c>
@@ -11973,7 +11976,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" s="3">
         <v>109</v>
       </c>
@@ -12005,7 +12008,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" s="3">
         <v>110</v>
       </c>
@@ -12037,7 +12040,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" s="3">
         <v>111</v>
       </c>
@@ -12066,7 +12069,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113" s="3">
         <v>112</v>
       </c>
@@ -12098,7 +12101,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114" s="3">
         <v>113</v>
       </c>
@@ -12130,7 +12133,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115" s="3">
         <v>114</v>
       </c>
@@ -12162,7 +12165,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A116" s="3">
         <v>115</v>
       </c>
@@ -12191,7 +12194,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A117" s="3">
         <v>116</v>
       </c>
@@ -12220,289 +12223,289 @@
         <v>914</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J118" s="17"/>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J119" s="17"/>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J120" s="17"/>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J121" s="17"/>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J122" s="17"/>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J123" s="17"/>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J124" s="17"/>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J125" s="17"/>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J126" s="17"/>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J127" s="17"/>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J128" s="17"/>
     </row>
-    <row r="129" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J129" s="17"/>
     </row>
-    <row r="130" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J130" s="17"/>
     </row>
-    <row r="131" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J131" s="17"/>
     </row>
-    <row r="132" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J132" s="17"/>
     </row>
-    <row r="133" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J133" s="17"/>
     </row>
-    <row r="134" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J134" s="17"/>
     </row>
-    <row r="135" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J135" s="17"/>
     </row>
-    <row r="136" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J136" s="17"/>
     </row>
-    <row r="137" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J137" s="17"/>
     </row>
-    <row r="138" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J138" s="17"/>
     </row>
-    <row r="139" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J139" s="17"/>
     </row>
-    <row r="140" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J140" s="17"/>
     </row>
-    <row r="141" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J141" s="17"/>
     </row>
-    <row r="142" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J142" s="17"/>
     </row>
-    <row r="143" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J143" s="17"/>
     </row>
-    <row r="144" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J144" s="17"/>
     </row>
-    <row r="145" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J145" s="17"/>
     </row>
-    <row r="146" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J146" s="17"/>
     </row>
-    <row r="147" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J147" s="17"/>
     </row>
-    <row r="148" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J148" s="17"/>
     </row>
-    <row r="149" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J149" s="17"/>
     </row>
-    <row r="150" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J150" s="17"/>
     </row>
-    <row r="151" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J151" s="17"/>
     </row>
-    <row r="152" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J152" s="17"/>
     </row>
-    <row r="153" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J153" s="17"/>
     </row>
-    <row r="154" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J154" s="17"/>
     </row>
-    <row r="155" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J155" s="17"/>
     </row>
-    <row r="156" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J156" s="17"/>
     </row>
-    <row r="157" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J157" s="17"/>
     </row>
-    <row r="158" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J158" s="17"/>
     </row>
-    <row r="159" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J159" s="17"/>
     </row>
-    <row r="160" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J160" s="17"/>
     </row>
-    <row r="161" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J161" s="17"/>
     </row>
-    <row r="162" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J162" s="17"/>
     </row>
-    <row r="163" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J163" s="17"/>
     </row>
-    <row r="164" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J164" s="17"/>
     </row>
-    <row r="165" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J165" s="17"/>
     </row>
-    <row r="166" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J166" s="17"/>
     </row>
-    <row r="167" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J167" s="17"/>
     </row>
-    <row r="168" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J168" s="17"/>
     </row>
-    <row r="169" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J169" s="17"/>
     </row>
-    <row r="170" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J170" s="17"/>
     </row>
-    <row r="171" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J171" s="17"/>
     </row>
-    <row r="172" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J172" s="17"/>
     </row>
-    <row r="173" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J173" s="17"/>
     </row>
-    <row r="174" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J174" s="17"/>
     </row>
-    <row r="175" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J175" s="17"/>
     </row>
-    <row r="176" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J176" s="17"/>
     </row>
-    <row r="177" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J177" s="17"/>
     </row>
-    <row r="178" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J178" s="17"/>
     </row>
-    <row r="179" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J179" s="17"/>
     </row>
-    <row r="180" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J180" s="17"/>
     </row>
-    <row r="181" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J181" s="17"/>
     </row>
-    <row r="182" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J182" s="17"/>
     </row>
-    <row r="183" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J183" s="17"/>
     </row>
-    <row r="184" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J184" s="17"/>
     </row>
-    <row r="185" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J185" s="17"/>
     </row>
-    <row r="186" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J186" s="17"/>
     </row>
-    <row r="187" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J187" s="17"/>
     </row>
-    <row r="188" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J188" s="17"/>
     </row>
-    <row r="189" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J189" s="17"/>
     </row>
-    <row r="190" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J190" s="17"/>
     </row>
-    <row r="191" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J191" s="17"/>
     </row>
-    <row r="192" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J192" s="17"/>
     </row>
-    <row r="193" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J193" s="17"/>
     </row>
-    <row r="194" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J194" s="17"/>
     </row>
-    <row r="195" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J195" s="17"/>
     </row>
-    <row r="196" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J196" s="17"/>
     </row>
-    <row r="197" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J197" s="17"/>
     </row>
-    <row r="198" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J198" s="17"/>
     </row>
-    <row r="199" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J199" s="17"/>
     </row>
-    <row r="200" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J200" s="17"/>
     </row>
-    <row r="201" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J201" s="17"/>
     </row>
-    <row r="202" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J202" s="17"/>
     </row>
-    <row r="203" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J203" s="17"/>
     </row>
-    <row r="204" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J204" s="17"/>
     </row>
-    <row r="205" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J205" s="17"/>
     </row>
-    <row r="206" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="206" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J206" s="17"/>
     </row>
-    <row r="207" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="207" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J207" s="17"/>
     </row>
-    <row r="208" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="208" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J208" s="17"/>
     </row>
-    <row r="209" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J209" s="17"/>
     </row>
-    <row r="210" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J210" s="17"/>
     </row>
-    <row r="211" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J211" s="17"/>
     </row>
-    <row r="212" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J212" s="17"/>
     </row>
   </sheetData>
@@ -12650,22 +12653,22 @@
       <selection pane="bottomLeft" activeCell="E96" sqref="E96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.453125" customWidth="1"/>
-    <col min="2" max="2" width="16.90625" customWidth="1"/>
-    <col min="3" max="3" width="15.54296875" customWidth="1"/>
-    <col min="4" max="4" width="25.453125" customWidth="1"/>
-    <col min="5" max="5" width="16.90625" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="33.08984375" customWidth="1"/>
-    <col min="8" max="8" width="9.453125" customWidth="1"/>
-    <col min="9" max="9" width="17.453125" customWidth="1"/>
-    <col min="10" max="10" width="33.08984375" customWidth="1"/>
-    <col min="11" max="16" width="21.453125" customWidth="1"/>
+    <col min="7" max="7" width="33.140625" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="10" max="10" width="33.140625" customWidth="1"/>
+    <col min="11" max="16" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>875</v>
       </c>
@@ -12703,7 +12706,7 @@
       <c r="O1" s="13"/>
       <c r="P1" s="13"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -12735,7 +12738,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -12767,7 +12770,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -12799,7 +12802,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -12831,7 +12834,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -12863,7 +12866,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -12895,7 +12898,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -12927,7 +12930,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -12959,7 +12962,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -12991,7 +12994,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -13023,7 +13026,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -13055,7 +13058,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -13087,7 +13090,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -13119,7 +13122,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -13151,7 +13154,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -13183,7 +13186,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -13215,7 +13218,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -13247,7 +13250,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -13279,7 +13282,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -13311,7 +13314,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -13343,7 +13346,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -13375,7 +13378,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -13407,7 +13410,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -13439,7 +13442,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -13471,7 +13474,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -13503,7 +13506,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -13535,7 +13538,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -13567,7 +13570,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -13599,7 +13602,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -13631,7 +13634,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -13663,7 +13666,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -13695,7 +13698,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -13727,7 +13730,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -13759,7 +13762,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -13791,7 +13794,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -13823,7 +13826,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -13855,7 +13858,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -13887,7 +13890,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -13919,7 +13922,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -13951,7 +13954,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -13983,7 +13986,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -14015,7 +14018,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -14047,7 +14050,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -14079,7 +14082,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -14111,7 +14114,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -14143,7 +14146,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -14175,7 +14178,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -14207,7 +14210,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -14239,7 +14242,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -14271,7 +14274,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -14303,7 +14306,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -14335,7 +14338,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -14367,7 +14370,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -14399,7 +14402,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -14431,7 +14434,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -14463,7 +14466,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -14495,7 +14498,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -14527,7 +14530,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -14559,7 +14562,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -14591,7 +14594,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -14623,7 +14626,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -14655,7 +14658,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -14687,7 +14690,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -14719,7 +14722,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -14751,7 +14754,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -14783,7 +14786,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -14815,7 +14818,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -14847,7 +14850,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -14879,7 +14882,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -14911,7 +14914,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -14943,7 +14946,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -14975,7 +14978,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -15007,7 +15010,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -15039,7 +15042,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -15071,7 +15074,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -15103,7 +15106,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -15135,7 +15138,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -15167,7 +15170,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -15199,7 +15202,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -15231,7 +15234,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -15263,7 +15266,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -15295,7 +15298,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -15327,7 +15330,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" s="3">
         <v>83</v>
       </c>
@@ -15359,7 +15362,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
         <v>84</v>
       </c>
@@ -15391,7 +15394,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" s="3">
         <v>85</v>
       </c>
@@ -15423,7 +15426,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>86</v>
       </c>
@@ -15455,7 +15458,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" s="3">
         <v>87</v>
       </c>
@@ -15484,7 +15487,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
         <v>88</v>
       </c>
@@ -15513,7 +15516,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" s="3">
         <v>89</v>
       </c>
@@ -15545,7 +15548,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" s="3">
         <v>90</v>
       </c>
@@ -15577,7 +15580,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" s="3">
         <v>91</v>
       </c>
@@ -15609,7 +15612,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" s="3">
         <v>92</v>
       </c>
@@ -15641,7 +15644,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94" s="3">
         <v>93</v>
       </c>
@@ -15673,7 +15676,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" s="3">
         <v>94</v>
       </c>
@@ -15705,7 +15708,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" s="3">
         <v>95</v>
       </c>
@@ -15737,7 +15740,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" s="3">
         <v>96</v>
       </c>
@@ -15769,7 +15772,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" s="3">
         <v>97</v>
       </c>
@@ -15798,7 +15801,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" s="3">
         <v>98</v>
       </c>
@@ -15830,7 +15833,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" s="3">
         <v>99</v>
       </c>
@@ -15862,7 +15865,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" s="3">
         <v>100</v>
       </c>
@@ -15894,7 +15897,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" s="3">
         <v>101</v>
       </c>
@@ -15926,7 +15929,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" s="3">
         <v>102</v>
       </c>
@@ -15958,7 +15961,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" s="3">
         <v>103</v>
       </c>
@@ -15990,7 +15993,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" s="3">
         <v>104</v>
       </c>
@@ -16022,7 +16025,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" s="3">
         <v>105</v>
       </c>
@@ -16054,7 +16057,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" s="3">
         <v>106</v>
       </c>
@@ -16086,7 +16089,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" s="3">
         <v>107</v>
       </c>
@@ -16118,7 +16121,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" s="3">
         <v>108</v>
       </c>
@@ -16150,7 +16153,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" s="3">
         <v>109</v>
       </c>
@@ -16182,268 +16185,268 @@
         <v>862</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J111" s="17"/>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J112" s="17"/>
     </row>
-    <row r="113" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J113" s="17"/>
     </row>
-    <row r="114" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J114" s="17"/>
     </row>
-    <row r="115" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J115" s="17"/>
     </row>
-    <row r="116" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J116" s="17"/>
     </row>
-    <row r="117" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J117" s="17"/>
     </row>
-    <row r="118" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J118" s="17"/>
     </row>
-    <row r="119" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J119" s="17"/>
     </row>
-    <row r="120" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J120" s="17"/>
     </row>
-    <row r="121" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J121" s="17"/>
     </row>
-    <row r="122" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J122" s="17"/>
     </row>
-    <row r="123" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J123" s="17"/>
     </row>
-    <row r="124" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J124" s="17"/>
     </row>
-    <row r="125" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J125" s="17"/>
     </row>
-    <row r="126" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J126" s="17"/>
     </row>
-    <row r="127" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J127" s="17"/>
     </row>
-    <row r="128" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J128" s="17"/>
     </row>
-    <row r="129" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J129" s="17"/>
     </row>
-    <row r="130" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J130" s="17"/>
     </row>
-    <row r="131" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J131" s="17"/>
     </row>
-    <row r="132" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J132" s="17"/>
     </row>
-    <row r="133" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J133" s="17"/>
     </row>
-    <row r="134" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J134" s="17"/>
     </row>
-    <row r="135" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J135" s="17"/>
     </row>
-    <row r="136" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J136" s="17"/>
     </row>
-    <row r="137" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J137" s="17"/>
     </row>
-    <row r="138" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J138" s="17"/>
     </row>
-    <row r="139" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J139" s="17"/>
     </row>
-    <row r="140" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J140" s="17"/>
     </row>
-    <row r="141" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J141" s="17"/>
     </row>
-    <row r="142" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J142" s="17"/>
     </row>
-    <row r="143" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J143" s="17"/>
     </row>
-    <row r="144" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J144" s="17"/>
     </row>
-    <row r="145" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J145" s="17"/>
     </row>
-    <row r="146" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J146" s="17"/>
     </row>
-    <row r="147" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J147" s="17"/>
     </row>
-    <row r="148" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J148" s="17"/>
     </row>
-    <row r="149" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J149" s="17"/>
     </row>
-    <row r="150" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J150" s="17"/>
     </row>
-    <row r="151" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J151" s="17"/>
     </row>
-    <row r="152" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J152" s="17"/>
     </row>
-    <row r="153" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J153" s="17"/>
     </row>
-    <row r="154" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J154" s="17"/>
     </row>
-    <row r="155" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J155" s="17"/>
     </row>
-    <row r="156" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J156" s="17"/>
     </row>
-    <row r="157" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J157" s="17"/>
     </row>
-    <row r="158" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J158" s="17"/>
     </row>
-    <row r="159" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J159" s="17"/>
     </row>
-    <row r="160" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J160" s="17"/>
     </row>
-    <row r="161" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J161" s="17"/>
     </row>
-    <row r="162" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J162" s="17"/>
     </row>
-    <row r="163" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J163" s="17"/>
     </row>
-    <row r="164" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J164" s="17"/>
     </row>
-    <row r="165" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J165" s="17"/>
     </row>
-    <row r="166" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J166" s="17"/>
     </row>
-    <row r="167" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J167" s="17"/>
     </row>
-    <row r="168" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J168" s="17"/>
     </row>
-    <row r="169" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J169" s="17"/>
     </row>
-    <row r="170" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J170" s="17"/>
     </row>
-    <row r="171" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J171" s="17"/>
     </row>
-    <row r="172" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J172" s="17"/>
     </row>
-    <row r="173" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J173" s="17"/>
     </row>
-    <row r="174" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J174" s="17"/>
     </row>
-    <row r="175" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J175" s="17"/>
     </row>
-    <row r="176" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J176" s="17"/>
     </row>
-    <row r="177" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J177" s="17"/>
     </row>
-    <row r="178" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J178" s="17"/>
     </row>
-    <row r="179" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J179" s="17"/>
     </row>
-    <row r="180" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J180" s="17"/>
     </row>
-    <row r="181" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J181" s="17"/>
     </row>
-    <row r="182" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J182" s="17"/>
     </row>
-    <row r="183" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J183" s="17"/>
     </row>
-    <row r="184" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J184" s="17"/>
     </row>
-    <row r="185" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J185" s="17"/>
     </row>
-    <row r="186" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J186" s="17"/>
     </row>
-    <row r="187" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J187" s="17"/>
     </row>
-    <row r="188" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J188" s="17"/>
     </row>
-    <row r="189" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J189" s="17"/>
     </row>
-    <row r="190" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J190" s="17"/>
     </row>
-    <row r="191" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J191" s="17"/>
     </row>
-    <row r="192" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J192" s="17"/>
     </row>
-    <row r="193" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J193" s="17"/>
     </row>
-    <row r="194" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J194" s="17"/>
     </row>
-    <row r="195" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J195" s="17"/>
     </row>
-    <row r="196" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J196" s="17"/>
     </row>
-    <row r="197" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J197" s="17"/>
     </row>
-    <row r="198" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J198" s="17"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Dion Kapfumvuti's details
</commit_message>
<xml_diff>
--- a/CS335/GitHub Info sans duplicates.xlsx
+++ b/CS335/GitHub Info sans duplicates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\Desktop\aligit\staffcard\cs335\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59068B20-D18D-4A37-8992-578BA6684581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B1E035D-3E5B-4497-8EEE-ED1123FF4AAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3256" uniqueCount="882">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3265" uniqueCount="882">
   <si>
     <t>Timestamp</t>
   </si>
@@ -3452,11 +3452,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:R127"/>
+  <dimension ref="A1:R128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C127" sqref="C127"/>
+      <selection pane="bottomLeft" activeCell="B128" sqref="B128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8231,6 +8231,38 @@
       </c>
       <c r="I127" s="3" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="128" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B128" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D128" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E128" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F128" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G128" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H128" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I128" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J128">
+        <v>3</v>
+      </c>
+      <c r="K128" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -8363,6 +8395,7 @@
     <hyperlink ref="G125" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
     <hyperlink ref="G126" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
     <hyperlink ref="G127" r:id="rId128" xr:uid="{7532BFD0-8793-404E-B456-A9A4C5A5AC68}"/>
+    <hyperlink ref="G128" r:id="rId129" xr:uid="{CB99F1D8-5DD6-4F73-8761-DD4BD5E0CBE1}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
added my details in the excel file
</commit_message>
<xml_diff>
--- a/CS335/GitHub Info sans duplicates.xlsx
+++ b/CS335/GitHub Info sans duplicates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\staffcard\CS335\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD296660-AD3E-4801-9649-104DCACCD931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3BBB50-496F-438C-9B4E-A50781C4C0B9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3308" uniqueCount="903">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3317" uniqueCount="910">
   <si>
     <t>Timestamp</t>
   </si>
@@ -2736,6 +2736,27 @@
   </si>
   <si>
     <t>https://github.com/Bibahbaanda</t>
+  </si>
+  <si>
+    <t>2019-04-07078</t>
+  </si>
+  <si>
+    <t>MHANDO</t>
+  </si>
+  <si>
+    <t>ISSA RAMADHANI</t>
+  </si>
+  <si>
+    <t>0788719867</t>
+  </si>
+  <si>
+    <t>issamhando@gmail.com</t>
+  </si>
+  <si>
+    <t>issalito</t>
+  </si>
+  <si>
+    <t>https://github.com/issalito</t>
   </si>
 </sst>
 </file>
@@ -2822,7 +2843,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -2853,6 +2874,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -8282,8 +8304,8 @@
   </sheetPr>
   <dimension ref="A1:P212"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K116" sqref="K116"/>
     </sheetView>
   </sheetViews>
@@ -12014,8 +12036,36 @@
       </c>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="E117" s="16"/>
-      <c r="J117" s="15"/>
+      <c r="A117" s="3">
+        <v>116</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>903</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>904</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>905</v>
+      </c>
+      <c r="E117" s="16" t="s">
+        <v>906</v>
+      </c>
+      <c r="F117" s="3" t="s">
+        <v>880</v>
+      </c>
+      <c r="G117" s="20" t="s">
+        <v>907</v>
+      </c>
+      <c r="H117" s="3" t="s">
+        <v>883</v>
+      </c>
+      <c r="I117" s="3" t="s">
+        <v>908</v>
+      </c>
+      <c r="J117" s="19" t="s">
+        <v>909</v>
+      </c>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.2">
       <c r="J118" s="15"/>
@@ -12303,7 +12353,7 @@
       <c r="J212" s="15"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B113 B116">
+  <conditionalFormatting sqref="B2:B113 B116:B117">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>COUNTIF($A$2:$A$14,A2)&gt;1</formula>
     </cfRule>
@@ -12426,10 +12476,12 @@
     <hyperlink ref="J115" r:id="rId115" xr:uid="{00000000-0004-0000-0100-000072000000}"/>
     <hyperlink ref="G116" r:id="rId116" xr:uid="{69660F94-B912-416E-A061-7BD913D93359}"/>
     <hyperlink ref="J116" r:id="rId117" xr:uid="{E95EF49E-00FD-48BD-AB03-997CB0E19159}"/>
+    <hyperlink ref="G117" r:id="rId118" xr:uid="{050D6865-4798-4940-A113-5AEC094DA3AD}"/>
+    <hyperlink ref="J117" r:id="rId119" xr:uid="{229E0B3D-59CA-4122-B9F8-61F16D61809F}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" fitToHeight="0" pageOrder="overThenDown" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId118"/>
+  <pageSetup paperSize="9" firstPageNumber="0" fitToHeight="0" pageOrder="overThenDown" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId120"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
removed a single letter
</commit_message>
<xml_diff>
--- a/CS335/GitHub Info sans duplicates.xlsx
+++ b/CS335/GitHub Info sans duplicates.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\staffcard\CS335\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\makambi\Documents\GitHub\staffcard\CS335\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D1C2F38-034B-447A-BDF6-467E1B3ACFBE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
     <sheet name="GitHub Info" sheetId="2" r:id="rId2"/>
     <sheet name="GitHub Info sans duplicates" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3297" uniqueCount="890">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3297" uniqueCount="891">
   <si>
     <t>Timestamp</t>
   </si>
@@ -2697,12 +2696,15 @@
   </si>
   <si>
     <t>DANIEL SOLOMON</t>
+  </si>
+  <si>
+    <t>JAME</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
@@ -3475,7 +3477,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -8338,137 +8340,137 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="L3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="L4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="L5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="L6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="L7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="L8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="L9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="L10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="L11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="L12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="L13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="L14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="L15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="L16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="L17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="L18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="L19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="L20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="L21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="L22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="L23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="L24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="L25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="L26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="L27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="L28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="L29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="L30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="L31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="L32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="L33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="L34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="L35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="L36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="L37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="L38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="L39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="L40" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="L41" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="L42" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="L43" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="L44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="L45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="L46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="L47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="L48" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="L49" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="L50" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="L51" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="L52" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="L53" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="L54" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="L55" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="L56" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="L57" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="L58" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="L59" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="L60" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="L61" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="L62" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="L63" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="L64" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="L65" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="L66" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="L67" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="L68" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="L69" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="L70" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="L71" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="L72" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="L73" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="L74" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="L75" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="L76" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="L77" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="L78" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="L79" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="L80" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="L81" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="L82" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="L83" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="L84" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="L85" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="L86" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="L87" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="L88" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="L89" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="L90" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="L91" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="L92" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="L93" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="L94" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="L95" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="L96" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="L97" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="L98" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="L99" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="L100" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="L101" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="L102" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="L103" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
-    <hyperlink ref="L104" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
-    <hyperlink ref="L105" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="L106" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
-    <hyperlink ref="L107" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="L108" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
-    <hyperlink ref="L109" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
-    <hyperlink ref="L110" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
-    <hyperlink ref="L111" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="L112" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
-    <hyperlink ref="L113" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
-    <hyperlink ref="L114" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
-    <hyperlink ref="L115" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="L116" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
-    <hyperlink ref="L117" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
-    <hyperlink ref="L118" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
-    <hyperlink ref="L119" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
-    <hyperlink ref="L120" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
-    <hyperlink ref="L121" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
-    <hyperlink ref="L122" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
-    <hyperlink ref="G123" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
-    <hyperlink ref="L123" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
-    <hyperlink ref="G124" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
-    <hyperlink ref="L124" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
-    <hyperlink ref="G125" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
-    <hyperlink ref="G126" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
-    <hyperlink ref="G127" r:id="rId128" xr:uid="{7532BFD0-8793-404E-B456-A9A4C5A5AC68}"/>
-    <hyperlink ref="G128" r:id="rId129" xr:uid="{CB99F1D8-5DD6-4F73-8761-DD4BD5E0CBE1}"/>
-    <hyperlink ref="G129" r:id="rId130" xr:uid="{43FE3FD3-7C28-40AD-94AA-407881D4ED7E}"/>
-    <hyperlink ref="L129" r:id="rId131" xr:uid="{43A6072C-DEA2-41E6-8B80-F7290ACAC14A}"/>
+    <hyperlink ref="L2" r:id="rId1"/>
+    <hyperlink ref="L3" r:id="rId2"/>
+    <hyperlink ref="L4" r:id="rId3"/>
+    <hyperlink ref="L5" r:id="rId4"/>
+    <hyperlink ref="L6" r:id="rId5"/>
+    <hyperlink ref="L7" r:id="rId6"/>
+    <hyperlink ref="L8" r:id="rId7"/>
+    <hyperlink ref="L9" r:id="rId8"/>
+    <hyperlink ref="L10" r:id="rId9"/>
+    <hyperlink ref="L11" r:id="rId10"/>
+    <hyperlink ref="L12" r:id="rId11"/>
+    <hyperlink ref="L13" r:id="rId12"/>
+    <hyperlink ref="L14" r:id="rId13"/>
+    <hyperlink ref="L15" r:id="rId14"/>
+    <hyperlink ref="L16" r:id="rId15"/>
+    <hyperlink ref="L17" r:id="rId16"/>
+    <hyperlink ref="L18" r:id="rId17"/>
+    <hyperlink ref="L19" r:id="rId18"/>
+    <hyperlink ref="L20" r:id="rId19"/>
+    <hyperlink ref="L21" r:id="rId20"/>
+    <hyperlink ref="L22" r:id="rId21"/>
+    <hyperlink ref="L23" r:id="rId22"/>
+    <hyperlink ref="L24" r:id="rId23"/>
+    <hyperlink ref="L25" r:id="rId24"/>
+    <hyperlink ref="L26" r:id="rId25"/>
+    <hyperlink ref="L27" r:id="rId26"/>
+    <hyperlink ref="L28" r:id="rId27"/>
+    <hyperlink ref="L29" r:id="rId28"/>
+    <hyperlink ref="L30" r:id="rId29"/>
+    <hyperlink ref="L31" r:id="rId30"/>
+    <hyperlink ref="L32" r:id="rId31"/>
+    <hyperlink ref="L33" r:id="rId32"/>
+    <hyperlink ref="L34" r:id="rId33"/>
+    <hyperlink ref="L35" r:id="rId34"/>
+    <hyperlink ref="L36" r:id="rId35"/>
+    <hyperlink ref="L37" r:id="rId36"/>
+    <hyperlink ref="L38" r:id="rId37"/>
+    <hyperlink ref="L39" r:id="rId38"/>
+    <hyperlink ref="L40" r:id="rId39"/>
+    <hyperlink ref="L41" r:id="rId40"/>
+    <hyperlink ref="L42" r:id="rId41"/>
+    <hyperlink ref="L43" r:id="rId42"/>
+    <hyperlink ref="L44" r:id="rId43"/>
+    <hyperlink ref="L45" r:id="rId44"/>
+    <hyperlink ref="L46" r:id="rId45"/>
+    <hyperlink ref="L47" r:id="rId46"/>
+    <hyperlink ref="L48" r:id="rId47"/>
+    <hyperlink ref="L49" r:id="rId48"/>
+    <hyperlink ref="L50" r:id="rId49"/>
+    <hyperlink ref="L51" r:id="rId50"/>
+    <hyperlink ref="L52" r:id="rId51"/>
+    <hyperlink ref="L53" r:id="rId52"/>
+    <hyperlink ref="L54" r:id="rId53"/>
+    <hyperlink ref="L55" r:id="rId54"/>
+    <hyperlink ref="L56" r:id="rId55"/>
+    <hyperlink ref="L57" r:id="rId56"/>
+    <hyperlink ref="L58" r:id="rId57"/>
+    <hyperlink ref="L59" r:id="rId58"/>
+    <hyperlink ref="L60" r:id="rId59"/>
+    <hyperlink ref="L61" r:id="rId60"/>
+    <hyperlink ref="L62" r:id="rId61"/>
+    <hyperlink ref="L63" r:id="rId62"/>
+    <hyperlink ref="L64" r:id="rId63"/>
+    <hyperlink ref="L65" r:id="rId64"/>
+    <hyperlink ref="L66" r:id="rId65"/>
+    <hyperlink ref="L67" r:id="rId66"/>
+    <hyperlink ref="L68" r:id="rId67"/>
+    <hyperlink ref="L69" r:id="rId68"/>
+    <hyperlink ref="L70" r:id="rId69"/>
+    <hyperlink ref="L71" r:id="rId70"/>
+    <hyperlink ref="L72" r:id="rId71"/>
+    <hyperlink ref="L73" r:id="rId72"/>
+    <hyperlink ref="L74" r:id="rId73"/>
+    <hyperlink ref="L75" r:id="rId74"/>
+    <hyperlink ref="L76" r:id="rId75"/>
+    <hyperlink ref="L77" r:id="rId76"/>
+    <hyperlink ref="L78" r:id="rId77"/>
+    <hyperlink ref="L79" r:id="rId78"/>
+    <hyperlink ref="L80" r:id="rId79"/>
+    <hyperlink ref="L81" r:id="rId80"/>
+    <hyperlink ref="L82" r:id="rId81"/>
+    <hyperlink ref="L83" r:id="rId82"/>
+    <hyperlink ref="L84" r:id="rId83"/>
+    <hyperlink ref="L85" r:id="rId84"/>
+    <hyperlink ref="L86" r:id="rId85"/>
+    <hyperlink ref="L87" r:id="rId86"/>
+    <hyperlink ref="L88" r:id="rId87"/>
+    <hyperlink ref="L89" r:id="rId88"/>
+    <hyperlink ref="L90" r:id="rId89"/>
+    <hyperlink ref="L91" r:id="rId90"/>
+    <hyperlink ref="L92" r:id="rId91"/>
+    <hyperlink ref="L93" r:id="rId92"/>
+    <hyperlink ref="L94" r:id="rId93"/>
+    <hyperlink ref="L95" r:id="rId94"/>
+    <hyperlink ref="L96" r:id="rId95"/>
+    <hyperlink ref="L97" r:id="rId96"/>
+    <hyperlink ref="L98" r:id="rId97"/>
+    <hyperlink ref="L99" r:id="rId98"/>
+    <hyperlink ref="L100" r:id="rId99"/>
+    <hyperlink ref="L101" r:id="rId100"/>
+    <hyperlink ref="L102" r:id="rId101"/>
+    <hyperlink ref="L103" r:id="rId102"/>
+    <hyperlink ref="L104" r:id="rId103"/>
+    <hyperlink ref="L105" r:id="rId104"/>
+    <hyperlink ref="L106" r:id="rId105"/>
+    <hyperlink ref="L107" r:id="rId106"/>
+    <hyperlink ref="L108" r:id="rId107"/>
+    <hyperlink ref="L109" r:id="rId108"/>
+    <hyperlink ref="L110" r:id="rId109"/>
+    <hyperlink ref="L111" r:id="rId110"/>
+    <hyperlink ref="L112" r:id="rId111"/>
+    <hyperlink ref="L113" r:id="rId112"/>
+    <hyperlink ref="L114" r:id="rId113"/>
+    <hyperlink ref="L115" r:id="rId114"/>
+    <hyperlink ref="L116" r:id="rId115"/>
+    <hyperlink ref="L117" r:id="rId116"/>
+    <hyperlink ref="L118" r:id="rId117"/>
+    <hyperlink ref="L119" r:id="rId118"/>
+    <hyperlink ref="L120" r:id="rId119"/>
+    <hyperlink ref="L121" r:id="rId120"/>
+    <hyperlink ref="L122" r:id="rId121"/>
+    <hyperlink ref="G123" r:id="rId122"/>
+    <hyperlink ref="L123" r:id="rId123"/>
+    <hyperlink ref="G124" r:id="rId124"/>
+    <hyperlink ref="L124" r:id="rId125"/>
+    <hyperlink ref="G125" r:id="rId126"/>
+    <hyperlink ref="G126" r:id="rId127"/>
+    <hyperlink ref="G127" r:id="rId128"/>
+    <hyperlink ref="G128" r:id="rId129"/>
+    <hyperlink ref="G129" r:id="rId130"/>
+    <hyperlink ref="L129" r:id="rId131"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -8481,7 +8483,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
@@ -12511,123 +12513,123 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="J3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="J4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="J5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="J6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="J7" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="J8" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="J9" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
-    <hyperlink ref="J10" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="J11" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
-    <hyperlink ref="J12" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
-    <hyperlink ref="J13" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
-    <hyperlink ref="J14" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
-    <hyperlink ref="J15" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
-    <hyperlink ref="J16" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
-    <hyperlink ref="J17" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
-    <hyperlink ref="J18" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
-    <hyperlink ref="J19" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
-    <hyperlink ref="J20" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
-    <hyperlink ref="J21" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
-    <hyperlink ref="J22" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
-    <hyperlink ref="J23" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
-    <hyperlink ref="J24" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
-    <hyperlink ref="J25" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
-    <hyperlink ref="J26" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
-    <hyperlink ref="J27" r:id="rId26" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
-    <hyperlink ref="J28" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
-    <hyperlink ref="J29" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
-    <hyperlink ref="J30" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
-    <hyperlink ref="J31" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
-    <hyperlink ref="J32" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
-    <hyperlink ref="J33" r:id="rId32" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
-    <hyperlink ref="J34" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
-    <hyperlink ref="J35" r:id="rId34" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
-    <hyperlink ref="J36" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
-    <hyperlink ref="J37" r:id="rId36" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
-    <hyperlink ref="J38" r:id="rId37" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
-    <hyperlink ref="J39" r:id="rId38" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
-    <hyperlink ref="J40" r:id="rId39" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
-    <hyperlink ref="J41" r:id="rId40" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
-    <hyperlink ref="J42" r:id="rId41" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
-    <hyperlink ref="J43" r:id="rId42" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
-    <hyperlink ref="J44" r:id="rId43" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
-    <hyperlink ref="J45" r:id="rId44" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
-    <hyperlink ref="J46" r:id="rId45" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
-    <hyperlink ref="J47" r:id="rId46" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
-    <hyperlink ref="J48" r:id="rId47" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
-    <hyperlink ref="J49" r:id="rId48" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
-    <hyperlink ref="J50" r:id="rId49" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
-    <hyperlink ref="J51" r:id="rId50" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
-    <hyperlink ref="J52" r:id="rId51" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
-    <hyperlink ref="J53" r:id="rId52" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
-    <hyperlink ref="J54" r:id="rId53" xr:uid="{00000000-0004-0000-0100-000034000000}"/>
-    <hyperlink ref="J55" r:id="rId54" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
-    <hyperlink ref="J56" r:id="rId55" xr:uid="{00000000-0004-0000-0100-000036000000}"/>
-    <hyperlink ref="J57" r:id="rId56" xr:uid="{00000000-0004-0000-0100-000037000000}"/>
-    <hyperlink ref="J58" r:id="rId57" xr:uid="{00000000-0004-0000-0100-000038000000}"/>
-    <hyperlink ref="J59" r:id="rId58" xr:uid="{00000000-0004-0000-0100-000039000000}"/>
-    <hyperlink ref="J60" r:id="rId59" xr:uid="{00000000-0004-0000-0100-00003A000000}"/>
-    <hyperlink ref="J61" r:id="rId60" xr:uid="{00000000-0004-0000-0100-00003B000000}"/>
-    <hyperlink ref="J62" r:id="rId61" xr:uid="{00000000-0004-0000-0100-00003C000000}"/>
-    <hyperlink ref="J63" r:id="rId62" xr:uid="{00000000-0004-0000-0100-00003D000000}"/>
-    <hyperlink ref="J64" r:id="rId63" xr:uid="{00000000-0004-0000-0100-00003E000000}"/>
-    <hyperlink ref="J65" r:id="rId64" xr:uid="{00000000-0004-0000-0100-00003F000000}"/>
-    <hyperlink ref="J66" r:id="rId65" xr:uid="{00000000-0004-0000-0100-000040000000}"/>
-    <hyperlink ref="J67" r:id="rId66" xr:uid="{00000000-0004-0000-0100-000041000000}"/>
-    <hyperlink ref="J68" r:id="rId67" xr:uid="{00000000-0004-0000-0100-000042000000}"/>
-    <hyperlink ref="J69" r:id="rId68" xr:uid="{00000000-0004-0000-0100-000043000000}"/>
-    <hyperlink ref="J70" r:id="rId69" xr:uid="{00000000-0004-0000-0100-000044000000}"/>
-    <hyperlink ref="J71" r:id="rId70" xr:uid="{00000000-0004-0000-0100-000045000000}"/>
-    <hyperlink ref="J72" r:id="rId71" xr:uid="{00000000-0004-0000-0100-000046000000}"/>
-    <hyperlink ref="J73" r:id="rId72" xr:uid="{00000000-0004-0000-0100-000047000000}"/>
-    <hyperlink ref="J74" r:id="rId73" xr:uid="{00000000-0004-0000-0100-000048000000}"/>
-    <hyperlink ref="J75" r:id="rId74" xr:uid="{00000000-0004-0000-0100-000049000000}"/>
-    <hyperlink ref="J76" r:id="rId75" xr:uid="{00000000-0004-0000-0100-00004A000000}"/>
-    <hyperlink ref="J77" r:id="rId76" xr:uid="{00000000-0004-0000-0100-00004B000000}"/>
-    <hyperlink ref="J78" r:id="rId77" xr:uid="{00000000-0004-0000-0100-00004C000000}"/>
-    <hyperlink ref="J79" r:id="rId78" xr:uid="{00000000-0004-0000-0100-00004D000000}"/>
-    <hyperlink ref="J80" r:id="rId79" xr:uid="{00000000-0004-0000-0100-00004E000000}"/>
-    <hyperlink ref="J81" r:id="rId80" xr:uid="{00000000-0004-0000-0100-00004F000000}"/>
-    <hyperlink ref="J82" r:id="rId81" xr:uid="{00000000-0004-0000-0100-000050000000}"/>
-    <hyperlink ref="J83" r:id="rId82" xr:uid="{00000000-0004-0000-0100-000051000000}"/>
-    <hyperlink ref="J84" r:id="rId83" xr:uid="{00000000-0004-0000-0100-000052000000}"/>
-    <hyperlink ref="J85" r:id="rId84" xr:uid="{00000000-0004-0000-0100-000053000000}"/>
-    <hyperlink ref="J86" r:id="rId85" xr:uid="{00000000-0004-0000-0100-000054000000}"/>
-    <hyperlink ref="J87" r:id="rId86" xr:uid="{00000000-0004-0000-0100-000055000000}"/>
-    <hyperlink ref="J88" r:id="rId87" xr:uid="{00000000-0004-0000-0100-000056000000}"/>
-    <hyperlink ref="J89" r:id="rId88" xr:uid="{00000000-0004-0000-0100-000057000000}"/>
-    <hyperlink ref="J90" r:id="rId89" xr:uid="{00000000-0004-0000-0100-000058000000}"/>
-    <hyperlink ref="J91" r:id="rId90" xr:uid="{00000000-0004-0000-0100-000059000000}"/>
-    <hyperlink ref="J92" r:id="rId91" xr:uid="{00000000-0004-0000-0100-00005A000000}"/>
-    <hyperlink ref="J93" r:id="rId92" xr:uid="{00000000-0004-0000-0100-00005B000000}"/>
-    <hyperlink ref="J94" r:id="rId93" xr:uid="{00000000-0004-0000-0100-00005C000000}"/>
-    <hyperlink ref="J95" r:id="rId94" xr:uid="{00000000-0004-0000-0100-00005D000000}"/>
-    <hyperlink ref="J96" r:id="rId95" xr:uid="{00000000-0004-0000-0100-00005E000000}"/>
-    <hyperlink ref="J97" r:id="rId96" xr:uid="{00000000-0004-0000-0100-00005F000000}"/>
-    <hyperlink ref="J98" r:id="rId97" xr:uid="{00000000-0004-0000-0100-000060000000}"/>
-    <hyperlink ref="J99" r:id="rId98" xr:uid="{00000000-0004-0000-0100-000061000000}"/>
-    <hyperlink ref="J100" r:id="rId99" xr:uid="{00000000-0004-0000-0100-000062000000}"/>
-    <hyperlink ref="J101" r:id="rId100" xr:uid="{00000000-0004-0000-0100-000063000000}"/>
-    <hyperlink ref="J102" r:id="rId101" xr:uid="{00000000-0004-0000-0100-000064000000}"/>
-    <hyperlink ref="J103" r:id="rId102" xr:uid="{00000000-0004-0000-0100-000065000000}"/>
-    <hyperlink ref="J104" r:id="rId103" xr:uid="{00000000-0004-0000-0100-000066000000}"/>
-    <hyperlink ref="J105" r:id="rId104" xr:uid="{00000000-0004-0000-0100-000067000000}"/>
-    <hyperlink ref="J106" r:id="rId105" xr:uid="{00000000-0004-0000-0100-000068000000}"/>
-    <hyperlink ref="J107" r:id="rId106" xr:uid="{00000000-0004-0000-0100-000069000000}"/>
-    <hyperlink ref="J108" r:id="rId107" xr:uid="{00000000-0004-0000-0100-00006A000000}"/>
-    <hyperlink ref="J109" r:id="rId108" xr:uid="{00000000-0004-0000-0100-00006B000000}"/>
-    <hyperlink ref="J110" r:id="rId109" xr:uid="{00000000-0004-0000-0100-00006C000000}"/>
-    <hyperlink ref="J111" r:id="rId110" xr:uid="{00000000-0004-0000-0100-00006D000000}"/>
-    <hyperlink ref="J112" r:id="rId111" xr:uid="{00000000-0004-0000-0100-00006E000000}"/>
-    <hyperlink ref="J113" r:id="rId112" xr:uid="{00000000-0004-0000-0100-00006F000000}"/>
-    <hyperlink ref="J114" r:id="rId113" xr:uid="{00000000-0004-0000-0100-000070000000}"/>
-    <hyperlink ref="G115" r:id="rId114" xr:uid="{986B288E-2B44-4904-A56E-6E855440D20F}"/>
-    <hyperlink ref="J115" r:id="rId115" xr:uid="{21408C62-1D1A-4F59-BB22-BF7FBDB0BD3F}"/>
-    <hyperlink ref="G116" r:id="rId116" xr:uid="{79B37CD3-81D4-49D3-8ADB-A2F742CC9547}"/>
-    <hyperlink ref="J116" r:id="rId117" xr:uid="{E8BFC75E-3B3F-463E-B6C0-FFA1470E441B}"/>
+    <hyperlink ref="J2" r:id="rId1"/>
+    <hyperlink ref="J3" r:id="rId2"/>
+    <hyperlink ref="J4" r:id="rId3"/>
+    <hyperlink ref="J5" r:id="rId4"/>
+    <hyperlink ref="J6" r:id="rId5"/>
+    <hyperlink ref="J7" r:id="rId6"/>
+    <hyperlink ref="J8" r:id="rId7"/>
+    <hyperlink ref="J9" r:id="rId8"/>
+    <hyperlink ref="J10" r:id="rId9"/>
+    <hyperlink ref="J11" r:id="rId10"/>
+    <hyperlink ref="J12" r:id="rId11"/>
+    <hyperlink ref="J13" r:id="rId12"/>
+    <hyperlink ref="J14" r:id="rId13"/>
+    <hyperlink ref="J15" r:id="rId14"/>
+    <hyperlink ref="J16" r:id="rId15"/>
+    <hyperlink ref="J17" r:id="rId16"/>
+    <hyperlink ref="J18" r:id="rId17"/>
+    <hyperlink ref="J19" r:id="rId18"/>
+    <hyperlink ref="J20" r:id="rId19"/>
+    <hyperlink ref="J21" r:id="rId20"/>
+    <hyperlink ref="J22" r:id="rId21"/>
+    <hyperlink ref="J23" r:id="rId22"/>
+    <hyperlink ref="J24" r:id="rId23"/>
+    <hyperlink ref="J25" r:id="rId24"/>
+    <hyperlink ref="J26" r:id="rId25"/>
+    <hyperlink ref="J27" r:id="rId26"/>
+    <hyperlink ref="J28" r:id="rId27"/>
+    <hyperlink ref="J29" r:id="rId28"/>
+    <hyperlink ref="J30" r:id="rId29"/>
+    <hyperlink ref="J31" r:id="rId30"/>
+    <hyperlink ref="J32" r:id="rId31"/>
+    <hyperlink ref="J33" r:id="rId32"/>
+    <hyperlink ref="J34" r:id="rId33"/>
+    <hyperlink ref="J35" r:id="rId34"/>
+    <hyperlink ref="J36" r:id="rId35"/>
+    <hyperlink ref="J37" r:id="rId36"/>
+    <hyperlink ref="J38" r:id="rId37"/>
+    <hyperlink ref="J39" r:id="rId38"/>
+    <hyperlink ref="J40" r:id="rId39"/>
+    <hyperlink ref="J41" r:id="rId40"/>
+    <hyperlink ref="J42" r:id="rId41"/>
+    <hyperlink ref="J43" r:id="rId42"/>
+    <hyperlink ref="J44" r:id="rId43"/>
+    <hyperlink ref="J45" r:id="rId44"/>
+    <hyperlink ref="J46" r:id="rId45"/>
+    <hyperlink ref="J47" r:id="rId46"/>
+    <hyperlink ref="J48" r:id="rId47"/>
+    <hyperlink ref="J49" r:id="rId48"/>
+    <hyperlink ref="J50" r:id="rId49"/>
+    <hyperlink ref="J51" r:id="rId50"/>
+    <hyperlink ref="J52" r:id="rId51"/>
+    <hyperlink ref="J53" r:id="rId52"/>
+    <hyperlink ref="J54" r:id="rId53"/>
+    <hyperlink ref="J55" r:id="rId54"/>
+    <hyperlink ref="J56" r:id="rId55"/>
+    <hyperlink ref="J57" r:id="rId56"/>
+    <hyperlink ref="J58" r:id="rId57"/>
+    <hyperlink ref="J59" r:id="rId58"/>
+    <hyperlink ref="J60" r:id="rId59"/>
+    <hyperlink ref="J61" r:id="rId60"/>
+    <hyperlink ref="J62" r:id="rId61"/>
+    <hyperlink ref="J63" r:id="rId62"/>
+    <hyperlink ref="J64" r:id="rId63"/>
+    <hyperlink ref="J65" r:id="rId64"/>
+    <hyperlink ref="J66" r:id="rId65"/>
+    <hyperlink ref="J67" r:id="rId66"/>
+    <hyperlink ref="J68" r:id="rId67"/>
+    <hyperlink ref="J69" r:id="rId68"/>
+    <hyperlink ref="J70" r:id="rId69"/>
+    <hyperlink ref="J71" r:id="rId70"/>
+    <hyperlink ref="J72" r:id="rId71"/>
+    <hyperlink ref="J73" r:id="rId72"/>
+    <hyperlink ref="J74" r:id="rId73"/>
+    <hyperlink ref="J75" r:id="rId74"/>
+    <hyperlink ref="J76" r:id="rId75"/>
+    <hyperlink ref="J77" r:id="rId76"/>
+    <hyperlink ref="J78" r:id="rId77"/>
+    <hyperlink ref="J79" r:id="rId78"/>
+    <hyperlink ref="J80" r:id="rId79"/>
+    <hyperlink ref="J81" r:id="rId80"/>
+    <hyperlink ref="J82" r:id="rId81"/>
+    <hyperlink ref="J83" r:id="rId82"/>
+    <hyperlink ref="J84" r:id="rId83"/>
+    <hyperlink ref="J85" r:id="rId84"/>
+    <hyperlink ref="J86" r:id="rId85"/>
+    <hyperlink ref="J87" r:id="rId86"/>
+    <hyperlink ref="J88" r:id="rId87"/>
+    <hyperlink ref="J89" r:id="rId88"/>
+    <hyperlink ref="J90" r:id="rId89"/>
+    <hyperlink ref="J91" r:id="rId90"/>
+    <hyperlink ref="J92" r:id="rId91"/>
+    <hyperlink ref="J93" r:id="rId92"/>
+    <hyperlink ref="J94" r:id="rId93"/>
+    <hyperlink ref="J95" r:id="rId94"/>
+    <hyperlink ref="J96" r:id="rId95"/>
+    <hyperlink ref="J97" r:id="rId96"/>
+    <hyperlink ref="J98" r:id="rId97"/>
+    <hyperlink ref="J99" r:id="rId98"/>
+    <hyperlink ref="J100" r:id="rId99"/>
+    <hyperlink ref="J101" r:id="rId100"/>
+    <hyperlink ref="J102" r:id="rId101"/>
+    <hyperlink ref="J103" r:id="rId102"/>
+    <hyperlink ref="J104" r:id="rId103"/>
+    <hyperlink ref="J105" r:id="rId104"/>
+    <hyperlink ref="J106" r:id="rId105"/>
+    <hyperlink ref="J107" r:id="rId106"/>
+    <hyperlink ref="J108" r:id="rId107"/>
+    <hyperlink ref="J109" r:id="rId108"/>
+    <hyperlink ref="J110" r:id="rId109"/>
+    <hyperlink ref="J111" r:id="rId110"/>
+    <hyperlink ref="J112" r:id="rId111"/>
+    <hyperlink ref="J113" r:id="rId112"/>
+    <hyperlink ref="J114" r:id="rId113"/>
+    <hyperlink ref="G115" r:id="rId114"/>
+    <hyperlink ref="J115" r:id="rId115"/>
+    <hyperlink ref="G116" r:id="rId116"/>
+    <hyperlink ref="J116" r:id="rId117"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -12641,7 +12643,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
@@ -12649,8 +12651,8 @@
   <dimension ref="A1:P198"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -14762,7 +14764,7 @@
         <v>551</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>252</v>
+        <v>890</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>552</v>
@@ -16455,116 +16457,116 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="J3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="J4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="J5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="J6" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
-    <hyperlink ref="J7" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
-    <hyperlink ref="J8" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
-    <hyperlink ref="J9" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
-    <hyperlink ref="J10" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
-    <hyperlink ref="J11" r:id="rId10" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
-    <hyperlink ref="J12" r:id="rId11" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
-    <hyperlink ref="J13" r:id="rId12" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
-    <hyperlink ref="J14" r:id="rId13" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
-    <hyperlink ref="J15" r:id="rId14" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
-    <hyperlink ref="J16" r:id="rId15" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
-    <hyperlink ref="J17" r:id="rId16" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
-    <hyperlink ref="J18" r:id="rId17" xr:uid="{00000000-0004-0000-0200-000010000000}"/>
-    <hyperlink ref="J19" r:id="rId18" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
-    <hyperlink ref="J20" r:id="rId19" xr:uid="{00000000-0004-0000-0200-000012000000}"/>
-    <hyperlink ref="J21" r:id="rId20" xr:uid="{00000000-0004-0000-0200-000013000000}"/>
-    <hyperlink ref="J22" r:id="rId21" xr:uid="{00000000-0004-0000-0200-000014000000}"/>
-    <hyperlink ref="J23" r:id="rId22" xr:uid="{00000000-0004-0000-0200-000015000000}"/>
-    <hyperlink ref="J24" r:id="rId23" xr:uid="{00000000-0004-0000-0200-000016000000}"/>
-    <hyperlink ref="J25" r:id="rId24" xr:uid="{00000000-0004-0000-0200-000017000000}"/>
-    <hyperlink ref="J26" r:id="rId25" xr:uid="{00000000-0004-0000-0200-000018000000}"/>
-    <hyperlink ref="J27" r:id="rId26" xr:uid="{00000000-0004-0000-0200-000019000000}"/>
-    <hyperlink ref="J28" r:id="rId27" xr:uid="{00000000-0004-0000-0200-00001A000000}"/>
-    <hyperlink ref="J29" r:id="rId28" xr:uid="{00000000-0004-0000-0200-00001B000000}"/>
-    <hyperlink ref="J30" r:id="rId29" xr:uid="{00000000-0004-0000-0200-00001C000000}"/>
-    <hyperlink ref="J31" r:id="rId30" xr:uid="{00000000-0004-0000-0200-00001D000000}"/>
-    <hyperlink ref="J32" r:id="rId31" xr:uid="{00000000-0004-0000-0200-00001E000000}"/>
-    <hyperlink ref="J33" r:id="rId32" xr:uid="{00000000-0004-0000-0200-00001F000000}"/>
-    <hyperlink ref="J34" r:id="rId33" xr:uid="{00000000-0004-0000-0200-000020000000}"/>
-    <hyperlink ref="J35" r:id="rId34" xr:uid="{00000000-0004-0000-0200-000021000000}"/>
-    <hyperlink ref="J36" r:id="rId35" xr:uid="{00000000-0004-0000-0200-000022000000}"/>
-    <hyperlink ref="J37" r:id="rId36" xr:uid="{00000000-0004-0000-0200-000023000000}"/>
-    <hyperlink ref="J38" r:id="rId37" xr:uid="{00000000-0004-0000-0200-000024000000}"/>
-    <hyperlink ref="J39" r:id="rId38" xr:uid="{00000000-0004-0000-0200-000025000000}"/>
-    <hyperlink ref="J40" r:id="rId39" xr:uid="{00000000-0004-0000-0200-000026000000}"/>
-    <hyperlink ref="J41" r:id="rId40" xr:uid="{00000000-0004-0000-0200-000027000000}"/>
-    <hyperlink ref="J42" r:id="rId41" xr:uid="{00000000-0004-0000-0200-000028000000}"/>
-    <hyperlink ref="J43" r:id="rId42" xr:uid="{00000000-0004-0000-0200-000029000000}"/>
-    <hyperlink ref="J44" r:id="rId43" xr:uid="{00000000-0004-0000-0200-00002A000000}"/>
-    <hyperlink ref="J45" r:id="rId44" xr:uid="{00000000-0004-0000-0200-00002B000000}"/>
-    <hyperlink ref="J46" r:id="rId45" xr:uid="{00000000-0004-0000-0200-00002C000000}"/>
-    <hyperlink ref="J47" r:id="rId46" xr:uid="{00000000-0004-0000-0200-00002D000000}"/>
-    <hyperlink ref="J48" r:id="rId47" xr:uid="{00000000-0004-0000-0200-00002E000000}"/>
-    <hyperlink ref="J49" r:id="rId48" xr:uid="{00000000-0004-0000-0200-00002F000000}"/>
-    <hyperlink ref="J50" r:id="rId49" xr:uid="{00000000-0004-0000-0200-000030000000}"/>
-    <hyperlink ref="J51" r:id="rId50" xr:uid="{00000000-0004-0000-0200-000031000000}"/>
-    <hyperlink ref="J52" r:id="rId51" xr:uid="{00000000-0004-0000-0200-000032000000}"/>
-    <hyperlink ref="J53" r:id="rId52" xr:uid="{00000000-0004-0000-0200-000033000000}"/>
-    <hyperlink ref="J54" r:id="rId53" xr:uid="{00000000-0004-0000-0200-000034000000}"/>
-    <hyperlink ref="J55" r:id="rId54" xr:uid="{00000000-0004-0000-0200-000035000000}"/>
-    <hyperlink ref="J56" r:id="rId55" xr:uid="{00000000-0004-0000-0200-000036000000}"/>
-    <hyperlink ref="J57" r:id="rId56" xr:uid="{00000000-0004-0000-0200-000037000000}"/>
-    <hyperlink ref="J58" r:id="rId57" xr:uid="{00000000-0004-0000-0200-000038000000}"/>
-    <hyperlink ref="J59" r:id="rId58" xr:uid="{00000000-0004-0000-0200-000039000000}"/>
-    <hyperlink ref="J60" r:id="rId59" xr:uid="{00000000-0004-0000-0200-00003A000000}"/>
-    <hyperlink ref="J61" r:id="rId60" xr:uid="{00000000-0004-0000-0200-00003B000000}"/>
-    <hyperlink ref="J62" r:id="rId61" xr:uid="{00000000-0004-0000-0200-00003C000000}"/>
-    <hyperlink ref="J63" r:id="rId62" xr:uid="{00000000-0004-0000-0200-00003D000000}"/>
-    <hyperlink ref="J64" r:id="rId63" xr:uid="{00000000-0004-0000-0200-00003E000000}"/>
-    <hyperlink ref="J65" r:id="rId64" xr:uid="{00000000-0004-0000-0200-00003F000000}"/>
-    <hyperlink ref="J66" r:id="rId65" xr:uid="{00000000-0004-0000-0200-000040000000}"/>
-    <hyperlink ref="J67" r:id="rId66" xr:uid="{00000000-0004-0000-0200-000041000000}"/>
-    <hyperlink ref="J68" r:id="rId67" xr:uid="{00000000-0004-0000-0200-000042000000}"/>
-    <hyperlink ref="J69" r:id="rId68" xr:uid="{00000000-0004-0000-0200-000043000000}"/>
-    <hyperlink ref="J70" r:id="rId69" xr:uid="{00000000-0004-0000-0200-000044000000}"/>
-    <hyperlink ref="J71" r:id="rId70" xr:uid="{00000000-0004-0000-0200-000045000000}"/>
-    <hyperlink ref="J72" r:id="rId71" xr:uid="{00000000-0004-0000-0200-000046000000}"/>
-    <hyperlink ref="J73" r:id="rId72" xr:uid="{00000000-0004-0000-0200-000047000000}"/>
-    <hyperlink ref="J74" r:id="rId73" xr:uid="{00000000-0004-0000-0200-000048000000}"/>
-    <hyperlink ref="J75" r:id="rId74" xr:uid="{00000000-0004-0000-0200-000049000000}"/>
-    <hyperlink ref="J76" r:id="rId75" xr:uid="{00000000-0004-0000-0200-00004A000000}"/>
-    <hyperlink ref="J77" r:id="rId76" xr:uid="{00000000-0004-0000-0200-00004B000000}"/>
-    <hyperlink ref="J78" r:id="rId77" xr:uid="{00000000-0004-0000-0200-00004C000000}"/>
-    <hyperlink ref="J79" r:id="rId78" xr:uid="{00000000-0004-0000-0200-00004D000000}"/>
-    <hyperlink ref="J80" r:id="rId79" xr:uid="{00000000-0004-0000-0200-00004E000000}"/>
-    <hyperlink ref="J81" r:id="rId80" xr:uid="{00000000-0004-0000-0200-00004F000000}"/>
-    <hyperlink ref="J82" r:id="rId81" xr:uid="{00000000-0004-0000-0200-000050000000}"/>
-    <hyperlink ref="J83" r:id="rId82" xr:uid="{00000000-0004-0000-0200-000051000000}"/>
-    <hyperlink ref="J84" r:id="rId83" xr:uid="{00000000-0004-0000-0200-000052000000}"/>
-    <hyperlink ref="J85" r:id="rId84" xr:uid="{00000000-0004-0000-0200-000053000000}"/>
-    <hyperlink ref="J86" r:id="rId85" xr:uid="{00000000-0004-0000-0200-000054000000}"/>
-    <hyperlink ref="J87" r:id="rId86" xr:uid="{00000000-0004-0000-0200-000055000000}"/>
-    <hyperlink ref="J88" r:id="rId87" xr:uid="{00000000-0004-0000-0200-000056000000}"/>
-    <hyperlink ref="J89" r:id="rId88" xr:uid="{00000000-0004-0000-0200-000057000000}"/>
-    <hyperlink ref="J90" r:id="rId89" xr:uid="{00000000-0004-0000-0200-000058000000}"/>
-    <hyperlink ref="J91" r:id="rId90" xr:uid="{00000000-0004-0000-0200-000059000000}"/>
-    <hyperlink ref="J92" r:id="rId91" xr:uid="{00000000-0004-0000-0200-00005A000000}"/>
-    <hyperlink ref="J93" r:id="rId92" xr:uid="{00000000-0004-0000-0200-00005B000000}"/>
-    <hyperlink ref="J94" r:id="rId93" xr:uid="{00000000-0004-0000-0200-00005C000000}"/>
-    <hyperlink ref="J95" r:id="rId94" xr:uid="{00000000-0004-0000-0200-00005D000000}"/>
-    <hyperlink ref="J96" r:id="rId95" xr:uid="{00000000-0004-0000-0200-00005E000000}"/>
-    <hyperlink ref="J97" r:id="rId96" xr:uid="{00000000-0004-0000-0200-00005F000000}"/>
-    <hyperlink ref="J98" r:id="rId97" xr:uid="{00000000-0004-0000-0200-000060000000}"/>
-    <hyperlink ref="J99" r:id="rId98" xr:uid="{00000000-0004-0000-0200-000061000000}"/>
-    <hyperlink ref="J100" r:id="rId99" xr:uid="{00000000-0004-0000-0200-000062000000}"/>
-    <hyperlink ref="J101" r:id="rId100" xr:uid="{00000000-0004-0000-0200-000063000000}"/>
-    <hyperlink ref="J102" r:id="rId101" xr:uid="{00000000-0004-0000-0200-000064000000}"/>
-    <hyperlink ref="J103" r:id="rId102" xr:uid="{00000000-0004-0000-0200-000065000000}"/>
-    <hyperlink ref="J104" r:id="rId103" xr:uid="{00000000-0004-0000-0200-000066000000}"/>
-    <hyperlink ref="J105" r:id="rId104" xr:uid="{00000000-0004-0000-0200-000067000000}"/>
-    <hyperlink ref="J106" r:id="rId105" xr:uid="{00000000-0004-0000-0200-000068000000}"/>
-    <hyperlink ref="J107" r:id="rId106" xr:uid="{00000000-0004-0000-0200-000069000000}"/>
-    <hyperlink ref="J108" r:id="rId107" xr:uid="{00000000-0004-0000-0200-00006A000000}"/>
-    <hyperlink ref="J109" r:id="rId108" xr:uid="{00000000-0004-0000-0200-00006B000000}"/>
-    <hyperlink ref="G110" r:id="rId109" xr:uid="{D5A2BDD1-328C-47C9-888E-8877726A2C8F}"/>
-    <hyperlink ref="J110" r:id="rId110" xr:uid="{3A5F2A4E-7A05-46BC-8991-7A9D9E407428}"/>
+    <hyperlink ref="J2" r:id="rId1"/>
+    <hyperlink ref="J3" r:id="rId2"/>
+    <hyperlink ref="J4" r:id="rId3"/>
+    <hyperlink ref="J5" r:id="rId4"/>
+    <hyperlink ref="J6" r:id="rId5"/>
+    <hyperlink ref="J7" r:id="rId6"/>
+    <hyperlink ref="J8" r:id="rId7"/>
+    <hyperlink ref="J9" r:id="rId8"/>
+    <hyperlink ref="J10" r:id="rId9"/>
+    <hyperlink ref="J11" r:id="rId10"/>
+    <hyperlink ref="J12" r:id="rId11"/>
+    <hyperlink ref="J13" r:id="rId12"/>
+    <hyperlink ref="J14" r:id="rId13"/>
+    <hyperlink ref="J15" r:id="rId14"/>
+    <hyperlink ref="J16" r:id="rId15"/>
+    <hyperlink ref="J17" r:id="rId16"/>
+    <hyperlink ref="J18" r:id="rId17"/>
+    <hyperlink ref="J19" r:id="rId18"/>
+    <hyperlink ref="J20" r:id="rId19"/>
+    <hyperlink ref="J21" r:id="rId20"/>
+    <hyperlink ref="J22" r:id="rId21"/>
+    <hyperlink ref="J23" r:id="rId22"/>
+    <hyperlink ref="J24" r:id="rId23"/>
+    <hyperlink ref="J25" r:id="rId24"/>
+    <hyperlink ref="J26" r:id="rId25"/>
+    <hyperlink ref="J27" r:id="rId26"/>
+    <hyperlink ref="J28" r:id="rId27"/>
+    <hyperlink ref="J29" r:id="rId28"/>
+    <hyperlink ref="J30" r:id="rId29"/>
+    <hyperlink ref="J31" r:id="rId30"/>
+    <hyperlink ref="J32" r:id="rId31"/>
+    <hyperlink ref="J33" r:id="rId32"/>
+    <hyperlink ref="J34" r:id="rId33"/>
+    <hyperlink ref="J35" r:id="rId34"/>
+    <hyperlink ref="J36" r:id="rId35"/>
+    <hyperlink ref="J37" r:id="rId36"/>
+    <hyperlink ref="J38" r:id="rId37"/>
+    <hyperlink ref="J39" r:id="rId38"/>
+    <hyperlink ref="J40" r:id="rId39"/>
+    <hyperlink ref="J41" r:id="rId40"/>
+    <hyperlink ref="J42" r:id="rId41"/>
+    <hyperlink ref="J43" r:id="rId42"/>
+    <hyperlink ref="J44" r:id="rId43"/>
+    <hyperlink ref="J45" r:id="rId44"/>
+    <hyperlink ref="J46" r:id="rId45"/>
+    <hyperlink ref="J47" r:id="rId46"/>
+    <hyperlink ref="J48" r:id="rId47"/>
+    <hyperlink ref="J49" r:id="rId48"/>
+    <hyperlink ref="J50" r:id="rId49"/>
+    <hyperlink ref="J51" r:id="rId50"/>
+    <hyperlink ref="J52" r:id="rId51"/>
+    <hyperlink ref="J53" r:id="rId52"/>
+    <hyperlink ref="J54" r:id="rId53"/>
+    <hyperlink ref="J55" r:id="rId54"/>
+    <hyperlink ref="J56" r:id="rId55"/>
+    <hyperlink ref="J57" r:id="rId56"/>
+    <hyperlink ref="J58" r:id="rId57"/>
+    <hyperlink ref="J59" r:id="rId58"/>
+    <hyperlink ref="J60" r:id="rId59"/>
+    <hyperlink ref="J61" r:id="rId60"/>
+    <hyperlink ref="J62" r:id="rId61"/>
+    <hyperlink ref="J63" r:id="rId62"/>
+    <hyperlink ref="J64" r:id="rId63"/>
+    <hyperlink ref="J65" r:id="rId64"/>
+    <hyperlink ref="J66" r:id="rId65"/>
+    <hyperlink ref="J67" r:id="rId66"/>
+    <hyperlink ref="J68" r:id="rId67"/>
+    <hyperlink ref="J69" r:id="rId68"/>
+    <hyperlink ref="J70" r:id="rId69"/>
+    <hyperlink ref="J71" r:id="rId70"/>
+    <hyperlink ref="J72" r:id="rId71"/>
+    <hyperlink ref="J73" r:id="rId72"/>
+    <hyperlink ref="J74" r:id="rId73"/>
+    <hyperlink ref="J75" r:id="rId74"/>
+    <hyperlink ref="J76" r:id="rId75"/>
+    <hyperlink ref="J77" r:id="rId76"/>
+    <hyperlink ref="J78" r:id="rId77"/>
+    <hyperlink ref="J79" r:id="rId78"/>
+    <hyperlink ref="J80" r:id="rId79"/>
+    <hyperlink ref="J81" r:id="rId80"/>
+    <hyperlink ref="J82" r:id="rId81"/>
+    <hyperlink ref="J83" r:id="rId82"/>
+    <hyperlink ref="J84" r:id="rId83"/>
+    <hyperlink ref="J85" r:id="rId84"/>
+    <hyperlink ref="J86" r:id="rId85"/>
+    <hyperlink ref="J87" r:id="rId86"/>
+    <hyperlink ref="J88" r:id="rId87"/>
+    <hyperlink ref="J89" r:id="rId88"/>
+    <hyperlink ref="J90" r:id="rId89"/>
+    <hyperlink ref="J91" r:id="rId90"/>
+    <hyperlink ref="J92" r:id="rId91"/>
+    <hyperlink ref="J93" r:id="rId92"/>
+    <hyperlink ref="J94" r:id="rId93"/>
+    <hyperlink ref="J95" r:id="rId94"/>
+    <hyperlink ref="J96" r:id="rId95"/>
+    <hyperlink ref="J97" r:id="rId96"/>
+    <hyperlink ref="J98" r:id="rId97"/>
+    <hyperlink ref="J99" r:id="rId98"/>
+    <hyperlink ref="J100" r:id="rId99"/>
+    <hyperlink ref="J101" r:id="rId100"/>
+    <hyperlink ref="J102" r:id="rId101"/>
+    <hyperlink ref="J103" r:id="rId102"/>
+    <hyperlink ref="J104" r:id="rId103"/>
+    <hyperlink ref="J105" r:id="rId104"/>
+    <hyperlink ref="J106" r:id="rId105"/>
+    <hyperlink ref="J107" r:id="rId106"/>
+    <hyperlink ref="J108" r:id="rId107"/>
+    <hyperlink ref="J109" r:id="rId108"/>
+    <hyperlink ref="G110" r:id="rId109"/>
+    <hyperlink ref="J110" r:id="rId110"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
added the removed letter
</commit_message>
<xml_diff>
--- a/CS335/GitHub Info sans duplicates.xlsx
+++ b/CS335/GitHub Info sans duplicates.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3297" uniqueCount="891">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3297" uniqueCount="890">
   <si>
     <t>Timestamp</t>
   </si>
@@ -2696,9 +2696,6 @@
   </si>
   <si>
     <t>DANIEL SOLOMON</t>
-  </si>
-  <si>
-    <t>JAME</t>
   </si>
 </sst>
 </file>
@@ -14764,7 +14761,7 @@
         <v>551</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>890</v>
+        <v>252</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>552</v>

</xml_diff>

<commit_message>
Update GitHub Info sans duplicates.xlsx
edited my name
</commit_message>
<xml_diff>
--- a/CS335/GitHub Info sans duplicates.xlsx
+++ b/CS335/GitHub Info sans duplicates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\staffcard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neemafaraja\Documents\GitHub\staffcard\CS335\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9795CA07-9D82-4C0D-89FD-F4DDFBC785C5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20779C37-C152-49FE-B504-F6E1A4A85983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -12304,8 +12304,8 @@
   <dimension ref="A1:P198"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
+      <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D107" sqref="D107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15720,10 +15720,10 @@
         <v>158</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>830</v>
+        <v>159</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>831</v>
+        <v>160</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>832</v>

</xml_diff>

<commit_message>
Added some changes to my phone numbers
</commit_message>
<xml_diff>
--- a/CS335/GitHub Info sans duplicates.xlsx
+++ b/CS335/GitHub Info sans duplicates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\staffcard\CS335\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter Kaisi\Desktop\git\staffcard\CS335\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A5A75C-3FEF-40E2-A64B-315A35DE1B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{589BC2C6-7FDC-4B85-A03B-1F1540831BA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3294" uniqueCount="908">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3293" uniqueCount="908">
   <si>
     <t>Timestamp</t>
   </si>
@@ -3242,14 +3242,14 @@
       <selection pane="bottomLeft" activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="26.28515625" customWidth="1"/>
-    <col min="6" max="18" width="21.42578125" customWidth="1"/>
+    <col min="1" max="4" width="21.453125" customWidth="1"/>
+    <col min="5" max="5" width="26.26953125" customWidth="1"/>
+    <col min="6" max="18" width="21.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3287,7 +3287,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44517.7927395718</v>
       </c>
@@ -3325,7 +3325,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>44517.829278495403</v>
       </c>
@@ -3363,7 +3363,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>44517.829803020803</v>
       </c>
@@ -3401,7 +3401,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>44517.832974606499</v>
       </c>
@@ -3439,7 +3439,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>44517.833342615697</v>
       </c>
@@ -3477,7 +3477,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>44517.834096585699</v>
       </c>
@@ -3515,7 +3515,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>44517.834304884302</v>
       </c>
@@ -3553,7 +3553,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>44517.834315161999</v>
       </c>
@@ -3591,7 +3591,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>44517.834467222201</v>
       </c>
@@ -3629,7 +3629,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>44517.836256620401</v>
       </c>
@@ -3667,7 +3667,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>44517.840131203702</v>
       </c>
@@ -3705,7 +3705,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>44517.840687338001</v>
       </c>
@@ -3743,7 +3743,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>44517.840723900503</v>
       </c>
@@ -3781,7 +3781,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>44517.848194363403</v>
       </c>
@@ -3819,7 +3819,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>44517.849799363401</v>
       </c>
@@ -3857,7 +3857,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>44517.851121805601</v>
       </c>
@@ -3895,7 +3895,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>44517.853374618098</v>
       </c>
@@ -3933,7 +3933,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>44517.855156886602</v>
       </c>
@@ -3971,7 +3971,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>44517.8585572917</v>
       </c>
@@ -4009,7 +4009,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>44517.8591194213</v>
       </c>
@@ -4047,7 +4047,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>44517.860663136598</v>
       </c>
@@ -4085,7 +4085,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>44517.863773090299</v>
       </c>
@@ -4123,7 +4123,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>44517.867895196803</v>
       </c>
@@ -4161,7 +4161,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>44517.868303217598</v>
       </c>
@@ -4199,7 +4199,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>44517.8691914468</v>
       </c>
@@ -4237,7 +4237,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>44517.874595833302</v>
       </c>
@@ -4275,7 +4275,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>44517.877297905099</v>
       </c>
@@ -4313,7 +4313,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>44517.877863588001</v>
       </c>
@@ -4351,7 +4351,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>44517.886029872701</v>
       </c>
@@ -4389,7 +4389,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>44517.888174652799</v>
       </c>
@@ -4427,7 +4427,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>44517.890895740697</v>
       </c>
@@ -4465,7 +4465,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>44517.898055138903</v>
       </c>
@@ -4503,7 +4503,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>44517.9033859259</v>
       </c>
@@ -4541,7 +4541,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>44517.916796608799</v>
       </c>
@@ -4579,7 +4579,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>44517.919944965302</v>
       </c>
@@ -4617,7 +4617,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>44517.920174733801</v>
       </c>
@@ -4655,7 +4655,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>44517.920207002302</v>
       </c>
@@ -4693,7 +4693,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>44517.925676088002</v>
       </c>
@@ -4731,7 +4731,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>44517.942313136598</v>
       </c>
@@ -4769,7 +4769,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>44517.967181493099</v>
       </c>
@@ -4807,7 +4807,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>44517.9708563889</v>
       </c>
@@ -4845,7 +4845,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>44517.974103865701</v>
       </c>
@@ -4883,7 +4883,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>44517.995788911998</v>
       </c>
@@ -4921,7 +4921,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44518.053331921299</v>
       </c>
@@ -4959,7 +4959,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>44518.1416807407</v>
       </c>
@@ -4997,7 +4997,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>44518.338707534698</v>
       </c>
@@ -5035,7 +5035,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>44518.348475844898</v>
       </c>
@@ -5073,7 +5073,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>44518.368981018502</v>
       </c>
@@ -5111,7 +5111,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>44518.376564247701</v>
       </c>
@@ -5149,7 +5149,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>44518.395640312498</v>
       </c>
@@ -5187,7 +5187,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>44518.396610844902</v>
       </c>
@@ -5225,7 +5225,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>44518.416108634301</v>
       </c>
@@ -5263,7 +5263,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>44518.419745173604</v>
       </c>
@@ -5301,7 +5301,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>44518.433273449104</v>
       </c>
@@ -5339,7 +5339,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>44518.433606898201</v>
       </c>
@@ -5377,7 +5377,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>44518.462937638898</v>
       </c>
@@ -5415,7 +5415,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>44518.4791463773</v>
       </c>
@@ -5453,7 +5453,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>44518.500450555599</v>
       </c>
@@ -5491,7 +5491,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>44518.545351886598</v>
       </c>
@@ -5529,7 +5529,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>44518.5769178357</v>
       </c>
@@ -5567,7 +5567,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>44518.580951863398</v>
       </c>
@@ -5605,7 +5605,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>44518.584114340301</v>
       </c>
@@ -5643,7 +5643,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>44518.599512685199</v>
       </c>
@@ -5681,7 +5681,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>44518.6111335069</v>
       </c>
@@ -5719,7 +5719,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>44518.639018194401</v>
       </c>
@@ -5757,7 +5757,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>44518.656796018498</v>
       </c>
@@ -5795,7 +5795,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>44518.669622650501</v>
       </c>
@@ -5833,7 +5833,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>44518.675713946803</v>
       </c>
@@ -5871,7 +5871,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>44518.678410173598</v>
       </c>
@@ -5909,7 +5909,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>44518.679047175901</v>
       </c>
@@ -5947,7 +5947,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>44518.681073298598</v>
       </c>
@@ -5985,7 +5985,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>44518.681981574096</v>
       </c>
@@ -6023,7 +6023,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>44518.682995844902</v>
       </c>
@@ -6061,7 +6061,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>44518.684843472198</v>
       </c>
@@ -6099,7 +6099,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>44518.690567743099</v>
       </c>
@@ -6137,7 +6137,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>44518.704118368099</v>
       </c>
@@ -6175,7 +6175,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>44518.7172751736</v>
       </c>
@@ -6213,7 +6213,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>44518.718211203697</v>
       </c>
@@ -6251,7 +6251,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="80" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>44518.7218906829</v>
       </c>
@@ -6289,7 +6289,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="81" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>44518.845550972197</v>
       </c>
@@ -6327,7 +6327,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="82" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>44518.845807673599</v>
       </c>
@@ -6365,7 +6365,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="83" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>44518.847130671304</v>
       </c>
@@ -6403,7 +6403,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="84" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>44518.8480487384</v>
       </c>
@@ -6441,7 +6441,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="85" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>44518.848206620401</v>
       </c>
@@ -6479,7 +6479,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="86" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>44518.851609803198</v>
       </c>
@@ -6517,7 +6517,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="87" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>44518.853343229202</v>
       </c>
@@ -6555,7 +6555,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="88" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>44518.854456469897</v>
       </c>
@@ -6593,7 +6593,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="89" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>44518.857002847202</v>
       </c>
@@ -6631,7 +6631,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="90" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>44518.857458969898</v>
       </c>
@@ -6669,7 +6669,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="91" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>44518.864664201399</v>
       </c>
@@ -6707,7 +6707,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="92" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>44518.865544432898</v>
       </c>
@@ -6745,7 +6745,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="93" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>44518.8734887963</v>
       </c>
@@ -6783,7 +6783,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="94" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>44518.880978576402</v>
       </c>
@@ -6821,7 +6821,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="95" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>44518.890144791701</v>
       </c>
@@ -6859,7 +6859,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="96" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>44518.8926736227</v>
       </c>
@@ -6897,7 +6897,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="97" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>44518.893882627301</v>
       </c>
@@ -6935,7 +6935,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="98" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>44518.895629976803</v>
       </c>
@@ -6973,7 +6973,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="99" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>44518.8972680324</v>
       </c>
@@ -7011,7 +7011,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="100" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>44518.901678900504</v>
       </c>
@@ -7049,7 +7049,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="101" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>44518.905369791697</v>
       </c>
@@ -7087,7 +7087,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="102" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>44518.914951886603</v>
       </c>
@@ -7125,7 +7125,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="103" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>44518.926460324103</v>
       </c>
@@ -7160,7 +7160,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="104" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>44518.9439103357</v>
       </c>
@@ -7195,7 +7195,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="105" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>44518.949051713003</v>
       </c>
@@ -7233,7 +7233,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="106" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>44518.949835740699</v>
       </c>
@@ -7271,7 +7271,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="107" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>44518.954430393504</v>
       </c>
@@ -7309,7 +7309,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="108" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>44518.964523217597</v>
       </c>
@@ -7347,7 +7347,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="109" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>44518.971188981501</v>
       </c>
@@ -7385,7 +7385,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="110" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>44518.9722345833</v>
       </c>
@@ -7423,7 +7423,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="111" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>44518.972730138899</v>
       </c>
@@ -7461,7 +7461,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="112" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>44518.977785532399</v>
       </c>
@@ -7499,7 +7499,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="113" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="7">
         <v>44519.003693425897</v>
       </c>
@@ -7541,7 +7541,7 @@
       <c r="Q113" s="9"/>
       <c r="R113" s="9"/>
     </row>
-    <row r="114" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>44521.695289421303</v>
       </c>
@@ -7579,7 +7579,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="115" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>44521.703645162001</v>
       </c>
@@ -7617,7 +7617,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="116" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>44521.798439618098</v>
       </c>
@@ -7655,7 +7655,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="117" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>44521.806830486101</v>
       </c>
@@ -7693,7 +7693,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="118" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>44521.997838750001</v>
       </c>
@@ -7731,7 +7731,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="119" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>44522.038008958298</v>
       </c>
@@ -7769,7 +7769,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="120" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>44522.396687349501</v>
       </c>
@@ -7807,7 +7807,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="121" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <v>44522.424870671297</v>
       </c>
@@ -7845,7 +7845,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="122" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>44522.601772291702</v>
       </c>
@@ -7883,7 +7883,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="123" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="11">
         <v>44532</v>
       </c>
@@ -7918,7 +7918,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="124" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B124" s="3" t="s">
         <v>423</v>
       </c>
@@ -7953,7 +7953,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="125" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B125" s="3" t="s">
         <v>852</v>
       </c>
@@ -7979,7 +7979,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="126" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B126" s="3" t="s">
         <v>458</v>
       </c>
@@ -8002,7 +8002,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="127" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B127" s="3" t="s">
         <v>856</v>
       </c>
@@ -8182,27 +8182,27 @@
   <dimension ref="A1:P212"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="D104" sqref="D104"/>
+      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="33.140625" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" customWidth="1"/>
-    <col min="10" max="10" width="33.140625" customWidth="1"/>
-    <col min="11" max="16" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="4.26953125" customWidth="1"/>
+    <col min="2" max="2" width="16.81640625" customWidth="1"/>
+    <col min="3" max="3" width="15.7265625" customWidth="1"/>
+    <col min="4" max="4" width="25.453125" customWidth="1"/>
+    <col min="5" max="5" width="16.81640625" customWidth="1"/>
+    <col min="6" max="6" width="20.90625" customWidth="1"/>
+    <col min="7" max="7" width="33.1796875" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" customWidth="1"/>
+    <col min="9" max="9" width="17.453125" customWidth="1"/>
+    <col min="10" max="10" width="33.1796875" customWidth="1"/>
+    <col min="11" max="16" width="21.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>864</v>
       </c>
@@ -8240,7 +8240,7 @@
       <c r="O1" s="13"/>
       <c r="P1" s="13"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -8272,7 +8272,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -8304,7 +8304,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -8336,7 +8336,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -8368,7 +8368,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -8400,7 +8400,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -8432,7 +8432,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -8464,7 +8464,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -8496,7 +8496,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -8528,7 +8528,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -8560,7 +8560,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -8592,7 +8592,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -8624,7 +8624,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -8656,7 +8656,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -8688,7 +8688,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -8720,7 +8720,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -8752,7 +8752,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -8784,7 +8784,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -8816,7 +8816,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -8848,7 +8848,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -8880,7 +8880,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -8912,7 +8912,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -8944,7 +8944,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -8976,7 +8976,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -9008,7 +9008,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -9040,7 +9040,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -9072,7 +9072,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -9104,7 +9104,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -9136,7 +9136,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -9168,7 +9168,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -9200,7 +9200,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -9232,7 +9232,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -9264,7 +9264,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -9296,7 +9296,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -9312,8 +9312,8 @@
       <c r="E35" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="F35" s="3" t="s">
-        <v>871</v>
+      <c r="F35" s="3">
+        <v>255762434093</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>263</v>
@@ -9328,7 +9328,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -9360,7 +9360,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -9392,7 +9392,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -9424,7 +9424,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -9456,7 +9456,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -9488,7 +9488,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -9520,7 +9520,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -9552,7 +9552,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -9584,7 +9584,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -9616,7 +9616,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -9648,7 +9648,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -9680,7 +9680,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -9712,7 +9712,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -9744,7 +9744,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -9776,7 +9776,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -9808,7 +9808,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -9840,7 +9840,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -9872,7 +9872,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -9904,7 +9904,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -9936,7 +9936,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -9968,7 +9968,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -10000,7 +10000,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -10032,7 +10032,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -10064,7 +10064,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -10096,7 +10096,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -10128,7 +10128,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -10160,7 +10160,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -10192,7 +10192,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -10224,7 +10224,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -10256,7 +10256,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -10288,7 +10288,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -10320,7 +10320,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -10352,7 +10352,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -10384,7 +10384,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -10416,7 +10416,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -10448,7 +10448,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -10480,7 +10480,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -10512,7 +10512,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -10544,7 +10544,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10" ht="25" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -10576,7 +10576,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -10608,7 +10608,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -10640,7 +10640,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -10672,7 +10672,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -10704,7 +10704,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -10736,7 +10736,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10" ht="25" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -10768,7 +10768,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -10800,7 +10800,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -10832,7 +10832,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -10864,7 +10864,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>83</v>
       </c>
@@ -10896,7 +10896,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>84</v>
       </c>
@@ -10928,7 +10928,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>85</v>
       </c>
@@ -10960,7 +10960,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>86</v>
       </c>
@@ -10992,7 +10992,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>87</v>
       </c>
@@ -11024,7 +11024,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>88</v>
       </c>
@@ -11056,7 +11056,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>89</v>
       </c>
@@ -11088,7 +11088,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>90</v>
       </c>
@@ -11120,7 +11120,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>91</v>
       </c>
@@ -11152,7 +11152,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>92</v>
       </c>
@@ -11184,7 +11184,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>93</v>
       </c>
@@ -11216,7 +11216,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>94</v>
       </c>
@@ -11248,7 +11248,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>95</v>
       </c>
@@ -11280,7 +11280,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>96</v>
       </c>
@@ -11312,7 +11312,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>97</v>
       </c>
@@ -11344,7 +11344,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>98</v>
       </c>
@@ -11376,7 +11376,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>99</v>
       </c>
@@ -11408,7 +11408,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>100</v>
       </c>
@@ -11440,7 +11440,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>101</v>
       </c>
@@ -11469,7 +11469,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <v>102</v>
       </c>
@@ -11498,7 +11498,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <v>103</v>
       </c>
@@ -11530,7 +11530,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>104</v>
       </c>
@@ -11562,7 +11562,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
         <v>105</v>
       </c>
@@ -11594,7 +11594,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
         <v>106</v>
       </c>
@@ -11626,7 +11626,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
         <v>107</v>
       </c>
@@ -11658,7 +11658,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
         <v>108</v>
       </c>
@@ -11690,7 +11690,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
         <v>109</v>
       </c>
@@ -11722,7 +11722,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
         <v>110</v>
       </c>
@@ -11754,7 +11754,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
         <v>111</v>
       </c>
@@ -11783,7 +11783,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
         <v>112</v>
       </c>
@@ -11815,7 +11815,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
         <v>113</v>
       </c>
@@ -11847,7 +11847,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
         <v>114</v>
       </c>
@@ -11879,295 +11879,295 @@
         <v>863</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J116" s="17"/>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J117" s="17"/>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J118" s="17"/>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J119" s="17"/>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J120" s="17"/>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J121" s="17"/>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J122" s="17"/>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J123" s="17"/>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J124" s="17"/>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J125" s="17"/>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J126" s="17"/>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J127" s="17"/>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J128" s="17"/>
     </row>
-    <row r="129" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="129" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J129" s="17"/>
     </row>
-    <row r="130" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="130" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J130" s="17"/>
     </row>
-    <row r="131" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="131" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J131" s="17"/>
     </row>
-    <row r="132" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="132" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J132" s="17"/>
     </row>
-    <row r="133" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="133" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J133" s="17"/>
     </row>
-    <row r="134" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="134" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J134" s="17"/>
     </row>
-    <row r="135" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="135" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J135" s="17"/>
     </row>
-    <row r="136" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="136" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J136" s="17"/>
     </row>
-    <row r="137" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="137" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J137" s="17"/>
     </row>
-    <row r="138" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="138" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J138" s="17"/>
     </row>
-    <row r="139" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="139" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J139" s="17"/>
     </row>
-    <row r="140" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="140" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J140" s="17"/>
     </row>
-    <row r="141" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="141" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J141" s="17"/>
     </row>
-    <row r="142" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="142" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J142" s="17"/>
     </row>
-    <row r="143" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="143" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J143" s="17"/>
     </row>
-    <row r="144" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="144" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J144" s="17"/>
     </row>
-    <row r="145" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="145" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J145" s="17"/>
     </row>
-    <row r="146" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="146" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J146" s="17"/>
     </row>
-    <row r="147" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="147" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J147" s="17"/>
     </row>
-    <row r="148" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="148" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J148" s="17"/>
     </row>
-    <row r="149" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="149" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J149" s="17"/>
     </row>
-    <row r="150" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="150" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J150" s="17"/>
     </row>
-    <row r="151" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="151" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J151" s="17"/>
     </row>
-    <row r="152" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="152" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J152" s="17"/>
     </row>
-    <row r="153" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="153" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J153" s="17"/>
     </row>
-    <row r="154" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="154" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J154" s="17"/>
     </row>
-    <row r="155" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="155" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J155" s="17"/>
     </row>
-    <row r="156" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="156" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J156" s="17"/>
     </row>
-    <row r="157" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="157" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J157" s="17"/>
     </row>
-    <row r="158" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="158" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J158" s="17"/>
     </row>
-    <row r="159" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="159" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J159" s="17"/>
     </row>
-    <row r="160" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="160" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J160" s="17"/>
     </row>
-    <row r="161" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="161" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J161" s="17"/>
     </row>
-    <row r="162" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="162" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J162" s="17"/>
     </row>
-    <row r="163" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="163" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J163" s="17"/>
     </row>
-    <row r="164" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="164" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J164" s="17"/>
     </row>
-    <row r="165" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="165" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J165" s="17"/>
     </row>
-    <row r="166" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="166" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J166" s="17"/>
     </row>
-    <row r="167" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="167" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J167" s="17"/>
     </row>
-    <row r="168" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="168" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J168" s="17"/>
     </row>
-    <row r="169" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="169" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J169" s="17"/>
     </row>
-    <row r="170" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="170" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J170" s="17"/>
     </row>
-    <row r="171" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="171" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J171" s="17"/>
     </row>
-    <row r="172" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="172" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J172" s="17"/>
     </row>
-    <row r="173" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="173" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J173" s="17"/>
     </row>
-    <row r="174" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="174" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J174" s="17"/>
     </row>
-    <row r="175" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="175" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J175" s="17"/>
     </row>
-    <row r="176" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="176" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J176" s="17"/>
     </row>
-    <row r="177" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="177" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J177" s="17"/>
     </row>
-    <row r="178" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="178" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J178" s="17"/>
     </row>
-    <row r="179" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="179" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J179" s="17"/>
     </row>
-    <row r="180" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="180" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J180" s="17"/>
     </row>
-    <row r="181" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="181" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J181" s="17"/>
     </row>
-    <row r="182" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="182" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J182" s="17"/>
     </row>
-    <row r="183" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="183" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J183" s="17"/>
     </row>
-    <row r="184" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="184" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J184" s="17"/>
     </row>
-    <row r="185" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="185" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J185" s="17"/>
     </row>
-    <row r="186" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="186" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J186" s="17"/>
     </row>
-    <row r="187" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="187" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J187" s="17"/>
     </row>
-    <row r="188" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="188" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J188" s="17"/>
     </row>
-    <row r="189" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="189" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J189" s="17"/>
     </row>
-    <row r="190" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="190" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J190" s="17"/>
     </row>
-    <row r="191" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="191" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J191" s="17"/>
     </row>
-    <row r="192" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="192" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J192" s="17"/>
     </row>
-    <row r="193" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="193" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J193" s="17"/>
     </row>
-    <row r="194" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="194" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J194" s="17"/>
     </row>
-    <row r="195" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="195" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J195" s="17"/>
     </row>
-    <row r="196" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="196" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J196" s="17"/>
     </row>
-    <row r="197" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="197" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J197" s="17"/>
     </row>
-    <row r="198" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="198" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J198" s="17"/>
     </row>
-    <row r="199" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="199" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J199" s="17"/>
     </row>
-    <row r="200" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="200" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J200" s="17"/>
     </row>
-    <row r="201" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="201" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J201" s="17"/>
     </row>
-    <row r="202" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="202" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J202" s="17"/>
     </row>
-    <row r="203" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="203" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J203" s="17"/>
     </row>
-    <row r="204" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="204" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J204" s="17"/>
     </row>
-    <row r="205" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="205" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J205" s="17"/>
     </row>
-    <row r="206" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="206" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J206" s="17"/>
     </row>
-    <row r="207" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="207" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J207" s="17"/>
     </row>
-    <row r="208" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="208" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J208" s="17"/>
     </row>
-    <row r="209" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="209" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J209" s="17"/>
     </row>
-    <row r="210" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="210" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J210" s="17"/>
     </row>
-    <row r="211" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="211" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J211" s="17"/>
     </row>
-    <row r="212" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="212" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J212" s="17"/>
     </row>
   </sheetData>
@@ -12311,22 +12311,22 @@
       <selection pane="bottomLeft" activeCell="D107" sqref="D107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="4.26953125" customWidth="1"/>
+    <col min="2" max="2" width="16.81640625" customWidth="1"/>
+    <col min="3" max="3" width="15.7265625" customWidth="1"/>
+    <col min="4" max="4" width="25.453125" customWidth="1"/>
+    <col min="5" max="5" width="16.81640625" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="33.140625" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" customWidth="1"/>
-    <col min="10" max="10" width="33.140625" customWidth="1"/>
-    <col min="11" max="16" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="33.1796875" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" customWidth="1"/>
+    <col min="9" max="9" width="17.453125" customWidth="1"/>
+    <col min="10" max="10" width="33.1796875" customWidth="1"/>
+    <col min="11" max="16" width="21.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>864</v>
       </c>
@@ -12364,7 +12364,7 @@
       <c r="O1" s="13"/>
       <c r="P1" s="13"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -12396,7 +12396,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -12428,7 +12428,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -12460,7 +12460,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -12492,7 +12492,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -12524,7 +12524,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -12556,7 +12556,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -12588,7 +12588,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -12620,7 +12620,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -12652,7 +12652,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -12684,7 +12684,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -12716,7 +12716,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -12748,7 +12748,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -12780,7 +12780,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -12812,7 +12812,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -12844,7 +12844,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -12876,7 +12876,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -12908,7 +12908,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -12940,7 +12940,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -12972,7 +12972,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -13004,7 +13004,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -13036,7 +13036,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -13068,7 +13068,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -13100,7 +13100,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -13132,7 +13132,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -13164,7 +13164,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -13196,7 +13196,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -13228,7 +13228,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -13260,7 +13260,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -13292,7 +13292,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -13324,7 +13324,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -13356,7 +13356,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -13388,7 +13388,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -13420,7 +13420,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -13452,7 +13452,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -13484,7 +13484,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -13516,7 +13516,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -13548,7 +13548,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -13580,7 +13580,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -13612,7 +13612,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -13644,7 +13644,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -13676,7 +13676,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -13708,7 +13708,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -13740,7 +13740,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -13772,7 +13772,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -13804,7 +13804,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -13836,7 +13836,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -13868,7 +13868,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -13900,7 +13900,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -13932,7 +13932,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -13964,7 +13964,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -13996,7 +13996,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -14028,7 +14028,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -14060,7 +14060,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -14092,7 +14092,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -14124,7 +14124,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -14156,7 +14156,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -14188,7 +14188,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -14220,7 +14220,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -14252,7 +14252,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -14284,7 +14284,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -14316,7 +14316,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -14348,7 +14348,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" ht="25" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -14380,7 +14380,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -14412,7 +14412,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -14444,7 +14444,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -14476,7 +14476,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -14508,7 +14508,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -14540,7 +14540,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -14572,7 +14572,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -14604,7 +14604,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -14636,7 +14636,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -14668,7 +14668,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -14700,7 +14700,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -14732,7 +14732,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -14764,7 +14764,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -14796,7 +14796,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -14828,7 +14828,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -14860,7 +14860,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -14892,7 +14892,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -14924,7 +14924,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -14956,7 +14956,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -14988,7 +14988,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>83</v>
       </c>
@@ -15020,7 +15020,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>84</v>
       </c>
@@ -15052,7 +15052,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>85</v>
       </c>
@@ -15084,7 +15084,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>86</v>
       </c>
@@ -15116,7 +15116,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>87</v>
       </c>
@@ -15145,7 +15145,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>88</v>
       </c>
@@ -15174,7 +15174,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>89</v>
       </c>
@@ -15206,7 +15206,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>90</v>
       </c>
@@ -15238,7 +15238,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>91</v>
       </c>
@@ -15270,7 +15270,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>92</v>
       </c>
@@ -15302,7 +15302,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>93</v>
       </c>
@@ -15334,7 +15334,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>94</v>
       </c>
@@ -15366,7 +15366,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>95</v>
       </c>
@@ -15398,7 +15398,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>96</v>
       </c>
@@ -15430,7 +15430,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>97</v>
       </c>
@@ -15459,7 +15459,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>98</v>
       </c>
@@ -15491,7 +15491,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>99</v>
       </c>
@@ -15523,7 +15523,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>100</v>
       </c>
@@ -15555,7 +15555,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>101</v>
       </c>
@@ -15587,7 +15587,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <v>102</v>
       </c>
@@ -15619,7 +15619,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <v>103</v>
       </c>
@@ -15651,7 +15651,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>104</v>
       </c>
@@ -15683,7 +15683,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
         <v>105</v>
       </c>
@@ -15715,7 +15715,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
         <v>106</v>
       </c>
@@ -15747,7 +15747,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
         <v>107</v>
       </c>
@@ -15779,7 +15779,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
         <v>108</v>
       </c>
@@ -15811,7 +15811,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
         <v>109</v>
       </c>
@@ -15843,7 +15843,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
         <v>110</v>
       </c>
@@ -15875,7 +15875,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
@@ -15907,262 +15907,262 @@
         <v>904</v>
       </c>
     </row>
-    <row r="113" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="113" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J113" s="17"/>
     </row>
-    <row r="114" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="114" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J114" s="17"/>
     </row>
-    <row r="115" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="115" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J115" s="17"/>
     </row>
-    <row r="116" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="116" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J116" s="17"/>
     </row>
-    <row r="117" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="117" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J117" s="17"/>
     </row>
-    <row r="118" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="118" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J118" s="17"/>
     </row>
-    <row r="119" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="119" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J119" s="17"/>
     </row>
-    <row r="120" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="120" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J120" s="17"/>
     </row>
-    <row r="121" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="121" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J121" s="17"/>
     </row>
-    <row r="122" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="122" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J122" s="17"/>
     </row>
-    <row r="123" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="123" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J123" s="17"/>
     </row>
-    <row r="124" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="124" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J124" s="17"/>
     </row>
-    <row r="125" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="125" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J125" s="17"/>
     </row>
-    <row r="126" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="126" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J126" s="17"/>
     </row>
-    <row r="127" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="127" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J127" s="17"/>
     </row>
-    <row r="128" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="128" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J128" s="17"/>
     </row>
-    <row r="129" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="129" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J129" s="17"/>
     </row>
-    <row r="130" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="130" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J130" s="17"/>
     </row>
-    <row r="131" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="131" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J131" s="17"/>
     </row>
-    <row r="132" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="132" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J132" s="17"/>
     </row>
-    <row r="133" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="133" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J133" s="17"/>
     </row>
-    <row r="134" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="134" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J134" s="17"/>
     </row>
-    <row r="135" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="135" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J135" s="17"/>
     </row>
-    <row r="136" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="136" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J136" s="17"/>
     </row>
-    <row r="137" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="137" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J137" s="17"/>
     </row>
-    <row r="138" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="138" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J138" s="17"/>
     </row>
-    <row r="139" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="139" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J139" s="17"/>
     </row>
-    <row r="140" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="140" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J140" s="17"/>
     </row>
-    <row r="141" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="141" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J141" s="17"/>
     </row>
-    <row r="142" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="142" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J142" s="17"/>
     </row>
-    <row r="143" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="143" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J143" s="17"/>
     </row>
-    <row r="144" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="144" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J144" s="17"/>
     </row>
-    <row r="145" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="145" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J145" s="17"/>
     </row>
-    <row r="146" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="146" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J146" s="17"/>
     </row>
-    <row r="147" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="147" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J147" s="17"/>
     </row>
-    <row r="148" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="148" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J148" s="17"/>
     </row>
-    <row r="149" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="149" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J149" s="17"/>
     </row>
-    <row r="150" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="150" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J150" s="17"/>
     </row>
-    <row r="151" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="151" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J151" s="17"/>
     </row>
-    <row r="152" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="152" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J152" s="17"/>
     </row>
-    <row r="153" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="153" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J153" s="17"/>
     </row>
-    <row r="154" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="154" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J154" s="17"/>
     </row>
-    <row r="155" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="155" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J155" s="17"/>
     </row>
-    <row r="156" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="156" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J156" s="17"/>
     </row>
-    <row r="157" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="157" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J157" s="17"/>
     </row>
-    <row r="158" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="158" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J158" s="17"/>
     </row>
-    <row r="159" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="159" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J159" s="17"/>
     </row>
-    <row r="160" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="160" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J160" s="17"/>
     </row>
-    <row r="161" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="161" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J161" s="17"/>
     </row>
-    <row r="162" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="162" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J162" s="17"/>
     </row>
-    <row r="163" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="163" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J163" s="17"/>
     </row>
-    <row r="164" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="164" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J164" s="17"/>
     </row>
-    <row r="165" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="165" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J165" s="17"/>
     </row>
-    <row r="166" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="166" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J166" s="17"/>
     </row>
-    <row r="167" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="167" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J167" s="17"/>
     </row>
-    <row r="168" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="168" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J168" s="17"/>
     </row>
-    <row r="169" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="169" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J169" s="17"/>
     </row>
-    <row r="170" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="170" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J170" s="17"/>
     </row>
-    <row r="171" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="171" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J171" s="17"/>
     </row>
-    <row r="172" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="172" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J172" s="17"/>
     </row>
-    <row r="173" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="173" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J173" s="17"/>
     </row>
-    <row r="174" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="174" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J174" s="17"/>
     </row>
-    <row r="175" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="175" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J175" s="17"/>
     </row>
-    <row r="176" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="176" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J176" s="17"/>
     </row>
-    <row r="177" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="177" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J177" s="17"/>
     </row>
-    <row r="178" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="178" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J178" s="17"/>
     </row>
-    <row r="179" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="179" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J179" s="17"/>
     </row>
-    <row r="180" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="180" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J180" s="17"/>
     </row>
-    <row r="181" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="181" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J181" s="17"/>
     </row>
-    <row r="182" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="182" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J182" s="17"/>
     </row>
-    <row r="183" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="183" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J183" s="17"/>
     </row>
-    <row r="184" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="184" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J184" s="17"/>
     </row>
-    <row r="185" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="185" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J185" s="17"/>
     </row>
-    <row r="186" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="186" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J186" s="17"/>
     </row>
-    <row r="187" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="187" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J187" s="17"/>
     </row>
-    <row r="188" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="188" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J188" s="17"/>
     </row>
-    <row r="189" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="189" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J189" s="17"/>
     </row>
-    <row r="190" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="190" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J190" s="17"/>
     </row>
-    <row r="191" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="191" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J191" s="17"/>
     </row>
-    <row r="192" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="192" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J192" s="17"/>
     </row>
-    <row r="193" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="193" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J193" s="17"/>
     </row>
-    <row r="194" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="194" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J194" s="17"/>
     </row>
-    <row r="195" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="195" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J195" s="17"/>
     </row>
-    <row r="196" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="196" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J196" s="17"/>
     </row>
-    <row r="197" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="197" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J197" s="17"/>
     </row>
-    <row r="198" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="198" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J198" s="17"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the middle name
</commit_message>
<xml_diff>
--- a/CS335/GitHub Info sans duplicates.xlsx
+++ b/CS335/GitHub Info sans duplicates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter Kaisi\Desktop\git\staffcard\CS335\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\staffcard\CS335\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{589BC2C6-7FDC-4B85-A03B-1F1540831BA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB88B0F-E212-4740-9FB0-5088681374C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -2750,7 +2750,7 @@
     <t>DANIEL SOLOMON</t>
   </si>
   <si>
-    <t>PHILIP JOSEPH</t>
+    <t>PHILIP J</t>
   </si>
 </sst>
 </file>
@@ -3242,14 +3242,14 @@
       <selection pane="bottomLeft" activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="21.453125" customWidth="1"/>
-    <col min="5" max="5" width="26.26953125" customWidth="1"/>
-    <col min="6" max="18" width="21.453125" customWidth="1"/>
+    <col min="1" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" customWidth="1"/>
+    <col min="6" max="18" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3287,7 +3287,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>44517.7927395718</v>
       </c>
@@ -3325,7 +3325,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>44517.829278495403</v>
       </c>
@@ -3363,7 +3363,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>44517.829803020803</v>
       </c>
@@ -3401,7 +3401,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>44517.832974606499</v>
       </c>
@@ -3439,7 +3439,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>44517.833342615697</v>
       </c>
@@ -3477,7 +3477,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>44517.834096585699</v>
       </c>
@@ -3515,7 +3515,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>44517.834304884302</v>
       </c>
@@ -3553,7 +3553,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>44517.834315161999</v>
       </c>
@@ -3591,7 +3591,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>44517.834467222201</v>
       </c>
@@ -3629,7 +3629,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>44517.836256620401</v>
       </c>
@@ -3667,7 +3667,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>44517.840131203702</v>
       </c>
@@ -3705,7 +3705,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>44517.840687338001</v>
       </c>
@@ -3743,7 +3743,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>44517.840723900503</v>
       </c>
@@ -3781,7 +3781,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>44517.848194363403</v>
       </c>
@@ -3819,7 +3819,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>44517.849799363401</v>
       </c>
@@ -3857,7 +3857,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>44517.851121805601</v>
       </c>
@@ -3895,7 +3895,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>44517.853374618098</v>
       </c>
@@ -3933,7 +3933,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>44517.855156886602</v>
       </c>
@@ -3971,7 +3971,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>44517.8585572917</v>
       </c>
@@ -4009,7 +4009,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>44517.8591194213</v>
       </c>
@@ -4047,7 +4047,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>44517.860663136598</v>
       </c>
@@ -4085,7 +4085,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>44517.863773090299</v>
       </c>
@@ -4123,7 +4123,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>44517.867895196803</v>
       </c>
@@ -4161,7 +4161,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>44517.868303217598</v>
       </c>
@@ -4199,7 +4199,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>44517.8691914468</v>
       </c>
@@ -4237,7 +4237,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>44517.874595833302</v>
       </c>
@@ -4275,7 +4275,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>44517.877297905099</v>
       </c>
@@ -4313,7 +4313,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>44517.877863588001</v>
       </c>
@@ -4351,7 +4351,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>44517.886029872701</v>
       </c>
@@ -4389,7 +4389,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>44517.888174652799</v>
       </c>
@@ -4427,7 +4427,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>44517.890895740697</v>
       </c>
@@ -4465,7 +4465,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>44517.898055138903</v>
       </c>
@@ -4503,7 +4503,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>44517.9033859259</v>
       </c>
@@ -4541,7 +4541,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>44517.916796608799</v>
       </c>
@@ -4579,7 +4579,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>44517.919944965302</v>
       </c>
@@ -4617,7 +4617,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>44517.920174733801</v>
       </c>
@@ -4655,7 +4655,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>44517.920207002302</v>
       </c>
@@ -4693,7 +4693,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>44517.925676088002</v>
       </c>
@@ -4731,7 +4731,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>44517.942313136598</v>
       </c>
@@ -4769,7 +4769,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>44517.967181493099</v>
       </c>
@@ -4807,7 +4807,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>44517.9708563889</v>
       </c>
@@ -4845,7 +4845,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>44517.974103865701</v>
       </c>
@@ -4883,7 +4883,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>44517.995788911998</v>
       </c>
@@ -4921,7 +4921,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>44518.053331921299</v>
       </c>
@@ -4959,7 +4959,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>44518.1416807407</v>
       </c>
@@ -4997,7 +4997,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>44518.338707534698</v>
       </c>
@@ -5035,7 +5035,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>44518.348475844898</v>
       </c>
@@ -5073,7 +5073,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>44518.368981018502</v>
       </c>
@@ -5111,7 +5111,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>44518.376564247701</v>
       </c>
@@ -5149,7 +5149,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>44518.395640312498</v>
       </c>
@@ -5187,7 +5187,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>44518.396610844902</v>
       </c>
@@ -5225,7 +5225,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>44518.416108634301</v>
       </c>
@@ -5263,7 +5263,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>44518.419745173604</v>
       </c>
@@ -5301,7 +5301,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>44518.433273449104</v>
       </c>
@@ -5339,7 +5339,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>44518.433606898201</v>
       </c>
@@ -5377,7 +5377,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>44518.462937638898</v>
       </c>
@@ -5415,7 +5415,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>44518.4791463773</v>
       </c>
@@ -5453,7 +5453,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>44518.500450555599</v>
       </c>
@@ -5491,7 +5491,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>44518.545351886598</v>
       </c>
@@ -5529,7 +5529,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>44518.5769178357</v>
       </c>
@@ -5567,7 +5567,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>44518.580951863398</v>
       </c>
@@ -5605,7 +5605,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>44518.584114340301</v>
       </c>
@@ -5643,7 +5643,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>44518.599512685199</v>
       </c>
@@ -5681,7 +5681,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>44518.6111335069</v>
       </c>
@@ -5719,7 +5719,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>44518.639018194401</v>
       </c>
@@ -5757,7 +5757,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>44518.656796018498</v>
       </c>
@@ -5795,7 +5795,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>44518.669622650501</v>
       </c>
@@ -5833,7 +5833,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>44518.675713946803</v>
       </c>
@@ -5871,7 +5871,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>44518.678410173598</v>
       </c>
@@ -5909,7 +5909,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>44518.679047175901</v>
       </c>
@@ -5947,7 +5947,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>44518.681073298598</v>
       </c>
@@ -5985,7 +5985,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>44518.681981574096</v>
       </c>
@@ -6023,7 +6023,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>44518.682995844902</v>
       </c>
@@ -6061,7 +6061,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>44518.684843472198</v>
       </c>
@@ -6099,7 +6099,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>44518.690567743099</v>
       </c>
@@ -6137,7 +6137,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>44518.704118368099</v>
       </c>
@@ -6175,7 +6175,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>44518.7172751736</v>
       </c>
@@ -6213,7 +6213,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>44518.718211203697</v>
       </c>
@@ -6251,7 +6251,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="80" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>44518.7218906829</v>
       </c>
@@ -6289,7 +6289,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="81" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>44518.845550972197</v>
       </c>
@@ -6327,7 +6327,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="82" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>44518.845807673599</v>
       </c>
@@ -6365,7 +6365,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="83" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>44518.847130671304</v>
       </c>
@@ -6403,7 +6403,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="84" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>44518.8480487384</v>
       </c>
@@ -6441,7 +6441,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="85" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>44518.848206620401</v>
       </c>
@@ -6479,7 +6479,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="86" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>44518.851609803198</v>
       </c>
@@ -6517,7 +6517,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="87" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>44518.853343229202</v>
       </c>
@@ -6555,7 +6555,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="88" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>44518.854456469897</v>
       </c>
@@ -6593,7 +6593,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="89" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>44518.857002847202</v>
       </c>
@@ -6631,7 +6631,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="90" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>44518.857458969898</v>
       </c>
@@ -6669,7 +6669,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="91" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>44518.864664201399</v>
       </c>
@@ -6707,7 +6707,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="92" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>44518.865544432898</v>
       </c>
@@ -6745,7 +6745,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="93" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>44518.8734887963</v>
       </c>
@@ -6783,7 +6783,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="94" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>44518.880978576402</v>
       </c>
@@ -6821,7 +6821,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="95" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>44518.890144791701</v>
       </c>
@@ -6859,7 +6859,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="96" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>44518.8926736227</v>
       </c>
@@ -6897,7 +6897,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="97" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>44518.893882627301</v>
       </c>
@@ -6935,7 +6935,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="98" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>44518.895629976803</v>
       </c>
@@ -6973,7 +6973,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="99" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <v>44518.8972680324</v>
       </c>
@@ -7011,7 +7011,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="100" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>44518.901678900504</v>
       </c>
@@ -7049,7 +7049,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="101" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
         <v>44518.905369791697</v>
       </c>
@@ -7087,7 +7087,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="102" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>44518.914951886603</v>
       </c>
@@ -7125,7 +7125,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="103" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>44518.926460324103</v>
       </c>
@@ -7160,7 +7160,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="104" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>44518.9439103357</v>
       </c>
@@ -7195,7 +7195,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="105" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
         <v>44518.949051713003</v>
       </c>
@@ -7233,7 +7233,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="106" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
         <v>44518.949835740699</v>
       </c>
@@ -7271,7 +7271,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="107" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
         <v>44518.954430393504</v>
       </c>
@@ -7309,7 +7309,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="108" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <v>44518.964523217597</v>
       </c>
@@ -7347,7 +7347,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="109" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
         <v>44518.971188981501</v>
       </c>
@@ -7385,7 +7385,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="110" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
         <v>44518.9722345833</v>
       </c>
@@ -7423,7 +7423,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="111" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
         <v>44518.972730138899</v>
       </c>
@@ -7461,7 +7461,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="112" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
         <v>44518.977785532399</v>
       </c>
@@ -7499,7 +7499,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="113" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="7">
         <v>44519.003693425897</v>
       </c>
@@ -7541,7 +7541,7 @@
       <c r="Q113" s="9"/>
       <c r="R113" s="9"/>
     </row>
-    <row r="114" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
         <v>44521.695289421303</v>
       </c>
@@ -7579,7 +7579,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="115" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
         <v>44521.703645162001</v>
       </c>
@@ -7617,7 +7617,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="116" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
         <v>44521.798439618098</v>
       </c>
@@ -7655,7 +7655,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="117" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
         <v>44521.806830486101</v>
       </c>
@@ -7693,7 +7693,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="118" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
         <v>44521.997838750001</v>
       </c>
@@ -7731,7 +7731,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="119" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
         <v>44522.038008958298</v>
       </c>
@@ -7769,7 +7769,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="120" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
         <v>44522.396687349501</v>
       </c>
@@ -7807,7 +7807,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="121" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
         <v>44522.424870671297</v>
       </c>
@@ -7845,7 +7845,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="122" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
         <v>44522.601772291702</v>
       </c>
@@ -7883,7 +7883,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="123" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="11">
         <v>44532</v>
       </c>
@@ -7918,7 +7918,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="124" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B124" s="3" t="s">
         <v>423</v>
       </c>
@@ -7953,7 +7953,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="125" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B125" s="3" t="s">
         <v>852</v>
       </c>
@@ -7979,7 +7979,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="126" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B126" s="3" t="s">
         <v>458</v>
       </c>
@@ -8002,7 +8002,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="127" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B127" s="3" t="s">
         <v>856</v>
       </c>
@@ -8182,27 +8182,27 @@
   <dimension ref="A1:P212"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
+      <selection pane="bottomLeft" activeCell="D104" sqref="D104"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.26953125" customWidth="1"/>
-    <col min="2" max="2" width="16.81640625" customWidth="1"/>
-    <col min="3" max="3" width="15.7265625" customWidth="1"/>
-    <col min="4" max="4" width="25.453125" customWidth="1"/>
-    <col min="5" max="5" width="16.81640625" customWidth="1"/>
-    <col min="6" max="6" width="20.90625" customWidth="1"/>
-    <col min="7" max="7" width="33.1796875" customWidth="1"/>
-    <col min="8" max="8" width="9.453125" customWidth="1"/>
-    <col min="9" max="9" width="17.453125" customWidth="1"/>
-    <col min="10" max="10" width="33.1796875" customWidth="1"/>
-    <col min="11" max="16" width="21.453125" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" customWidth="1"/>
+    <col min="7" max="7" width="33.140625" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="10" max="10" width="33.140625" customWidth="1"/>
+    <col min="11" max="16" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>864</v>
       </c>
@@ -8240,7 +8240,7 @@
       <c r="O1" s="13"/>
       <c r="P1" s="13"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -8272,7 +8272,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -8304,7 +8304,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -8336,7 +8336,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -8368,7 +8368,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -8400,7 +8400,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -8432,7 +8432,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -8464,7 +8464,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -8496,7 +8496,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -8528,7 +8528,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -8560,7 +8560,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -8592,7 +8592,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -8624,7 +8624,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -8656,7 +8656,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -8688,7 +8688,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -8720,7 +8720,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -8752,7 +8752,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -8784,7 +8784,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -8816,7 +8816,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -8848,7 +8848,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -8880,7 +8880,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -8912,7 +8912,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -8944,7 +8944,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -8976,7 +8976,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -9008,7 +9008,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -9040,7 +9040,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -9072,7 +9072,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -9104,7 +9104,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -9136,7 +9136,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -9168,7 +9168,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -9200,7 +9200,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -9232,7 +9232,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -9264,7 +9264,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -9296,7 +9296,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -9328,7 +9328,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -9360,7 +9360,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -9392,7 +9392,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -9424,7 +9424,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -9456,7 +9456,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -9488,7 +9488,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -9520,7 +9520,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -9552,7 +9552,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -9584,7 +9584,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -9616,7 +9616,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -9648,7 +9648,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -9680,7 +9680,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -9712,7 +9712,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -9744,7 +9744,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -9776,7 +9776,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -9808,7 +9808,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -9840,7 +9840,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -9872,7 +9872,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -9904,7 +9904,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -9936,7 +9936,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -9968,7 +9968,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -10000,7 +10000,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -10032,7 +10032,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -10064,7 +10064,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -10096,7 +10096,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -10128,7 +10128,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -10160,7 +10160,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -10192,7 +10192,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -10224,7 +10224,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -10256,7 +10256,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -10288,7 +10288,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -10320,7 +10320,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -10352,7 +10352,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -10384,7 +10384,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -10416,7 +10416,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -10448,7 +10448,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -10480,7 +10480,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -10512,7 +10512,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -10544,7 +10544,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="25" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -10576,7 +10576,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -10608,7 +10608,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -10640,7 +10640,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -10672,7 +10672,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -10704,7 +10704,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -10736,7 +10736,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="25" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -10768,7 +10768,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -10800,7 +10800,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -10832,7 +10832,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -10864,7 +10864,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" s="3">
         <v>83</v>
       </c>
@@ -10896,7 +10896,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
         <v>84</v>
       </c>
@@ -10928,7 +10928,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A86" s="3">
         <v>85</v>
       </c>
@@ -10960,7 +10960,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>86</v>
       </c>
@@ -10992,7 +10992,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" s="3">
         <v>87</v>
       </c>
@@ -11024,7 +11024,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
         <v>88</v>
       </c>
@@ -11056,7 +11056,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" s="3">
         <v>89</v>
       </c>
@@ -11088,7 +11088,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" s="3">
         <v>90</v>
       </c>
@@ -11120,7 +11120,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" s="3">
         <v>91</v>
       </c>
@@ -11152,7 +11152,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" s="3">
         <v>92</v>
       </c>
@@ -11184,7 +11184,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94" s="3">
         <v>93</v>
       </c>
@@ -11216,7 +11216,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" s="3">
         <v>94</v>
       </c>
@@ -11248,7 +11248,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" s="3">
         <v>95</v>
       </c>
@@ -11280,7 +11280,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" s="3">
         <v>96</v>
       </c>
@@ -11312,7 +11312,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" s="3">
         <v>97</v>
       </c>
@@ -11344,7 +11344,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" s="3">
         <v>98</v>
       </c>
@@ -11376,7 +11376,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" s="3">
         <v>99</v>
       </c>
@@ -11408,7 +11408,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" s="3">
         <v>100</v>
       </c>
@@ -11440,7 +11440,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" s="3">
         <v>101</v>
       </c>
@@ -11469,7 +11469,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" s="3">
         <v>102</v>
       </c>
@@ -11498,7 +11498,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" s="3">
         <v>103</v>
       </c>
@@ -11530,7 +11530,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" s="3">
         <v>104</v>
       </c>
@@ -11562,7 +11562,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" s="3">
         <v>105</v>
       </c>
@@ -11594,7 +11594,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" s="3">
         <v>106</v>
       </c>
@@ -11626,7 +11626,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" s="3">
         <v>107</v>
       </c>
@@ -11658,7 +11658,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" s="3">
         <v>108</v>
       </c>
@@ -11690,7 +11690,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" s="3">
         <v>109</v>
       </c>
@@ -11722,7 +11722,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" s="3">
         <v>110</v>
       </c>
@@ -11754,7 +11754,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" s="3">
         <v>111</v>
       </c>
@@ -11783,7 +11783,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113" s="3">
         <v>112</v>
       </c>
@@ -11815,7 +11815,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114" s="3">
         <v>113</v>
       </c>
@@ -11847,7 +11847,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115" s="3">
         <v>114</v>
       </c>
@@ -11879,295 +11879,295 @@
         <v>863</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J116" s="17"/>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J117" s="17"/>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J118" s="17"/>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J119" s="17"/>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J120" s="17"/>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J121" s="17"/>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J122" s="17"/>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J123" s="17"/>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J124" s="17"/>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J125" s="17"/>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J126" s="17"/>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J127" s="17"/>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J128" s="17"/>
     </row>
-    <row r="129" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J129" s="17"/>
     </row>
-    <row r="130" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J130" s="17"/>
     </row>
-    <row r="131" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J131" s="17"/>
     </row>
-    <row r="132" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J132" s="17"/>
     </row>
-    <row r="133" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J133" s="17"/>
     </row>
-    <row r="134" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J134" s="17"/>
     </row>
-    <row r="135" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J135" s="17"/>
     </row>
-    <row r="136" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J136" s="17"/>
     </row>
-    <row r="137" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J137" s="17"/>
     </row>
-    <row r="138" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J138" s="17"/>
     </row>
-    <row r="139" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J139" s="17"/>
     </row>
-    <row r="140" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J140" s="17"/>
     </row>
-    <row r="141" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J141" s="17"/>
     </row>
-    <row r="142" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J142" s="17"/>
     </row>
-    <row r="143" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J143" s="17"/>
     </row>
-    <row r="144" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J144" s="17"/>
     </row>
-    <row r="145" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J145" s="17"/>
     </row>
-    <row r="146" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J146" s="17"/>
     </row>
-    <row r="147" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J147" s="17"/>
     </row>
-    <row r="148" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J148" s="17"/>
     </row>
-    <row r="149" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J149" s="17"/>
     </row>
-    <row r="150" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J150" s="17"/>
     </row>
-    <row r="151" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J151" s="17"/>
     </row>
-    <row r="152" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J152" s="17"/>
     </row>
-    <row r="153" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J153" s="17"/>
     </row>
-    <row r="154" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J154" s="17"/>
     </row>
-    <row r="155" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J155" s="17"/>
     </row>
-    <row r="156" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J156" s="17"/>
     </row>
-    <row r="157" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J157" s="17"/>
     </row>
-    <row r="158" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J158" s="17"/>
     </row>
-    <row r="159" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J159" s="17"/>
     </row>
-    <row r="160" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J160" s="17"/>
     </row>
-    <row r="161" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J161" s="17"/>
     </row>
-    <row r="162" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J162" s="17"/>
     </row>
-    <row r="163" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J163" s="17"/>
     </row>
-    <row r="164" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J164" s="17"/>
     </row>
-    <row r="165" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J165" s="17"/>
     </row>
-    <row r="166" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J166" s="17"/>
     </row>
-    <row r="167" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J167" s="17"/>
     </row>
-    <row r="168" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J168" s="17"/>
     </row>
-    <row r="169" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J169" s="17"/>
     </row>
-    <row r="170" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J170" s="17"/>
     </row>
-    <row r="171" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J171" s="17"/>
     </row>
-    <row r="172" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J172" s="17"/>
     </row>
-    <row r="173" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J173" s="17"/>
     </row>
-    <row r="174" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J174" s="17"/>
     </row>
-    <row r="175" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J175" s="17"/>
     </row>
-    <row r="176" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J176" s="17"/>
     </row>
-    <row r="177" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J177" s="17"/>
     </row>
-    <row r="178" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J178" s="17"/>
     </row>
-    <row r="179" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J179" s="17"/>
     </row>
-    <row r="180" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J180" s="17"/>
     </row>
-    <row r="181" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J181" s="17"/>
     </row>
-    <row r="182" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J182" s="17"/>
     </row>
-    <row r="183" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J183" s="17"/>
     </row>
-    <row r="184" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J184" s="17"/>
     </row>
-    <row r="185" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J185" s="17"/>
     </row>
-    <row r="186" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J186" s="17"/>
     </row>
-    <row r="187" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J187" s="17"/>
     </row>
-    <row r="188" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J188" s="17"/>
     </row>
-    <row r="189" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J189" s="17"/>
     </row>
-    <row r="190" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J190" s="17"/>
     </row>
-    <row r="191" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J191" s="17"/>
     </row>
-    <row r="192" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J192" s="17"/>
     </row>
-    <row r="193" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J193" s="17"/>
     </row>
-    <row r="194" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J194" s="17"/>
     </row>
-    <row r="195" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J195" s="17"/>
     </row>
-    <row r="196" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J196" s="17"/>
     </row>
-    <row r="197" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J197" s="17"/>
     </row>
-    <row r="198" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J198" s="17"/>
     </row>
-    <row r="199" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J199" s="17"/>
     </row>
-    <row r="200" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J200" s="17"/>
     </row>
-    <row r="201" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J201" s="17"/>
     </row>
-    <row r="202" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J202" s="17"/>
     </row>
-    <row r="203" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J203" s="17"/>
     </row>
-    <row r="204" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J204" s="17"/>
     </row>
-    <row r="205" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J205" s="17"/>
     </row>
-    <row r="206" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="206" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J206" s="17"/>
     </row>
-    <row r="207" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="207" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J207" s="17"/>
     </row>
-    <row r="208" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="208" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J208" s="17"/>
     </row>
-    <row r="209" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J209" s="17"/>
     </row>
-    <row r="210" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J210" s="17"/>
     </row>
-    <row r="211" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J211" s="17"/>
     </row>
-    <row r="212" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J212" s="17"/>
     </row>
   </sheetData>
@@ -12311,22 +12311,22 @@
       <selection pane="bottomLeft" activeCell="D107" sqref="D107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.26953125" customWidth="1"/>
-    <col min="2" max="2" width="16.81640625" customWidth="1"/>
-    <col min="3" max="3" width="15.7265625" customWidth="1"/>
-    <col min="4" max="4" width="25.453125" customWidth="1"/>
-    <col min="5" max="5" width="16.81640625" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="33.1796875" customWidth="1"/>
-    <col min="8" max="8" width="9.453125" customWidth="1"/>
-    <col min="9" max="9" width="17.453125" customWidth="1"/>
-    <col min="10" max="10" width="33.1796875" customWidth="1"/>
-    <col min="11" max="16" width="21.453125" customWidth="1"/>
+    <col min="7" max="7" width="33.140625" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="10" max="10" width="33.140625" customWidth="1"/>
+    <col min="11" max="16" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>864</v>
       </c>
@@ -12364,7 +12364,7 @@
       <c r="O1" s="13"/>
       <c r="P1" s="13"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -12396,7 +12396,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -12428,7 +12428,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -12460,7 +12460,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -12492,7 +12492,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -12524,7 +12524,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -12556,7 +12556,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -12588,7 +12588,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -12620,7 +12620,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -12652,7 +12652,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -12684,7 +12684,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -12716,7 +12716,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -12748,7 +12748,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -12780,7 +12780,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -12812,7 +12812,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -12844,7 +12844,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -12876,7 +12876,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -12908,7 +12908,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -12940,7 +12940,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -12972,7 +12972,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -13004,7 +13004,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -13036,7 +13036,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -13068,7 +13068,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -13100,7 +13100,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -13132,7 +13132,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -13164,7 +13164,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -13196,7 +13196,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -13228,7 +13228,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -13260,7 +13260,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -13292,7 +13292,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -13324,7 +13324,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -13356,7 +13356,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -13388,7 +13388,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -13420,7 +13420,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -13452,7 +13452,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -13484,7 +13484,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -13516,7 +13516,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -13548,7 +13548,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -13580,7 +13580,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -13612,7 +13612,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -13644,7 +13644,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -13676,7 +13676,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -13708,7 +13708,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -13740,7 +13740,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -13772,7 +13772,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -13804,7 +13804,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -13836,7 +13836,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -13868,7 +13868,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -13900,7 +13900,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -13932,7 +13932,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -13964,7 +13964,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -13996,7 +13996,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -14028,7 +14028,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -14060,7 +14060,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -14092,7 +14092,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -14124,7 +14124,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -14156,7 +14156,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -14188,7 +14188,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -14220,7 +14220,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -14252,7 +14252,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -14284,7 +14284,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -14316,7 +14316,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -14348,7 +14348,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -14380,7 +14380,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -14412,7 +14412,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -14444,7 +14444,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -14476,7 +14476,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -14508,7 +14508,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -14540,7 +14540,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -14572,7 +14572,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -14604,7 +14604,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -14636,7 +14636,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -14668,7 +14668,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -14700,7 +14700,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -14732,7 +14732,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -14764,7 +14764,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -14796,7 +14796,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -14828,7 +14828,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -14860,7 +14860,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -14892,7 +14892,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -14924,7 +14924,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -14956,7 +14956,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -14988,7 +14988,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" s="3">
         <v>83</v>
       </c>
@@ -15020,7 +15020,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
         <v>84</v>
       </c>
@@ -15052,7 +15052,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" s="3">
         <v>85</v>
       </c>
@@ -15084,7 +15084,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>86</v>
       </c>
@@ -15116,7 +15116,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" s="3">
         <v>87</v>
       </c>
@@ -15145,7 +15145,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
         <v>88</v>
       </c>
@@ -15174,7 +15174,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" s="3">
         <v>89</v>
       </c>
@@ -15206,7 +15206,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" s="3">
         <v>90</v>
       </c>
@@ -15238,7 +15238,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" s="3">
         <v>91</v>
       </c>
@@ -15270,7 +15270,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" s="3">
         <v>92</v>
       </c>
@@ -15302,7 +15302,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94" s="3">
         <v>93</v>
       </c>
@@ -15334,7 +15334,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" s="3">
         <v>94</v>
       </c>
@@ -15366,7 +15366,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" s="3">
         <v>95</v>
       </c>
@@ -15398,7 +15398,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" s="3">
         <v>96</v>
       </c>
@@ -15430,7 +15430,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" s="3">
         <v>97</v>
       </c>
@@ -15459,7 +15459,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" s="3">
         <v>98</v>
       </c>
@@ -15491,7 +15491,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" s="3">
         <v>99</v>
       </c>
@@ -15523,7 +15523,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" s="3">
         <v>100</v>
       </c>
@@ -15555,7 +15555,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" s="3">
         <v>101</v>
       </c>
@@ -15587,7 +15587,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" s="3">
         <v>102</v>
       </c>
@@ -15619,7 +15619,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" s="3">
         <v>103</v>
       </c>
@@ -15651,7 +15651,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" s="3">
         <v>104</v>
       </c>
@@ -15683,7 +15683,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" s="3">
         <v>105</v>
       </c>
@@ -15715,7 +15715,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" s="3">
         <v>106</v>
       </c>
@@ -15747,7 +15747,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" s="3">
         <v>107</v>
       </c>
@@ -15779,7 +15779,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" s="3">
         <v>108</v>
       </c>
@@ -15811,7 +15811,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" s="3">
         <v>109</v>
       </c>
@@ -15843,7 +15843,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" s="3">
         <v>110</v>
       </c>
@@ -15875,7 +15875,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>111</v>
       </c>
@@ -15907,262 +15907,262 @@
         <v>904</v>
       </c>
     </row>
-    <row r="113" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J113" s="17"/>
     </row>
-    <row r="114" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J114" s="17"/>
     </row>
-    <row r="115" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J115" s="17"/>
     </row>
-    <row r="116" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J116" s="17"/>
     </row>
-    <row r="117" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J117" s="17"/>
     </row>
-    <row r="118" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J118" s="17"/>
     </row>
-    <row r="119" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J119" s="17"/>
     </row>
-    <row r="120" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J120" s="17"/>
     </row>
-    <row r="121" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J121" s="17"/>
     </row>
-    <row r="122" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J122" s="17"/>
     </row>
-    <row r="123" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J123" s="17"/>
     </row>
-    <row r="124" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J124" s="17"/>
     </row>
-    <row r="125" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J125" s="17"/>
     </row>
-    <row r="126" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J126" s="17"/>
     </row>
-    <row r="127" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J127" s="17"/>
     </row>
-    <row r="128" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J128" s="17"/>
     </row>
-    <row r="129" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J129" s="17"/>
     </row>
-    <row r="130" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J130" s="17"/>
     </row>
-    <row r="131" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J131" s="17"/>
     </row>
-    <row r="132" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J132" s="17"/>
     </row>
-    <row r="133" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J133" s="17"/>
     </row>
-    <row r="134" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J134" s="17"/>
     </row>
-    <row r="135" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J135" s="17"/>
     </row>
-    <row r="136" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J136" s="17"/>
     </row>
-    <row r="137" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J137" s="17"/>
     </row>
-    <row r="138" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J138" s="17"/>
     </row>
-    <row r="139" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J139" s="17"/>
     </row>
-    <row r="140" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J140" s="17"/>
     </row>
-    <row r="141" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J141" s="17"/>
     </row>
-    <row r="142" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J142" s="17"/>
     </row>
-    <row r="143" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J143" s="17"/>
     </row>
-    <row r="144" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J144" s="17"/>
     </row>
-    <row r="145" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J145" s="17"/>
     </row>
-    <row r="146" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J146" s="17"/>
     </row>
-    <row r="147" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J147" s="17"/>
     </row>
-    <row r="148" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J148" s="17"/>
     </row>
-    <row r="149" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J149" s="17"/>
     </row>
-    <row r="150" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J150" s="17"/>
     </row>
-    <row r="151" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J151" s="17"/>
     </row>
-    <row r="152" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J152" s="17"/>
     </row>
-    <row r="153" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J153" s="17"/>
     </row>
-    <row r="154" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J154" s="17"/>
     </row>
-    <row r="155" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J155" s="17"/>
     </row>
-    <row r="156" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J156" s="17"/>
     </row>
-    <row r="157" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J157" s="17"/>
     </row>
-    <row r="158" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J158" s="17"/>
     </row>
-    <row r="159" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J159" s="17"/>
     </row>
-    <row r="160" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J160" s="17"/>
     </row>
-    <row r="161" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J161" s="17"/>
     </row>
-    <row r="162" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J162" s="17"/>
     </row>
-    <row r="163" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J163" s="17"/>
     </row>
-    <row r="164" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J164" s="17"/>
     </row>
-    <row r="165" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J165" s="17"/>
     </row>
-    <row r="166" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J166" s="17"/>
     </row>
-    <row r="167" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J167" s="17"/>
     </row>
-    <row r="168" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J168" s="17"/>
     </row>
-    <row r="169" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J169" s="17"/>
     </row>
-    <row r="170" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J170" s="17"/>
     </row>
-    <row r="171" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J171" s="17"/>
     </row>
-    <row r="172" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J172" s="17"/>
     </row>
-    <row r="173" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J173" s="17"/>
     </row>
-    <row r="174" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J174" s="17"/>
     </row>
-    <row r="175" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J175" s="17"/>
     </row>
-    <row r="176" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J176" s="17"/>
     </row>
-    <row r="177" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J177" s="17"/>
     </row>
-    <row r="178" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J178" s="17"/>
     </row>
-    <row r="179" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J179" s="17"/>
     </row>
-    <row r="180" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J180" s="17"/>
     </row>
-    <row r="181" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J181" s="17"/>
     </row>
-    <row r="182" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J182" s="17"/>
     </row>
-    <row r="183" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J183" s="17"/>
     </row>
-    <row r="184" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J184" s="17"/>
     </row>
-    <row r="185" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J185" s="17"/>
     </row>
-    <row r="186" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J186" s="17"/>
     </row>
-    <row r="187" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J187" s="17"/>
     </row>
-    <row r="188" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J188" s="17"/>
     </row>
-    <row r="189" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J189" s="17"/>
     </row>
-    <row r="190" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J190" s="17"/>
     </row>
-    <row r="191" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J191" s="17"/>
     </row>
-    <row r="192" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J192" s="17"/>
     </row>
-    <row r="193" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J193" s="17"/>
     </row>
-    <row r="194" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J194" s="17"/>
     </row>
-    <row r="195" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J195" s="17"/>
     </row>
-    <row r="196" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J196" s="17"/>
     </row>
-    <row r="197" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J197" s="17"/>
     </row>
-    <row r="198" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J198" s="17"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated my github data
</commit_message>
<xml_diff>
--- a/CS335/GitHub Info sans duplicates.xlsx
+++ b/CS335/GitHub Info sans duplicates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\staffcard\CS335\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joane\Desktop\staffcard\CS335\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{117837A6-B2B7-4677-A870-D79E9EF57F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBFDB654-5E3E-4F97-9143-C54639F09CD0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3799" uniqueCount="1166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3799" uniqueCount="1169">
   <si>
     <t>Timestamp</t>
   </si>
@@ -3520,6 +3520,15 @@
   </si>
   <si>
     <t>https;//github.com/MartinMsuya</t>
+  </si>
+  <si>
+    <t>joaneliamuganda@gmail.com</t>
+  </si>
+  <si>
+    <t>Joannah123</t>
+  </si>
+  <si>
+    <t>https://github.com/Joannah123</t>
   </si>
 </sst>
 </file>
@@ -3564,7 +3573,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -3572,6 +3581,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3913,15 +3928,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L127"/>
+  <dimension ref="A1:P127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="L104" sqref="L104:M104"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3959,7 +3978,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3997,7 +4016,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -4035,7 +4054,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -4073,7 +4092,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -4111,7 +4130,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -4149,7 +4168,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -4187,7 +4206,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>65</v>
       </c>
@@ -4225,7 +4244,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>74</v>
       </c>
@@ -4263,7 +4282,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>82</v>
       </c>
@@ -4301,7 +4320,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>90</v>
       </c>
@@ -4339,7 +4358,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>98</v>
       </c>
@@ -4377,7 +4396,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>106</v>
       </c>
@@ -4415,7 +4434,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>113</v>
       </c>
@@ -4453,7 +4472,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>121</v>
       </c>
@@ -4491,7 +4510,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>130</v>
       </c>
@@ -4529,7 +4548,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>138</v>
       </c>
@@ -4567,7 +4586,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>146</v>
       </c>
@@ -4605,7 +4624,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>154</v>
       </c>
@@ -4643,7 +4662,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>163</v>
       </c>
@@ -4681,7 +4700,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>171</v>
       </c>
@@ -4719,7 +4738,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>179</v>
       </c>
@@ -4757,7 +4776,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>187</v>
       </c>
@@ -4795,7 +4814,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>195</v>
       </c>
@@ -4833,7 +4852,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>203</v>
       </c>
@@ -4871,7 +4890,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>212</v>
       </c>
@@ -4909,7 +4928,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>221</v>
       </c>
@@ -4947,7 +4966,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>229</v>
       </c>
@@ -4985,7 +5004,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>237</v>
       </c>
@@ -5023,7 +5042,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>245</v>
       </c>
@@ -5061,7 +5080,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>253</v>
       </c>
@@ -5099,7 +5118,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>261</v>
       </c>
@@ -5137,7 +5156,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>269</v>
       </c>
@@ -5175,7 +5194,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>277</v>
       </c>
@@ -5213,7 +5232,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>285</v>
       </c>
@@ -5251,7 +5270,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>294</v>
       </c>
@@ -5289,7 +5308,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>302</v>
       </c>
@@ -5327,7 +5346,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>311</v>
       </c>
@@ -5365,7 +5384,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>319</v>
       </c>
@@ -5403,7 +5422,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>327</v>
       </c>
@@ -5441,7 +5460,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>336</v>
       </c>
@@ -5479,7 +5498,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>344</v>
       </c>
@@ -5517,7 +5536,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>352</v>
       </c>
@@ -5555,7 +5574,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>360</v>
       </c>
@@ -5593,7 +5612,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>368</v>
       </c>
@@ -5631,7 +5650,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>376</v>
       </c>
@@ -5669,7 +5688,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>384</v>
       </c>
@@ -5707,7 +5726,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>392</v>
       </c>
@@ -5745,7 +5764,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>400</v>
       </c>
@@ -5783,7 +5802,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>408</v>
       </c>
@@ -5821,7 +5840,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>416</v>
       </c>
@@ -5859,7 +5878,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>424</v>
       </c>
@@ -5897,7 +5916,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>432</v>
       </c>
@@ -5935,7 +5954,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>440</v>
       </c>
@@ -5973,7 +5992,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>448</v>
       </c>
@@ -6011,7 +6030,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>456</v>
       </c>
@@ -6049,7 +6068,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>464</v>
       </c>
@@ -6087,7 +6106,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>472</v>
       </c>
@@ -6125,7 +6144,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>481</v>
       </c>
@@ -6163,7 +6182,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>488</v>
       </c>
@@ -6201,7 +6220,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>496</v>
       </c>
@@ -6239,7 +6258,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>505</v>
       </c>
@@ -6277,7 +6296,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>513</v>
       </c>
@@ -6315,7 +6334,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>521</v>
       </c>
@@ -6353,7 +6372,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>530</v>
       </c>
@@ -6391,7 +6410,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>538</v>
       </c>
@@ -6429,7 +6448,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>546</v>
       </c>
@@ -6467,7 +6486,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>554</v>
       </c>
@@ -6505,7 +6524,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>562</v>
       </c>
@@ -6543,7 +6562,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>571</v>
       </c>
@@ -6581,7 +6600,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>579</v>
       </c>
@@ -6619,7 +6638,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>587</v>
       </c>
@@ -6657,7 +6676,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>595</v>
       </c>
@@ -6695,7 +6714,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>603</v>
       </c>
@@ -6733,7 +6752,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>611</v>
       </c>
@@ -6771,7 +6790,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>619</v>
       </c>
@@ -6809,7 +6828,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>628</v>
       </c>
@@ -6847,7 +6866,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>635</v>
       </c>
@@ -6885,7 +6904,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>642</v>
       </c>
@@ -6923,7 +6942,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>650</v>
       </c>
@@ -6961,7 +6980,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>658</v>
       </c>
@@ -6999,7 +7018,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>666</v>
       </c>
@@ -7037,7 +7056,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>674</v>
       </c>
@@ -7075,7 +7094,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>683</v>
       </c>
@@ -7113,7 +7132,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>690</v>
       </c>
@@ -7151,7 +7170,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>698</v>
       </c>
@@ -7189,7 +7208,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>706</v>
       </c>
@@ -7227,7 +7246,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>714</v>
       </c>
@@ -7265,7 +7284,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>722</v>
       </c>
@@ -7303,7 +7322,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>730</v>
       </c>
@@ -7341,7 +7360,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>738</v>
       </c>
@@ -7379,7 +7398,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>746</v>
       </c>
@@ -7417,7 +7436,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>754</v>
       </c>
@@ -7455,7 +7474,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>762</v>
       </c>
@@ -7493,7 +7512,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>770</v>
       </c>
@@ -7531,7 +7550,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>772</v>
       </c>
@@ -7569,7 +7588,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>780</v>
       </c>
@@ -7607,7 +7626,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>788</v>
       </c>
@@ -7645,7 +7664,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>796</v>
       </c>
@@ -7683,7 +7702,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>804</v>
       </c>
@@ -7721,7 +7740,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>812</v>
       </c>
@@ -7759,7 +7778,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>820</v>
       </c>
@@ -7797,7 +7816,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>828</v>
       </c>
@@ -7832,7 +7851,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>835</v>
       </c>
@@ -7845,12 +7864,15 @@
       <c r="D104" t="s">
         <v>838</v>
       </c>
-      <c r="E104" t="s">
-        <v>839</v>
+      <c r="E104">
+        <v>716689793</v>
       </c>
       <c r="F104" t="s">
         <v>17</v>
       </c>
+      <c r="G104" s="1" t="s">
+        <v>1166</v>
+      </c>
       <c r="H104" t="s">
         <v>71</v>
       </c>
@@ -7861,13 +7883,15 @@
         <v>21</v>
       </c>
       <c r="K104" t="s">
-        <v>840</v>
-      </c>
-      <c r="L104" t="s">
-        <v>841</v>
-      </c>
-    </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.35">
+        <v>1167</v>
+      </c>
+      <c r="L104" s="5" t="s">
+        <v>1168</v>
+      </c>
+      <c r="M104" s="4"/>
+      <c r="P104" s="1"/>
+    </row>
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>842</v>
       </c>
@@ -7905,7 +7929,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>850</v>
       </c>
@@ -7943,7 +7967,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>858</v>
       </c>
@@ -7981,7 +8005,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>866</v>
       </c>
@@ -8019,7 +8043,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>874</v>
       </c>
@@ -8057,7 +8081,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>883</v>
       </c>
@@ -8095,7 +8119,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>891</v>
       </c>
@@ -8133,7 +8157,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>893</v>
       </c>
@@ -8171,7 +8195,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>901</v>
       </c>
@@ -8206,7 +8230,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>903</v>
       </c>
@@ -8244,7 +8268,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>911</v>
       </c>
@@ -8282,7 +8306,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>919</v>
       </c>
@@ -8320,7 +8344,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>927</v>
       </c>
@@ -8358,7 +8382,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>934</v>
       </c>
@@ -8396,7 +8420,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>942</v>
       </c>
@@ -8434,7 +8458,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>950</v>
       </c>
@@ -8472,7 +8496,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>957</v>
       </c>
@@ -8510,7 +8534,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>965</v>
       </c>
@@ -8548,7 +8572,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>973</v>
       </c>
@@ -8583,7 +8607,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
         <v>482</v>
       </c>
@@ -8618,7 +8642,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
         <v>977</v>
       </c>
@@ -8644,7 +8668,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>522</v>
       </c>
@@ -8667,7 +8691,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
         <v>983</v>
       </c>
@@ -8703,9 +8727,16 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="L104:M104"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G104" r:id="rId1" xr:uid="{0637F5CB-A740-4582-ACD8-E461EEC2F40F}"/>
+    <hyperlink ref="L104" r:id="rId2" xr:uid="{961EA30F-21E6-45DA-B0A1-8705C72691BA}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:L33 A35:L127 A34:E34 G34:L34" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:L33 A35:L103 A34:E34 G34:L34 A105:L127 A104:D104 F104 H104:J104" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -8718,15 +8749,15 @@
       <selection activeCell="B117" sqref="B117:L117"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="17.5" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.875" customWidth="1"/>
+    <col min="5" max="5" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>991</v>
       </c>
@@ -8758,7 +8789,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>998</v>
       </c>
@@ -8790,7 +8821,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1001</v>
       </c>
@@ -8822,7 +8853,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -8854,7 +8885,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1002</v>
       </c>
@@ -8886,7 +8917,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1004</v>
       </c>
@@ -8918,7 +8949,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1005</v>
       </c>
@@ -8950,7 +8981,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1007</v>
       </c>
@@ -8982,7 +9013,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1008</v>
       </c>
@@ -9014,7 +9045,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1009</v>
       </c>
@@ -9046,7 +9077,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1010</v>
       </c>
@@ -9078,7 +9109,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1011</v>
       </c>
@@ -9110,7 +9141,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1012</v>
       </c>
@@ -9142,7 +9173,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1013</v>
       </c>
@@ -9174,7 +9205,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>1014</v>
       </c>
@@ -9206,7 +9237,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1015</v>
       </c>
@@ -9238,7 +9269,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1016</v>
       </c>
@@ -9270,7 +9301,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>1017</v>
       </c>
@@ -9302,7 +9333,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>1018</v>
       </c>
@@ -9334,7 +9365,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>1019</v>
       </c>
@@ -9366,7 +9397,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>1020</v>
       </c>
@@ -9398,7 +9429,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>1021</v>
       </c>
@@ -9430,7 +9461,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>1022</v>
       </c>
@@ -9462,7 +9493,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>1024</v>
       </c>
@@ -9494,7 +9525,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>1025</v>
       </c>
@@ -9526,7 +9557,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>1026</v>
       </c>
@@ -9558,7 +9589,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>1027</v>
       </c>
@@ -9590,7 +9621,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>1028</v>
       </c>
@@ -9622,7 +9653,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>1029</v>
       </c>
@@ -9654,7 +9685,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>1030</v>
       </c>
@@ -9686,7 +9717,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>1031</v>
       </c>
@@ -9718,7 +9749,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>1032</v>
       </c>
@@ -9750,7 +9781,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>1034</v>
       </c>
@@ -9782,7 +9813,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>1035</v>
       </c>
@@ -9814,7 +9845,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>1036</v>
       </c>
@@ -9846,7 +9877,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>1038</v>
       </c>
@@ -9878,7 +9909,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>1039</v>
       </c>
@@ -9910,7 +9941,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>1040</v>
       </c>
@@ -9942,7 +9973,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>1041</v>
       </c>
@@ -9974,7 +10005,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>1042</v>
       </c>
@@ -10006,7 +10037,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>1043</v>
       </c>
@@ -10038,7 +10069,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>1044</v>
       </c>
@@ -10070,7 +10101,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>1045</v>
       </c>
@@ -10102,7 +10133,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>1046</v>
       </c>
@@ -10134,7 +10165,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>1047</v>
       </c>
@@ -10166,7 +10197,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>1048</v>
       </c>
@@ -10198,7 +10229,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>1049</v>
       </c>
@@ -10230,7 +10261,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>1050</v>
       </c>
@@ -10262,7 +10293,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>1051</v>
       </c>
@@ -10294,7 +10325,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>1052</v>
       </c>
@@ -10326,7 +10357,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>1054</v>
       </c>
@@ -10358,7 +10389,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>1055</v>
       </c>
@@ -10390,7 +10421,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>1056</v>
       </c>
@@ -10422,7 +10453,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>1057</v>
       </c>
@@ -10454,7 +10485,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>1058</v>
       </c>
@@ -10486,7 +10517,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>1059</v>
       </c>
@@ -10518,7 +10549,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>1060</v>
       </c>
@@ -10550,7 +10581,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>1062</v>
       </c>
@@ -10582,7 +10613,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>1063</v>
       </c>
@@ -10614,7 +10645,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>1064</v>
       </c>
@@ -10646,7 +10677,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>1065</v>
       </c>
@@ -10678,7 +10709,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>1066</v>
       </c>
@@ -10710,7 +10741,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>1067</v>
       </c>
@@ -10742,7 +10773,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>1068</v>
       </c>
@@ -10774,7 +10805,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>1069</v>
       </c>
@@ -10806,7 +10837,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>1070</v>
       </c>
@@ -10838,7 +10869,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>1071</v>
       </c>
@@ -10870,7 +10901,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>1072</v>
       </c>
@@ -10902,7 +10933,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>1073</v>
       </c>
@@ -10934,7 +10965,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>1074</v>
       </c>
@@ -10966,7 +10997,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>1075</v>
       </c>
@@ -10998,7 +11029,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>1076</v>
       </c>
@@ -11030,7 +11061,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>1077</v>
       </c>
@@ -11062,7 +11093,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>1078</v>
       </c>
@@ -11094,7 +11125,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>1079</v>
       </c>
@@ -11126,7 +11157,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>1080</v>
       </c>
@@ -11158,7 +11189,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>1081</v>
       </c>
@@ -11190,7 +11221,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>1083</v>
       </c>
@@ -11222,7 +11253,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>1084</v>
       </c>
@@ -11254,7 +11285,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>1085</v>
       </c>
@@ -11286,7 +11317,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>1086</v>
       </c>
@@ -11318,7 +11349,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>1087</v>
       </c>
@@ -11350,7 +11381,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>1088</v>
       </c>
@@ -11382,7 +11413,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>1089</v>
       </c>
@@ -11414,7 +11445,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>1090</v>
       </c>
@@ -11446,7 +11477,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>1091</v>
       </c>
@@ -11478,7 +11509,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>1092</v>
       </c>
@@ -11510,7 +11541,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>1093</v>
       </c>
@@ -11542,7 +11573,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>1094</v>
       </c>
@@ -11574,7 +11605,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>1095</v>
       </c>
@@ -11606,7 +11637,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>1096</v>
       </c>
@@ -11638,7 +11669,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>1097</v>
       </c>
@@ -11670,7 +11701,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>1098</v>
       </c>
@@ -11702,7 +11733,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>1099</v>
       </c>
@@ -11734,7 +11765,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>1100</v>
       </c>
@@ -11766,7 +11797,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>1101</v>
       </c>
@@ -11798,7 +11829,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>1102</v>
       </c>
@@ -11830,7 +11861,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>1103</v>
       </c>
@@ -11862,7 +11893,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>1104</v>
       </c>
@@ -11894,7 +11925,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>1105</v>
       </c>
@@ -11926,7 +11957,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>1107</v>
       </c>
@@ -11958,7 +11989,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>1108</v>
       </c>
@@ -11987,7 +12018,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>1109</v>
       </c>
@@ -12016,7 +12047,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>1110</v>
       </c>
@@ -12048,7 +12079,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>1112</v>
       </c>
@@ -12080,7 +12111,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>1113</v>
       </c>
@@ -12112,7 +12143,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>1114</v>
       </c>
@@ -12144,7 +12175,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>1115</v>
       </c>
@@ -12176,7 +12207,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>1116</v>
       </c>
@@ -12208,7 +12239,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>1117</v>
       </c>
@@ -12240,7 +12271,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>1118</v>
       </c>
@@ -12272,7 +12303,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>1119</v>
       </c>
@@ -12301,7 +12332,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>1120</v>
       </c>
@@ -12333,7 +12364,7 @@
         <v>1122</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>1123</v>
       </c>
@@ -12365,7 +12396,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>1131</v>
       </c>
@@ -12397,7 +12428,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>1132</v>
       </c>
@@ -12429,7 +12460,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>117</v>
       </c>
@@ -12481,16 +12512,16 @@
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="29.25" style="2" customWidth="1"/>
-    <col min="9" max="9" width="17.08203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="17.125" style="2" customWidth="1"/>
     <col min="10" max="10" width="30.25" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>991</v>
       </c>
@@ -12522,7 +12553,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>998</v>
       </c>
@@ -12554,7 +12585,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1001</v>
       </c>
@@ -12586,7 +12617,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -12618,7 +12649,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1002</v>
       </c>
@@ -12650,7 +12681,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1004</v>
       </c>
@@ -12682,7 +12713,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1005</v>
       </c>
@@ -12714,7 +12745,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1007</v>
       </c>
@@ -12746,7 +12777,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1008</v>
       </c>
@@ -12778,7 +12809,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1009</v>
       </c>
@@ -12810,7 +12841,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1010</v>
       </c>
@@ -12842,7 +12873,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1011</v>
       </c>
@@ -12874,7 +12905,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1012</v>
       </c>
@@ -12906,7 +12937,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1013</v>
       </c>
@@ -12938,7 +12969,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>1014</v>
       </c>
@@ -12970,7 +13001,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1015</v>
       </c>
@@ -13002,7 +13033,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1016</v>
       </c>
@@ -13034,7 +13065,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>1017</v>
       </c>
@@ -13066,7 +13097,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>1018</v>
       </c>
@@ -13098,7 +13129,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>1019</v>
       </c>
@@ -13130,7 +13161,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>1020</v>
       </c>
@@ -13162,7 +13193,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>1021</v>
       </c>
@@ -13194,7 +13225,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>1022</v>
       </c>
@@ -13226,7 +13257,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>1024</v>
       </c>
@@ -13258,7 +13289,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>1025</v>
       </c>
@@ -13290,7 +13321,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>1026</v>
       </c>
@@ -13322,7 +13353,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>1027</v>
       </c>
@@ -13354,7 +13385,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>1028</v>
       </c>
@@ -13386,7 +13417,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>1029</v>
       </c>
@@ -13418,7 +13449,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>1030</v>
       </c>
@@ -13450,7 +13481,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>1031</v>
       </c>
@@ -13482,7 +13513,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>1032</v>
       </c>
@@ -13514,7 +13545,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>1034</v>
       </c>
@@ -13546,7 +13577,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>1035</v>
       </c>
@@ -13578,7 +13609,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>1036</v>
       </c>
@@ -13610,7 +13641,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>1038</v>
       </c>
@@ -13642,7 +13673,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>1039</v>
       </c>
@@ -13674,7 +13705,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>1040</v>
       </c>
@@ -13706,7 +13737,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>1041</v>
       </c>
@@ -13738,7 +13769,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>1042</v>
       </c>
@@ -13770,7 +13801,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>1043</v>
       </c>
@@ -13802,7 +13833,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>1044</v>
       </c>
@@ -13834,7 +13865,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>1045</v>
       </c>
@@ -13866,7 +13897,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>1046</v>
       </c>
@@ -13898,7 +13929,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>1047</v>
       </c>
@@ -13930,7 +13961,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>1048</v>
       </c>
@@ -13962,7 +13993,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>1049</v>
       </c>
@@ -13994,7 +14025,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>1050</v>
       </c>
@@ -14026,7 +14057,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>1051</v>
       </c>
@@ -14058,7 +14089,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>1052</v>
       </c>
@@ -14090,7 +14121,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>1054</v>
       </c>
@@ -14122,7 +14153,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>1055</v>
       </c>
@@ -14154,7 +14185,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>1056</v>
       </c>
@@ -14186,7 +14217,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>1057</v>
       </c>
@@ -14218,7 +14249,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>1058</v>
       </c>
@@ -14250,7 +14281,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>1059</v>
       </c>
@@ -14282,7 +14313,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>1060</v>
       </c>
@@ -14314,7 +14345,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>1062</v>
       </c>
@@ -14346,7 +14377,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>1063</v>
       </c>
@@ -14378,7 +14409,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>1064</v>
       </c>
@@ -14410,7 +14441,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>1065</v>
       </c>
@@ -14442,7 +14473,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>1066</v>
       </c>
@@ -14474,7 +14505,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>1067</v>
       </c>
@@ -14506,7 +14537,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>1068</v>
       </c>
@@ -14538,7 +14569,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>1069</v>
       </c>
@@ -14570,7 +14601,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>1070</v>
       </c>
@@ -14602,7 +14633,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>1071</v>
       </c>
@@ -14634,7 +14665,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>1072</v>
       </c>
@@ -14666,7 +14697,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>1073</v>
       </c>
@@ -14698,7 +14729,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>1074</v>
       </c>
@@ -14730,7 +14761,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>1075</v>
       </c>
@@ -14762,7 +14793,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>1076</v>
       </c>
@@ -14794,7 +14825,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>1077</v>
       </c>
@@ -14826,7 +14857,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>1078</v>
       </c>
@@ -14858,7 +14889,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>1079</v>
       </c>
@@ -14890,7 +14921,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>1080</v>
       </c>
@@ -14922,7 +14953,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>1081</v>
       </c>
@@ -14954,7 +14985,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>1083</v>
       </c>
@@ -14986,7 +15017,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>1084</v>
       </c>
@@ -15018,7 +15049,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>1085</v>
       </c>
@@ -15050,7 +15081,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>1086</v>
       </c>
@@ -15082,7 +15113,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>1087</v>
       </c>
@@ -15114,7 +15145,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>1088</v>
       </c>
@@ -15146,7 +15177,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>1089</v>
       </c>
@@ -15178,7 +15209,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>1090</v>
       </c>
@@ -15210,7 +15241,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>1091</v>
       </c>
@@ -15242,7 +15273,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>1092</v>
       </c>
@@ -15274,7 +15305,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>1093</v>
       </c>
@@ -15303,7 +15334,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>1094</v>
       </c>
@@ -15332,7 +15363,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>1095</v>
       </c>
@@ -15364,7 +15395,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>1096</v>
       </c>
@@ -15396,7 +15427,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>1097</v>
       </c>
@@ -15428,7 +15459,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>1098</v>
       </c>
@@ -15460,7 +15491,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>1099</v>
       </c>
@@ -15492,7 +15523,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>1100</v>
       </c>
@@ -15524,7 +15555,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>1101</v>
       </c>
@@ -15556,7 +15587,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>1102</v>
       </c>
@@ -15588,7 +15619,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>1103</v>
       </c>
@@ -15617,7 +15648,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>1104</v>
       </c>
@@ -15649,7 +15680,7 @@
         <v>1122</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>1105</v>
       </c>
@@ -15681,7 +15712,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>1107</v>
       </c>
@@ -15713,7 +15744,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>1108</v>
       </c>
@@ -15745,7 +15776,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>1109</v>
       </c>
@@ -15777,7 +15808,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>1110</v>
       </c>
@@ -15809,7 +15840,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>1112</v>
       </c>
@@ -15841,7 +15872,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>1113</v>
       </c>
@@ -15873,7 +15904,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>1114</v>
       </c>
@@ -15905,7 +15936,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>1115</v>
       </c>
@@ -15937,7 +15968,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>1116</v>
       </c>
@@ -15969,7 +16000,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>1117</v>
       </c>
@@ -16001,7 +16032,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>1118</v>
       </c>
@@ -16033,7 +16064,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>1119</v>
       </c>
@@ -16065,7 +16096,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>

</xml_diff>

<commit_message>
Added a reccord on line 116
</commit_message>
<xml_diff>
--- a/CS335/GitHub Info sans duplicates.xlsx
+++ b/CS335/GitHub Info sans duplicates.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Documents\UDSM\Third Year\IS 335\git\staffcard\CS335\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\staffcard\CS335\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E956657E-78FC-4DAA-B745-6CA811B950C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7810" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="756" yWindow="756" windowWidth="14400" windowHeight="7812" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3802" uniqueCount="1180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3808" uniqueCount="1184">
   <si>
     <t>Timestamp</t>
   </si>
@@ -3567,12 +3566,24 @@
   </si>
   <si>
     <t>https://github.com/ARwaich911</t>
+  </si>
+  <si>
+    <t>2019-04-05208</t>
+  </si>
+  <si>
+    <t>Lyaganda</t>
+  </si>
+  <si>
+    <t>Masanja</t>
+  </si>
+  <si>
+    <t>lyagandaml@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -3617,7 +3628,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -3632,6 +3643,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3947,21 +3961,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P127"/>
   <sheetViews>
     <sheetView topLeftCell="A112" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="9.83203125" customWidth="1"/>
-    <col min="11" max="11" width="9.83203125" customWidth="1"/>
+    <col min="5" max="5" width="9.796875" customWidth="1"/>
+    <col min="11" max="11" width="9.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3999,7 +4013,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -4037,7 +4051,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -4075,7 +4089,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -4113,7 +4127,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -4151,7 +4165,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -4189,7 +4203,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -4227,7 +4241,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>65</v>
       </c>
@@ -4265,7 +4279,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>74</v>
       </c>
@@ -4303,7 +4317,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>82</v>
       </c>
@@ -4341,7 +4355,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>90</v>
       </c>
@@ -4379,7 +4393,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>98</v>
       </c>
@@ -4417,7 +4431,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>106</v>
       </c>
@@ -4455,7 +4469,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>113</v>
       </c>
@@ -4493,7 +4507,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>121</v>
       </c>
@@ -4531,7 +4545,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>130</v>
       </c>
@@ -4569,7 +4583,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>138</v>
       </c>
@@ -4607,7 +4621,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>146</v>
       </c>
@@ -4645,7 +4659,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>154</v>
       </c>
@@ -4683,7 +4697,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>163</v>
       </c>
@@ -4721,7 +4735,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>171</v>
       </c>
@@ -4759,7 +4773,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>179</v>
       </c>
@@ -4797,7 +4811,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>187</v>
       </c>
@@ -4835,7 +4849,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>195</v>
       </c>
@@ -4873,7 +4887,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>203</v>
       </c>
@@ -4911,7 +4925,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>212</v>
       </c>
@@ -4949,7 +4963,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>221</v>
       </c>
@@ -4987,7 +5001,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>229</v>
       </c>
@@ -5025,7 +5039,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>237</v>
       </c>
@@ -5063,7 +5077,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>245</v>
       </c>
@@ -5101,7 +5115,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>253</v>
       </c>
@@ -5139,7 +5153,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>261</v>
       </c>
@@ -5177,7 +5191,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>269</v>
       </c>
@@ -5215,7 +5229,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>277</v>
       </c>
@@ -5253,7 +5267,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>286</v>
       </c>
@@ -5291,7 +5305,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>295</v>
       </c>
@@ -5329,7 +5343,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>303</v>
       </c>
@@ -5367,7 +5381,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>312</v>
       </c>
@@ -5405,7 +5419,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>320</v>
       </c>
@@ -5443,7 +5457,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>328</v>
       </c>
@@ -5481,7 +5495,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>337</v>
       </c>
@@ -5519,7 +5533,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>345</v>
       </c>
@@ -5557,7 +5571,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>353</v>
       </c>
@@ -5595,7 +5609,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>361</v>
       </c>
@@ -5633,7 +5647,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>369</v>
       </c>
@@ -5671,7 +5685,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>377</v>
       </c>
@@ -5709,7 +5723,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>385</v>
       </c>
@@ -5747,7 +5761,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>393</v>
       </c>
@@ -5785,7 +5799,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>401</v>
       </c>
@@ -5823,7 +5837,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>409</v>
       </c>
@@ -5861,7 +5875,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>417</v>
       </c>
@@ -5899,7 +5913,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>425</v>
       </c>
@@ -5937,7 +5951,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>433</v>
       </c>
@@ -5975,7 +5989,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>441</v>
       </c>
@@ -6013,7 +6027,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>449</v>
       </c>
@@ -6051,7 +6065,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>457</v>
       </c>
@@ -6089,7 +6103,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>465</v>
       </c>
@@ -6127,7 +6141,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>473</v>
       </c>
@@ -6165,7 +6179,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>482</v>
       </c>
@@ -6203,7 +6217,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>489</v>
       </c>
@@ -6241,7 +6255,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>497</v>
       </c>
@@ -6279,7 +6293,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>506</v>
       </c>
@@ -6317,7 +6331,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>514</v>
       </c>
@@ -6355,7 +6369,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>522</v>
       </c>
@@ -6393,7 +6407,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>531</v>
       </c>
@@ -6431,7 +6445,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>539</v>
       </c>
@@ -6469,7 +6483,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>547</v>
       </c>
@@ -6507,7 +6521,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>555</v>
       </c>
@@ -6545,7 +6559,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>563</v>
       </c>
@@ -6583,7 +6597,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>572</v>
       </c>
@@ -6621,7 +6635,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>580</v>
       </c>
@@ -6659,7 +6673,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>588</v>
       </c>
@@ -6697,7 +6711,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>596</v>
       </c>
@@ -6735,7 +6749,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>604</v>
       </c>
@@ -6773,7 +6787,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>612</v>
       </c>
@@ -6811,7 +6825,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>620</v>
       </c>
@@ -6849,7 +6863,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>629</v>
       </c>
@@ -6887,7 +6901,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>636</v>
       </c>
@@ -6925,7 +6939,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>643</v>
       </c>
@@ -6963,7 +6977,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>651</v>
       </c>
@@ -7001,7 +7015,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>659</v>
       </c>
@@ -7039,7 +7053,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>667</v>
       </c>
@@ -7077,7 +7091,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>675</v>
       </c>
@@ -7115,7 +7129,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>684</v>
       </c>
@@ -7153,7 +7167,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>691</v>
       </c>
@@ -7191,7 +7205,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>699</v>
       </c>
@@ -7229,7 +7243,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>707</v>
       </c>
@@ -7267,7 +7281,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>715</v>
       </c>
@@ -7305,7 +7319,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>723</v>
       </c>
@@ -7343,7 +7357,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>731</v>
       </c>
@@ -7381,7 +7395,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>739</v>
       </c>
@@ -7419,7 +7433,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>747</v>
       </c>
@@ -7457,7 +7471,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>755</v>
       </c>
@@ -7495,7 +7509,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>763</v>
       </c>
@@ -7533,7 +7547,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>771</v>
       </c>
@@ -7571,7 +7585,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>773</v>
       </c>
@@ -7609,7 +7623,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>781</v>
       </c>
@@ -7647,7 +7661,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>789</v>
       </c>
@@ -7685,7 +7699,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>797</v>
       </c>
@@ -7723,7 +7737,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>805</v>
       </c>
@@ -7761,7 +7775,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>813</v>
       </c>
@@ -7799,7 +7813,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>821</v>
       </c>
@@ -7837,7 +7851,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>829</v>
       </c>
@@ -7872,7 +7886,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>836</v>
       </c>
@@ -7912,7 +7926,7 @@
       <c r="M104" s="8"/>
       <c r="P104" s="1"/>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>843</v>
       </c>
@@ -7950,7 +7964,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>851</v>
       </c>
@@ -7988,7 +8002,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A107" s="2">
         <v>44518.9544328704</v>
       </c>
@@ -8026,7 +8040,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>866</v>
       </c>
@@ -8064,7 +8078,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>874</v>
       </c>
@@ -8102,7 +8116,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>883</v>
       </c>
@@ -8140,7 +8154,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>891</v>
       </c>
@@ -8178,7 +8192,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>893</v>
       </c>
@@ -8216,7 +8230,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>901</v>
       </c>
@@ -8251,7 +8265,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>903</v>
       </c>
@@ -8289,7 +8303,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>911</v>
       </c>
@@ -8327,7 +8341,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>919</v>
       </c>
@@ -8365,7 +8379,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>927</v>
       </c>
@@ -8403,7 +8417,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>934</v>
       </c>
@@ -8441,7 +8455,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>942</v>
       </c>
@@ -8479,7 +8493,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>950</v>
       </c>
@@ -8517,7 +8531,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>957</v>
       </c>
@@ -8555,7 +8569,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>965</v>
       </c>
@@ -8593,7 +8607,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>973</v>
       </c>
@@ -8628,7 +8642,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B124" t="s">
         <v>483</v>
       </c>
@@ -8663,7 +8677,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B125" t="s">
         <v>977</v>
       </c>
@@ -8689,7 +8703,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B126" t="s">
         <v>523</v>
       </c>
@@ -8712,7 +8726,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B127" t="s">
         <v>982</v>
       </c>
@@ -8752,8 +8766,8 @@
     <mergeCell ref="L104:M104"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G104" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="L104" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G104" r:id="rId1"/>
+    <hyperlink ref="L104" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -8761,23 +8775,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J117"/>
   <sheetViews>
     <sheetView topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="17.5" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" customWidth="1"/>
-    <col min="5" max="5" width="14.58203125" customWidth="1"/>
-    <col min="6" max="6" width="9.83203125" customWidth="1"/>
+    <col min="4" max="4" width="15.796875" customWidth="1"/>
+    <col min="5" max="5" width="14.59765625" customWidth="1"/>
+    <col min="6" max="6" width="9.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>990</v>
       </c>
@@ -8809,7 +8823,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>997</v>
       </c>
@@ -8841,7 +8855,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1000</v>
       </c>
@@ -8873,7 +8887,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -8905,7 +8919,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1001</v>
       </c>
@@ -8937,7 +8951,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1003</v>
       </c>
@@ -8969,7 +8983,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1004</v>
       </c>
@@ -9001,7 +9015,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1006</v>
       </c>
@@ -9033,7 +9047,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1007</v>
       </c>
@@ -9065,7 +9079,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1008</v>
       </c>
@@ -9097,7 +9111,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1009</v>
       </c>
@@ -9129,7 +9143,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1010</v>
       </c>
@@ -9161,7 +9175,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>1011</v>
       </c>
@@ -9193,7 +9207,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>1012</v>
       </c>
@@ -9225,7 +9239,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>1013</v>
       </c>
@@ -9257,7 +9271,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>1014</v>
       </c>
@@ -9289,7 +9303,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>1015</v>
       </c>
@@ -9321,7 +9335,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>1016</v>
       </c>
@@ -9353,7 +9367,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>1017</v>
       </c>
@@ -9385,7 +9399,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>1018</v>
       </c>
@@ -9417,7 +9431,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>1019</v>
       </c>
@@ -9449,7 +9463,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>1020</v>
       </c>
@@ -9481,7 +9495,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>1021</v>
       </c>
@@ -9513,7 +9527,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>1023</v>
       </c>
@@ -9545,7 +9559,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>1024</v>
       </c>
@@ -9577,7 +9591,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>1025</v>
       </c>
@@ -9609,7 +9623,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>1026</v>
       </c>
@@ -9641,7 +9655,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>1027</v>
       </c>
@@ -9673,7 +9687,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>1028</v>
       </c>
@@ -9705,7 +9719,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>1029</v>
       </c>
@@ -9737,7 +9751,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>1030</v>
       </c>
@@ -9769,7 +9783,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>1031</v>
       </c>
@@ -9801,7 +9815,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>1033</v>
       </c>
@@ -9833,7 +9847,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>1034</v>
       </c>
@@ -9865,7 +9879,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>1035</v>
       </c>
@@ -9897,7 +9911,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>1037</v>
       </c>
@@ -9929,7 +9943,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>1038</v>
       </c>
@@ -9961,7 +9975,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>1039</v>
       </c>
@@ -9993,7 +10007,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>1040</v>
       </c>
@@ -10025,7 +10039,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>1041</v>
       </c>
@@ -10057,7 +10071,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>1042</v>
       </c>
@@ -10089,7 +10103,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>1043</v>
       </c>
@@ -10121,7 +10135,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>1044</v>
       </c>
@@ -10153,7 +10167,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>1045</v>
       </c>
@@ -10185,7 +10199,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>1046</v>
       </c>
@@ -10217,7 +10231,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>1047</v>
       </c>
@@ -10249,7 +10263,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>1048</v>
       </c>
@@ -10281,7 +10295,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>1049</v>
       </c>
@@ -10313,7 +10327,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>1050</v>
       </c>
@@ -10345,7 +10359,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>1051</v>
       </c>
@@ -10377,7 +10391,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>1053</v>
       </c>
@@ -10409,7 +10423,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>1054</v>
       </c>
@@ -10441,7 +10455,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>1055</v>
       </c>
@@ -10473,7 +10487,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>1056</v>
       </c>
@@ -10505,7 +10519,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>1057</v>
       </c>
@@ -10537,7 +10551,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>1058</v>
       </c>
@@ -10569,7 +10583,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>1059</v>
       </c>
@@ -10601,7 +10615,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>1061</v>
       </c>
@@ -10633,7 +10647,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>1062</v>
       </c>
@@ -10665,7 +10679,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>1063</v>
       </c>
@@ -10697,7 +10711,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>1064</v>
       </c>
@@ -10729,7 +10743,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>1065</v>
       </c>
@@ -10761,7 +10775,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>1066</v>
       </c>
@@ -10793,7 +10807,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>1067</v>
       </c>
@@ -10825,7 +10839,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>1068</v>
       </c>
@@ -10857,7 +10871,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>1069</v>
       </c>
@@ -10889,7 +10903,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>1070</v>
       </c>
@@ -10921,7 +10935,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>1071</v>
       </c>
@@ -10953,7 +10967,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>1072</v>
       </c>
@@ -10985,7 +10999,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>1073</v>
       </c>
@@ -11017,7 +11031,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>1074</v>
       </c>
@@ -11049,7 +11063,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>1075</v>
       </c>
@@ -11081,7 +11095,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>1076</v>
       </c>
@@ -11113,7 +11127,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>1077</v>
       </c>
@@ -11145,7 +11159,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>1078</v>
       </c>
@@ -11177,7 +11191,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>1079</v>
       </c>
@@ -11209,7 +11223,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>1080</v>
       </c>
@@ -11241,7 +11255,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>1082</v>
       </c>
@@ -11273,7 +11287,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>1083</v>
       </c>
@@ -11305,7 +11319,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>1084</v>
       </c>
@@ -11337,7 +11351,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>1085</v>
       </c>
@@ -11369,7 +11383,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>1086</v>
       </c>
@@ -11401,7 +11415,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>1087</v>
       </c>
@@ -11433,7 +11447,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>1088</v>
       </c>
@@ -11465,7 +11479,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>1089</v>
       </c>
@@ -11497,7 +11511,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>1090</v>
       </c>
@@ -11529,7 +11543,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>1091</v>
       </c>
@@ -11561,7 +11575,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>1092</v>
       </c>
@@ -11593,7 +11607,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>1093</v>
       </c>
@@ -11625,7 +11639,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>1094</v>
       </c>
@@ -11657,7 +11671,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>1095</v>
       </c>
@@ -11689,7 +11703,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>1096</v>
       </c>
@@ -11721,7 +11735,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>1097</v>
       </c>
@@ -11753,7 +11767,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>1098</v>
       </c>
@@ -11785,7 +11799,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>1099</v>
       </c>
@@ -11817,7 +11831,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>1100</v>
       </c>
@@ -11849,7 +11863,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>1101</v>
       </c>
@@ -11881,7 +11895,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>1102</v>
       </c>
@@ -11913,7 +11927,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>1103</v>
       </c>
@@ -11945,7 +11959,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>1104</v>
       </c>
@@ -11977,7 +11991,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>1106</v>
       </c>
@@ -12009,7 +12023,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>1107</v>
       </c>
@@ -12038,7 +12052,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>1108</v>
       </c>
@@ -12067,7 +12081,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>1112</v>
       </c>
@@ -12099,7 +12113,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>1114</v>
       </c>
@@ -12131,7 +12145,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>1115</v>
       </c>
@@ -12163,7 +12177,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>1117</v>
       </c>
@@ -12195,7 +12209,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>1118</v>
       </c>
@@ -12227,7 +12241,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>1119</v>
       </c>
@@ -12259,7 +12273,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>1120</v>
       </c>
@@ -12291,7 +12305,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>1121</v>
       </c>
@@ -12320,7 +12334,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>1122</v>
       </c>
@@ -12352,7 +12366,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>1125</v>
       </c>
@@ -12384,7 +12398,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>1133</v>
       </c>
@@ -12416,7 +12430,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>1134</v>
       </c>
@@ -12448,7 +12462,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>117</v>
       </c>
@@ -12482,7 +12496,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G117" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="G117" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -12490,26 +12504,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J116"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E110" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J118" sqref="J118"/>
+    <sheetView tabSelected="1" topLeftCell="A102" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="8.5" style="9"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="16.5" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="9.83203125" customWidth="1"/>
-    <col min="7" max="7" width="29.25" style="5" customWidth="1"/>
-    <col min="9" max="9" width="17.08203125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="30.25" style="5" customWidth="1"/>
+    <col min="5" max="5" width="16.5" customWidth="1"/>
+    <col min="7" max="7" width="32" style="5" customWidth="1"/>
+    <col min="9" max="9" width="17.09765625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="33.8984375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
         <v>990</v>
       </c>
       <c r="B1" t="s">
@@ -12540,8 +12555,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>997</v>
       </c>
       <c r="B2" t="s">
@@ -12572,8 +12587,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
         <v>1000</v>
       </c>
       <c r="B3" t="s">
@@ -12604,8 +12619,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
         <v>21</v>
       </c>
       <c r="B4" t="s">
@@ -12636,8 +12651,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
         <v>1001</v>
       </c>
       <c r="B5" t="s">
@@ -12668,8 +12683,8 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
         <v>1003</v>
       </c>
       <c r="B6" t="s">
@@ -12700,8 +12715,8 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
         <v>1004</v>
       </c>
       <c r="B7" t="s">
@@ -12732,8 +12747,8 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
         <v>1006</v>
       </c>
       <c r="B8" t="s">
@@ -12764,8 +12779,8 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
         <v>1007</v>
       </c>
       <c r="B9" t="s">
@@ -12796,8 +12811,8 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
         <v>1008</v>
       </c>
       <c r="B10" t="s">
@@ -12828,8 +12843,8 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
         <v>1009</v>
       </c>
       <c r="B11" t="s">
@@ -12860,8 +12875,8 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="31" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    <row r="12" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
         <v>1010</v>
       </c>
       <c r="B12" t="s">
@@ -12892,8 +12907,8 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
         <v>1011</v>
       </c>
       <c r="B13" t="s">
@@ -12924,8 +12939,8 @@
         <v>129</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
         <v>1012</v>
       </c>
       <c r="B14" t="s">
@@ -12956,8 +12971,8 @@
         <v>137</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
         <v>1013</v>
       </c>
       <c r="B15" t="s">
@@ -12988,8 +13003,8 @@
         <v>145</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
         <v>1014</v>
       </c>
       <c r="B16" t="s">
@@ -13020,8 +13035,8 @@
         <v>153</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
         <v>1015</v>
       </c>
       <c r="B17" t="s">
@@ -13052,8 +13067,8 @@
         <v>162</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+    <row r="18" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
         <v>1016</v>
       </c>
       <c r="B18" t="s">
@@ -13084,8 +13099,8 @@
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
         <v>1017</v>
       </c>
       <c r="B19" t="s">
@@ -13116,8 +13131,8 @@
         <v>178</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
         <v>1018</v>
       </c>
       <c r="B20" t="s">
@@ -13148,8 +13163,8 @@
         <v>194</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="9" t="s">
         <v>1019</v>
       </c>
       <c r="B21" t="s">
@@ -13180,8 +13195,8 @@
         <v>202</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
         <v>1020</v>
       </c>
       <c r="B22" t="s">
@@ -13212,8 +13227,8 @@
         <v>211</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="9" t="s">
         <v>1021</v>
       </c>
       <c r="B23" t="s">
@@ -13244,8 +13259,8 @@
         <v>220</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="31" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+    <row r="24" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
         <v>1023</v>
       </c>
       <c r="B24" t="s">
@@ -13276,8 +13291,8 @@
         <v>228</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="9" t="s">
         <v>1024</v>
       </c>
       <c r="B25" t="s">
@@ -13308,8 +13323,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="9" t="s">
         <v>1025</v>
       </c>
       <c r="B26" t="s">
@@ -13340,8 +13355,8 @@
         <v>260</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="9" t="s">
         <v>1026</v>
       </c>
       <c r="B27" t="s">
@@ -13372,8 +13387,8 @@
         <v>268</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+    <row r="28" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="9" t="s">
         <v>1027</v>
       </c>
       <c r="B28" t="s">
@@ -13404,8 +13419,8 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="31" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+    <row r="29" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="9" t="s">
         <v>1028</v>
       </c>
       <c r="B29" t="s">
@@ -13436,8 +13451,8 @@
         <v>285</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="31" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+    <row r="30" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="9" t="s">
         <v>1029</v>
       </c>
       <c r="B30" t="s">
@@ -13468,8 +13483,8 @@
         <v>294</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="9" t="s">
         <v>1030</v>
       </c>
       <c r="B31" t="s">
@@ -13500,8 +13515,8 @@
         <v>302</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="9" t="s">
         <v>1031</v>
       </c>
       <c r="B32" t="s">
@@ -13532,8 +13547,8 @@
         <v>311</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="9" t="s">
         <v>1033</v>
       </c>
       <c r="B33" t="s">
@@ -13564,8 +13579,8 @@
         <v>319</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="9" t="s">
         <v>1034</v>
       </c>
       <c r="B34" t="s">
@@ -13596,8 +13611,8 @@
         <v>327</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="9" t="s">
         <v>1035</v>
       </c>
       <c r="B35" t="s">
@@ -13628,8 +13643,8 @@
         <v>336</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="9" t="s">
         <v>1037</v>
       </c>
       <c r="B36" t="s">
@@ -13660,8 +13675,8 @@
         <v>344</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="9" t="s">
         <v>1038</v>
       </c>
       <c r="B37" t="s">
@@ -13692,8 +13707,8 @@
         <v>360</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+    <row r="38" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A38" s="9" t="s">
         <v>1039</v>
       </c>
       <c r="B38" t="s">
@@ -13724,8 +13739,8 @@
         <v>368</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="31" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+    <row r="39" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A39" s="9" t="s">
         <v>1040</v>
       </c>
       <c r="B39" t="s">
@@ -13756,8 +13771,8 @@
         <v>384</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" s="9" t="s">
         <v>1041</v>
       </c>
       <c r="B40" t="s">
@@ -13788,8 +13803,8 @@
         <v>392</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+    <row r="41" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A41" s="9" t="s">
         <v>1042</v>
       </c>
       <c r="B41" t="s">
@@ -13820,8 +13835,8 @@
         <v>400</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" s="9" t="s">
         <v>1043</v>
       </c>
       <c r="B42" t="s">
@@ -13852,8 +13867,8 @@
         <v>408</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" s="9" t="s">
         <v>1044</v>
       </c>
       <c r="B43" t="s">
@@ -13884,8 +13899,8 @@
         <v>416</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" s="9" t="s">
         <v>1045</v>
       </c>
       <c r="B44" t="s">
@@ -13916,8 +13931,8 @@
         <v>432</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" s="9" t="s">
         <v>1046</v>
       </c>
       <c r="B45" t="s">
@@ -13948,8 +13963,8 @@
         <v>440</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" s="9" t="s">
         <v>1047</v>
       </c>
       <c r="B46" t="s">
@@ -13980,8 +13995,8 @@
         <v>456</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" s="9" t="s">
         <v>1048</v>
       </c>
       <c r="B47" t="s">
@@ -14012,8 +14027,8 @@
         <v>464</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" s="9" t="s">
         <v>1049</v>
       </c>
       <c r="B48" t="s">
@@ -14044,8 +14059,8 @@
         <v>472</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49" s="9" t="s">
         <v>1050</v>
       </c>
       <c r="B49" t="s">
@@ -14076,8 +14091,8 @@
         <v>481</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50" s="9" t="s">
         <v>1051</v>
       </c>
       <c r="B50" t="s">
@@ -14108,8 +14123,8 @@
         <v>488</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51" s="9" t="s">
         <v>1053</v>
       </c>
       <c r="B51" t="s">
@@ -14140,8 +14155,8 @@
         <v>496</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52" s="9" t="s">
         <v>1054</v>
       </c>
       <c r="B52" t="s">
@@ -14172,8 +14187,8 @@
         <v>505</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="31" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
+    <row r="53" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A53" s="9" t="s">
         <v>1055</v>
       </c>
       <c r="B53" t="s">
@@ -14204,8 +14219,8 @@
         <v>513</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A54" s="9" t="s">
         <v>1056</v>
       </c>
       <c r="B54" t="s">
@@ -14236,8 +14251,8 @@
         <v>521</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A55" s="9" t="s">
         <v>1057</v>
       </c>
       <c r="B55" t="s">
@@ -14268,8 +14283,8 @@
         <v>530</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A56" s="9" t="s">
         <v>1058</v>
       </c>
       <c r="B56" t="s">
@@ -14300,8 +14315,8 @@
         <v>538</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A57" s="9" t="s">
         <v>1059</v>
       </c>
       <c r="B57" t="s">
@@ -14332,8 +14347,8 @@
         <v>546</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A58" s="9" t="s">
         <v>1061</v>
       </c>
       <c r="B58" t="s">
@@ -14364,8 +14379,8 @@
         <v>554</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A59" s="9" t="s">
         <v>1062</v>
       </c>
       <c r="B59" t="s">
@@ -14396,8 +14411,8 @@
         <v>562</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A60" s="9" t="s">
         <v>1063</v>
       </c>
       <c r="B60" t="s">
@@ -14428,8 +14443,8 @@
         <v>571</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A61" s="9" t="s">
         <v>1064</v>
       </c>
       <c r="B61" t="s">
@@ -14460,8 +14475,8 @@
         <v>587</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A62" s="9" t="s">
         <v>1065</v>
       </c>
       <c r="B62" t="s">
@@ -14492,8 +14507,8 @@
         <v>595</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="31" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
+    <row r="63" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A63" s="9" t="s">
         <v>1066</v>
       </c>
       <c r="B63" t="s">
@@ -14524,8 +14539,8 @@
         <v>603</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="31" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
+    <row r="64" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A64" s="9" t="s">
         <v>1067</v>
       </c>
       <c r="B64" t="s">
@@ -14556,8 +14571,8 @@
         <v>619</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A65" s="9" t="s">
         <v>1068</v>
       </c>
       <c r="B65" t="s">
@@ -14588,8 +14603,8 @@
         <v>628</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="31" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
+    <row r="66" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A66" s="9" t="s">
         <v>1069</v>
       </c>
       <c r="B66" t="s">
@@ -14620,8 +14635,8 @@
         <v>635</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
+    <row r="67" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A67" s="9" t="s">
         <v>1070</v>
       </c>
       <c r="B67" t="s">
@@ -14652,8 +14667,8 @@
         <v>642</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A68" s="9" t="s">
         <v>1071</v>
       </c>
       <c r="B68" t="s">
@@ -14684,8 +14699,8 @@
         <v>650</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A69" s="9" t="s">
         <v>1072</v>
       </c>
       <c r="B69" t="s">
@@ -14716,8 +14731,8 @@
         <v>658</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A70" s="9" t="s">
         <v>1073</v>
       </c>
       <c r="B70" t="s">
@@ -14748,8 +14763,8 @@
         <v>674</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
+    <row r="71" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A71" s="9" t="s">
         <v>1074</v>
       </c>
       <c r="B71" t="s">
@@ -14780,8 +14795,8 @@
         <v>683</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A72" s="9" t="s">
         <v>1075</v>
       </c>
       <c r="B72" t="s">
@@ -14812,8 +14827,8 @@
         <v>690</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A73" s="9" t="s">
         <v>1076</v>
       </c>
       <c r="B73" t="s">
@@ -14844,8 +14859,8 @@
         <v>698</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A74" s="9" t="s">
         <v>1077</v>
       </c>
       <c r="B74" t="s">
@@ -14876,8 +14891,8 @@
         <v>706</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="31" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
+    <row r="75" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A75" s="9" t="s">
         <v>1078</v>
       </c>
       <c r="B75" t="s">
@@ -14908,8 +14923,8 @@
         <v>714</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A76" s="9" t="s">
         <v>1079</v>
       </c>
       <c r="B76" t="s">
@@ -14940,8 +14955,8 @@
         <v>722</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A77" s="9" t="s">
         <v>1080</v>
       </c>
       <c r="B77" t="s">
@@ -14972,8 +14987,8 @@
         <v>730</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A78" s="9" t="s">
         <v>1082</v>
       </c>
       <c r="B78" t="s">
@@ -15004,8 +15019,8 @@
         <v>738</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A79" t="s">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A79" s="9" t="s">
         <v>1083</v>
       </c>
       <c r="B79" t="s">
@@ -15036,8 +15051,8 @@
         <v>746</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A80" t="s">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A80" s="9" t="s">
         <v>1084</v>
       </c>
       <c r="B80" t="s">
@@ -15068,8 +15083,8 @@
         <v>762</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="31" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
+    <row r="81" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A81" s="9" t="s">
         <v>1085</v>
       </c>
       <c r="B81" t="s">
@@ -15100,8 +15115,8 @@
         <v>780</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="31" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
+    <row r="82" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A82" s="9" t="s">
         <v>1086</v>
       </c>
       <c r="B82" t="s">
@@ -15132,8 +15147,8 @@
         <v>788</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A83" t="s">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A83" s="9" t="s">
         <v>1087</v>
       </c>
       <c r="B83" t="s">
@@ -15164,8 +15179,8 @@
         <v>796</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A84" s="9" t="s">
         <v>1088</v>
       </c>
       <c r="B84" t="s">
@@ -15196,8 +15211,8 @@
         <v>804</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A85" s="9" t="s">
         <v>1089</v>
       </c>
       <c r="B85" t="s">
@@ -15228,8 +15243,8 @@
         <v>812</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A86" t="s">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A86" s="9" t="s">
         <v>1090</v>
       </c>
       <c r="B86" t="s">
@@ -15260,8 +15275,8 @@
         <v>820</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A87" t="s">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A87" s="9" t="s">
         <v>1091</v>
       </c>
       <c r="B87" t="s">
@@ -15292,8 +15307,8 @@
         <v>828</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="31" x14ac:dyDescent="0.35">
-      <c r="A88" t="s">
+    <row r="88" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A88" s="9" t="s">
         <v>1092</v>
       </c>
       <c r="B88" t="s">
@@ -15321,8 +15336,8 @@
         <v>835</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A89" t="s">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A89" s="9" t="s">
         <v>1093</v>
       </c>
       <c r="B89" t="s">
@@ -15350,8 +15365,8 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A90" t="s">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A90" s="9" t="s">
         <v>1094</v>
       </c>
       <c r="B90" t="s">
@@ -15382,8 +15397,8 @@
         <v>850</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A91" t="s">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A91" s="9" t="s">
         <v>1095</v>
       </c>
       <c r="B91" t="s">
@@ -15414,8 +15429,8 @@
         <v>858</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="31" x14ac:dyDescent="0.35">
-      <c r="A92" t="s">
+    <row r="92" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A92" s="9" t="s">
         <v>1096</v>
       </c>
       <c r="B92" t="s">
@@ -15446,8 +15461,8 @@
         <v>865</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A93" t="s">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A93" s="9" t="s">
         <v>1097</v>
       </c>
       <c r="B93" t="s">
@@ -15478,8 +15493,8 @@
         <v>873</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="31" x14ac:dyDescent="0.35">
-      <c r="A94" t="s">
+    <row r="94" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A94" s="9" t="s">
         <v>1098</v>
       </c>
       <c r="B94" t="s">
@@ -15510,8 +15525,8 @@
         <v>882</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A95" t="s">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A95" s="9" t="s">
         <v>1099</v>
       </c>
       <c r="B95" t="s">
@@ -15542,8 +15557,8 @@
         <v>890</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A96" t="s">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A96" s="9" t="s">
         <v>1100</v>
       </c>
       <c r="B96" t="s">
@@ -15574,8 +15589,8 @@
         <v>730</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A97" t="s">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A97" s="9" t="s">
         <v>1101</v>
       </c>
       <c r="B97" t="s">
@@ -15606,8 +15621,8 @@
         <v>900</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A98" t="s">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A98" s="9" t="s">
         <v>1102</v>
       </c>
       <c r="B98" t="s">
@@ -15635,8 +15650,8 @@
         <v>285</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A99" t="s">
+    <row r="99" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A99" s="9" t="s">
         <v>1103</v>
       </c>
       <c r="B99" t="s">
@@ -15667,8 +15682,8 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="31" x14ac:dyDescent="0.35">
-      <c r="A100" t="s">
+    <row r="100" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="9" t="s">
         <v>1104</v>
       </c>
       <c r="B100" t="s">
@@ -15699,8 +15714,8 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A101" t="s">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A101" s="9" t="s">
         <v>1106</v>
       </c>
       <c r="B101" t="s">
@@ -15731,8 +15746,8 @@
         <v>910</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A102" t="s">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A102" s="9" t="s">
         <v>1107</v>
       </c>
       <c r="B102" t="s">
@@ -15763,8 +15778,8 @@
         <v>918</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A103" t="s">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A103" s="9" t="s">
         <v>1108</v>
       </c>
       <c r="B103" t="s">
@@ -15795,8 +15810,8 @@
         <v>926</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A104" t="s">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A104" s="9" t="s">
         <v>1112</v>
       </c>
       <c r="B104" t="s">
@@ -15827,8 +15842,8 @@
         <v>933</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A105" t="s">
+    <row r="105" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="9" t="s">
         <v>1114</v>
       </c>
       <c r="B105" t="s">
@@ -15859,8 +15874,8 @@
         <v>941</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A106" t="s">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A106" s="9" t="s">
         <v>1115</v>
       </c>
       <c r="B106" t="s">
@@ -15891,8 +15906,8 @@
         <v>949</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A107" t="s">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A107" s="9" t="s">
         <v>1117</v>
       </c>
       <c r="B107" t="s">
@@ -15923,8 +15938,8 @@
         <v>956</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A108" t="s">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A108" s="9" t="s">
         <v>1118</v>
       </c>
       <c r="B108" t="s">
@@ -15955,8 +15970,8 @@
         <v>964</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A109" t="s">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A109" s="9" t="s">
         <v>1119</v>
       </c>
       <c r="B109" t="s">
@@ -15987,8 +16002,8 @@
         <v>972</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A110" t="s">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A110" s="9" t="s">
         <v>1150</v>
       </c>
       <c r="B110" t="s">
@@ -16019,8 +16034,8 @@
         <v>989</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A111" t="s">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A111" s="9" t="s">
         <v>1120</v>
       </c>
       <c r="B111" t="s">
@@ -16051,8 +16066,8 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="31" x14ac:dyDescent="0.35">
-      <c r="A112" t="s">
+    <row r="112" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="9" t="s">
         <v>1121</v>
       </c>
       <c r="B112" t="s">
@@ -16083,8 +16098,8 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A114">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A114" s="9">
         <v>113</v>
       </c>
       <c r="B114" t="s">
@@ -16115,8 +16130,8 @@
         <v>1147</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A115">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A115" s="9">
         <v>114</v>
       </c>
       <c r="B115" t="s">
@@ -16147,8 +16162,8 @@
         <v>120</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A116">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A116" s="9">
         <v>115</v>
       </c>
       <c r="B116" t="s">
@@ -16177,20 +16192,47 @@
       </c>
       <c r="J116" s="7" t="s">
         <v>1179</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A117" s="9">
+        <v>116</v>
+      </c>
+      <c r="B117" t="s">
+        <v>1180</v>
+      </c>
+      <c r="C117" t="s">
+        <v>1181</v>
+      </c>
+      <c r="D117" t="s">
+        <v>1182</v>
+      </c>
+      <c r="E117">
+        <v>765279045</v>
+      </c>
+      <c r="G117" s="7" t="s">
+        <v>1183</v>
+      </c>
+      <c r="H117" t="s">
+        <v>1002</v>
+      </c>
+      <c r="I117" s="5" t="s">
+        <v>1181</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="G114" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="G59" r:id="rId2" xr:uid="{8AD43A06-3CFA-4E13-A776-A2195F019507}"/>
-    <hyperlink ref="J59" r:id="rId3" xr:uid="{C4FF8B53-949E-46D7-A9DD-C552A2CA3857}"/>
-    <hyperlink ref="G115" r:id="rId4" xr:uid="{C76D56C7-8B8E-4D40-8F05-2B8C526A3873}"/>
-    <hyperlink ref="J115" r:id="rId5" xr:uid="{8FD24C44-7E7B-4DE6-A4C7-66BE611A505A}"/>
-    <hyperlink ref="G116" r:id="rId6" xr:uid="{99BC76D9-F434-42B6-BB62-184EB8365519}"/>
-    <hyperlink ref="J116" r:id="rId7" xr:uid="{EBA2F8D3-BEE8-4CE0-AD83-C7E780260833}"/>
+    <hyperlink ref="G114" r:id="rId1"/>
+    <hyperlink ref="G59" r:id="rId2"/>
+    <hyperlink ref="J59" r:id="rId3"/>
+    <hyperlink ref="G115" r:id="rId4"/>
+    <hyperlink ref="J115" r:id="rId5"/>
+    <hyperlink ref="G116" r:id="rId6"/>
+    <hyperlink ref="J116" r:id="rId7"/>
+    <hyperlink ref="G117" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added number and info
</commit_message>
<xml_diff>
--- a/CS335/GitHub Info sans duplicates.xlsx
+++ b/CS335/GitHub Info sans duplicates.xlsx
@@ -3641,11 +3641,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="yyyy/mm/dd\ h:mm"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -3680,7 +3680,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3691,6 +3691,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -3705,17 +3721,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3752,14 +3768,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -3767,9 +3775,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3792,13 +3799,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -3806,7 +3806,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3821,7 +3821,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3833,55 +3905,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3893,19 +3923,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3917,25 +3935,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3947,31 +3947,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3989,19 +3971,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4019,6 +4019,17 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -4078,17 +4089,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -4115,146 +4115,146 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -13144,8 +13144,8 @@
   <sheetPr/>
   <dimension ref="A1:J122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B114" workbookViewId="0">
-      <selection activeCell="J124" sqref="J124"/>
+    <sheetView tabSelected="1" topLeftCell="B105" workbookViewId="0">
+      <selection activeCell="G122" sqref="G122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.75"/>
@@ -17005,7 +17005,7 @@
         <v>758286451</v>
       </c>
       <c r="F122" t="s">
-        <v>998</v>
+        <v>17</v>
       </c>
       <c r="G122" s="2" t="s">
         <v>752</v>

</xml_diff>

<commit_message>
Added a second number
</commit_message>
<xml_diff>
--- a/CS335/GitHub Info sans duplicates.xlsx
+++ b/CS335/GitHub Info sans duplicates.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jarvis Rwabuyongo\staffcard\CS335\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A3962D-7A65-473C-9E7C-86B0BFBAD3C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="20475" windowHeight="8415" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3849" uniqueCount="1206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3849" uniqueCount="1207">
   <si>
     <t>Timestamp</t>
   </si>
@@ -3634,20 +3640,19 @@
   </si>
   <si>
     <t>Machuche M</t>
+  </si>
+  <si>
+    <t>+255764014746</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="yyyy/mm/dd\ h:mm"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy/mm/dd\ h:mm"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -3669,344 +3674,21 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -4014,324 +3696,43 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -4589,26 +3990,26 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P127"/>
   <sheetViews>
     <sheetView topLeftCell="A115" workbookViewId="0">
       <selection activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
     <col min="5" max="5" width="9.875" customWidth="1"/>
     <col min="11" max="11" width="9.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4646,7 +4047,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -4684,7 +4085,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -4722,7 +4123,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -4760,7 +4161,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -4798,7 +4199,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -4836,7 +4237,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -4874,7 +4275,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>65</v>
       </c>
@@ -4912,7 +4313,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>74</v>
       </c>
@@ -4950,7 +4351,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>82</v>
       </c>
@@ -4988,7 +4389,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>90</v>
       </c>
@@ -5026,7 +4427,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>98</v>
       </c>
@@ -5064,7 +4465,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>106</v>
       </c>
@@ -5102,7 +4503,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>113</v>
       </c>
@@ -5140,7 +4541,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>121</v>
       </c>
@@ -5178,7 +4579,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>130</v>
       </c>
@@ -5216,7 +4617,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>138</v>
       </c>
@@ -5254,7 +4655,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>146</v>
       </c>
@@ -5292,7 +4693,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>154</v>
       </c>
@@ -5330,7 +4731,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>163</v>
       </c>
@@ -5368,7 +4769,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>171</v>
       </c>
@@ -5406,7 +4807,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>179</v>
       </c>
@@ -5444,7 +4845,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>187</v>
       </c>
@@ -5482,7 +4883,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>195</v>
       </c>
@@ -5520,7 +4921,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>203</v>
       </c>
@@ -5558,7 +4959,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>212</v>
       </c>
@@ -5596,7 +4997,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>221</v>
       </c>
@@ -5634,7 +5035,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>229</v>
       </c>
@@ -5672,7 +5073,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>237</v>
       </c>
@@ -5710,7 +5111,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>245</v>
       </c>
@@ -5748,7 +5149,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>253</v>
       </c>
@@ -5786,7 +5187,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>261</v>
       </c>
@@ -5824,7 +5225,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>269</v>
       </c>
@@ -5862,7 +5263,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>277</v>
       </c>
@@ -5900,7 +5301,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>286</v>
       </c>
@@ -5938,7 +5339,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>295</v>
       </c>
@@ -5976,7 +5377,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>303</v>
       </c>
@@ -6014,7 +5415,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>312</v>
       </c>
@@ -6052,7 +5453,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>320</v>
       </c>
@@ -6090,7 +5491,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>328</v>
       </c>
@@ -6128,7 +5529,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>337</v>
       </c>
@@ -6166,7 +5567,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>345</v>
       </c>
@@ -6204,7 +5605,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>353</v>
       </c>
@@ -6242,7 +5643,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>361</v>
       </c>
@@ -6280,7 +5681,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>369</v>
       </c>
@@ -6318,7 +5719,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>377</v>
       </c>
@@ -6356,7 +5757,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>385</v>
       </c>
@@ -6394,7 +5795,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>393</v>
       </c>
@@ -6432,7 +5833,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>401</v>
       </c>
@@ -6470,7 +5871,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="50" spans="1:12">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>409</v>
       </c>
@@ -6508,7 +5909,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>417</v>
       </c>
@@ -6546,7 +5947,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="52" spans="1:12">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>425</v>
       </c>
@@ -6584,7 +5985,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="53" spans="1:12">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>433</v>
       </c>
@@ -6622,7 +6023,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="54" spans="1:12">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>441</v>
       </c>
@@ -6660,7 +6061,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="55" spans="1:12">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>449</v>
       </c>
@@ -6698,7 +6099,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="56" spans="1:12">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>457</v>
       </c>
@@ -6736,7 +6137,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="57" spans="1:12">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>465</v>
       </c>
@@ -6774,7 +6175,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="58" spans="1:12">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>473</v>
       </c>
@@ -6812,7 +6213,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="59" spans="1:12">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>482</v>
       </c>
@@ -6850,7 +6251,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="60" spans="1:12">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>489</v>
       </c>
@@ -6888,7 +6289,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="61" spans="1:12">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>497</v>
       </c>
@@ -6926,7 +6327,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="62" spans="1:12">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>506</v>
       </c>
@@ -6964,7 +6365,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="63" spans="1:12">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>514</v>
       </c>
@@ -7002,7 +6403,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="64" spans="1:12">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>522</v>
       </c>
@@ -7040,7 +6441,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="65" spans="1:12">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>531</v>
       </c>
@@ -7078,7 +6479,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="66" spans="1:12">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>539</v>
       </c>
@@ -7116,7 +6517,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="67" spans="1:12">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>547</v>
       </c>
@@ -7154,7 +6555,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="68" spans="1:12">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>555</v>
       </c>
@@ -7192,7 +6593,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="69" spans="1:12">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>563</v>
       </c>
@@ -7230,7 +6631,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="70" spans="1:12">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>572</v>
       </c>
@@ -7268,7 +6669,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="71" spans="1:12">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>580</v>
       </c>
@@ -7306,7 +6707,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="72" spans="1:12">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>588</v>
       </c>
@@ -7344,7 +6745,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="73" spans="1:12">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>596</v>
       </c>
@@ -7382,7 +6783,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="74" spans="1:12">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>604</v>
       </c>
@@ -7420,7 +6821,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="75" spans="1:12">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>612</v>
       </c>
@@ -7458,7 +6859,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="76" spans="1:12">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>620</v>
       </c>
@@ -7496,7 +6897,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="77" spans="1:12">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>629</v>
       </c>
@@ -7534,7 +6935,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="78" spans="1:12">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>636</v>
       </c>
@@ -7572,7 +6973,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="79" spans="1:12">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>643</v>
       </c>
@@ -7610,7 +7011,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="80" spans="1:12">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>651</v>
       </c>
@@ -7648,7 +7049,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="81" spans="1:12">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>659</v>
       </c>
@@ -7686,7 +7087,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="82" spans="1:12">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>667</v>
       </c>
@@ -7724,7 +7125,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="83" spans="1:12">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>675</v>
       </c>
@@ -7762,7 +7163,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="84" spans="1:12">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>684</v>
       </c>
@@ -7800,7 +7201,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="85" spans="1:12">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>691</v>
       </c>
@@ -7838,7 +7239,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="86" spans="1:12">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>699</v>
       </c>
@@ -7876,7 +7277,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="87" spans="1:12">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>707</v>
       </c>
@@ -7914,7 +7315,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="88" spans="1:12">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>715</v>
       </c>
@@ -7952,7 +7353,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="89" spans="1:12">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>723</v>
       </c>
@@ -7990,7 +7391,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="90" spans="1:12">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>731</v>
       </c>
@@ -8028,7 +7429,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="91" spans="1:12">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>739</v>
       </c>
@@ -8066,7 +7467,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="92" spans="1:12">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>747</v>
       </c>
@@ -8104,7 +7505,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="93" spans="1:12">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>755</v>
       </c>
@@ -8142,7 +7543,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="94" spans="1:12">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>763</v>
       </c>
@@ -8180,7 +7581,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="95" spans="1:12">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>771</v>
       </c>
@@ -8218,7 +7619,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="96" spans="1:12">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>773</v>
       </c>
@@ -8256,7 +7657,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="97" spans="1:12">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>781</v>
       </c>
@@ -8294,7 +7695,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="98" spans="1:12">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>789</v>
       </c>
@@ -8332,7 +7733,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="99" spans="1:12">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>797</v>
       </c>
@@ -8370,7 +7771,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="100" spans="1:12">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>805</v>
       </c>
@@ -8408,7 +7809,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="101" spans="1:12">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>813</v>
       </c>
@@ -8446,7 +7847,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="102" spans="1:12">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>821</v>
       </c>
@@ -8484,7 +7885,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="103" spans="1:12">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>829</v>
       </c>
@@ -8519,7 +7920,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="104" spans="1:16">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>836</v>
       </c>
@@ -8553,13 +7954,13 @@
       <c r="K104" t="s">
         <v>841</v>
       </c>
-      <c r="L104" s="9" t="s">
+      <c r="L104" s="10" t="s">
         <v>842</v>
       </c>
-      <c r="M104" s="9"/>
+      <c r="M104" s="10"/>
       <c r="P104" s="7"/>
     </row>
-    <row r="105" spans="1:12">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>843</v>
       </c>
@@ -8597,7 +7998,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="106" spans="1:12">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>851</v>
       </c>
@@ -8635,7 +8036,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="107" spans="1:12">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" s="8">
         <v>44518.9544328704</v>
       </c>
@@ -8673,7 +8074,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="108" spans="1:12">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>866</v>
       </c>
@@ -8711,7 +8112,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="109" spans="1:12">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>874</v>
       </c>
@@ -8749,7 +8150,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="110" spans="1:12">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>883</v>
       </c>
@@ -8787,7 +8188,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="111" spans="1:12">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>891</v>
       </c>
@@ -8825,7 +8226,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="112" spans="1:12">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>893</v>
       </c>
@@ -8863,7 +8264,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="113" spans="1:12">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>901</v>
       </c>
@@ -8898,7 +8299,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="114" spans="1:12">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>903</v>
       </c>
@@ -8936,7 +8337,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="115" spans="1:12">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>911</v>
       </c>
@@ -8974,7 +8375,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="116" spans="1:12">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>919</v>
       </c>
@@ -9012,7 +8413,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="117" spans="1:12">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>927</v>
       </c>
@@ -9050,7 +8451,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="118" spans="1:12">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>934</v>
       </c>
@@ -9088,7 +8489,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="119" spans="1:12">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>942</v>
       </c>
@@ -9126,7 +8527,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="120" spans="1:12">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>950</v>
       </c>
@@ -9164,7 +8565,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="121" spans="1:12">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>957</v>
       </c>
@@ -9202,7 +8603,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="122" spans="1:12">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>965</v>
       </c>
@@ -9240,7 +8641,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="123" spans="1:12">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>973</v>
       </c>
@@ -9275,7 +8676,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="124" spans="2:12">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
         <v>483</v>
       </c>
@@ -9310,7 +8711,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="125" spans="2:9">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
         <v>977</v>
       </c>
@@ -9336,7 +8737,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="126" spans="2:8">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>523</v>
       </c>
@@ -9359,7 +8760,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="127" spans="2:12">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
         <v>982</v>
       </c>
@@ -9399,25 +8800,23 @@
     <mergeCell ref="L104:M104"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G104" r:id="rId1" display="joaneliamuganda@gmail.com"/>
-    <hyperlink ref="L104" r:id="rId2" display="https://github.com/Joannah123"/>
+    <hyperlink ref="G104" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="L104" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="17.5" customWidth="1"/>
@@ -9426,7 +8825,7 @@
     <col min="6" max="6" width="9.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>990</v>
       </c>
@@ -9458,7 +8857,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>997</v>
       </c>
@@ -9490,7 +8889,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1000</v>
       </c>
@@ -9522,7 +8921,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -9554,7 +8953,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1001</v>
       </c>
@@ -9586,7 +8985,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1003</v>
       </c>
@@ -9618,7 +9017,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1004</v>
       </c>
@@ -9650,7 +9049,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1006</v>
       </c>
@@ -9682,7 +9081,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1007</v>
       </c>
@@ -9714,7 +9113,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1008</v>
       </c>
@@ -9746,7 +9145,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1009</v>
       </c>
@@ -9778,7 +9177,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1010</v>
       </c>
@@ -9810,7 +9209,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1011</v>
       </c>
@@ -9842,7 +9241,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1012</v>
       </c>
@@ -9874,7 +9273,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>1013</v>
       </c>
@@ -9906,7 +9305,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1014</v>
       </c>
@@ -9938,7 +9337,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1015</v>
       </c>
@@ -9970,7 +9369,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>1016</v>
       </c>
@@ -10002,7 +9401,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>1017</v>
       </c>
@@ -10034,7 +9433,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>1018</v>
       </c>
@@ -10066,7 +9465,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>1019</v>
       </c>
@@ -10098,7 +9497,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>1020</v>
       </c>
@@ -10130,7 +9529,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>1021</v>
       </c>
@@ -10162,7 +9561,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>1023</v>
       </c>
@@ -10194,7 +9593,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>1024</v>
       </c>
@@ -10226,7 +9625,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>1025</v>
       </c>
@@ -10258,7 +9657,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>1026</v>
       </c>
@@ -10290,7 +9689,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>1027</v>
       </c>
@@ -10322,7 +9721,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>1028</v>
       </c>
@@ -10354,7 +9753,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>1029</v>
       </c>
@@ -10386,7 +9785,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>1030</v>
       </c>
@@ -10418,7 +9817,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>1031</v>
       </c>
@@ -10450,7 +9849,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>1033</v>
       </c>
@@ -10482,7 +9881,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>1034</v>
       </c>
@@ -10514,7 +9913,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>1035</v>
       </c>
@@ -10546,7 +9945,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>1037</v>
       </c>
@@ -10578,7 +9977,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>1038</v>
       </c>
@@ -10610,7 +10009,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>1039</v>
       </c>
@@ -10642,7 +10041,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>1040</v>
       </c>
@@ -10674,7 +10073,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>1041</v>
       </c>
@@ -10706,7 +10105,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>1042</v>
       </c>
@@ -10738,7 +10137,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>1043</v>
       </c>
@@ -10770,7 +10169,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>1044</v>
       </c>
@@ -10802,7 +10201,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>1045</v>
       </c>
@@ -10834,7 +10233,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>1046</v>
       </c>
@@ -10866,7 +10265,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>1047</v>
       </c>
@@ -10898,7 +10297,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>1048</v>
       </c>
@@ -10930,7 +10329,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>1049</v>
       </c>
@@ -10962,7 +10361,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>1050</v>
       </c>
@@ -10994,7 +10393,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>1051</v>
       </c>
@@ -11026,7 +10425,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>1053</v>
       </c>
@@ -11058,7 +10457,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>1054</v>
       </c>
@@ -11090,7 +10489,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>1055</v>
       </c>
@@ -11122,7 +10521,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>1056</v>
       </c>
@@ -11154,7 +10553,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>1057</v>
       </c>
@@ -11186,7 +10585,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>1058</v>
       </c>
@@ -11218,7 +10617,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>1059</v>
       </c>
@@ -11250,7 +10649,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>1061</v>
       </c>
@@ -11282,7 +10681,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>1062</v>
       </c>
@@ -11314,7 +10713,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>1063</v>
       </c>
@@ -11346,7 +10745,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>1064</v>
       </c>
@@ -11378,7 +10777,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>1065</v>
       </c>
@@ -11410,7 +10809,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>1066</v>
       </c>
@@ -11442,7 +10841,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>1067</v>
       </c>
@@ -11474,7 +10873,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>1068</v>
       </c>
@@ -11506,7 +10905,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>1069</v>
       </c>
@@ -11538,7 +10937,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>1070</v>
       </c>
@@ -11570,7 +10969,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>1071</v>
       </c>
@@ -11602,7 +11001,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>1072</v>
       </c>
@@ -11634,7 +11033,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>1073</v>
       </c>
@@ -11666,7 +11065,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>1074</v>
       </c>
@@ -11698,7 +11097,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>1075</v>
       </c>
@@ -11730,7 +11129,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>1076</v>
       </c>
@@ -11762,7 +11161,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>1077</v>
       </c>
@@ -11794,7 +11193,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>1078</v>
       </c>
@@ -11826,7 +11225,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>1079</v>
       </c>
@@ -11858,7 +11257,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>1080</v>
       </c>
@@ -11890,7 +11289,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>1082</v>
       </c>
@@ -11922,7 +11321,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>1083</v>
       </c>
@@ -11954,7 +11353,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>1084</v>
       </c>
@@ -11986,7 +11385,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>1085</v>
       </c>
@@ -12018,7 +11417,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>1086</v>
       </c>
@@ -12050,7 +11449,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>1087</v>
       </c>
@@ -12082,7 +11481,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>1088</v>
       </c>
@@ -12114,7 +11513,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>1089</v>
       </c>
@@ -12146,7 +11545,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>1090</v>
       </c>
@@ -12178,7 +11577,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>1091</v>
       </c>
@@ -12210,7 +11609,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>1092</v>
       </c>
@@ -12242,7 +11641,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>1093</v>
       </c>
@@ -12274,7 +11673,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>1094</v>
       </c>
@@ -12306,7 +11705,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>1095</v>
       </c>
@@ -12338,7 +11737,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>1096</v>
       </c>
@@ -12370,7 +11769,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>1097</v>
       </c>
@@ -12402,7 +11801,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>1098</v>
       </c>
@@ -12434,7 +11833,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>1099</v>
       </c>
@@ -12466,7 +11865,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>1100</v>
       </c>
@@ -12498,7 +11897,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>1101</v>
       </c>
@@ -12530,7 +11929,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>1102</v>
       </c>
@@ -12562,7 +11961,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>1103</v>
       </c>
@@ -12594,7 +11993,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>1104</v>
       </c>
@@ -12626,7 +12025,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>1106</v>
       </c>
@@ -12658,7 +12057,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>1107</v>
       </c>
@@ -12687,7 +12086,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>1108</v>
       </c>
@@ -12716,7 +12115,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="104" spans="1:10">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>1112</v>
       </c>
@@ -12748,7 +12147,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>1114</v>
       </c>
@@ -12780,7 +12179,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>1115</v>
       </c>
@@ -12812,7 +12211,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>1117</v>
       </c>
@@ -12844,7 +12243,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>1118</v>
       </c>
@@ -12876,7 +12275,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>1119</v>
       </c>
@@ -12908,7 +12307,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>1120</v>
       </c>
@@ -12940,7 +12339,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>1121</v>
       </c>
@@ -12969,7 +12368,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="113" spans="1:10">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>1122</v>
       </c>
@@ -13001,7 +12400,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>1125</v>
       </c>
@@ -13033,7 +12432,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>1133</v>
       </c>
@@ -13065,7 +12464,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>1134</v>
       </c>
@@ -13097,7 +12496,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="117" spans="1:10">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>117</v>
       </c>
@@ -13131,36 +12530,34 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G117" r:id="rId1" display="martincalvin731@gmail.com"/>
+    <hyperlink ref="G117" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B105" workbookViewId="0">
-      <selection activeCell="G122" sqref="G122"/>
+    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="16.5" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="9.875" customWidth="1"/>
-    <col min="6" max="6" width="7.375" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
+    <col min="6" max="6" width="18.375" customWidth="1"/>
     <col min="7" max="7" width="29.25" style="1" customWidth="1"/>
     <col min="9" max="9" width="17.125" style="1" customWidth="1"/>
     <col min="10" max="10" width="30.25" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>990</v>
       </c>
@@ -13192,7 +12589,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>997</v>
       </c>
@@ -13224,7 +12621,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1000</v>
       </c>
@@ -13256,7 +12653,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -13288,7 +12685,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1001</v>
       </c>
@@ -13320,7 +12717,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1003</v>
       </c>
@@ -13352,7 +12749,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1004</v>
       </c>
@@ -13384,7 +12781,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1006</v>
       </c>
@@ -13416,7 +12813,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1007</v>
       </c>
@@ -13448,7 +12845,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1008</v>
       </c>
@@ -13480,7 +12877,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1009</v>
       </c>
@@ -13512,7 +12909,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1010</v>
       </c>
@@ -13544,7 +12941,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1011</v>
       </c>
@@ -13576,7 +12973,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1012</v>
       </c>
@@ -13608,7 +13005,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>1013</v>
       </c>
@@ -13640,7 +13037,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1014</v>
       </c>
@@ -13672,7 +13069,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1015</v>
       </c>
@@ -13704,7 +13101,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="18" ht="47.25" spans="1:10">
+    <row r="18" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>1016</v>
       </c>
@@ -13736,7 +13133,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>1017</v>
       </c>
@@ -13768,7 +13165,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>1018</v>
       </c>
@@ -13800,7 +13197,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>1019</v>
       </c>
@@ -13832,7 +13229,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>1020</v>
       </c>
@@ -13864,7 +13261,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>1021</v>
       </c>
@@ -13896,7 +13293,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>1023</v>
       </c>
@@ -13928,7 +13325,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>1024</v>
       </c>
@@ -13960,7 +13357,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>1025</v>
       </c>
@@ -13992,7 +13389,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>1026</v>
       </c>
@@ -14024,7 +13421,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>1027</v>
       </c>
@@ -14056,7 +13453,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="29" ht="31.5" spans="1:10">
+    <row r="29" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>1028</v>
       </c>
@@ -14088,7 +13485,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="30" ht="31.5" spans="1:10">
+    <row r="30" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>1029</v>
       </c>
@@ -14120,7 +13517,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>1030</v>
       </c>
@@ -14152,7 +13549,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>1031</v>
       </c>
@@ -14184,7 +13581,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>1033</v>
       </c>
@@ -14216,7 +13613,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>1034</v>
       </c>
@@ -14248,7 +13645,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>1035</v>
       </c>
@@ -14280,7 +13677,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>1037</v>
       </c>
@@ -14312,7 +13709,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>1038</v>
       </c>
@@ -14344,7 +13741,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>1039</v>
       </c>
@@ -14376,7 +13773,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="39" ht="31.5" spans="1:10">
+    <row r="39" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>1040</v>
       </c>
@@ -14408,7 +13805,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>1041</v>
       </c>
@@ -14440,7 +13837,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>1042</v>
       </c>
@@ -14472,7 +13869,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>1043</v>
       </c>
@@ -14504,7 +13901,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>1044</v>
       </c>
@@ -14536,7 +13933,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>1045</v>
       </c>
@@ -14568,7 +13965,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>1046</v>
       </c>
@@ -14584,8 +13981,8 @@
       <c r="E45" t="s">
         <v>437</v>
       </c>
-      <c r="F45" t="s">
-        <v>998</v>
+      <c r="F45" s="11" t="s">
+        <v>1206</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>438</v>
@@ -14600,7 +13997,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>1047</v>
       </c>
@@ -14632,7 +14029,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>1048</v>
       </c>
@@ -14664,7 +14061,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>1049</v>
       </c>
@@ -14696,7 +14093,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>1050</v>
       </c>
@@ -14728,7 +14125,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>1051</v>
       </c>
@@ -14760,7 +14157,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>1053</v>
       </c>
@@ -14776,7 +14173,7 @@
       <c r="E51" t="s">
         <v>493</v>
       </c>
-      <c r="F51" s="10" t="s">
+      <c r="F51" s="9" t="s">
         <v>1149</v>
       </c>
       <c r="G51" s="1" t="s">
@@ -14792,7 +14189,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>1054</v>
       </c>
@@ -14824,7 +14221,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>1055</v>
       </c>
@@ -14856,7 +14253,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>1056</v>
       </c>
@@ -14888,7 +14285,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>1057</v>
       </c>
@@ -14920,7 +14317,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>1058</v>
       </c>
@@ -14952,7 +14349,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>1059</v>
       </c>
@@ -14984,7 +14381,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>1061</v>
       </c>
@@ -15016,7 +14413,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>1062</v>
       </c>
@@ -15048,7 +14445,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>1063</v>
       </c>
@@ -15080,7 +14477,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>1064</v>
       </c>
@@ -15112,7 +14509,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>1065</v>
       </c>
@@ -15144,7 +14541,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>1066</v>
       </c>
@@ -15176,7 +14573,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="64" ht="31.5" spans="1:10">
+    <row r="64" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>1067</v>
       </c>
@@ -15208,7 +14605,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>1068</v>
       </c>
@@ -15240,7 +14637,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>1069</v>
       </c>
@@ -15272,7 +14669,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>1070</v>
       </c>
@@ -15304,7 +14701,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>1071</v>
       </c>
@@ -15336,7 +14733,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>1072</v>
       </c>
@@ -15368,7 +14765,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>1073</v>
       </c>
@@ -15400,7 +14797,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>1074</v>
       </c>
@@ -15432,7 +14829,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>1075</v>
       </c>
@@ -15464,7 +14861,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>1076</v>
       </c>
@@ -15496,7 +14893,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>1077</v>
       </c>
@@ -15528,7 +14925,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="75" ht="31.5" spans="1:10">
+    <row r="75" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>1078</v>
       </c>
@@ -15560,7 +14957,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>1079</v>
       </c>
@@ -15592,7 +14989,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>1080</v>
       </c>
@@ -15624,7 +15021,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>1082</v>
       </c>
@@ -15656,7 +15053,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>1083</v>
       </c>
@@ -15688,7 +15085,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>1084</v>
       </c>
@@ -15720,7 +15117,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>1085</v>
       </c>
@@ -15752,7 +15149,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>1086</v>
       </c>
@@ -15784,7 +15181,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>1087</v>
       </c>
@@ -15816,7 +15213,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>1088</v>
       </c>
@@ -15848,7 +15245,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>1089</v>
       </c>
@@ -15880,7 +15277,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>1090</v>
       </c>
@@ -15912,7 +15309,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>1091</v>
       </c>
@@ -15944,7 +15341,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>1092</v>
       </c>
@@ -15973,7 +15370,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>1093</v>
       </c>
@@ -16002,7 +15399,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>1094</v>
       </c>
@@ -16034,7 +15431,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>1095</v>
       </c>
@@ -16066,7 +15463,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>1096</v>
       </c>
@@ -16098,7 +15495,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>1097</v>
       </c>
@@ -16130,7 +15527,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="94" ht="31.5" spans="1:10">
+    <row r="94" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>1098</v>
       </c>
@@ -16162,7 +15559,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>1099</v>
       </c>
@@ -16194,7 +15591,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>1100</v>
       </c>
@@ -16226,7 +15623,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>1101</v>
       </c>
@@ -16258,7 +15655,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>1102</v>
       </c>
@@ -16287,7 +15684,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>1103</v>
       </c>
@@ -16319,7 +15716,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>1104</v>
       </c>
@@ -16351,7 +15748,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>1106</v>
       </c>
@@ -16383,7 +15780,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>1107</v>
       </c>
@@ -16415,7 +15812,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>1108</v>
       </c>
@@ -16447,7 +15844,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="104" spans="1:10">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>1112</v>
       </c>
@@ -16479,7 +15876,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>1114</v>
       </c>
@@ -16511,7 +15908,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>1115</v>
       </c>
@@ -16543,7 +15940,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>1117</v>
       </c>
@@ -16575,7 +15972,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>1118</v>
       </c>
@@ -16607,7 +16004,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>1119</v>
       </c>
@@ -16639,7 +16036,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>1154</v>
       </c>
@@ -16671,7 +16068,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>1120</v>
       </c>
@@ -16703,7 +16100,7 @@
         <v>1164</v>
       </c>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>1121</v>
       </c>
@@ -16735,7 +16132,7 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
@@ -16767,7 +16164,7 @@
         <v>1147</v>
       </c>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
@@ -16799,7 +16196,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
@@ -16831,7 +16228,7 @@
         <v>1181</v>
       </c>
     </row>
-    <row r="117" spans="1:10">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -16860,7 +16257,7 @@
         <v>1187</v>
       </c>
     </row>
-    <row r="118" spans="1:10">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
@@ -16892,7 +16289,7 @@
         <v>1194</v>
       </c>
     </row>
-    <row r="119" spans="1:10">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
@@ -16924,7 +16321,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="120" spans="1:10">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
@@ -16956,7 +16353,7 @@
         <v>1197</v>
       </c>
     </row>
-    <row r="121" spans="1:10">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
@@ -16988,7 +16385,7 @@
         <v>1203</v>
       </c>
     </row>
-    <row r="122" spans="1:10">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
@@ -17022,28 +16419,27 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G114" r:id="rId1" display="martincalvin731@gmail.com"/>
-    <hyperlink ref="G59" r:id="rId2" display="irenescarion88@gmail.com"/>
-    <hyperlink ref="J59" r:id="rId3" display="https://github.com/IreneScarion"/>
-    <hyperlink ref="G115" r:id="rId4" display="candymutagaywa@gmail.com"/>
-    <hyperlink ref="J115" r:id="rId5" display="https://github.com/CandyTheophil"/>
-    <hyperlink ref="G116" r:id="rId6" display="aminja901@gmail.com"/>
-    <hyperlink ref="J116" r:id="rId7" display="https://github.com/ARwaich911"/>
-    <hyperlink ref="G117" r:id="rId8" display="stanleyrichardmbuya@gmail.com"/>
-    <hyperlink ref="J117" r:id="rId9" display="https://github.com/stan-lee98"/>
-    <hyperlink ref="G118" r:id="rId10" display="chusechusechuse09@gmail.com"/>
-    <hyperlink ref="J118" r:id="rId11" display="https://github.com/kilonzoH"/>
-    <hyperlink ref="G119" r:id="rId12" display="omaryzainab55@gmail.com"/>
-    <hyperlink ref="J119" r:id="rId13" display="https://github.com/Zay26"/>
-    <hyperlink ref="G120" r:id="rId14" display="Juma4aziz@gmail.com"/>
-    <hyperlink ref="J120" r:id="rId15" display="https://github.com/Jay4-bit"/>
-    <hyperlink ref="G121" r:id="rId16" display="mlaki3434@gmail.com"/>
-    <hyperlink ref="J121" r:id="rId17" display="https://github.com/jay-mlaki34"/>
-    <hyperlink ref="G122" r:id="rId18" display="machuchesteven@gmail.com"/>
-    <hyperlink ref="J122" r:id="rId19" display="https://github.com/machuchesteven" tooltip="https://github.com/machuchesteven"/>
+    <hyperlink ref="G114" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="G59" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="J59" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="G115" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="J115" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="G116" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="J116" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="G117" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="J117" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="G118" r:id="rId10" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="J118" r:id="rId11" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
+    <hyperlink ref="G119" r:id="rId12" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
+    <hyperlink ref="J119" r:id="rId13" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
+    <hyperlink ref="G120" r:id="rId14" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
+    <hyperlink ref="J120" r:id="rId15" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
+    <hyperlink ref="G121" r:id="rId16" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
+    <hyperlink ref="J121" r:id="rId17" xr:uid="{00000000-0004-0000-0200-000010000000}"/>
+    <hyperlink ref="G122" r:id="rId18" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
+    <hyperlink ref="J122" r:id="rId19" tooltip="https://github.com/machuchesteven" xr:uid="{00000000-0004-0000-0200-000012000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added my phone number
</commit_message>
<xml_diff>
--- a/CS335/GitHub Info sans duplicates.xlsx
+++ b/CS335/GitHub Info sans duplicates.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\staffcard\CS335\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\staffcard\CS335\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE69D4BE-7905-47BE-8CFD-8337A8145282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3891" uniqueCount="1236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3890" uniqueCount="1236">
   <si>
     <t>Timestamp</t>
   </si>
@@ -3734,7 +3735,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd\ h:mm"/>
   </numFmts>
@@ -4081,21 +4082,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P127"/>
   <sheetViews>
-    <sheetView topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="C107" sqref="C107"/>
+    <sheetView topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="G83" sqref="G83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="9.875" customWidth="1"/>
-    <col min="11" max="11" width="9.875" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" customWidth="1"/>
+    <col min="11" max="11" width="9.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4133,7 +4134,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -4171,7 +4172,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -4209,7 +4210,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -4247,7 +4248,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -4285,7 +4286,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -4323,7 +4324,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -4361,7 +4362,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>65</v>
       </c>
@@ -4399,7 +4400,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>74</v>
       </c>
@@ -4437,7 +4438,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>82</v>
       </c>
@@ -4475,7 +4476,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>90</v>
       </c>
@@ -4513,7 +4514,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>98</v>
       </c>
@@ -4551,7 +4552,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>106</v>
       </c>
@@ -4589,7 +4590,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>113</v>
       </c>
@@ -4627,7 +4628,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>121</v>
       </c>
@@ -4665,7 +4666,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>130</v>
       </c>
@@ -4703,7 +4704,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>138</v>
       </c>
@@ -4741,7 +4742,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>146</v>
       </c>
@@ -4779,7 +4780,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>154</v>
       </c>
@@ -4817,7 +4818,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>163</v>
       </c>
@@ -4855,7 +4856,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>171</v>
       </c>
@@ -4893,7 +4894,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>179</v>
       </c>
@@ -4931,7 +4932,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>187</v>
       </c>
@@ -4969,7 +4970,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>195</v>
       </c>
@@ -5007,7 +5008,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>203</v>
       </c>
@@ -5045,7 +5046,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>212</v>
       </c>
@@ -5083,7 +5084,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>221</v>
       </c>
@@ -5121,7 +5122,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>229</v>
       </c>
@@ -5159,7 +5160,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>237</v>
       </c>
@@ -5197,7 +5198,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>245</v>
       </c>
@@ -5235,7 +5236,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>253</v>
       </c>
@@ -5273,7 +5274,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>261</v>
       </c>
@@ -5311,7 +5312,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>269</v>
       </c>
@@ -5349,7 +5350,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>277</v>
       </c>
@@ -5387,7 +5388,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>286</v>
       </c>
@@ -5425,7 +5426,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>295</v>
       </c>
@@ -5463,7 +5464,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>303</v>
       </c>
@@ -5501,7 +5502,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>312</v>
       </c>
@@ -5539,7 +5540,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>320</v>
       </c>
@@ -5577,7 +5578,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>328</v>
       </c>
@@ -5615,7 +5616,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>337</v>
       </c>
@@ -5653,7 +5654,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>345</v>
       </c>
@@ -5691,7 +5692,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>353</v>
       </c>
@@ -5729,7 +5730,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>361</v>
       </c>
@@ -5767,7 +5768,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>369</v>
       </c>
@@ -5805,7 +5806,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>377</v>
       </c>
@@ -5843,7 +5844,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>385</v>
       </c>
@@ -5881,7 +5882,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>393</v>
       </c>
@@ -5919,7 +5920,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>401</v>
       </c>
@@ -5957,7 +5958,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>409</v>
       </c>
@@ -5995,7 +5996,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>417</v>
       </c>
@@ -6033,7 +6034,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>425</v>
       </c>
@@ -6071,7 +6072,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>433</v>
       </c>
@@ -6109,7 +6110,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>441</v>
       </c>
@@ -6147,7 +6148,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>449</v>
       </c>
@@ -6185,7 +6186,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>457</v>
       </c>
@@ -6223,7 +6224,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>465</v>
       </c>
@@ -6261,7 +6262,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>473</v>
       </c>
@@ -6299,7 +6300,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>482</v>
       </c>
@@ -6337,7 +6338,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>489</v>
       </c>
@@ -6375,7 +6376,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>497</v>
       </c>
@@ -6413,7 +6414,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>506</v>
       </c>
@@ -6451,7 +6452,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>514</v>
       </c>
@@ -6489,7 +6490,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>522</v>
       </c>
@@ -6527,7 +6528,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>531</v>
       </c>
@@ -6565,7 +6566,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>539</v>
       </c>
@@ -6603,7 +6604,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>547</v>
       </c>
@@ -6641,7 +6642,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>555</v>
       </c>
@@ -6679,7 +6680,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>563</v>
       </c>
@@ -6717,7 +6718,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>572</v>
       </c>
@@ -6755,7 +6756,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>580</v>
       </c>
@@ -6793,7 +6794,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>588</v>
       </c>
@@ -6831,7 +6832,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>596</v>
       </c>
@@ -6869,7 +6870,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>604</v>
       </c>
@@ -6907,7 +6908,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>612</v>
       </c>
@@ -6945,7 +6946,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>620</v>
       </c>
@@ -6983,7 +6984,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>629</v>
       </c>
@@ -7021,7 +7022,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>636</v>
       </c>
@@ -7059,7 +7060,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>643</v>
       </c>
@@ -7097,7 +7098,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>651</v>
       </c>
@@ -7135,7 +7136,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>659</v>
       </c>
@@ -7173,7 +7174,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>667</v>
       </c>
@@ -7211,7 +7212,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>675</v>
       </c>
@@ -7249,7 +7250,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>684</v>
       </c>
@@ -7287,7 +7288,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>691</v>
       </c>
@@ -7325,7 +7326,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>699</v>
       </c>
@@ -7363,7 +7364,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>707</v>
       </c>
@@ -7401,7 +7402,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>715</v>
       </c>
@@ -7439,7 +7440,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>723</v>
       </c>
@@ -7477,7 +7478,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>731</v>
       </c>
@@ -7515,7 +7516,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>739</v>
       </c>
@@ -7553,7 +7554,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>747</v>
       </c>
@@ -7591,7 +7592,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>755</v>
       </c>
@@ -7629,7 +7630,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>763</v>
       </c>
@@ -7667,7 +7668,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>771</v>
       </c>
@@ -7705,7 +7706,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>773</v>
       </c>
@@ -7743,7 +7744,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>781</v>
       </c>
@@ -7781,7 +7782,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>789</v>
       </c>
@@ -7819,7 +7820,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>797</v>
       </c>
@@ -7857,7 +7858,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>805</v>
       </c>
@@ -7895,7 +7896,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>813</v>
       </c>
@@ -7933,7 +7934,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>821</v>
       </c>
@@ -7971,7 +7972,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>829</v>
       </c>
@@ -8006,7 +8007,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>836</v>
       </c>
@@ -8046,7 +8047,7 @@
       <c r="M104" s="11"/>
       <c r="P104" s="7"/>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>843</v>
       </c>
@@ -8084,7 +8085,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>851</v>
       </c>
@@ -8122,7 +8123,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A107" s="8">
         <v>44518.9544328704</v>
       </c>
@@ -8160,7 +8161,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>866</v>
       </c>
@@ -8198,7 +8199,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>874</v>
       </c>
@@ -8236,7 +8237,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>883</v>
       </c>
@@ -8274,7 +8275,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>891</v>
       </c>
@@ -8312,7 +8313,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>893</v>
       </c>
@@ -8350,7 +8351,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>901</v>
       </c>
@@ -8385,7 +8386,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>903</v>
       </c>
@@ -8423,7 +8424,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>911</v>
       </c>
@@ -8461,7 +8462,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>919</v>
       </c>
@@ -8499,7 +8500,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>927</v>
       </c>
@@ -8537,7 +8538,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>934</v>
       </c>
@@ -8575,7 +8576,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>942</v>
       </c>
@@ -8613,7 +8614,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>950</v>
       </c>
@@ -8651,7 +8652,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>957</v>
       </c>
@@ -8689,7 +8690,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>965</v>
       </c>
@@ -8727,7 +8728,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>973</v>
       </c>
@@ -8762,7 +8763,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B124" t="s">
         <v>483</v>
       </c>
@@ -8797,7 +8798,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B125" t="s">
         <v>977</v>
       </c>
@@ -8823,7 +8824,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B126" t="s">
         <v>523</v>
       </c>
@@ -8846,7 +8847,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B127" t="s">
         <v>982</v>
       </c>
@@ -8886,8 +8887,8 @@
     <mergeCell ref="L104:M104"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G104" r:id="rId1"/>
-    <hyperlink ref="L104" r:id="rId2"/>
+    <hyperlink ref="G104" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="L104" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -8895,23 +8896,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J117"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="G82" sqref="G82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="17.5" customWidth="1"/>
-    <col min="4" max="4" width="15.875" customWidth="1"/>
-    <col min="5" max="5" width="14.625" customWidth="1"/>
-    <col min="6" max="6" width="9.875" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" customWidth="1"/>
+    <col min="5" max="5" width="14.58203125" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>990</v>
       </c>
@@ -8943,7 +8944,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>997</v>
       </c>
@@ -8975,7 +8976,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1000</v>
       </c>
@@ -9007,7 +9008,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -9039,7 +9040,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1001</v>
       </c>
@@ -9071,7 +9072,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1003</v>
       </c>
@@ -9103,7 +9104,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1004</v>
       </c>
@@ -9135,7 +9136,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>1006</v>
       </c>
@@ -9167,7 +9168,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>1007</v>
       </c>
@@ -9199,7 +9200,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>1008</v>
       </c>
@@ -9231,7 +9232,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>1009</v>
       </c>
@@ -9263,7 +9264,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>1010</v>
       </c>
@@ -9295,7 +9296,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>1011</v>
       </c>
@@ -9327,7 +9328,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>1012</v>
       </c>
@@ -9359,7 +9360,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>1013</v>
       </c>
@@ -9391,7 +9392,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>1014</v>
       </c>
@@ -9423,7 +9424,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>1015</v>
       </c>
@@ -9455,7 +9456,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>1016</v>
       </c>
@@ -9487,7 +9488,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>1017</v>
       </c>
@@ -9519,7 +9520,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>1018</v>
       </c>
@@ -9551,7 +9552,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>1019</v>
       </c>
@@ -9583,7 +9584,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>1020</v>
       </c>
@@ -9615,7 +9616,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>1021</v>
       </c>
@@ -9647,7 +9648,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>1023</v>
       </c>
@@ -9679,7 +9680,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>1024</v>
       </c>
@@ -9711,7 +9712,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>1025</v>
       </c>
@@ -9743,7 +9744,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>1026</v>
       </c>
@@ -9775,7 +9776,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>1027</v>
       </c>
@@ -9807,7 +9808,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>1028</v>
       </c>
@@ -9839,7 +9840,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>1029</v>
       </c>
@@ -9871,7 +9872,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>1030</v>
       </c>
@@ -9903,7 +9904,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>1031</v>
       </c>
@@ -9935,7 +9936,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>1033</v>
       </c>
@@ -9967,7 +9968,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>1034</v>
       </c>
@@ -9999,7 +10000,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>1035</v>
       </c>
@@ -10031,7 +10032,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>1037</v>
       </c>
@@ -10063,7 +10064,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>1038</v>
       </c>
@@ -10095,7 +10096,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>1039</v>
       </c>
@@ -10127,7 +10128,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>1040</v>
       </c>
@@ -10159,7 +10160,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>1041</v>
       </c>
@@ -10191,7 +10192,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>1042</v>
       </c>
@@ -10223,7 +10224,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>1043</v>
       </c>
@@ -10255,7 +10256,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>1044</v>
       </c>
@@ -10287,7 +10288,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>1045</v>
       </c>
@@ -10319,7 +10320,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>1046</v>
       </c>
@@ -10351,7 +10352,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>1047</v>
       </c>
@@ -10383,7 +10384,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>1048</v>
       </c>
@@ -10415,7 +10416,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>1049</v>
       </c>
@@ -10447,7 +10448,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>1050</v>
       </c>
@@ -10479,7 +10480,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>1051</v>
       </c>
@@ -10511,7 +10512,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>1053</v>
       </c>
@@ -10543,7 +10544,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>1054</v>
       </c>
@@ -10575,7 +10576,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>1055</v>
       </c>
@@ -10607,7 +10608,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>1056</v>
       </c>
@@ -10639,7 +10640,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>1057</v>
       </c>
@@ -10671,7 +10672,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>1058</v>
       </c>
@@ -10703,7 +10704,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>1059</v>
       </c>
@@ -10735,7 +10736,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>1061</v>
       </c>
@@ -10767,7 +10768,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>1062</v>
       </c>
@@ -10799,7 +10800,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>1063</v>
       </c>
@@ -10831,7 +10832,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>1064</v>
       </c>
@@ -10863,7 +10864,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>1065</v>
       </c>
@@ -10895,7 +10896,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>1066</v>
       </c>
@@ -10927,7 +10928,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>1067</v>
       </c>
@@ -10959,7 +10960,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>1068</v>
       </c>
@@ -10991,7 +10992,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>1069</v>
       </c>
@@ -11023,7 +11024,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>1070</v>
       </c>
@@ -11055,7 +11056,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>1071</v>
       </c>
@@ -11087,7 +11088,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>1072</v>
       </c>
@@ -11119,7 +11120,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>1073</v>
       </c>
@@ -11151,7 +11152,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>1074</v>
       </c>
@@ -11183,7 +11184,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>1075</v>
       </c>
@@ -11215,7 +11216,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>1076</v>
       </c>
@@ -11247,7 +11248,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>1077</v>
       </c>
@@ -11279,7 +11280,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>1078</v>
       </c>
@@ -11311,7 +11312,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>1079</v>
       </c>
@@ -11343,7 +11344,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>1080</v>
       </c>
@@ -11375,7 +11376,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>1082</v>
       </c>
@@ -11407,7 +11408,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>1083</v>
       </c>
@@ -11439,7 +11440,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>1084</v>
       </c>
@@ -11471,7 +11472,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>1085</v>
       </c>
@@ -11503,7 +11504,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>1086</v>
       </c>
@@ -11535,7 +11536,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>1087</v>
       </c>
@@ -11567,7 +11568,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>1088</v>
       </c>
@@ -11599,7 +11600,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>1089</v>
       </c>
@@ -11631,7 +11632,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>1090</v>
       </c>
@@ -11663,7 +11664,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>1091</v>
       </c>
@@ -11695,7 +11696,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>1092</v>
       </c>
@@ -11727,7 +11728,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>1093</v>
       </c>
@@ -11759,7 +11760,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>1094</v>
       </c>
@@ -11791,7 +11792,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>1095</v>
       </c>
@@ -11823,7 +11824,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>1096</v>
       </c>
@@ -11855,7 +11856,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>1097</v>
       </c>
@@ -11887,7 +11888,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>1098</v>
       </c>
@@ -11919,7 +11920,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>1099</v>
       </c>
@@ -11951,7 +11952,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>1100</v>
       </c>
@@ -11983,7 +11984,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>1101</v>
       </c>
@@ -12015,7 +12016,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>1102</v>
       </c>
@@ -12047,7 +12048,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>1103</v>
       </c>
@@ -12079,7 +12080,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>1104</v>
       </c>
@@ -12111,7 +12112,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>1106</v>
       </c>
@@ -12143,7 +12144,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>1107</v>
       </c>
@@ -12172,7 +12173,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>1108</v>
       </c>
@@ -12201,7 +12202,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>1112</v>
       </c>
@@ -12233,7 +12234,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>1114</v>
       </c>
@@ -12265,7 +12266,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>1115</v>
       </c>
@@ -12297,7 +12298,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>1117</v>
       </c>
@@ -12329,7 +12330,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>1118</v>
       </c>
@@ -12361,7 +12362,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>1119</v>
       </c>
@@ -12393,7 +12394,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>1120</v>
       </c>
@@ -12425,7 +12426,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>1121</v>
       </c>
@@ -12454,7 +12455,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>1122</v>
       </c>
@@ -12486,7 +12487,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>1125</v>
       </c>
@@ -12518,7 +12519,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>1133</v>
       </c>
@@ -12550,7 +12551,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>1134</v>
       </c>
@@ -12582,7 +12583,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>117</v>
       </c>
@@ -12616,7 +12617,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G117" r:id="rId1"/>
+    <hyperlink ref="G117" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -12624,26 +12625,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="A128" sqref="A128"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="16.5" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="18.375" customWidth="1"/>
-    <col min="7" max="7" width="29.125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="30.125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="29.08203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.08203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="30.08203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>990</v>
       </c>
@@ -12675,7 +12676,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>997</v>
       </c>
@@ -12707,7 +12708,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1000</v>
       </c>
@@ -12739,7 +12740,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -12771,7 +12772,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1001</v>
       </c>
@@ -12803,7 +12804,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1003</v>
       </c>
@@ -12835,7 +12836,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1004</v>
       </c>
@@ -12867,7 +12868,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>1006</v>
       </c>
@@ -12899,7 +12900,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>1007</v>
       </c>
@@ -12931,7 +12932,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>1008</v>
       </c>
@@ -12963,7 +12964,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>1009</v>
       </c>
@@ -12995,7 +12996,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>1010</v>
       </c>
@@ -13027,7 +13028,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>1011</v>
       </c>
@@ -13059,7 +13060,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>1012</v>
       </c>
@@ -13091,7 +13092,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>1013</v>
       </c>
@@ -13123,7 +13124,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>1014</v>
       </c>
@@ -13155,7 +13156,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>1015</v>
       </c>
@@ -13187,7 +13188,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>1016</v>
       </c>
@@ -13219,7 +13220,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>1017</v>
       </c>
@@ -13251,7 +13252,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>1018</v>
       </c>
@@ -13283,7 +13284,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>1019</v>
       </c>
@@ -13315,7 +13316,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>1020</v>
       </c>
@@ -13347,7 +13348,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>1021</v>
       </c>
@@ -13379,7 +13380,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>1023</v>
       </c>
@@ -13411,7 +13412,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>1024</v>
       </c>
@@ -13443,7 +13444,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>1025</v>
       </c>
@@ -13475,7 +13476,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>1026</v>
       </c>
@@ -13507,7 +13508,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>1027</v>
       </c>
@@ -13539,7 +13540,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>1028</v>
       </c>
@@ -13571,7 +13572,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>1029</v>
       </c>
@@ -13603,7 +13604,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>1030</v>
       </c>
@@ -13635,7 +13636,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>1031</v>
       </c>
@@ -13651,9 +13652,6 @@
       <c r="E32" t="s">
         <v>307</v>
       </c>
-      <c r="F32" t="s">
-        <v>308</v>
-      </c>
       <c r="G32" s="1" t="s">
         <v>309</v>
       </c>
@@ -13667,7 +13665,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>1033</v>
       </c>
@@ -13699,7 +13697,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>1034</v>
       </c>
@@ -13731,7 +13729,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>1035</v>
       </c>
@@ -13763,7 +13761,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>1037</v>
       </c>
@@ -13795,7 +13793,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>1038</v>
       </c>
@@ -13827,7 +13825,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>1039</v>
       </c>
@@ -13859,7 +13857,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>1040</v>
       </c>
@@ -13891,7 +13889,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>1041</v>
       </c>
@@ -13923,7 +13921,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>1042</v>
       </c>
@@ -13955,7 +13953,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>1043</v>
       </c>
@@ -13987,7 +13985,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>1044</v>
       </c>
@@ -14019,7 +14017,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>1045</v>
       </c>
@@ -14051,7 +14049,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>1046</v>
       </c>
@@ -14083,7 +14081,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>1047</v>
       </c>
@@ -14115,7 +14113,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>1048</v>
       </c>
@@ -14147,7 +14145,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>1049</v>
       </c>
@@ -14179,7 +14177,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>1050</v>
       </c>
@@ -14211,7 +14209,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>1051</v>
       </c>
@@ -14243,7 +14241,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>1053</v>
       </c>
@@ -14275,7 +14273,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>1054</v>
       </c>
@@ -14307,7 +14305,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>1055</v>
       </c>
@@ -14339,7 +14337,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>1056</v>
       </c>
@@ -14371,7 +14369,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>1057</v>
       </c>
@@ -14403,7 +14401,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>1058</v>
       </c>
@@ -14435,7 +14433,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>1059</v>
       </c>
@@ -14467,7 +14465,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>1061</v>
       </c>
@@ -14499,7 +14497,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>1062</v>
       </c>
@@ -14531,7 +14529,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>1063</v>
       </c>
@@ -14563,7 +14561,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>1064</v>
       </c>
@@ -14595,7 +14593,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>1065</v>
       </c>
@@ -14627,7 +14625,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>1066</v>
       </c>
@@ -14659,7 +14657,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>1067</v>
       </c>
@@ -14691,7 +14689,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>1068</v>
       </c>
@@ -14723,7 +14721,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>1069</v>
       </c>
@@ -14755,7 +14753,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>1070</v>
       </c>
@@ -14787,7 +14785,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>1071</v>
       </c>
@@ -14819,7 +14817,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>1072</v>
       </c>
@@ -14851,7 +14849,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>1073</v>
       </c>
@@ -14883,7 +14881,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>1074</v>
       </c>
@@ -14915,7 +14913,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>1075</v>
       </c>
@@ -14947,7 +14945,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>1076</v>
       </c>
@@ -14979,7 +14977,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>1077</v>
       </c>
@@ -15011,7 +15009,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>1078</v>
       </c>
@@ -15043,7 +15041,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>1079</v>
       </c>
@@ -15075,7 +15073,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>1080</v>
       </c>
@@ -15107,7 +15105,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>1082</v>
       </c>
@@ -15139,7 +15137,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>1083</v>
       </c>
@@ -15171,7 +15169,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>1084</v>
       </c>
@@ -15203,7 +15201,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>1085</v>
       </c>
@@ -15235,7 +15233,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>1086</v>
       </c>
@@ -15267,7 +15265,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>1087</v>
       </c>
@@ -15299,7 +15297,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>1088</v>
       </c>
@@ -15331,7 +15329,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>1089</v>
       </c>
@@ -15363,7 +15361,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>1090</v>
       </c>
@@ -15395,7 +15393,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>1091</v>
       </c>
@@ -15427,7 +15425,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>1092</v>
       </c>
@@ -15456,7 +15454,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>1093</v>
       </c>
@@ -15485,7 +15483,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>1094</v>
       </c>
@@ -15517,7 +15515,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>1095</v>
       </c>
@@ -15549,7 +15547,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>1096</v>
       </c>
@@ -15581,7 +15579,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>1097</v>
       </c>
@@ -15613,7 +15611,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>1098</v>
       </c>
@@ -15645,7 +15643,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>1099</v>
       </c>
@@ -15677,7 +15675,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>1100</v>
       </c>
@@ -15709,7 +15707,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>1101</v>
       </c>
@@ -15741,7 +15739,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>1102</v>
       </c>
@@ -15770,7 +15768,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>1103</v>
       </c>
@@ -15802,7 +15800,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>1104</v>
       </c>
@@ -15834,7 +15832,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>1106</v>
       </c>
@@ -15866,7 +15864,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>1107</v>
       </c>
@@ -15898,7 +15896,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>1108</v>
       </c>
@@ -15930,7 +15928,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>1112</v>
       </c>
@@ -15962,7 +15960,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>1114</v>
       </c>
@@ -15994,7 +15992,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>1115</v>
       </c>
@@ -16026,7 +16024,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>1117</v>
       </c>
@@ -16058,7 +16056,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>1118</v>
       </c>
@@ -16090,7 +16088,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>1119</v>
       </c>
@@ -16122,7 +16120,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>1154</v>
       </c>
@@ -16154,7 +16152,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>1120</v>
       </c>
@@ -16186,7 +16184,7 @@
         <v>1164</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>1121</v>
       </c>
@@ -16218,7 +16216,7 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>113</v>
       </c>
@@ -16250,7 +16248,7 @@
         <v>1147</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>114</v>
       </c>
@@ -16282,7 +16280,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>115</v>
       </c>
@@ -16314,7 +16312,7 @@
         <v>1181</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>116</v>
       </c>
@@ -16343,7 +16341,7 @@
         <v>1187</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>117</v>
       </c>
@@ -16375,7 +16373,7 @@
         <v>1194</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>118</v>
       </c>
@@ -16407,7 +16405,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>119</v>
       </c>
@@ -16439,7 +16437,7 @@
         <v>1197</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>120</v>
       </c>
@@ -16471,7 +16469,7 @@
         <v>1203</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>121</v>
       </c>
@@ -16503,7 +16501,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>122</v>
       </c>
@@ -16535,7 +16533,7 @@
         <v>1212</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B124" t="s">
         <v>1218</v>
       </c>
@@ -16564,7 +16562,7 @@
         <v>1217</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B125" t="s">
         <v>1219</v>
       </c>
@@ -16590,7 +16588,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B126" t="s">
         <v>644</v>
       </c>
@@ -16616,7 +16614,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B127" t="s">
         <v>1228</v>
       </c>
@@ -16639,10 +16637,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A128">
-        <v>127</v>
-      </c>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B128" t="s">
         <v>532</v>
       </c>
@@ -16667,31 +16662,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G114" r:id="rId1"/>
-    <hyperlink ref="G59" r:id="rId2"/>
-    <hyperlink ref="J59" r:id="rId3"/>
-    <hyperlink ref="G115" r:id="rId4"/>
-    <hyperlink ref="J115" r:id="rId5"/>
-    <hyperlink ref="G116" r:id="rId6"/>
-    <hyperlink ref="J116" r:id="rId7"/>
-    <hyperlink ref="G117" r:id="rId8"/>
-    <hyperlink ref="J117" r:id="rId9"/>
-    <hyperlink ref="G118" r:id="rId10"/>
-    <hyperlink ref="J118" r:id="rId11"/>
-    <hyperlink ref="G119" r:id="rId12"/>
-    <hyperlink ref="J119" r:id="rId13"/>
-    <hyperlink ref="G120" r:id="rId14"/>
-    <hyperlink ref="J120" r:id="rId15"/>
-    <hyperlink ref="G121" r:id="rId16"/>
-    <hyperlink ref="J121" r:id="rId17"/>
-    <hyperlink ref="G122" r:id="rId18"/>
-    <hyperlink ref="J122" r:id="rId19" tooltip="https://github.com/machuchesteven"/>
-    <hyperlink ref="G123" r:id="rId20"/>
-    <hyperlink ref="J123" r:id="rId21"/>
-    <hyperlink ref="G124" r:id="rId22"/>
-    <hyperlink ref="J124" r:id="rId23"/>
-    <hyperlink ref="G127" r:id="rId24"/>
-    <hyperlink ref="G128" r:id="rId25"/>
+    <hyperlink ref="G114" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="G59" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="J59" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="G115" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="J115" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="G116" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="J116" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="G117" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="J117" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="G118" r:id="rId10" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="J118" r:id="rId11" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
+    <hyperlink ref="G119" r:id="rId12" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
+    <hyperlink ref="J119" r:id="rId13" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
+    <hyperlink ref="G120" r:id="rId14" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
+    <hyperlink ref="J120" r:id="rId15" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
+    <hyperlink ref="G121" r:id="rId16" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
+    <hyperlink ref="J121" r:id="rId17" xr:uid="{00000000-0004-0000-0200-000010000000}"/>
+    <hyperlink ref="G122" r:id="rId18" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
+    <hyperlink ref="J122" r:id="rId19" tooltip="https://github.com/machuchesteven" xr:uid="{00000000-0004-0000-0200-000012000000}"/>
+    <hyperlink ref="G123" r:id="rId20" xr:uid="{00000000-0004-0000-0200-000013000000}"/>
+    <hyperlink ref="J123" r:id="rId21" xr:uid="{00000000-0004-0000-0200-000014000000}"/>
+    <hyperlink ref="G124" r:id="rId22" xr:uid="{00000000-0004-0000-0200-000015000000}"/>
+    <hyperlink ref="J124" r:id="rId23" xr:uid="{00000000-0004-0000-0200-000016000000}"/>
+    <hyperlink ref="G127" r:id="rId24" xr:uid="{00000000-0004-0000-0200-000017000000}"/>
+    <hyperlink ref="G128" r:id="rId25" xr:uid="{00000000-0004-0000-0200-000018000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId26"/>

</xml_diff>

<commit_message>
Added my name in Excel sheet
</commit_message>
<xml_diff>
--- a/CS335/GitHub Info sans duplicates.xlsx
+++ b/CS335/GitHub Info sans duplicates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\staffcard\CS335\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\staffcard\CS335\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358DA6C2-7723-43D3-9C3F-9DEE2DDB506E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96F9620-F1A3-4C07-8FF4-2A1B64A0373C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3897" uniqueCount="1241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3905" uniqueCount="1245">
   <si>
     <t>Timestamp</t>
   </si>
@@ -3745,6 +3745,18 @@
   </si>
   <si>
     <t>charlesmgema</t>
+  </si>
+  <si>
+    <t>2019-04-05189</t>
+  </si>
+  <si>
+    <t>Lwanda</t>
+  </si>
+  <si>
+    <t>Erick Peter</t>
+  </si>
+  <si>
+    <t>cs</t>
   </si>
 </sst>
 </file>
@@ -4104,14 +4116,14 @@
       <selection activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="9.875" customWidth="1"/>
-    <col min="11" max="11" width="9.875" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" customWidth="1"/>
+    <col min="11" max="11" width="9.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4149,7 +4161,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -4187,7 +4199,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -4225,7 +4237,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -4263,7 +4275,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -4301,7 +4313,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -4339,7 +4351,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -4377,7 +4389,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>65</v>
       </c>
@@ -4415,7 +4427,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>74</v>
       </c>
@@ -4453,7 +4465,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>82</v>
       </c>
@@ -4491,7 +4503,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>90</v>
       </c>
@@ -4529,7 +4541,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>98</v>
       </c>
@@ -4567,7 +4579,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>106</v>
       </c>
@@ -4605,7 +4617,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>113</v>
       </c>
@@ -4643,7 +4655,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>121</v>
       </c>
@@ -4681,7 +4693,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>130</v>
       </c>
@@ -4719,7 +4731,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>138</v>
       </c>
@@ -4757,7 +4769,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>146</v>
       </c>
@@ -4795,7 +4807,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>154</v>
       </c>
@@ -4833,7 +4845,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>163</v>
       </c>
@@ -4871,7 +4883,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>171</v>
       </c>
@@ -4909,7 +4921,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>179</v>
       </c>
@@ -4947,7 +4959,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>187</v>
       </c>
@@ -4985,7 +4997,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>195</v>
       </c>
@@ -5023,7 +5035,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>203</v>
       </c>
@@ -5061,7 +5073,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>212</v>
       </c>
@@ -5099,7 +5111,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>221</v>
       </c>
@@ -5137,7 +5149,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>229</v>
       </c>
@@ -5175,7 +5187,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>237</v>
       </c>
@@ -5213,7 +5225,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>245</v>
       </c>
@@ -5251,7 +5263,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>253</v>
       </c>
@@ -5289,7 +5301,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>261</v>
       </c>
@@ -5327,7 +5339,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>269</v>
       </c>
@@ -5365,7 +5377,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>277</v>
       </c>
@@ -5403,7 +5415,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>286</v>
       </c>
@@ -5441,7 +5453,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>295</v>
       </c>
@@ -5479,7 +5491,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>303</v>
       </c>
@@ -5517,7 +5529,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>312</v>
       </c>
@@ -5555,7 +5567,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>320</v>
       </c>
@@ -5593,7 +5605,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>328</v>
       </c>
@@ -5631,7 +5643,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>337</v>
       </c>
@@ -5669,7 +5681,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>345</v>
       </c>
@@ -5707,7 +5719,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>353</v>
       </c>
@@ -5745,7 +5757,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>361</v>
       </c>
@@ -5783,7 +5795,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>369</v>
       </c>
@@ -5821,7 +5833,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>377</v>
       </c>
@@ -5859,7 +5871,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>385</v>
       </c>
@@ -5897,7 +5909,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>393</v>
       </c>
@@ -5935,7 +5947,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>401</v>
       </c>
@@ -5973,7 +5985,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>409</v>
       </c>
@@ -6011,7 +6023,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>417</v>
       </c>
@@ -6049,7 +6061,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>425</v>
       </c>
@@ -6087,7 +6099,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>433</v>
       </c>
@@ -6125,7 +6137,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>441</v>
       </c>
@@ -6163,7 +6175,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>449</v>
       </c>
@@ -6201,7 +6213,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>457</v>
       </c>
@@ -6239,7 +6251,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>465</v>
       </c>
@@ -6277,7 +6289,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>473</v>
       </c>
@@ -6315,7 +6327,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>482</v>
       </c>
@@ -6353,7 +6365,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>489</v>
       </c>
@@ -6391,7 +6403,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>497</v>
       </c>
@@ -6429,7 +6441,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>506</v>
       </c>
@@ -6467,7 +6479,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>514</v>
       </c>
@@ -6505,7 +6517,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>522</v>
       </c>
@@ -6543,7 +6555,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>531</v>
       </c>
@@ -6581,7 +6593,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>539</v>
       </c>
@@ -6619,7 +6631,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>547</v>
       </c>
@@ -6657,7 +6669,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>555</v>
       </c>
@@ -6695,7 +6707,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>563</v>
       </c>
@@ -6733,7 +6745,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>572</v>
       </c>
@@ -6771,7 +6783,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>580</v>
       </c>
@@ -6809,7 +6821,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>588</v>
       </c>
@@ -6847,7 +6859,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>596</v>
       </c>
@@ -6885,7 +6897,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>604</v>
       </c>
@@ -6923,7 +6935,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>612</v>
       </c>
@@ -6961,7 +6973,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>620</v>
       </c>
@@ -6999,7 +7011,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>629</v>
       </c>
@@ -7037,7 +7049,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>636</v>
       </c>
@@ -7075,7 +7087,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>643</v>
       </c>
@@ -7113,7 +7125,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>651</v>
       </c>
@@ -7151,7 +7163,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>659</v>
       </c>
@@ -7189,7 +7201,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>667</v>
       </c>
@@ -7227,7 +7239,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>675</v>
       </c>
@@ -7265,7 +7277,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>684</v>
       </c>
@@ -7303,7 +7315,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>691</v>
       </c>
@@ -7341,7 +7353,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>699</v>
       </c>
@@ -7379,7 +7391,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>707</v>
       </c>
@@ -7417,7 +7429,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>715</v>
       </c>
@@ -7455,7 +7467,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>723</v>
       </c>
@@ -7493,7 +7505,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>731</v>
       </c>
@@ -7531,7 +7543,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>739</v>
       </c>
@@ -7569,7 +7581,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>747</v>
       </c>
@@ -7607,7 +7619,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>755</v>
       </c>
@@ -7645,7 +7657,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>763</v>
       </c>
@@ -7683,7 +7695,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>771</v>
       </c>
@@ -7721,7 +7733,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>773</v>
       </c>
@@ -7759,7 +7771,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>781</v>
       </c>
@@ -7797,7 +7809,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>789</v>
       </c>
@@ -7835,7 +7847,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>797</v>
       </c>
@@ -7873,7 +7885,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>805</v>
       </c>
@@ -7911,7 +7923,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>813</v>
       </c>
@@ -7949,7 +7961,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>821</v>
       </c>
@@ -7987,7 +7999,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>829</v>
       </c>
@@ -8022,7 +8034,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>836</v>
       </c>
@@ -8062,7 +8074,7 @@
       <c r="M104" s="11"/>
       <c r="P104" s="7"/>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>843</v>
       </c>
@@ -8100,7 +8112,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>851</v>
       </c>
@@ -8138,7 +8150,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A107" s="8">
         <v>44518.9544328704</v>
       </c>
@@ -8176,7 +8188,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>866</v>
       </c>
@@ -8214,7 +8226,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>874</v>
       </c>
@@ -8252,7 +8264,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>883</v>
       </c>
@@ -8290,7 +8302,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>891</v>
       </c>
@@ -8328,7 +8340,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>893</v>
       </c>
@@ -8366,7 +8378,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>901</v>
       </c>
@@ -8401,7 +8413,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>903</v>
       </c>
@@ -8439,7 +8451,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>911</v>
       </c>
@@ -8477,7 +8489,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>919</v>
       </c>
@@ -8515,7 +8527,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>927</v>
       </c>
@@ -8553,7 +8565,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>934</v>
       </c>
@@ -8591,7 +8603,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>942</v>
       </c>
@@ -8629,7 +8641,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>950</v>
       </c>
@@ -8667,7 +8679,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>957</v>
       </c>
@@ -8705,7 +8717,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>965</v>
       </c>
@@ -8743,7 +8755,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>973</v>
       </c>
@@ -8778,7 +8790,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B124" t="s">
         <v>483</v>
       </c>
@@ -8813,7 +8825,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B125" t="s">
         <v>977</v>
       </c>
@@ -8839,7 +8851,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B126" t="s">
         <v>523</v>
       </c>
@@ -8862,7 +8874,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B127" t="s">
         <v>982</v>
       </c>
@@ -8918,16 +8930,16 @@
       <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="17.5" customWidth="1"/>
-    <col min="4" max="4" width="15.875" customWidth="1"/>
-    <col min="5" max="5" width="14.625" customWidth="1"/>
-    <col min="6" max="6" width="9.875" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" customWidth="1"/>
+    <col min="5" max="5" width="14.58203125" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>990</v>
       </c>
@@ -8959,7 +8971,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>997</v>
       </c>
@@ -8991,7 +9003,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1000</v>
       </c>
@@ -9023,7 +9035,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -9055,7 +9067,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1001</v>
       </c>
@@ -9087,7 +9099,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1003</v>
       </c>
@@ -9119,7 +9131,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1004</v>
       </c>
@@ -9151,7 +9163,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>1006</v>
       </c>
@@ -9183,7 +9195,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>1007</v>
       </c>
@@ -9215,7 +9227,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>1008</v>
       </c>
@@ -9247,7 +9259,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>1009</v>
       </c>
@@ -9279,7 +9291,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>1010</v>
       </c>
@@ -9311,7 +9323,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>1011</v>
       </c>
@@ -9343,7 +9355,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>1012</v>
       </c>
@@ -9375,7 +9387,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>1013</v>
       </c>
@@ -9407,7 +9419,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>1014</v>
       </c>
@@ -9439,7 +9451,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>1015</v>
       </c>
@@ -9471,7 +9483,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>1016</v>
       </c>
@@ -9503,7 +9515,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>1017</v>
       </c>
@@ -9535,7 +9547,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>1018</v>
       </c>
@@ -9567,7 +9579,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>1019</v>
       </c>
@@ -9599,7 +9611,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>1020</v>
       </c>
@@ -9631,7 +9643,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>1021</v>
       </c>
@@ -9663,7 +9675,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>1023</v>
       </c>
@@ -9695,7 +9707,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>1024</v>
       </c>
@@ -9727,7 +9739,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>1025</v>
       </c>
@@ -9759,7 +9771,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>1026</v>
       </c>
@@ -9791,7 +9803,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>1027</v>
       </c>
@@ -9823,7 +9835,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>1028</v>
       </c>
@@ -9855,7 +9867,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>1029</v>
       </c>
@@ -9887,7 +9899,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>1030</v>
       </c>
@@ -9919,7 +9931,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>1031</v>
       </c>
@@ -9951,7 +9963,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>1033</v>
       </c>
@@ -9983,7 +9995,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>1034</v>
       </c>
@@ -10015,7 +10027,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>1035</v>
       </c>
@@ -10047,7 +10059,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>1037</v>
       </c>
@@ -10079,7 +10091,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>1038</v>
       </c>
@@ -10111,7 +10123,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>1039</v>
       </c>
@@ -10143,7 +10155,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>1040</v>
       </c>
@@ -10175,7 +10187,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>1041</v>
       </c>
@@ -10207,7 +10219,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>1042</v>
       </c>
@@ -10239,7 +10251,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>1043</v>
       </c>
@@ -10271,7 +10283,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>1044</v>
       </c>
@@ -10303,7 +10315,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>1045</v>
       </c>
@@ -10335,7 +10347,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>1046</v>
       </c>
@@ -10367,7 +10379,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>1047</v>
       </c>
@@ -10399,7 +10411,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>1048</v>
       </c>
@@ -10431,7 +10443,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>1049</v>
       </c>
@@ -10463,7 +10475,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>1050</v>
       </c>
@@ -10495,7 +10507,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>1051</v>
       </c>
@@ -10527,7 +10539,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>1053</v>
       </c>
@@ -10559,7 +10571,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>1054</v>
       </c>
@@ -10591,7 +10603,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>1055</v>
       </c>
@@ -10623,7 +10635,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>1056</v>
       </c>
@@ -10655,7 +10667,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>1057</v>
       </c>
@@ -10687,7 +10699,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>1058</v>
       </c>
@@ -10719,7 +10731,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>1059</v>
       </c>
@@ -10751,7 +10763,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>1061</v>
       </c>
@@ -10783,7 +10795,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>1062</v>
       </c>
@@ -10815,7 +10827,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>1063</v>
       </c>
@@ -10847,7 +10859,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>1064</v>
       </c>
@@ -10879,7 +10891,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>1065</v>
       </c>
@@ -10911,7 +10923,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>1066</v>
       </c>
@@ -10943,7 +10955,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>1067</v>
       </c>
@@ -10975,7 +10987,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>1068</v>
       </c>
@@ -11007,7 +11019,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>1069</v>
       </c>
@@ -11039,7 +11051,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>1070</v>
       </c>
@@ -11071,7 +11083,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>1071</v>
       </c>
@@ -11103,7 +11115,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>1072</v>
       </c>
@@ -11135,7 +11147,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>1073</v>
       </c>
@@ -11167,7 +11179,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>1074</v>
       </c>
@@ -11199,7 +11211,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>1075</v>
       </c>
@@ -11231,7 +11243,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>1076</v>
       </c>
@@ -11263,7 +11275,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>1077</v>
       </c>
@@ -11295,7 +11307,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>1078</v>
       </c>
@@ -11327,7 +11339,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>1079</v>
       </c>
@@ -11359,7 +11371,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>1080</v>
       </c>
@@ -11391,7 +11403,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>1082</v>
       </c>
@@ -11423,7 +11435,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>1083</v>
       </c>
@@ -11455,7 +11467,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>1084</v>
       </c>
@@ -11487,7 +11499,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>1085</v>
       </c>
@@ -11519,7 +11531,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>1086</v>
       </c>
@@ -11551,7 +11563,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>1087</v>
       </c>
@@ -11583,7 +11595,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>1088</v>
       </c>
@@ -11615,7 +11627,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>1089</v>
       </c>
@@ -11647,7 +11659,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>1090</v>
       </c>
@@ -11679,7 +11691,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>1091</v>
       </c>
@@ -11711,7 +11723,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>1092</v>
       </c>
@@ -11743,7 +11755,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>1093</v>
       </c>
@@ -11775,7 +11787,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>1094</v>
       </c>
@@ -11807,7 +11819,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>1095</v>
       </c>
@@ -11839,7 +11851,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>1096</v>
       </c>
@@ -11871,7 +11883,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>1097</v>
       </c>
@@ -11903,7 +11915,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>1098</v>
       </c>
@@ -11935,7 +11947,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>1099</v>
       </c>
@@ -11967,7 +11979,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>1100</v>
       </c>
@@ -11999,7 +12011,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>1101</v>
       </c>
@@ -12031,7 +12043,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>1102</v>
       </c>
@@ -12063,7 +12075,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>1103</v>
       </c>
@@ -12095,7 +12107,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>1104</v>
       </c>
@@ -12127,7 +12139,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>1106</v>
       </c>
@@ -12159,7 +12171,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>1107</v>
       </c>
@@ -12188,7 +12200,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>1108</v>
       </c>
@@ -12217,7 +12229,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>1112</v>
       </c>
@@ -12249,7 +12261,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>1114</v>
       </c>
@@ -12281,7 +12293,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>1115</v>
       </c>
@@ -12313,7 +12325,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>1117</v>
       </c>
@@ -12345,7 +12357,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>1118</v>
       </c>
@@ -12377,7 +12389,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>1119</v>
       </c>
@@ -12409,7 +12421,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>1120</v>
       </c>
@@ -12441,7 +12453,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>1121</v>
       </c>
@@ -12470,7 +12482,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>1122</v>
       </c>
@@ -12502,7 +12514,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>1125</v>
       </c>
@@ -12534,7 +12546,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>1133</v>
       </c>
@@ -12566,7 +12578,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>1134</v>
       </c>
@@ -12598,7 +12610,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>117</v>
       </c>
@@ -12641,25 +12653,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J129"/>
+  <dimension ref="A1:J130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="F129" sqref="F129"/>
+    <sheetView tabSelected="1" topLeftCell="D121" workbookViewId="0">
+      <selection activeCell="J135" sqref="J135"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="16.5" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="18.375" customWidth="1"/>
-    <col min="7" max="7" width="29.125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="30.125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="29.08203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.08203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="30.08203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>990</v>
       </c>
@@ -12691,7 +12703,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>997</v>
       </c>
@@ -12723,7 +12735,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1000</v>
       </c>
@@ -12755,7 +12767,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -12787,7 +12799,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1001</v>
       </c>
@@ -12819,7 +12831,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1003</v>
       </c>
@@ -12851,7 +12863,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1004</v>
       </c>
@@ -12883,7 +12895,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>1006</v>
       </c>
@@ -12915,7 +12927,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>1007</v>
       </c>
@@ -12947,7 +12959,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>1008</v>
       </c>
@@ -12979,7 +12991,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>1009</v>
       </c>
@@ -13011,7 +13023,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>1010</v>
       </c>
@@ -13043,7 +13055,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>1011</v>
       </c>
@@ -13075,7 +13087,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>1012</v>
       </c>
@@ -13107,7 +13119,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>1013</v>
       </c>
@@ -13139,7 +13151,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>1014</v>
       </c>
@@ -13171,7 +13183,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>1015</v>
       </c>
@@ -13203,7 +13215,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>1016</v>
       </c>
@@ -13235,7 +13247,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>1017</v>
       </c>
@@ -13267,7 +13279,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>1018</v>
       </c>
@@ -13299,7 +13311,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>1019</v>
       </c>
@@ -13331,7 +13343,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>1020</v>
       </c>
@@ -13363,7 +13375,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>1021</v>
       </c>
@@ -13395,7 +13407,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>1023</v>
       </c>
@@ -13427,7 +13439,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>1024</v>
       </c>
@@ -13459,7 +13471,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>1025</v>
       </c>
@@ -13491,7 +13503,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>1026</v>
       </c>
@@ -13523,7 +13535,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>1027</v>
       </c>
@@ -13555,7 +13567,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>1028</v>
       </c>
@@ -13587,7 +13599,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>1029</v>
       </c>
@@ -13619,7 +13631,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>1030</v>
       </c>
@@ -13651,7 +13663,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>1031</v>
       </c>
@@ -13683,7 +13695,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>1033</v>
       </c>
@@ -13715,7 +13727,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>1034</v>
       </c>
@@ -13747,7 +13759,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>1035</v>
       </c>
@@ -13779,7 +13791,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>1037</v>
       </c>
@@ -13811,7 +13823,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>1038</v>
       </c>
@@ -13843,7 +13855,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>1039</v>
       </c>
@@ -13875,7 +13887,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>1040</v>
       </c>
@@ -13907,7 +13919,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>1041</v>
       </c>
@@ -13939,7 +13951,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>1042</v>
       </c>
@@ -13971,7 +13983,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>1043</v>
       </c>
@@ -14003,7 +14015,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>1044</v>
       </c>
@@ -14035,7 +14047,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>1045</v>
       </c>
@@ -14067,7 +14079,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>1046</v>
       </c>
@@ -14099,7 +14111,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>1047</v>
       </c>
@@ -14131,7 +14143,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>1048</v>
       </c>
@@ -14163,7 +14175,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>1049</v>
       </c>
@@ -14195,7 +14207,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>1050</v>
       </c>
@@ -14227,7 +14239,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>1051</v>
       </c>
@@ -14259,7 +14271,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>1053</v>
       </c>
@@ -14291,7 +14303,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>1054</v>
       </c>
@@ -14323,7 +14335,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>1055</v>
       </c>
@@ -14355,7 +14367,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>1056</v>
       </c>
@@ -14387,7 +14399,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>1057</v>
       </c>
@@ -14419,7 +14431,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>1058</v>
       </c>
@@ -14451,7 +14463,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>1059</v>
       </c>
@@ -14483,7 +14495,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>1061</v>
       </c>
@@ -14515,7 +14527,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>1062</v>
       </c>
@@ -14547,7 +14559,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>1063</v>
       </c>
@@ -14579,7 +14591,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>1064</v>
       </c>
@@ -14611,7 +14623,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>1065</v>
       </c>
@@ -14643,7 +14655,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>1066</v>
       </c>
@@ -14675,7 +14687,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>1067</v>
       </c>
@@ -14707,7 +14719,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>1068</v>
       </c>
@@ -14739,7 +14751,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>1069</v>
       </c>
@@ -14771,7 +14783,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>1070</v>
       </c>
@@ -14803,7 +14815,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>1071</v>
       </c>
@@ -14835,7 +14847,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>1072</v>
       </c>
@@ -14867,7 +14879,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>1073</v>
       </c>
@@ -14899,7 +14911,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>1074</v>
       </c>
@@ -14931,7 +14943,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>1075</v>
       </c>
@@ -14963,7 +14975,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>1076</v>
       </c>
@@ -14995,7 +15007,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>1077</v>
       </c>
@@ -15027,7 +15039,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>1078</v>
       </c>
@@ -15059,7 +15071,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>1079</v>
       </c>
@@ -15091,7 +15103,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>1080</v>
       </c>
@@ -15123,7 +15135,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>1082</v>
       </c>
@@ -15155,7 +15167,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>1083</v>
       </c>
@@ -15187,7 +15199,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>1084</v>
       </c>
@@ -15219,7 +15231,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>1085</v>
       </c>
@@ -15251,7 +15263,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>1086</v>
       </c>
@@ -15283,7 +15295,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>1087</v>
       </c>
@@ -15315,7 +15327,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>1088</v>
       </c>
@@ -15347,7 +15359,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>1089</v>
       </c>
@@ -15379,7 +15391,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>1090</v>
       </c>
@@ -15411,7 +15423,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>1091</v>
       </c>
@@ -15443,7 +15455,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>1092</v>
       </c>
@@ -15472,7 +15484,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>1093</v>
       </c>
@@ -15501,7 +15513,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>1094</v>
       </c>
@@ -15533,7 +15545,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>1095</v>
       </c>
@@ -15565,7 +15577,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>1096</v>
       </c>
@@ -15597,7 +15609,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>1097</v>
       </c>
@@ -15629,7 +15641,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>1098</v>
       </c>
@@ -15661,7 +15673,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>1099</v>
       </c>
@@ -15693,7 +15705,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>1100</v>
       </c>
@@ -15725,7 +15737,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>1101</v>
       </c>
@@ -15757,7 +15769,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>1102</v>
       </c>
@@ -15786,7 +15798,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>1103</v>
       </c>
@@ -15818,7 +15830,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>1104</v>
       </c>
@@ -15850,7 +15862,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>1106</v>
       </c>
@@ -15882,7 +15894,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>1107</v>
       </c>
@@ -15914,7 +15926,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>1108</v>
       </c>
@@ -15946,7 +15958,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>1112</v>
       </c>
@@ -15978,7 +15990,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>1114</v>
       </c>
@@ -16010,7 +16022,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>1115</v>
       </c>
@@ -16042,7 +16054,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>1117</v>
       </c>
@@ -16074,7 +16086,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>1118</v>
       </c>
@@ -16106,7 +16118,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>1119</v>
       </c>
@@ -16138,7 +16150,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>1154</v>
       </c>
@@ -16170,7 +16182,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>1120</v>
       </c>
@@ -16202,7 +16214,7 @@
         <v>1164</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>1121</v>
       </c>
@@ -16234,7 +16246,7 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>113</v>
       </c>
@@ -16266,7 +16278,7 @@
         <v>1147</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>114</v>
       </c>
@@ -16298,7 +16310,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>115</v>
       </c>
@@ -16330,7 +16342,7 @@
         <v>1181</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>116</v>
       </c>
@@ -16359,7 +16371,7 @@
         <v>1187</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>117</v>
       </c>
@@ -16391,7 +16403,7 @@
         <v>1194</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>118</v>
       </c>
@@ -16423,7 +16435,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>119</v>
       </c>
@@ -16455,7 +16467,7 @@
         <v>1197</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>120</v>
       </c>
@@ -16487,7 +16499,7 @@
         <v>1203</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>121</v>
       </c>
@@ -16519,7 +16531,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>122</v>
       </c>
@@ -16551,7 +16563,7 @@
         <v>1212</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B124" t="s">
         <v>1218</v>
       </c>
@@ -16580,7 +16592,7 @@
         <v>1217</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B125" t="s">
         <v>1219</v>
       </c>
@@ -16606,7 +16618,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B126" t="s">
         <v>644</v>
       </c>
@@ -16632,7 +16644,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B127" t="s">
         <v>1228</v>
       </c>
@@ -16655,7 +16667,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B128" t="s">
         <v>532</v>
       </c>
@@ -16678,7 +16690,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="129" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B129" t="s">
         <v>1236</v>
       </c>
@@ -16699,6 +16711,35 @@
       </c>
       <c r="I129" s="1" t="s">
         <v>1240</v>
+      </c>
+    </row>
+    <row r="130" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B130" t="s">
+        <v>1241</v>
+      </c>
+      <c r="C130" t="s">
+        <v>1242</v>
+      </c>
+      <c r="D130" t="s">
+        <v>1243</v>
+      </c>
+      <c r="E130">
+        <v>692041830</v>
+      </c>
+      <c r="F130" t="s">
+        <v>1161</v>
+      </c>
+      <c r="G130" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H130" t="s">
+        <v>1244</v>
+      </c>
+      <c r="I130" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J130" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -16729,8 +16770,9 @@
     <hyperlink ref="G127" r:id="rId24" xr:uid="{00000000-0004-0000-0200-000017000000}"/>
     <hyperlink ref="G128" r:id="rId25" xr:uid="{00000000-0004-0000-0200-000018000000}"/>
     <hyperlink ref="G129" r:id="rId26" xr:uid="{4D4F6C73-7B5B-465E-B35A-0EA7EA1E0F6C}"/>
+    <hyperlink ref="G130" r:id="rId27" xr:uid="{13CC8746-5F90-4CB5-B13B-581C0B2867D4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId27"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId28"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added my details to the excel
</commit_message>
<xml_diff>
--- a/CS335/GitHub Info sans duplicates.xlsx
+++ b/CS335/GitHub Info sans duplicates.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neemafaraja\Documents\staffcard\CS335\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\applications\Other applications\staffcard\CS335\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A61BEE-5F9D-46CF-9114-1EF0C830C6E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3904" uniqueCount="1246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3912" uniqueCount="1249">
   <si>
     <t>Timestamp</t>
   </si>
@@ -3760,12 +3759,21 @@
   </si>
   <si>
     <t>2019-04-03565</t>
+  </si>
+  <si>
+    <t>Mhuli</t>
+  </si>
+  <si>
+    <t>Stephen Robert</t>
+  </si>
+  <si>
+    <t>https://github.com/Stevo237</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd\ h:mm"/>
   </numFmts>
@@ -4112,7 +4120,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P127"/>
   <sheetViews>
     <sheetView topLeftCell="A115" workbookViewId="0">
@@ -8917,8 +8925,8 @@
     <mergeCell ref="L104:M104"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G104" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="L104" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G104" r:id="rId1"/>
+    <hyperlink ref="L104" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -8926,7 +8934,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12647,7 +12655,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G117" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="G117" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -12655,11 +12663,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J130"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="F118" workbookViewId="0">
+      <selection activeCell="J131" sqref="J131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -16745,37 +16753,67 @@
         <v>31</v>
       </c>
     </row>
+    <row r="131" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B131" t="s">
+        <v>573</v>
+      </c>
+      <c r="C131" t="s">
+        <v>1246</v>
+      </c>
+      <c r="D131" t="s">
+        <v>1247</v>
+      </c>
+      <c r="E131">
+        <v>742726716</v>
+      </c>
+      <c r="F131" t="s">
+        <v>17</v>
+      </c>
+      <c r="G131" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="H131" t="s">
+        <v>999</v>
+      </c>
+      <c r="I131" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="J131" s="1" t="s">
+        <v>1248</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G114" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="G59" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="J59" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="G115" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="J115" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
-    <hyperlink ref="G116" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
-    <hyperlink ref="J116" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
-    <hyperlink ref="G117" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
-    <hyperlink ref="J117" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
-    <hyperlink ref="G118" r:id="rId10" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
-    <hyperlink ref="J118" r:id="rId11" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
-    <hyperlink ref="G119" r:id="rId12" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
-    <hyperlink ref="J119" r:id="rId13" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
-    <hyperlink ref="G120" r:id="rId14" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
-    <hyperlink ref="J120" r:id="rId15" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
-    <hyperlink ref="G121" r:id="rId16" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
-    <hyperlink ref="J121" r:id="rId17" xr:uid="{00000000-0004-0000-0200-000010000000}"/>
-    <hyperlink ref="G122" r:id="rId18" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
-    <hyperlink ref="J122" r:id="rId19" tooltip="https://github.com/machuchesteven" xr:uid="{00000000-0004-0000-0200-000012000000}"/>
-    <hyperlink ref="G123" r:id="rId20" xr:uid="{00000000-0004-0000-0200-000013000000}"/>
-    <hyperlink ref="J123" r:id="rId21" xr:uid="{00000000-0004-0000-0200-000014000000}"/>
-    <hyperlink ref="G124" r:id="rId22" xr:uid="{00000000-0004-0000-0200-000015000000}"/>
-    <hyperlink ref="J124" r:id="rId23" xr:uid="{00000000-0004-0000-0200-000016000000}"/>
-    <hyperlink ref="G127" r:id="rId24" xr:uid="{00000000-0004-0000-0200-000017000000}"/>
-    <hyperlink ref="G128" r:id="rId25" xr:uid="{00000000-0004-0000-0200-000018000000}"/>
-    <hyperlink ref="G129" r:id="rId26" xr:uid="{4D4F6C73-7B5B-465E-B35A-0EA7EA1E0F6C}"/>
-    <hyperlink ref="G130" r:id="rId27" xr:uid="{13CC8746-5F90-4CB5-B13B-581C0B2867D4}"/>
+    <hyperlink ref="G114" r:id="rId1"/>
+    <hyperlink ref="G59" r:id="rId2"/>
+    <hyperlink ref="J59" r:id="rId3"/>
+    <hyperlink ref="G115" r:id="rId4"/>
+    <hyperlink ref="J115" r:id="rId5"/>
+    <hyperlink ref="G116" r:id="rId6"/>
+    <hyperlink ref="J116" r:id="rId7"/>
+    <hyperlink ref="G117" r:id="rId8"/>
+    <hyperlink ref="J117" r:id="rId9"/>
+    <hyperlink ref="G118" r:id="rId10"/>
+    <hyperlink ref="J118" r:id="rId11"/>
+    <hyperlink ref="G119" r:id="rId12"/>
+    <hyperlink ref="J119" r:id="rId13"/>
+    <hyperlink ref="G120" r:id="rId14"/>
+    <hyperlink ref="J120" r:id="rId15"/>
+    <hyperlink ref="G121" r:id="rId16"/>
+    <hyperlink ref="J121" r:id="rId17"/>
+    <hyperlink ref="G122" r:id="rId18"/>
+    <hyperlink ref="J122" r:id="rId19" tooltip="https://github.com/machuchesteven"/>
+    <hyperlink ref="G123" r:id="rId20"/>
+    <hyperlink ref="J123" r:id="rId21"/>
+    <hyperlink ref="G124" r:id="rId22"/>
+    <hyperlink ref="J124" r:id="rId23"/>
+    <hyperlink ref="G127" r:id="rId24"/>
+    <hyperlink ref="G128" r:id="rId25"/>
+    <hyperlink ref="G129" r:id="rId26"/>
+    <hyperlink ref="G130" r:id="rId27"/>
+    <hyperlink ref="G131" r:id="rId28"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId28"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId29"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change number and name
</commit_message>
<xml_diff>
--- a/CS335/GitHub Info sans duplicates.xlsx
+++ b/CS335/GitHub Info sans duplicates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\staffcard\CS335\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C5C3ED-ACFD-48DE-897D-0F2DDEF233BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93506A33-81BC-4DB1-9E99-6833D7FD62E5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="22692" windowHeight="14592" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3301" uniqueCount="910">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3300" uniqueCount="911">
   <si>
     <t>Timestamp</t>
   </si>
@@ -2763,6 +2763,9 @@
   </si>
   <si>
     <t>0719912159</t>
+  </si>
+  <si>
+    <t>DEOGRATIAS GASPER</t>
   </si>
 </sst>
 </file>
@@ -3280,14 +3283,14 @@
       <selection pane="bottomLeft" activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="21.46484375" customWidth="1"/>
-    <col min="7" max="7" width="29.796875" customWidth="1"/>
-    <col min="8" max="18" width="21.46484375" customWidth="1"/>
+    <col min="1" max="6" width="21.44140625" customWidth="1"/>
+    <col min="7" max="7" width="29.77734375" customWidth="1"/>
+    <col min="8" max="18" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3325,7 +3328,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44517.7927395718</v>
       </c>
@@ -3363,7 +3366,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>44517.829278495403</v>
       </c>
@@ -3401,7 +3404,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>44517.829803020803</v>
       </c>
@@ -3439,7 +3442,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>44517.832974606499</v>
       </c>
@@ -3477,7 +3480,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>44517.833342615697</v>
       </c>
@@ -3515,7 +3518,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>44517.834096585699</v>
       </c>
@@ -3553,7 +3556,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>44517.834304884302</v>
       </c>
@@ -3591,7 +3594,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>44517.834315161999</v>
       </c>
@@ -3629,7 +3632,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>44517.834467222201</v>
       </c>
@@ -3667,7 +3670,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>44517.836256620401</v>
       </c>
@@ -3705,7 +3708,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>44517.840131203702</v>
       </c>
@@ -3743,7 +3746,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>44517.840687338001</v>
       </c>
@@ -3781,7 +3784,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>44517.840723900503</v>
       </c>
@@ -3819,7 +3822,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>44517.848194363403</v>
       </c>
@@ -3857,7 +3860,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>44517.849799363401</v>
       </c>
@@ -3895,7 +3898,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>44517.851121805601</v>
       </c>
@@ -3933,7 +3936,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>44517.853374618098</v>
       </c>
@@ -3971,7 +3974,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>44517.855156886602</v>
       </c>
@@ -4009,7 +4012,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>44517.8585572917</v>
       </c>
@@ -4047,7 +4050,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>44517.8591194213</v>
       </c>
@@ -4085,7 +4088,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>44517.860663136598</v>
       </c>
@@ -4123,7 +4126,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>44517.863773090299</v>
       </c>
@@ -4161,7 +4164,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>44517.867895196803</v>
       </c>
@@ -4199,7 +4202,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>44517.868303217598</v>
       </c>
@@ -4237,7 +4240,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>44517.8691914468</v>
       </c>
@@ -4275,7 +4278,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>44517.874595833302</v>
       </c>
@@ -4313,7 +4316,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>44517.877297905099</v>
       </c>
@@ -4351,7 +4354,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>44517.877863588001</v>
       </c>
@@ -4389,7 +4392,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>44517.886029872701</v>
       </c>
@@ -4427,7 +4430,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>44517.888174652799</v>
       </c>
@@ -4465,7 +4468,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>44517.890895740697</v>
       </c>
@@ -4503,7 +4506,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>44517.898055138903</v>
       </c>
@@ -4541,7 +4544,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>44517.9033859259</v>
       </c>
@@ -4579,7 +4582,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>44517.916796608799</v>
       </c>
@@ -4617,7 +4620,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>44517.919944965302</v>
       </c>
@@ -4655,7 +4658,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>44517.920173611114</v>
       </c>
@@ -4693,7 +4696,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>44517.94259259259</v>
       </c>
@@ -4731,7 +4734,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>44517.920207002302</v>
       </c>
@@ -4769,7 +4772,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>44517.925676088002</v>
       </c>
@@ -4807,7 +4810,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>44517.942313136598</v>
       </c>
@@ -4845,7 +4848,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>44517.967181493099</v>
       </c>
@@ -4883,7 +4886,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>44517.9708563889</v>
       </c>
@@ -4921,7 +4924,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>44517.974103865701</v>
       </c>
@@ -4959,7 +4962,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44517.995788911998</v>
       </c>
@@ -4997,7 +5000,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>44518.053331921299</v>
       </c>
@@ -5035,7 +5038,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>44518.1416807407</v>
       </c>
@@ -5073,7 +5076,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>44518.338707534698</v>
       </c>
@@ -5111,7 +5114,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>44518.348475844898</v>
       </c>
@@ -5149,7 +5152,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>44518.368981018502</v>
       </c>
@@ -5187,7 +5190,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>44518.376564247701</v>
       </c>
@@ -5225,7 +5228,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>44518.395640312498</v>
       </c>
@@ -5263,7 +5266,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>44518.396610844902</v>
       </c>
@@ -5301,7 +5304,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>44518.416108634301</v>
       </c>
@@ -5339,7 +5342,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>44518.419745173604</v>
       </c>
@@ -5377,7 +5380,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>44518.433273449104</v>
       </c>
@@ -5415,7 +5418,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>44518.433606898201</v>
       </c>
@@ -5453,7 +5456,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>44518.462937638898</v>
       </c>
@@ -5491,7 +5494,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>44518.4791463773</v>
       </c>
@@ -5529,7 +5532,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>44518.500450555599</v>
       </c>
@@ -5567,7 +5570,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>44518.545351886598</v>
       </c>
@@ -5605,7 +5608,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>44518.5769178357</v>
       </c>
@@ -5643,7 +5646,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>44518.580951863398</v>
       </c>
@@ -5681,7 +5684,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>44518.584114340301</v>
       </c>
@@ -5719,7 +5722,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>44518.599512685199</v>
       </c>
@@ -5757,7 +5760,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>44518.6111335069</v>
       </c>
@@ -5795,7 +5798,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>44518.639018194401</v>
       </c>
@@ -5833,7 +5836,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>44518.656796018498</v>
       </c>
@@ -5871,7 +5874,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>44518.669622650501</v>
       </c>
@@ -5909,7 +5912,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>44518.675713946803</v>
       </c>
@@ -5947,7 +5950,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>44518.678410173598</v>
       </c>
@@ -5985,7 +5988,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>44518.679047175901</v>
       </c>
@@ -6023,7 +6026,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>44518.681073298598</v>
       </c>
@@ -6061,7 +6064,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>44518.681981574096</v>
       </c>
@@ -6099,7 +6102,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>44518.682995844902</v>
       </c>
@@ -6137,7 +6140,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>44518.684843472198</v>
       </c>
@@ -6175,7 +6178,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>44518.690567743099</v>
       </c>
@@ -6213,7 +6216,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>44518.704118368099</v>
       </c>
@@ -6251,7 +6254,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>44518.7172751736</v>
       </c>
@@ -6289,7 +6292,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="80" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>44518.718211203697</v>
       </c>
@@ -6327,7 +6330,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="81" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>44518.7218906829</v>
       </c>
@@ -6365,7 +6368,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="82" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>44518.845550972197</v>
       </c>
@@ -6403,7 +6406,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="83" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>44518.845807673599</v>
       </c>
@@ -6441,7 +6444,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="84" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>44518.847130671304</v>
       </c>
@@ -6479,7 +6482,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="85" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>44518.8480487384</v>
       </c>
@@ -6517,7 +6520,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="86" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>44518.848206620401</v>
       </c>
@@ -6555,7 +6558,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="87" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>44518.851609803198</v>
       </c>
@@ -6593,7 +6596,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="88" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>44518.853343229202</v>
       </c>
@@ -6631,7 +6634,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="89" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>44518.854456469897</v>
       </c>
@@ -6669,7 +6672,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="90" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>44518.857002847202</v>
       </c>
@@ -6707,7 +6710,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="91" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>44518.857458969898</v>
       </c>
@@ -6745,7 +6748,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="92" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>44518.864664201399</v>
       </c>
@@ -6783,7 +6786,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="93" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>44518.865544432898</v>
       </c>
@@ -6821,7 +6824,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="94" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>44518.8734887963</v>
       </c>
@@ -6859,7 +6862,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="95" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>44518.880978576402</v>
       </c>
@@ -6897,7 +6900,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="96" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>44518.890144791701</v>
       </c>
@@ -6935,7 +6938,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="97" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>44518.8926736227</v>
       </c>
@@ -6973,7 +6976,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="98" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>44518.893882627301</v>
       </c>
@@ -7011,7 +7014,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="99" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>44518.895629976803</v>
       </c>
@@ -7049,7 +7052,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="100" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>44518.8972680324</v>
       </c>
@@ -7087,7 +7090,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="101" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>44518.901678900504</v>
       </c>
@@ -7125,7 +7128,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="102" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>44518.905369791697</v>
       </c>
@@ -7163,7 +7166,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="103" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>44518.914951886603</v>
       </c>
@@ -7201,7 +7204,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="104" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>44518.926460324103</v>
       </c>
@@ -7236,7 +7239,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="105" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>44518.9439103357</v>
       </c>
@@ -7271,7 +7274,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="106" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>44518.949051713003</v>
       </c>
@@ -7309,7 +7312,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="107" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>44518.949835740699</v>
       </c>
@@ -7347,7 +7350,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="108" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>44518.954430393504</v>
       </c>
@@ -7385,7 +7388,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="109" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>44518.964523217597</v>
       </c>
@@ -7423,7 +7426,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="110" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>44518.971188981501</v>
       </c>
@@ -7461,7 +7464,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="111" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>44518.9722345833</v>
       </c>
@@ -7499,7 +7502,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="112" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>44518.972730138899</v>
       </c>
@@ -7537,7 +7540,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="113" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>44518.977785532399</v>
       </c>
@@ -7575,7 +7578,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="114" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="7">
         <v>44519.003693425897</v>
       </c>
@@ -7617,7 +7620,7 @@
       <c r="Q114" s="9"/>
       <c r="R114" s="9"/>
     </row>
-    <row r="115" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>44521.695289421303</v>
       </c>
@@ -7655,7 +7658,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="116" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>44521.703645162001</v>
       </c>
@@ -7693,7 +7696,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="117" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>44521.798439618098</v>
       </c>
@@ -7731,7 +7734,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="118" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>44521.806830486101</v>
       </c>
@@ -7769,7 +7772,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="119" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>44521.997838750001</v>
       </c>
@@ -7807,7 +7810,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="120" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>44522.038008958298</v>
       </c>
@@ -7845,7 +7848,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="121" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <v>44522.396687349501</v>
       </c>
@@ -7883,7 +7886,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="122" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>44522.424870671297</v>
       </c>
@@ -7921,7 +7924,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="123" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>44522.601772291702</v>
       </c>
@@ -7959,43 +7962,43 @@
         <v>849</v>
       </c>
     </row>
-    <row r="124" spans="1:18" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="125" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:18" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K125" s="12" t="s">
         <v>850</v>
       </c>
     </row>
-    <row r="126" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K126" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="127" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K127" t="s">
         <v>851</v>
       </c>
     </row>
-    <row r="128" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K128" t="s">
         <v>852</v>
       </c>
     </row>
-    <row r="129" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K129" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="130" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K130" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="131" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K131" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="132" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K132" t="s">
         <v>853</v>
       </c>
@@ -8141,26 +8144,26 @@
   <dimension ref="A1:P212"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G119" sqref="G119"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.265625" customWidth="1"/>
-    <col min="2" max="2" width="16.796875" customWidth="1"/>
-    <col min="3" max="3" width="15.73046875" customWidth="1"/>
-    <col min="4" max="4" width="25.46484375" customWidth="1"/>
-    <col min="5" max="5" width="16.796875" style="22" customWidth="1"/>
+    <col min="1" max="1" width="4.21875" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" customWidth="1"/>
+    <col min="3" max="3" width="15.77734375" customWidth="1"/>
+    <col min="4" max="4" width="25.44140625" customWidth="1"/>
+    <col min="5" max="5" width="16.77734375" style="22" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="33.19921875" customWidth="1"/>
-    <col min="8" max="8" width="9.46484375" customWidth="1"/>
-    <col min="9" max="9" width="17.46484375" customWidth="1"/>
-    <col min="10" max="10" width="33.19921875" customWidth="1"/>
-    <col min="11" max="16" width="21.46484375" customWidth="1"/>
+    <col min="7" max="7" width="33.21875" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" customWidth="1"/>
+    <col min="9" max="9" width="17.44140625" customWidth="1"/>
+    <col min="10" max="10" width="33.21875" customWidth="1"/>
+    <col min="11" max="16" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>854</v>
       </c>
@@ -8198,7 +8201,7 @@
       <c r="O1" s="13"/>
       <c r="P1" s="13"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -8230,7 +8233,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -8262,7 +8265,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -8294,7 +8297,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -8326,7 +8329,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -8358,7 +8361,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -8390,7 +8393,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -8422,7 +8425,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -8454,7 +8457,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -8486,7 +8489,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -8518,7 +8521,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -8550,7 +8553,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -8582,7 +8585,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -8614,7 +8617,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -8646,7 +8649,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -8678,7 +8681,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -8710,7 +8713,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -8742,7 +8745,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="38.25" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -8753,13 +8756,13 @@
         <v>145</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>146</v>
+        <v>910</v>
       </c>
       <c r="E19" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>861</v>
+      <c r="F19" s="3">
+        <v>68559145</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>148</v>
@@ -8774,7 +8777,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -8806,7 +8809,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -8838,7 +8841,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -8870,7 +8873,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -8902,7 +8905,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -8934,7 +8937,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -8966,7 +8969,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -8998,7 +9001,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -9030,7 +9033,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -9062,7 +9065,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -9094,7 +9097,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -9126,7 +9129,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -9158,7 +9161,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -9190,7 +9193,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -9222,7 +9225,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -9254,7 +9257,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -9286,7 +9289,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -9318,7 +9321,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -9350,7 +9353,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -9382,7 +9385,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -9414,7 +9417,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -9446,7 +9449,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -9478,7 +9481,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -9510,7 +9513,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -9542,7 +9545,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -9574,7 +9577,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -9606,7 +9609,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -9638,7 +9641,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -9670,7 +9673,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -9702,7 +9705,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -9734,7 +9737,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -9766,7 +9769,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -9798,7 +9801,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -9830,7 +9833,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -9862,7 +9865,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -9894,7 +9897,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -9926,7 +9929,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -9958,7 +9961,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -9990,7 +9993,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -10022,7 +10025,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -10054,7 +10057,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -10086,7 +10089,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -10118,7 +10121,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -10150,7 +10153,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -10182,7 +10185,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -10214,7 +10217,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -10246,7 +10249,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -10278,7 +10281,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -10310,7 +10313,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -10342,7 +10345,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -10374,7 +10377,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -10406,7 +10409,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -10438,7 +10441,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -10470,7 +10473,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -10502,7 +10505,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -10534,7 +10537,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -10566,7 +10569,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -10598,7 +10601,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -10630,7 +10633,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -10662,7 +10665,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -10694,7 +10697,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -10726,7 +10729,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -10758,7 +10761,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -10790,7 +10793,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -10822,7 +10825,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>83</v>
       </c>
@@ -10854,7 +10857,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>84</v>
       </c>
@@ -10886,7 +10889,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>85</v>
       </c>
@@ -10918,7 +10921,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>86</v>
       </c>
@@ -10950,7 +10953,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>87</v>
       </c>
@@ -10982,7 +10985,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>88</v>
       </c>
@@ -11014,7 +11017,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>89</v>
       </c>
@@ -11046,7 +11049,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>90</v>
       </c>
@@ -11078,7 +11081,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>91</v>
       </c>
@@ -11110,7 +11113,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>92</v>
       </c>
@@ -11142,7 +11145,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>93</v>
       </c>
@@ -11174,7 +11177,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>94</v>
       </c>
@@ -11206,7 +11209,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>95</v>
       </c>
@@ -11238,7 +11241,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>96</v>
       </c>
@@ -11270,7 +11273,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>97</v>
       </c>
@@ -11302,7 +11305,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>98</v>
       </c>
@@ -11334,7 +11337,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>99</v>
       </c>
@@ -11366,7 +11369,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>100</v>
       </c>
@@ -11398,7 +11401,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>101</v>
       </c>
@@ -11427,7 +11430,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <v>102</v>
       </c>
@@ -11456,7 +11459,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <v>103</v>
       </c>
@@ -11488,7 +11491,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>104</v>
       </c>
@@ -11520,7 +11523,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
         <v>105</v>
       </c>
@@ -11552,7 +11555,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
         <v>106</v>
       </c>
@@ -11584,7 +11587,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
         <v>107</v>
       </c>
@@ -11616,7 +11619,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
         <v>108</v>
       </c>
@@ -11648,7 +11651,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
         <v>109</v>
       </c>
@@ -11680,7 +11683,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
         <v>110</v>
       </c>
@@ -11712,7 +11715,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
         <v>111</v>
       </c>
@@ -11741,7 +11744,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
         <v>112</v>
       </c>
@@ -11773,7 +11776,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
         <v>113</v>
       </c>
@@ -11805,7 +11808,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
         <v>114</v>
       </c>
@@ -11837,7 +11840,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="3">
         <v>115</v>
       </c>
@@ -11869,7 +11872,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="3">
         <v>116</v>
       </c>
@@ -11901,7 +11904,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="3">
         <v>117</v>
       </c>
@@ -11933,7 +11936,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="3">
         <v>118</v>
       </c>
@@ -11965,283 +11968,283 @@
         <v>626</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J120" s="16"/>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J121" s="16"/>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J122" s="16"/>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J123" s="16"/>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J124" s="16"/>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J125" s="16"/>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J126" s="16"/>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J127" s="16"/>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J128" s="16"/>
     </row>
-    <row r="129" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="129" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J129" s="16"/>
     </row>
-    <row r="130" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="130" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J130" s="16"/>
     </row>
-    <row r="131" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="131" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J131" s="16"/>
     </row>
-    <row r="132" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="132" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J132" s="16"/>
     </row>
-    <row r="133" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="133" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J133" s="16"/>
     </row>
-    <row r="134" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="134" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J134" s="16"/>
     </row>
-    <row r="135" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="135" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J135" s="16"/>
     </row>
-    <row r="136" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="136" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J136" s="16"/>
     </row>
-    <row r="137" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="137" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J137" s="16"/>
     </row>
-    <row r="138" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="138" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J138" s="16"/>
     </row>
-    <row r="139" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="139" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J139" s="16"/>
     </row>
-    <row r="140" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="140" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J140" s="16"/>
     </row>
-    <row r="141" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="141" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J141" s="16"/>
     </row>
-    <row r="142" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="142" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J142" s="16"/>
     </row>
-    <row r="143" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="143" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J143" s="16"/>
     </row>
-    <row r="144" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="144" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J144" s="16"/>
     </row>
-    <row r="145" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="145" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J145" s="16"/>
     </row>
-    <row r="146" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="146" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J146" s="16"/>
     </row>
-    <row r="147" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="147" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J147" s="16"/>
     </row>
-    <row r="148" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="148" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J148" s="16"/>
     </row>
-    <row r="149" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="149" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J149" s="16"/>
     </row>
-    <row r="150" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="150" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J150" s="16"/>
     </row>
-    <row r="151" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="151" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J151" s="16"/>
     </row>
-    <row r="152" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="152" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J152" s="16"/>
     </row>
-    <row r="153" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="153" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J153" s="16"/>
     </row>
-    <row r="154" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="154" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J154" s="16"/>
     </row>
-    <row r="155" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="155" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J155" s="16"/>
     </row>
-    <row r="156" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="156" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J156" s="16"/>
     </row>
-    <row r="157" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="157" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J157" s="16"/>
     </row>
-    <row r="158" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="158" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J158" s="16"/>
     </row>
-    <row r="159" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="159" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J159" s="16"/>
     </row>
-    <row r="160" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="160" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J160" s="16"/>
     </row>
-    <row r="161" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="161" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J161" s="16"/>
     </row>
-    <row r="162" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="162" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J162" s="16"/>
     </row>
-    <row r="163" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="163" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J163" s="16"/>
     </row>
-    <row r="164" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="164" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J164" s="16"/>
     </row>
-    <row r="165" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="165" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J165" s="16"/>
     </row>
-    <row r="166" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="166" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J166" s="16"/>
     </row>
-    <row r="167" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="167" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J167" s="16"/>
     </row>
-    <row r="168" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="168" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J168" s="16"/>
     </row>
-    <row r="169" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="169" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J169" s="16"/>
     </row>
-    <row r="170" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="170" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J170" s="16"/>
     </row>
-    <row r="171" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="171" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J171" s="16"/>
     </row>
-    <row r="172" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="172" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J172" s="16"/>
     </row>
-    <row r="173" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="173" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J173" s="16"/>
     </row>
-    <row r="174" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="174" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J174" s="16"/>
     </row>
-    <row r="175" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="175" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J175" s="16"/>
     </row>
-    <row r="176" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="176" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J176" s="16"/>
     </row>
-    <row r="177" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="177" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J177" s="16"/>
     </row>
-    <row r="178" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="178" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J178" s="16"/>
     </row>
-    <row r="179" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="179" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J179" s="16"/>
     </row>
-    <row r="180" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="180" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J180" s="16"/>
     </row>
-    <row r="181" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="181" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J181" s="16"/>
     </row>
-    <row r="182" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="182" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J182" s="16"/>
     </row>
-    <row r="183" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="183" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J183" s="16"/>
     </row>
-    <row r="184" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="184" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J184" s="16"/>
     </row>
-    <row r="185" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="185" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J185" s="16"/>
     </row>
-    <row r="186" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="186" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J186" s="16"/>
     </row>
-    <row r="187" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="187" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J187" s="16"/>
     </row>
-    <row r="188" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="188" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J188" s="16"/>
     </row>
-    <row r="189" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="189" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J189" s="16"/>
     </row>
-    <row r="190" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="190" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J190" s="16"/>
     </row>
-    <row r="191" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="191" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J191" s="16"/>
     </row>
-    <row r="192" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="192" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J192" s="16"/>
     </row>
-    <row r="193" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="193" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J193" s="16"/>
     </row>
-    <row r="194" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="194" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J194" s="16"/>
     </row>
-    <row r="195" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="195" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J195" s="16"/>
     </row>
-    <row r="196" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="196" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J196" s="16"/>
     </row>
-    <row r="197" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="197" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J197" s="16"/>
     </row>
-    <row r="198" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="198" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J198" s="16"/>
     </row>
-    <row r="199" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="199" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J199" s="16"/>
     </row>
-    <row r="200" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="200" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J200" s="16"/>
     </row>
-    <row r="201" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="201" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J201" s="16"/>
     </row>
-    <row r="202" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="202" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J202" s="16"/>
     </row>
-    <row r="203" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="203" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J203" s="16"/>
     </row>
-    <row r="204" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="204" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J204" s="16"/>
     </row>
-    <row r="205" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="205" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J205" s="16"/>
     </row>
-    <row r="206" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="206" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J206" s="16"/>
     </row>
-    <row r="207" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="207" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J207" s="16"/>
     </row>
-    <row r="208" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="208" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J208" s="16"/>
     </row>
-    <row r="209" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="209" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J209" s="16"/>
     </row>
-    <row r="210" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="210" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J210" s="16"/>
     </row>
-    <row r="211" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="211" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J211" s="16"/>
     </row>
-    <row r="212" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="212" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J212" s="16"/>
     </row>
   </sheetData>
@@ -12392,22 +12395,22 @@
       <selection pane="bottomLeft" activeCell="E113" sqref="E113"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.265625" customWidth="1"/>
-    <col min="2" max="2" width="16.796875" customWidth="1"/>
-    <col min="3" max="3" width="15.73046875" customWidth="1"/>
-    <col min="4" max="4" width="25.46484375" customWidth="1"/>
-    <col min="5" max="5" width="16.796875" style="22" customWidth="1"/>
+    <col min="1" max="1" width="4.21875" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" customWidth="1"/>
+    <col min="3" max="3" width="15.77734375" customWidth="1"/>
+    <col min="4" max="4" width="25.44140625" customWidth="1"/>
+    <col min="5" max="5" width="16.77734375" style="22" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="33.19921875" customWidth="1"/>
-    <col min="8" max="8" width="9.46484375" customWidth="1"/>
-    <col min="9" max="9" width="17.46484375" customWidth="1"/>
-    <col min="10" max="10" width="33.19921875" customWidth="1"/>
-    <col min="11" max="16" width="21.46484375" customWidth="1"/>
+    <col min="7" max="7" width="33.21875" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" customWidth="1"/>
+    <col min="9" max="9" width="17.44140625" customWidth="1"/>
+    <col min="10" max="10" width="33.21875" customWidth="1"/>
+    <col min="11" max="16" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>854</v>
       </c>
@@ -12445,7 +12448,7 @@
       <c r="O1" s="13"/>
       <c r="P1" s="13"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -12477,7 +12480,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -12509,7 +12512,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -12541,7 +12544,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -12573,7 +12576,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -12605,7 +12608,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -12637,7 +12640,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -12669,7 +12672,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -12701,7 +12704,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -12733,7 +12736,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -12765,7 +12768,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -12797,7 +12800,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -12829,7 +12832,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -12861,7 +12864,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -12893,7 +12896,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -12925,7 +12928,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -12957,7 +12960,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="38.25" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -12989,7 +12992,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -13021,7 +13024,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -13053,7 +13056,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -13085,7 +13088,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -13117,7 +13120,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -13149,7 +13152,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -13181,7 +13184,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -13213,7 +13216,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -13245,7 +13248,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -13277,7 +13280,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -13309,7 +13312,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -13341,7 +13344,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -13373,7 +13376,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -13405,7 +13408,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -13437,7 +13440,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -13469,7 +13472,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -13501,7 +13504,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -13533,7 +13536,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -13565,7 +13568,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -13597,7 +13600,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -13629,7 +13632,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -13661,7 +13664,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -13693,7 +13696,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -13725,7 +13728,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -13757,7 +13760,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -13789,7 +13792,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -13821,7 +13824,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -13853,7 +13856,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -13885,7 +13888,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -13917,7 +13920,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -13949,7 +13952,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -13981,7 +13984,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -14013,7 +14016,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -14045,7 +14048,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -14077,7 +14080,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -14109,7 +14112,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -14141,7 +14144,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -14173,7 +14176,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -14205,7 +14208,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -14237,7 +14240,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -14269,7 +14272,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -14301,7 +14304,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -14333,7 +14336,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -14365,7 +14368,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -14397,7 +14400,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -14429,7 +14432,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -14461,7 +14464,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -14493,7 +14496,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -14525,7 +14528,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -14557,7 +14560,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -14589,7 +14592,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -14621,7 +14624,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -14653,7 +14656,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -14685,7 +14688,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -14717,7 +14720,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -14749,7 +14752,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -14781,7 +14784,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -14813,7 +14816,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -14845,7 +14848,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -14877,7 +14880,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -14909,7 +14912,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -14941,7 +14944,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -14973,7 +14976,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -15005,7 +15008,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -15037,7 +15040,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -15069,7 +15072,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>83</v>
       </c>
@@ -15101,7 +15104,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>84</v>
       </c>
@@ -15133,7 +15136,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>85</v>
       </c>
@@ -15165,7 +15168,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>86</v>
       </c>
@@ -15197,7 +15200,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>87</v>
       </c>
@@ -15226,7 +15229,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>88</v>
       </c>
@@ -15255,7 +15258,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>89</v>
       </c>
@@ -15287,7 +15290,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>90</v>
       </c>
@@ -15319,7 +15322,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>91</v>
       </c>
@@ -15351,7 +15354,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>92</v>
       </c>
@@ -15383,7 +15386,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>93</v>
       </c>
@@ -15415,7 +15418,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>94</v>
       </c>
@@ -15447,7 +15450,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>95</v>
       </c>
@@ -15479,7 +15482,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>96</v>
       </c>
@@ -15511,7 +15514,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>97</v>
       </c>
@@ -15540,7 +15543,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>98</v>
       </c>
@@ -15572,7 +15575,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>99</v>
       </c>
@@ -15604,7 +15607,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>100</v>
       </c>
@@ -15636,7 +15639,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>101</v>
       </c>
@@ -15668,7 +15671,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <v>102</v>
       </c>
@@ -15700,7 +15703,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <v>103</v>
       </c>
@@ -15732,7 +15735,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>104</v>
       </c>
@@ -15764,7 +15767,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
         <v>105</v>
       </c>
@@ -15796,7 +15799,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
         <v>106</v>
       </c>
@@ -15828,7 +15831,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
         <v>107</v>
       </c>
@@ -15860,7 +15863,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
         <v>108</v>
       </c>
@@ -15892,7 +15895,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
         <v>109</v>
       </c>
@@ -15924,7 +15927,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
         <v>110</v>
       </c>
@@ -15956,265 +15959,265 @@
         <v>898</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J112" s="16"/>
     </row>
-    <row r="113" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="113" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J113" s="16"/>
     </row>
-    <row r="114" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="114" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J114" s="16"/>
     </row>
-    <row r="115" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="115" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J115" s="16"/>
     </row>
-    <row r="116" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="116" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J116" s="16"/>
     </row>
-    <row r="117" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="117" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J117" s="16"/>
     </row>
-    <row r="118" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="118" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J118" s="16"/>
     </row>
-    <row r="119" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="119" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J119" s="16"/>
     </row>
-    <row r="120" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="120" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J120" s="16"/>
     </row>
-    <row r="121" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="121" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J121" s="16"/>
     </row>
-    <row r="122" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="122" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J122" s="16"/>
     </row>
-    <row r="123" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="123" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J123" s="16"/>
     </row>
-    <row r="124" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="124" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J124" s="16"/>
     </row>
-    <row r="125" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="125" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J125" s="16"/>
     </row>
-    <row r="126" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="126" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J126" s="16"/>
     </row>
-    <row r="127" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="127" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J127" s="16"/>
     </row>
-    <row r="128" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="128" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J128" s="16"/>
     </row>
-    <row r="129" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="129" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J129" s="16"/>
     </row>
-    <row r="130" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="130" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J130" s="16"/>
     </row>
-    <row r="131" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="131" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J131" s="16"/>
     </row>
-    <row r="132" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="132" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J132" s="16"/>
     </row>
-    <row r="133" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="133" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J133" s="16"/>
     </row>
-    <row r="134" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="134" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J134" s="16"/>
     </row>
-    <row r="135" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="135" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J135" s="16"/>
     </row>
-    <row r="136" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="136" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J136" s="16"/>
     </row>
-    <row r="137" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="137" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J137" s="16"/>
     </row>
-    <row r="138" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="138" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J138" s="16"/>
     </row>
-    <row r="139" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="139" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J139" s="16"/>
     </row>
-    <row r="140" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="140" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J140" s="16"/>
     </row>
-    <row r="141" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="141" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J141" s="16"/>
     </row>
-    <row r="142" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="142" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J142" s="16"/>
     </row>
-    <row r="143" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="143" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J143" s="16"/>
     </row>
-    <row r="144" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="144" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J144" s="16"/>
     </row>
-    <row r="145" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="145" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J145" s="16"/>
     </row>
-    <row r="146" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="146" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J146" s="16"/>
     </row>
-    <row r="147" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="147" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J147" s="16"/>
     </row>
-    <row r="148" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="148" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J148" s="16"/>
     </row>
-    <row r="149" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="149" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J149" s="16"/>
     </row>
-    <row r="150" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="150" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J150" s="16"/>
     </row>
-    <row r="151" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="151" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J151" s="16"/>
     </row>
-    <row r="152" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="152" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J152" s="16"/>
     </row>
-    <row r="153" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="153" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J153" s="16"/>
     </row>
-    <row r="154" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="154" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J154" s="16"/>
     </row>
-    <row r="155" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="155" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J155" s="16"/>
     </row>
-    <row r="156" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="156" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J156" s="16"/>
     </row>
-    <row r="157" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="157" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J157" s="16"/>
     </row>
-    <row r="158" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="158" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J158" s="16"/>
     </row>
-    <row r="159" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="159" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J159" s="16"/>
     </row>
-    <row r="160" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="160" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J160" s="16"/>
     </row>
-    <row r="161" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="161" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J161" s="16"/>
     </row>
-    <row r="162" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="162" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J162" s="16"/>
     </row>
-    <row r="163" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="163" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J163" s="16"/>
     </row>
-    <row r="164" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="164" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J164" s="16"/>
     </row>
-    <row r="165" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="165" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J165" s="16"/>
     </row>
-    <row r="166" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="166" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J166" s="16"/>
     </row>
-    <row r="167" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="167" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J167" s="16"/>
     </row>
-    <row r="168" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="168" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J168" s="16"/>
     </row>
-    <row r="169" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="169" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J169" s="16"/>
     </row>
-    <row r="170" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="170" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J170" s="16"/>
     </row>
-    <row r="171" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="171" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J171" s="16"/>
     </row>
-    <row r="172" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="172" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J172" s="16"/>
     </row>
-    <row r="173" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="173" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J173" s="16"/>
     </row>
-    <row r="174" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="174" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J174" s="16"/>
     </row>
-    <row r="175" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="175" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J175" s="16"/>
     </row>
-    <row r="176" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="176" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J176" s="16"/>
     </row>
-    <row r="177" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="177" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J177" s="16"/>
     </row>
-    <row r="178" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="178" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J178" s="16"/>
     </row>
-    <row r="179" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="179" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J179" s="16"/>
     </row>
-    <row r="180" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="180" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J180" s="16"/>
     </row>
-    <row r="181" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="181" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J181" s="16"/>
     </row>
-    <row r="182" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="182" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J182" s="16"/>
     </row>
-    <row r="183" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="183" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J183" s="16"/>
     </row>
-    <row r="184" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="184" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J184" s="16"/>
     </row>
-    <row r="185" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="185" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J185" s="16"/>
     </row>
-    <row r="186" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="186" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J186" s="16"/>
     </row>
-    <row r="187" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="187" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J187" s="16"/>
     </row>
-    <row r="188" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="188" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J188" s="16"/>
     </row>
-    <row r="189" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="189" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J189" s="16"/>
     </row>
-    <row r="190" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="190" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J190" s="16"/>
     </row>
-    <row r="191" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="191" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J191" s="16"/>
     </row>
-    <row r="192" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="192" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J192" s="16"/>
     </row>
-    <row r="193" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="193" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J193" s="16"/>
     </row>
-    <row r="194" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="194" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J194" s="16"/>
     </row>
-    <row r="195" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="195" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J195" s="16"/>
     </row>
-    <row r="196" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="196" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J196" s="16"/>
     </row>
-    <row r="197" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="197" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J197" s="16"/>
     </row>
-    <row r="198" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="198" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J198" s="16"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change other phone number
</commit_message>
<xml_diff>
--- a/CS335/GitHub Info sans duplicates.xlsx
+++ b/CS335/GitHub Info sans duplicates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Jlungo\staffcard\CS335\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E845516-9609-4A4C-8677-A7286FF73575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D742E88-603B-461C-94E1-E8FED0C9AF58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3890" uniqueCount="1236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3890" uniqueCount="1237">
   <si>
     <t>Timestamp</t>
   </si>
@@ -3730,6 +3730,9 @@
   </si>
   <si>
     <t>+255657990682</t>
+  </si>
+  <si>
+    <t>+255735990682</t>
   </si>
 </sst>
 </file>
@@ -12628,8 +12631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -14676,8 +14679,8 @@
       <c r="E64" s="9" t="s">
         <v>1235</v>
       </c>
-      <c r="F64" t="s">
-        <v>998</v>
+      <c r="F64" s="9" t="s">
+        <v>1236</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>617</v>

</xml_diff>

<commit_message>
FIXED NAME IN SPREADSHEET
</commit_message>
<xml_diff>
--- a/CS335/GitHub Info sans duplicates.xlsx
+++ b/CS335/GitHub Info sans duplicates.xlsx
@@ -3600,7 +3600,7 @@
     <t xml:space="preserve">SAITORIA</t>
   </si>
   <si>
-    <t xml:space="preserve">SARONI W</t>
+    <t xml:space="preserve">SARONI WILFRED</t>
   </si>
   <si>
     <t xml:space="preserve">DANIEL SOLOMON</t>
@@ -3750,7 +3750,7 @@
     <numFmt numFmtId="165" formatCode="m/d/yyyy\ h:mm"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -3780,12 +3780,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3833,7 +3827,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3870,10 +3864,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3902,7 +3892,7 @@
       <selection pane="topLeft" activeCell="I129" activeCellId="0" sqref="I129"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.51171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.25"/>
@@ -8797,10 +8787,10 @@
   <dimension ref="A1:J126"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A113" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J143" activeCellId="0" sqref="J143"/>
+      <selection pane="topLeft" activeCell="D126" activeCellId="0" sqref="D126"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.51171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.5"/>
@@ -12727,7 +12717,7 @@
       <c r="I126" s="0" t="s">
         <v>929</v>
       </c>
-      <c r="J126" s="9" t="s">
+      <c r="J126" s="7" t="s">
         <v>933</v>
       </c>
     </row>
@@ -12767,14 +12757,14 @@
       <selection pane="topLeft" activeCell="J104" activeCellId="0" sqref="J104"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.51171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="5" width="29.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="5" width="17.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="5" width="17.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="5" width="30.26"/>
   </cols>
   <sheetData>
@@ -16372,7 +16362,7 @@
       <c r="F114" s="0" t="s">
         <v>1012</v>
       </c>
-      <c r="G114" s="10" t="s">
+      <c r="G114" s="9" t="s">
         <v>1159</v>
       </c>
       <c r="H114" s="0" t="s">

</xml_diff>

<commit_message>
changed another cell color
</commit_message>
<xml_diff>
--- a/CS335/GitHub Info sans duplicates.xlsx
+++ b/CS335/GitHub Info sans duplicates.xlsx
@@ -3752,7 +3752,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -3788,8 +3788,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3807,6 +3814,11 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -3817,12 +3829,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -3840,16 +3853,20 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -8091,10 +8108,10 @@
       <c r="K104" t="s">
         <v>841</v>
       </c>
-      <c r="L104" s="11" t="s">
+      <c r="L104" s="12" t="s">
         <v>842</v>
       </c>
-      <c r="M104" s="11"/>
+      <c r="M104" s="12"/>
       <c r="P104" s="1"/>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.3">
@@ -12980,7 +12997,7 @@
   <dimension ref="A1:J121"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A100" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G109" sqref="G109"/>
+      <selection activeCell="I109" sqref="I109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -16460,13 +16477,13 @@
       <c r="F109" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G109" s="12" t="s">
+      <c r="G109" s="11" t="s">
         <v>970</v>
       </c>
       <c r="H109" t="s">
         <v>1001</v>
       </c>
-      <c r="I109" s="4" t="s">
+      <c r="I109" s="13" t="s">
         <v>971</v>
       </c>
       <c r="J109" s="4" t="s">

</xml_diff>

<commit_message>
Added phone number and changed github username
</commit_message>
<xml_diff>
--- a/CS335/GitHub Info sans duplicates.xlsx
+++ b/CS335/GitHub Info sans duplicates.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3911" uniqueCount="1239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3910" uniqueCount="1241">
   <si>
     <t xml:space="preserve">Timestamp</t>
   </si>
@@ -3604,6 +3604,12 @@
   </si>
   <si>
     <t xml:space="preserve">DANIEL SOLOMON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EvelynAjuna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://guthub.com/EvelynAjuna</t>
   </si>
   <si>
     <t xml:space="preserve">Scarion</t>
@@ -3750,7 +3756,7 @@
     <numFmt numFmtId="165" formatCode="m/d/yyyy\ h:mm"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -3780,12 +3786,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3870,11 +3870,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3899,10 +3899,10 @@
   <dimension ref="A1:P129"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E115" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I129" activeCellId="0" sqref="I129"/>
+      <selection pane="topLeft" activeCell="I129" activeCellId="2" sqref="F38 G33 I129"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.51953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.25"/>
@@ -8797,10 +8797,10 @@
   <dimension ref="A1:J126"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A113" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D126" activeCellId="0" sqref="D126"/>
+      <selection pane="topLeft" activeCell="D126" activeCellId="2" sqref="F38 G33 D126"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.51953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.5"/>
@@ -12763,16 +12763,17 @@
   </sheetPr>
   <dimension ref="A1:J121"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E102" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J121" activeCellId="0" sqref="J121"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G33" activeCellId="1" sqref="F38 G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.51953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="5" width="29.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="5" width="17.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="5" width="30.26"/>
@@ -13866,7 +13867,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>1048</v>
       </c>
@@ -13882,7 +13883,7 @@
       <c r="E35" s="0" t="s">
         <v>332</v>
       </c>
-      <c r="F35" s="0" t="s">
+      <c r="F35" s="9" t="s">
         <v>333</v>
       </c>
       <c r="G35" s="5" t="s">
@@ -13962,7 +13963,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>1052</v>
       </c>
@@ -13978,8 +13979,8 @@
       <c r="E38" s="0" t="s">
         <v>365</v>
       </c>
-      <c r="F38" s="0" t="s">
-        <v>1012</v>
+      <c r="F38" s="9" t="n">
+        <v>255752449074</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>366</v>
@@ -13988,10 +13989,10 @@
         <v>1018</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>367</v>
+        <v>1194</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>368</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14642,10 +14643,10 @@
         <v>556</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>1194</v>
+        <v>1196</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>1195</v>
+        <v>1197</v>
       </c>
       <c r="E59" s="0" t="s">
         <v>559</v>
@@ -15137,7 +15138,7 @@
         <v>704</v>
       </c>
       <c r="H74" s="0" t="s">
-        <v>1196</v>
+        <v>1198</v>
       </c>
       <c r="I74" s="5" t="s">
         <v>705</v>
@@ -16207,7 +16208,7 @@
         <v>960</v>
       </c>
       <c r="E108" s="0" t="s">
-        <v>1197</v>
+        <v>1199</v>
       </c>
       <c r="F108" s="0" t="s">
         <v>17</v>
@@ -16259,16 +16260,16 @@
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>1198</v>
+        <v>1200</v>
       </c>
       <c r="B110" s="0" t="s">
         <v>982</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>1199</v>
+        <v>1201</v>
       </c>
       <c r="D110" s="0" t="s">
-        <v>1200</v>
+        <v>1202</v>
       </c>
       <c r="E110" s="0" t="s">
         <v>985</v>
@@ -16294,31 +16295,31 @@
         <v>1134</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>1201</v>
+        <v>1203</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>1202</v>
+        <v>1204</v>
       </c>
       <c r="D111" s="0" t="s">
-        <v>1203</v>
+        <v>1205</v>
       </c>
       <c r="E111" s="0" t="s">
-        <v>1204</v>
+        <v>1206</v>
       </c>
       <c r="F111" s="0" t="s">
         <v>999</v>
       </c>
       <c r="G111" s="5" t="s">
-        <v>1205</v>
+        <v>1207</v>
       </c>
       <c r="H111" s="0" t="s">
         <v>1013</v>
       </c>
       <c r="I111" s="5" t="s">
-        <v>1206</v>
+        <v>1208</v>
       </c>
       <c r="J111" s="5" t="s">
-        <v>1207</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16326,31 +16327,31 @@
         <v>1135</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>1208</v>
+        <v>1210</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>1209</v>
+        <v>1211</v>
       </c>
       <c r="D112" s="0" t="s">
-        <v>1210</v>
+        <v>1212</v>
       </c>
       <c r="E112" s="0" t="s">
-        <v>1211</v>
+        <v>1213</v>
       </c>
       <c r="F112" s="0" t="s">
-        <v>1212</v>
+        <v>1214</v>
       </c>
       <c r="G112" s="5" t="s">
-        <v>1213</v>
+        <v>1215</v>
       </c>
       <c r="H112" s="0" t="s">
         <v>1018</v>
       </c>
       <c r="I112" s="5" t="s">
-        <v>1214</v>
+        <v>1216</v>
       </c>
       <c r="J112" s="5" t="s">
-        <v>1215</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16372,7 +16373,7 @@
       <c r="F114" s="0" t="s">
         <v>1012</v>
       </c>
-      <c r="G114" s="9" t="s">
+      <c r="G114" s="10" t="s">
         <v>1159</v>
       </c>
       <c r="H114" s="0" t="s">
@@ -16393,10 +16394,10 @@
         <v>114</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>1216</v>
+        <v>1218</v>
       </c>
       <c r="D115" s="0" t="s">
-        <v>1217</v>
+        <v>1219</v>
       </c>
       <c r="E115" s="0" t="n">
         <v>693641541</v>
@@ -16411,7 +16412,7 @@
         <v>1018</v>
       </c>
       <c r="I115" s="5" t="s">
-        <v>1218</v>
+        <v>1220</v>
       </c>
       <c r="J115" s="4" t="s">
         <v>120</v>
@@ -16422,13 +16423,13 @@
         <v>115</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>1219</v>
+        <v>1221</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>1220</v>
+        <v>1222</v>
       </c>
       <c r="D116" s="0" t="s">
-        <v>1221</v>
+        <v>1223</v>
       </c>
       <c r="E116" s="0" t="n">
         <v>620781851</v>
@@ -16437,16 +16438,16 @@
         <v>1012</v>
       </c>
       <c r="G116" s="4" t="s">
-        <v>1222</v>
+        <v>1224</v>
       </c>
       <c r="H116" s="0" t="s">
         <v>1018</v>
       </c>
       <c r="I116" s="5" t="s">
-        <v>1223</v>
+        <v>1225</v>
       </c>
       <c r="J116" s="4" t="s">
-        <v>1224</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16454,28 +16455,28 @@
         <v>116</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>1226</v>
+        <v>1228</v>
       </c>
       <c r="D117" s="0" t="s">
-        <v>1227</v>
+        <v>1229</v>
       </c>
       <c r="E117" s="0" t="n">
         <v>682958270</v>
       </c>
       <c r="G117" s="4" t="s">
-        <v>1228</v>
+        <v>1230</v>
       </c>
       <c r="H117" s="0" t="s">
         <v>1013</v>
       </c>
       <c r="I117" s="5" t="s">
-        <v>1229</v>
+        <v>1231</v>
       </c>
       <c r="J117" s="4" t="s">
-        <v>1230</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16486,10 +16487,10 @@
         <v>515</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>1231</v>
+        <v>1233</v>
       </c>
       <c r="D118" s="0" t="s">
-        <v>1232</v>
+        <v>1234</v>
       </c>
       <c r="E118" s="0" t="n">
         <v>710088836</v>
@@ -16498,7 +16499,7 @@
         <v>519</v>
       </c>
       <c r="H118" s="0" t="s">
-        <v>1233</v>
+        <v>1235</v>
       </c>
       <c r="I118" s="5" t="s">
         <v>520</v>
@@ -16509,13 +16510,13 @@
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="0" t="s">
-        <v>1234</v>
+        <v>1236</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>1235</v>
+        <v>1237</v>
       </c>
       <c r="D119" s="0" t="s">
-        <v>1236</v>
+        <v>1238</v>
       </c>
       <c r="E119" s="0" t="n">
         <v>710776796</v>
@@ -16524,13 +16525,13 @@
         <v>999</v>
       </c>
       <c r="G119" s="4" t="s">
-        <v>1237</v>
+        <v>1239</v>
       </c>
       <c r="H119" s="0" t="s">
         <v>1001</v>
       </c>
       <c r="I119" s="5" t="s">
-        <v>1238</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16587,28 +16588,29 @@
       <c r="I121" s="5" t="s">
         <v>929</v>
       </c>
-      <c r="J121" s="10" t="s">
+      <c r="J121" s="5" t="s">
         <v>933</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G59" r:id="rId1" display="irenescarion88@gmail.com"/>
-    <hyperlink ref="J59" r:id="rId2" display="https://github.com/IreneScarion"/>
-    <hyperlink ref="G114" r:id="rId3" display="martincalvin731@gmail.com"/>
-    <hyperlink ref="G115" r:id="rId4" display="candymutagaywa@gmail.com"/>
-    <hyperlink ref="J115" r:id="rId5" display="https://github.com/CandyTheophil"/>
-    <hyperlink ref="G116" r:id="rId6" display="aminja901@gmail.com"/>
-    <hyperlink ref="J116" r:id="rId7" display="https://github.com/ARwaich911"/>
-    <hyperlink ref="G117" r:id="rId8" display="stanleyrichardmbuya@gmail.com"/>
-    <hyperlink ref="J117" r:id="rId9" display="https://github.com/stan-lee98"/>
-    <hyperlink ref="G118" r:id="rId10" display="tomekawinfrida@gmail.com"/>
-    <hyperlink ref="J118" r:id="rId11" display="https://github.com/Windorah"/>
-    <hyperlink ref="G119" r:id="rId12" display="yohanastevenkasaila@gmail.com"/>
-    <hyperlink ref="G120" r:id="rId13" display="jumakbs@gmail.com"/>
-    <hyperlink ref="J120" r:id="rId14" display="https://github.com/jumakbs"/>
-    <hyperlink ref="G121" r:id="rId15" display="saronisaitoria@gmail.com"/>
-    <hyperlink ref="J121" r:id="rId16" display="https://github.com/Saitoria"/>
+    <hyperlink ref="J38" r:id="rId1" display="https://guthub.com/EvelynAjuna"/>
+    <hyperlink ref="G59" r:id="rId2" display="irenescarion88@gmail.com"/>
+    <hyperlink ref="J59" r:id="rId3" display="https://github.com/IreneScarion"/>
+    <hyperlink ref="G114" r:id="rId4" display="martincalvin731@gmail.com"/>
+    <hyperlink ref="G115" r:id="rId5" display="candymutagaywa@gmail.com"/>
+    <hyperlink ref="J115" r:id="rId6" display="https://github.com/CandyTheophil"/>
+    <hyperlink ref="G116" r:id="rId7" display="aminja901@gmail.com"/>
+    <hyperlink ref="J116" r:id="rId8" display="https://github.com/ARwaich911"/>
+    <hyperlink ref="G117" r:id="rId9" display="stanleyrichardmbuya@gmail.com"/>
+    <hyperlink ref="J117" r:id="rId10" display="https://github.com/stan-lee98"/>
+    <hyperlink ref="G118" r:id="rId11" display="tomekawinfrida@gmail.com"/>
+    <hyperlink ref="J118" r:id="rId12" display="https://github.com/Windorah"/>
+    <hyperlink ref="G119" r:id="rId13" display="yohanastevenkasaila@gmail.com"/>
+    <hyperlink ref="G120" r:id="rId14" display="jumakbs@gmail.com"/>
+    <hyperlink ref="J120" r:id="rId15" display="https://github.com/jumakbs"/>
+    <hyperlink ref="G121" r:id="rId16" display="saronisaitoria@gmail.com"/>
+    <hyperlink ref="J121" r:id="rId17" display="https://github.com/Saitoria"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Modified some data in our database table
</commit_message>
<xml_diff>
--- a/CS335/GitHub Info sans duplicates.xlsx
+++ b/CS335/GitHub Info sans duplicates.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\staffcard\CS335\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A4DE63-7C9D-49E1-A50D-8D2E8C50DD8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="25600" windowHeight="14340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -2651,7 +2645,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
@@ -3204,14 +3198,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -3412,23 +3398,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:R122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K54" sqref="K54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="18" width="21.42578125" customWidth="1"/>
+    <col min="1" max="18" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3466,7 +3452,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1">
       <c r="A2" s="2">
         <v>44517.792739571756</v>
       </c>
@@ -3504,7 +3490,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="15.75" customHeight="1">
       <c r="A3" s="2">
         <v>44517.829278495366</v>
       </c>
@@ -3542,7 +3528,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="15.75" customHeight="1">
       <c r="A4" s="2">
         <v>44517.829803020832</v>
       </c>
@@ -3580,7 +3566,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1">
       <c r="A5" s="2">
         <v>44517.832974606485</v>
       </c>
@@ -3618,7 +3604,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="15.75" customHeight="1">
       <c r="A6" s="2">
         <v>44517.833342615741</v>
       </c>
@@ -3656,7 +3642,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="15.75" customHeight="1">
       <c r="A7" s="2">
         <v>44517.834096585648</v>
       </c>
@@ -3694,7 +3680,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1">
       <c r="A8" s="2">
         <v>44517.834304884258</v>
       </c>
@@ -3732,7 +3718,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="15.75" customHeight="1">
       <c r="A9" s="2">
         <v>44517.834315162036</v>
       </c>
@@ -3770,7 +3756,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="15.75" customHeight="1">
       <c r="A10" s="2">
         <v>44517.834467222223</v>
       </c>
@@ -3808,7 +3794,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="15.75" customHeight="1">
       <c r="A11" s="2">
         <v>44517.836256620372</v>
       </c>
@@ -3846,7 +3832,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="15.75" customHeight="1">
       <c r="A12" s="2">
         <v>44517.840131203702</v>
       </c>
@@ -3884,7 +3870,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="15.75" customHeight="1">
       <c r="A13" s="2">
         <v>44517.840687337964</v>
       </c>
@@ -3922,7 +3908,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="15.75" customHeight="1">
       <c r="A14" s="2">
         <v>44517.840723900459</v>
       </c>
@@ -3960,7 +3946,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="15.75" customHeight="1">
       <c r="A15" s="2">
         <v>44517.848194363425</v>
       </c>
@@ -3998,7 +3984,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="15.75" customHeight="1">
       <c r="A16" s="2">
         <v>44517.849799363423</v>
       </c>
@@ -4036,7 +4022,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="15.75" customHeight="1">
       <c r="A17" s="2">
         <v>44517.851121805557</v>
       </c>
@@ -4074,7 +4060,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="15.75" customHeight="1">
       <c r="A18" s="2">
         <v>44517.853374618055</v>
       </c>
@@ -4112,7 +4098,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="15.75" customHeight="1">
       <c r="A19" s="2">
         <v>44517.855156886573</v>
       </c>
@@ -4150,7 +4136,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="15.75" customHeight="1">
       <c r="A20" s="2">
         <v>44517.858557291664</v>
       </c>
@@ -4188,7 +4174,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="15.75" customHeight="1">
       <c r="A21" s="2">
         <v>44517.859119421293</v>
       </c>
@@ -4226,7 +4212,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="15.75" customHeight="1">
       <c r="A22" s="2">
         <v>44517.860663136569</v>
       </c>
@@ -4264,7 +4250,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="15.75" customHeight="1">
       <c r="A23" s="2">
         <v>44517.863773090277</v>
       </c>
@@ -4302,7 +4288,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" ht="15.75" customHeight="1">
       <c r="A24" s="2">
         <v>44517.867895196759</v>
       </c>
@@ -4340,7 +4326,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="15.75" customHeight="1">
       <c r="A25" s="2">
         <v>44517.86830321759</v>
       </c>
@@ -4378,7 +4364,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="15.75" customHeight="1">
       <c r="A26" s="2">
         <v>44517.869191446764</v>
       </c>
@@ -4416,7 +4402,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" ht="15.75" customHeight="1">
       <c r="A27" s="2">
         <v>44517.874595833331</v>
       </c>
@@ -4454,7 +4440,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" ht="15.75" customHeight="1">
       <c r="A28" s="2">
         <v>44517.877297905092</v>
       </c>
@@ -4492,7 +4478,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" ht="15.75" customHeight="1">
       <c r="A29" s="2">
         <v>44517.877863587964</v>
       </c>
@@ -4530,7 +4516,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" ht="15.75" customHeight="1">
       <c r="A30" s="2">
         <v>44517.886029872687</v>
       </c>
@@ -4568,7 +4554,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="15.75" customHeight="1">
       <c r="A31" s="2">
         <v>44517.888174652777</v>
       </c>
@@ -4606,7 +4592,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" ht="15.75" customHeight="1">
       <c r="A32" s="2">
         <v>44517.89089574074</v>
       </c>
@@ -4644,7 +4630,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" ht="15.75" customHeight="1">
       <c r="A33" s="2">
         <v>44517.898055138889</v>
       </c>
@@ -4682,7 +4668,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" ht="15.75" customHeight="1">
       <c r="A34" s="2">
         <v>44517.903385925922</v>
       </c>
@@ -4720,7 +4706,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" ht="15.75" customHeight="1">
       <c r="A35" s="2">
         <v>44517.916796608799</v>
       </c>
@@ -4758,7 +4744,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" ht="15.75" customHeight="1">
       <c r="A36" s="2">
         <v>44517.919944965281</v>
       </c>
@@ -4796,7 +4782,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" ht="15.75" customHeight="1">
       <c r="A37" s="2">
         <v>44517.920174733794</v>
       </c>
@@ -4834,7 +4820,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" ht="15.75" customHeight="1">
       <c r="A38" s="2">
         <v>44517.920207002317</v>
       </c>
@@ -4872,7 +4858,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" ht="15.75" customHeight="1">
       <c r="A39" s="2">
         <v>44517.925676087965</v>
       </c>
@@ -4910,7 +4896,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" ht="15.75" customHeight="1">
       <c r="A40" s="2">
         <v>44517.942313136577</v>
       </c>
@@ -4948,7 +4934,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" ht="15.75" customHeight="1">
       <c r="A41" s="2">
         <v>44517.967181493055</v>
       </c>
@@ -4986,7 +4972,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" ht="15.75" customHeight="1">
       <c r="A42" s="2">
         <v>44517.970856388885</v>
       </c>
@@ -5024,7 +5010,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" ht="15.75" customHeight="1">
       <c r="A43" s="2">
         <v>44517.974103865738</v>
       </c>
@@ -5062,7 +5048,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" ht="15.75" customHeight="1">
       <c r="A44" s="2">
         <v>44517.995788912041</v>
       </c>
@@ -5100,7 +5086,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" ht="15.75" customHeight="1">
       <c r="A45" s="2">
         <v>44518.053331921299</v>
       </c>
@@ -5138,7 +5124,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" ht="15.75" customHeight="1">
       <c r="A46" s="2">
         <v>44518.141680740737</v>
       </c>
@@ -5176,7 +5162,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" ht="15.75" customHeight="1">
       <c r="A47" s="2">
         <v>44518.338707534727</v>
       </c>
@@ -5214,7 +5200,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" ht="15.75" customHeight="1">
       <c r="A48" s="2">
         <v>44518.348475844905</v>
       </c>
@@ -5252,7 +5238,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" ht="15.75" customHeight="1">
       <c r="A49" s="2">
         <v>44518.368981018517</v>
       </c>
@@ -5290,7 +5276,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" ht="15.75" customHeight="1">
       <c r="A50" s="2">
         <v>44518.376564247686</v>
       </c>
@@ -5328,7 +5314,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" ht="15.75" customHeight="1">
       <c r="A51" s="2">
         <v>44518.395640312505</v>
       </c>
@@ -5366,7 +5352,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" ht="15.75" customHeight="1">
       <c r="A52" s="2">
         <v>44518.396610844909</v>
       </c>
@@ -5404,7 +5390,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" ht="15.75" customHeight="1">
       <c r="A53" s="2">
         <v>44518.416108634265</v>
       </c>
@@ -5442,7 +5428,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" ht="15.75" customHeight="1">
       <c r="A54" s="2">
         <v>44518.419745173611</v>
       </c>
@@ -5480,7 +5466,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" ht="15.75" customHeight="1">
       <c r="A55" s="2">
         <v>44518.433273449074</v>
       </c>
@@ -5518,7 +5504,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" ht="15.75" customHeight="1">
       <c r="A56" s="2">
         <v>44518.43360689815</v>
       </c>
@@ -5556,7 +5542,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" ht="15.75" customHeight="1">
       <c r="A57" s="2">
         <v>44518.462937638891</v>
       </c>
@@ -5594,7 +5580,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" ht="15.75" customHeight="1">
       <c r="A58" s="2">
         <v>44518.479146377314</v>
       </c>
@@ -5632,7 +5618,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" ht="15.75" customHeight="1">
       <c r="A59" s="2">
         <v>44518.500450555555</v>
       </c>
@@ -5670,7 +5656,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" ht="15.75" customHeight="1">
       <c r="A60" s="2">
         <v>44518.545351886569</v>
       </c>
@@ -5708,7 +5694,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" ht="15.75" customHeight="1">
       <c r="A61" s="2">
         <v>44518.57691783565</v>
       </c>
@@ -5746,7 +5732,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" ht="15.75" customHeight="1">
       <c r="A62" s="2">
         <v>44518.580951863427</v>
       </c>
@@ -5784,7 +5770,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" ht="15.75" customHeight="1">
       <c r="A63" s="2">
         <v>44518.584114340279</v>
       </c>
@@ -5822,7 +5808,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" ht="15.75" customHeight="1">
       <c r="A64" s="2">
         <v>44518.599512685185</v>
       </c>
@@ -5860,7 +5846,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" ht="15.75" customHeight="1">
       <c r="A65" s="2">
         <v>44518.611133506944</v>
       </c>
@@ -5898,7 +5884,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12" ht="15.75" customHeight="1">
       <c r="A66" s="2">
         <v>44518.639018194444</v>
       </c>
@@ -5936,7 +5922,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:12" ht="15.75" customHeight="1">
       <c r="A67" s="2">
         <v>44518.65679601852</v>
       </c>
@@ -5974,7 +5960,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:12" ht="15.75" customHeight="1">
       <c r="A68" s="2">
         <v>44518.669622650465</v>
       </c>
@@ -6012,7 +5998,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:12" ht="15.75" customHeight="1">
       <c r="A69" s="2">
         <v>44518.675713946759</v>
       </c>
@@ -6050,7 +6036,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12" ht="15.75" customHeight="1">
       <c r="A70" s="2">
         <v>44518.678410173612</v>
       </c>
@@ -6088,7 +6074,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:12" ht="15.75" customHeight="1">
       <c r="A71" s="2">
         <v>44518.67904717593</v>
       </c>
@@ -6126,7 +6112,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12" ht="15.75" customHeight="1">
       <c r="A72" s="2">
         <v>44518.681073298612</v>
       </c>
@@ -6164,7 +6150,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12" ht="15.75" customHeight="1">
       <c r="A73" s="2">
         <v>44518.681981574075</v>
       </c>
@@ -6202,7 +6188,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12" ht="15.75" customHeight="1">
       <c r="A74" s="2">
         <v>44518.682995844909</v>
       </c>
@@ -6240,7 +6226,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" ht="15.75" customHeight="1">
       <c r="A75" s="2">
         <v>44518.68484347222</v>
       </c>
@@ -6278,7 +6264,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:12" ht="15.75" customHeight="1">
       <c r="A76" s="2">
         <v>44518.690567743055</v>
       </c>
@@ -6316,7 +6302,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12" ht="15.75" customHeight="1">
       <c r="A77" s="2">
         <v>44518.704118368056</v>
       </c>
@@ -6354,7 +6340,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:12" ht="15.75" customHeight="1">
       <c r="A78" s="2">
         <v>44518.717275173607</v>
       </c>
@@ -6392,7 +6378,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12" ht="15.75" customHeight="1">
       <c r="A79" s="2">
         <v>44518.718211203704</v>
       </c>
@@ -6430,7 +6416,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="80" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:12" ht="15.75" customHeight="1">
       <c r="A80" s="2">
         <v>44518.721890682871</v>
       </c>
@@ -6468,7 +6454,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="81" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12" ht="15.75" customHeight="1">
       <c r="A81" s="2">
         <v>44518.845550972226</v>
       </c>
@@ -6506,7 +6492,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="82" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12" ht="15.75" customHeight="1">
       <c r="A82" s="2">
         <v>44518.845807673613</v>
       </c>
@@ -6544,7 +6530,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="83" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:12" ht="15.75" customHeight="1">
       <c r="A83" s="2">
         <v>44518.847130671296</v>
       </c>
@@ -6582,7 +6568,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="84" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:12" ht="15.75" customHeight="1">
       <c r="A84" s="2">
         <v>44518.848048738422</v>
       </c>
@@ -6620,7 +6606,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="85" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:12" ht="15.75" customHeight="1">
       <c r="A85" s="2">
         <v>44518.848206620372</v>
       </c>
@@ -6658,7 +6644,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="86" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:12" ht="15.75" customHeight="1">
       <c r="A86" s="2">
         <v>44518.851609803241</v>
       </c>
@@ -6696,7 +6682,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="87" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:12" ht="15.75" customHeight="1">
       <c r="A87" s="2">
         <v>44518.853343229166</v>
       </c>
@@ -6734,7 +6720,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="88" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:12" ht="15.75" customHeight="1">
       <c r="A88" s="2">
         <v>44518.854456469911</v>
       </c>
@@ -6772,7 +6758,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="89" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:12" ht="15.75" customHeight="1">
       <c r="A89" s="2">
         <v>44518.857002847217</v>
       </c>
@@ -6810,7 +6796,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="90" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:12" ht="15.75" customHeight="1">
       <c r="A90" s="2">
         <v>44518.857458969913</v>
       </c>
@@ -6848,7 +6834,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="91" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:12" ht="15.75" customHeight="1">
       <c r="A91" s="2">
         <v>44518.864664201392</v>
       </c>
@@ -6886,7 +6872,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="92" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:12" ht="15.75" customHeight="1">
       <c r="A92" s="2">
         <v>44518.865544432869</v>
       </c>
@@ -6924,7 +6910,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="93" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:12" ht="15.75" customHeight="1">
       <c r="A93" s="2">
         <v>44518.873488796293</v>
       </c>
@@ -6962,7 +6948,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="94" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:12" ht="15.75" customHeight="1">
       <c r="A94" s="2">
         <v>44518.880978576388</v>
       </c>
@@ -7000,7 +6986,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="95" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:12" ht="15.75" customHeight="1">
       <c r="A95" s="2">
         <v>44518.890144791665</v>
       </c>
@@ -7038,7 +7024,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="96" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:12" ht="15.75" customHeight="1">
       <c r="A96" s="2">
         <v>44518.892673622686</v>
       </c>
@@ -7076,7 +7062,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="97" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:12" ht="15.75" customHeight="1">
       <c r="A97" s="2">
         <v>44518.893882627315</v>
       </c>
@@ -7114,7 +7100,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="98" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:12" ht="15.75" customHeight="1">
       <c r="A98" s="2">
         <v>44518.895629976847</v>
       </c>
@@ -7152,7 +7138,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="99" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:12" ht="15.75" customHeight="1">
       <c r="A99" s="2">
         <v>44518.897268032408</v>
       </c>
@@ -7190,7 +7176,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="100" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:12" ht="15.75" customHeight="1">
       <c r="A100" s="2">
         <v>44518.901678900467</v>
       </c>
@@ -7228,7 +7214,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="101" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:12" ht="15.75" customHeight="1">
       <c r="A101" s="2">
         <v>44518.905369791668</v>
       </c>
@@ -7266,7 +7252,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="102" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:12" ht="15.75" customHeight="1">
       <c r="A102" s="2">
         <v>44518.914951886574</v>
       </c>
@@ -7304,7 +7290,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="103" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:12" ht="15.75" customHeight="1">
       <c r="A103" s="2">
         <v>44518.926460324074</v>
       </c>
@@ -7339,7 +7325,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="104" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:12" ht="15.75" customHeight="1">
       <c r="A104" s="2">
         <v>44518.943910335649</v>
       </c>
@@ -7374,7 +7360,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="105" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:12" ht="15.75" customHeight="1">
       <c r="A105" s="2">
         <v>44518.94905171296</v>
       </c>
@@ -7412,7 +7398,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="106" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:12" ht="15.75" customHeight="1">
       <c r="A106" s="2">
         <v>44518.949835740743</v>
       </c>
@@ -7450,7 +7436,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="107" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:12" ht="15.75" customHeight="1">
       <c r="A107" s="2">
         <v>44518.954430393518</v>
       </c>
@@ -7488,7 +7474,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="108" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:12" ht="15.75" customHeight="1">
       <c r="A108" s="2">
         <v>44518.964523217597</v>
       </c>
@@ -7526,7 +7512,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="109" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:12" ht="15.75" customHeight="1">
       <c r="A109" s="2">
         <v>44518.971188981479</v>
       </c>
@@ -7564,7 +7550,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="110" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:12" ht="15.75" customHeight="1">
       <c r="A110" s="2">
         <v>44518.972234583329</v>
       </c>
@@ -7602,7 +7588,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="111" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:12" ht="15.75" customHeight="1">
       <c r="A111" s="2">
         <v>44518.972730138892</v>
       </c>
@@ -7640,7 +7626,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="112" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:12" ht="15.75" customHeight="1">
       <c r="A112" s="2">
         <v>44518.977785532406</v>
       </c>
@@ -7678,7 +7664,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="113" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:18" ht="15.75" customHeight="1">
       <c r="A113" s="6">
         <v>44519.003693425926</v>
       </c>
@@ -7720,7 +7706,7 @@
       <c r="Q113" s="9"/>
       <c r="R113" s="9"/>
     </row>
-    <row r="114" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:18" ht="15.75" customHeight="1">
       <c r="A114" s="2">
         <v>44521.695289421295</v>
       </c>
@@ -7758,7 +7744,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="115" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:18" ht="15.75" customHeight="1">
       <c r="A115" s="2">
         <v>44521.703645162037</v>
       </c>
@@ -7796,7 +7782,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="116" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:18" ht="15.75" customHeight="1">
       <c r="A116" s="2">
         <v>44521.798439618055</v>
       </c>
@@ -7834,7 +7820,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="117" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:18" ht="15.75" customHeight="1">
       <c r="A117" s="2">
         <v>44521.806830486108</v>
       </c>
@@ -7872,7 +7858,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="118" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:18" ht="15.75" customHeight="1">
       <c r="A118" s="2">
         <v>44521.997838750001</v>
       </c>
@@ -7910,7 +7896,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="119" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:18" ht="15.75" customHeight="1">
       <c r="A119" s="2">
         <v>44522.038008958334</v>
       </c>
@@ -7948,7 +7934,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="120" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:18" ht="15.75" customHeight="1">
       <c r="A120" s="2">
         <v>44522.396687349537</v>
       </c>
@@ -7986,7 +7972,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="121" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:18" ht="15.75" customHeight="1">
       <c r="A121" s="2">
         <v>44522.424870671297</v>
       </c>
@@ -8024,7 +8010,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="122" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:18" ht="15.75" customHeight="1">
       <c r="A122" s="2">
         <v>44522.601772291666</v>
       </c>
@@ -8064,127 +8050,127 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="L3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="L4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="L5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="L6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="L7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="L8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="L9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="L10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="L11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="L12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="L13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="L14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="L15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="L16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="L17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="L18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="L19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="L20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="L21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="L22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="L23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="L24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="L25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="L26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="L27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="L28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="L29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="L30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="L31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="L32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="L33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="L34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="L35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="L36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="L37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="L38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="L39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="L40" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="L41" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="L42" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="L43" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="L44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="L45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="L46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="L47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="L48" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="L49" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="L50" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="L51" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="L52" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="L53" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="L54" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="L55" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="L56" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="L57" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="L58" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="L59" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="L60" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="L61" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="L62" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="L63" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="L64" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="L65" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="L66" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="L67" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="L68" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="L69" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="L70" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="L71" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="L72" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="L73" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="L74" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="L75" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="L76" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="L77" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="L78" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="L79" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="L80" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="L81" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="L82" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="L83" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="L84" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="L85" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="L86" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="L87" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="L88" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="L89" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="L90" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="L91" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="L92" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="L93" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="L94" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="L95" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="L96" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="L97" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="L98" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="L99" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="L100" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="L101" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="L102" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="L103" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
-    <hyperlink ref="L104" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
-    <hyperlink ref="L105" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="L106" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
-    <hyperlink ref="L107" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="L108" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
-    <hyperlink ref="L109" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
-    <hyperlink ref="L110" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
-    <hyperlink ref="L111" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="L112" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
-    <hyperlink ref="L113" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
-    <hyperlink ref="L114" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
-    <hyperlink ref="L115" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="L116" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
-    <hyperlink ref="L117" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
-    <hyperlink ref="L118" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
-    <hyperlink ref="L119" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
-    <hyperlink ref="L120" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
-    <hyperlink ref="L121" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
-    <hyperlink ref="L122" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="L2" r:id="rId1"/>
+    <hyperlink ref="L3" r:id="rId2"/>
+    <hyperlink ref="L4" r:id="rId3"/>
+    <hyperlink ref="L5" r:id="rId4"/>
+    <hyperlink ref="L6" r:id="rId5"/>
+    <hyperlink ref="L7" r:id="rId6"/>
+    <hyperlink ref="L8" r:id="rId7"/>
+    <hyperlink ref="L9" r:id="rId8"/>
+    <hyperlink ref="L10" r:id="rId9"/>
+    <hyperlink ref="L11" r:id="rId10"/>
+    <hyperlink ref="L12" r:id="rId11"/>
+    <hyperlink ref="L13" r:id="rId12"/>
+    <hyperlink ref="L14" r:id="rId13"/>
+    <hyperlink ref="L15" r:id="rId14"/>
+    <hyperlink ref="L16" r:id="rId15"/>
+    <hyperlink ref="L17" r:id="rId16"/>
+    <hyperlink ref="L18" r:id="rId17"/>
+    <hyperlink ref="L19" r:id="rId18"/>
+    <hyperlink ref="L20" r:id="rId19"/>
+    <hyperlink ref="L21" r:id="rId20"/>
+    <hyperlink ref="L22" r:id="rId21"/>
+    <hyperlink ref="L23" r:id="rId22"/>
+    <hyperlink ref="L24" r:id="rId23"/>
+    <hyperlink ref="L25" r:id="rId24"/>
+    <hyperlink ref="L26" r:id="rId25"/>
+    <hyperlink ref="L27" r:id="rId26"/>
+    <hyperlink ref="L28" r:id="rId27"/>
+    <hyperlink ref="L29" r:id="rId28"/>
+    <hyperlink ref="L30" r:id="rId29"/>
+    <hyperlink ref="L31" r:id="rId30"/>
+    <hyperlink ref="L32" r:id="rId31"/>
+    <hyperlink ref="L33" r:id="rId32"/>
+    <hyperlink ref="L34" r:id="rId33"/>
+    <hyperlink ref="L35" r:id="rId34"/>
+    <hyperlink ref="L36" r:id="rId35"/>
+    <hyperlink ref="L37" r:id="rId36"/>
+    <hyperlink ref="L38" r:id="rId37"/>
+    <hyperlink ref="L39" r:id="rId38"/>
+    <hyperlink ref="L40" r:id="rId39"/>
+    <hyperlink ref="L41" r:id="rId40"/>
+    <hyperlink ref="L42" r:id="rId41"/>
+    <hyperlink ref="L43" r:id="rId42"/>
+    <hyperlink ref="L44" r:id="rId43"/>
+    <hyperlink ref="L45" r:id="rId44"/>
+    <hyperlink ref="L46" r:id="rId45"/>
+    <hyperlink ref="L47" r:id="rId46"/>
+    <hyperlink ref="L48" r:id="rId47"/>
+    <hyperlink ref="L49" r:id="rId48"/>
+    <hyperlink ref="L50" r:id="rId49"/>
+    <hyperlink ref="L51" r:id="rId50"/>
+    <hyperlink ref="L52" r:id="rId51"/>
+    <hyperlink ref="L53" r:id="rId52"/>
+    <hyperlink ref="L54" r:id="rId53"/>
+    <hyperlink ref="L55" r:id="rId54"/>
+    <hyperlink ref="L56" r:id="rId55"/>
+    <hyperlink ref="L57" r:id="rId56"/>
+    <hyperlink ref="L58" r:id="rId57"/>
+    <hyperlink ref="L59" r:id="rId58"/>
+    <hyperlink ref="L60" r:id="rId59"/>
+    <hyperlink ref="L61" r:id="rId60"/>
+    <hyperlink ref="L62" r:id="rId61"/>
+    <hyperlink ref="L63" r:id="rId62"/>
+    <hyperlink ref="L64" r:id="rId63"/>
+    <hyperlink ref="L65" r:id="rId64"/>
+    <hyperlink ref="L66" r:id="rId65"/>
+    <hyperlink ref="L67" r:id="rId66"/>
+    <hyperlink ref="L68" r:id="rId67"/>
+    <hyperlink ref="L69" r:id="rId68"/>
+    <hyperlink ref="L70" r:id="rId69"/>
+    <hyperlink ref="L71" r:id="rId70"/>
+    <hyperlink ref="L72" r:id="rId71"/>
+    <hyperlink ref="L73" r:id="rId72"/>
+    <hyperlink ref="L74" r:id="rId73"/>
+    <hyperlink ref="L75" r:id="rId74"/>
+    <hyperlink ref="L76" r:id="rId75"/>
+    <hyperlink ref="L77" r:id="rId76"/>
+    <hyperlink ref="L78" r:id="rId77"/>
+    <hyperlink ref="L79" r:id="rId78"/>
+    <hyperlink ref="L80" r:id="rId79"/>
+    <hyperlink ref="L81" r:id="rId80"/>
+    <hyperlink ref="L82" r:id="rId81"/>
+    <hyperlink ref="L83" r:id="rId82"/>
+    <hyperlink ref="L84" r:id="rId83"/>
+    <hyperlink ref="L85" r:id="rId84"/>
+    <hyperlink ref="L86" r:id="rId85"/>
+    <hyperlink ref="L87" r:id="rId86"/>
+    <hyperlink ref="L88" r:id="rId87"/>
+    <hyperlink ref="L89" r:id="rId88"/>
+    <hyperlink ref="L90" r:id="rId89"/>
+    <hyperlink ref="L91" r:id="rId90"/>
+    <hyperlink ref="L92" r:id="rId91"/>
+    <hyperlink ref="L93" r:id="rId92"/>
+    <hyperlink ref="L94" r:id="rId93"/>
+    <hyperlink ref="L95" r:id="rId94"/>
+    <hyperlink ref="L96" r:id="rId95"/>
+    <hyperlink ref="L97" r:id="rId96"/>
+    <hyperlink ref="L98" r:id="rId97"/>
+    <hyperlink ref="L99" r:id="rId98"/>
+    <hyperlink ref="L100" r:id="rId99"/>
+    <hyperlink ref="L101" r:id="rId100"/>
+    <hyperlink ref="L102" r:id="rId101"/>
+    <hyperlink ref="L103" r:id="rId102"/>
+    <hyperlink ref="L104" r:id="rId103"/>
+    <hyperlink ref="L105" r:id="rId104"/>
+    <hyperlink ref="L106" r:id="rId105"/>
+    <hyperlink ref="L107" r:id="rId106"/>
+    <hyperlink ref="L108" r:id="rId107"/>
+    <hyperlink ref="L109" r:id="rId108"/>
+    <hyperlink ref="L110" r:id="rId109"/>
+    <hyperlink ref="L111" r:id="rId110"/>
+    <hyperlink ref="L112" r:id="rId111"/>
+    <hyperlink ref="L113" r:id="rId112"/>
+    <hyperlink ref="L114" r:id="rId113"/>
+    <hyperlink ref="L115" r:id="rId114"/>
+    <hyperlink ref="L116" r:id="rId115"/>
+    <hyperlink ref="L117" r:id="rId116"/>
+    <hyperlink ref="L118" r:id="rId117"/>
+    <hyperlink ref="L119" r:id="rId118"/>
+    <hyperlink ref="L120" r:id="rId119"/>
+    <hyperlink ref="L121" r:id="rId120"/>
+    <hyperlink ref="L122" r:id="rId121"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -8197,8 +8183,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -8209,22 +8195,22 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="25.5" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="33.140625" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" customWidth="1"/>
-    <col min="10" max="10" width="33.140625" customWidth="1"/>
-    <col min="11" max="16" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="33.1640625" customWidth="1"/>
+    <col min="8" max="8" width="9.5" customWidth="1"/>
+    <col min="9" max="9" width="17.5" customWidth="1"/>
+    <col min="10" max="10" width="33.1640625" customWidth="1"/>
+    <col min="11" max="16" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="39.75" customHeight="1">
       <c r="A1" s="11" t="s">
         <v>850</v>
       </c>
@@ -8262,7 +8248,7 @@
       <c r="O1" s="12"/>
       <c r="P1" s="12"/>
     </row>
-    <row r="2" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="12">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -8294,7 +8280,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="12">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -8326,7 +8312,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="12">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -8358,7 +8344,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" ht="12">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -8390,7 +8376,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" ht="12">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -8422,7 +8408,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="12">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -8454,7 +8440,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="12">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -8486,7 +8472,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="12">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -8518,7 +8504,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="12">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -8550,7 +8536,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" ht="12">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -8582,7 +8568,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" ht="12">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -8614,7 +8600,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" ht="12">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -8646,7 +8632,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" ht="12">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -8678,7 +8664,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" ht="12">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -8710,7 +8696,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" ht="12">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -8742,7 +8728,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="12">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -8774,7 +8760,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="12">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -8806,7 +8792,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="36">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -8838,7 +8824,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="12">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -8870,7 +8856,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="12">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -8902,7 +8888,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="12">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -8934,7 +8920,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="12">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -8966,7 +8952,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="12">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -8998,7 +8984,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="12">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -9030,7 +9016,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="12">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -9062,7 +9048,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="12">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -9094,7 +9080,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="12">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -9126,7 +9112,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="12">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -9158,7 +9144,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" ht="12">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -9190,7 +9176,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="12">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -9222,7 +9208,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="12">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -9254,7 +9240,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" ht="12">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -9286,7 +9272,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" ht="12">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -9318,7 +9304,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="12">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -9350,7 +9336,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" ht="12">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -9382,7 +9368,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" ht="12">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -9414,7 +9400,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" ht="12">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -9446,7 +9432,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" ht="12">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -9478,7 +9464,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" ht="12">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -9510,7 +9496,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" ht="12">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -9542,7 +9528,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" ht="12">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -9574,7 +9560,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" ht="12">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -9606,7 +9592,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" ht="12">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -9638,7 +9624,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" ht="12">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -9670,7 +9656,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" ht="12">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -9702,7 +9688,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" ht="12">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -9734,7 +9720,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" ht="12">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -9766,7 +9752,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" ht="12">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -9798,7 +9784,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" ht="12">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -9830,7 +9816,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" ht="12">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -9862,7 +9848,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" ht="12">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -9894,7 +9880,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" ht="12">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -9926,7 +9912,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" ht="12">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -9958,7 +9944,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" ht="12">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -9990,7 +9976,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" ht="12">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -10022,7 +10008,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" ht="12">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -10054,7 +10040,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" ht="12">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -10086,7 +10072,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" ht="12">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -10118,7 +10104,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" ht="12">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -10150,7 +10136,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" ht="12">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -10182,7 +10168,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" ht="12">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -10214,7 +10200,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" ht="12">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -10246,7 +10232,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" ht="12">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -10278,7 +10264,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" ht="12">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -10310,7 +10296,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" ht="12">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -10342,7 +10328,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" ht="12">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -10374,7 +10360,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" ht="12">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -10406,7 +10392,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" ht="12">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -10438,7 +10424,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10" ht="12">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -10470,7 +10456,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10" ht="12">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -10502,7 +10488,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10" ht="12">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -10534,7 +10520,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10" ht="12">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -10566,7 +10552,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10" ht="24">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -10598,7 +10584,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10" ht="12">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -10630,7 +10616,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10" ht="12">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -10662,7 +10648,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10" ht="12">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -10694,7 +10680,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10" ht="12">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -10726,7 +10712,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10" ht="12">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -10758,7 +10744,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10" ht="12">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -10790,7 +10776,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" ht="12">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -10822,7 +10808,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10" ht="12">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -10854,7 +10840,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10" ht="12">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -10886,7 +10872,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10" ht="12">
       <c r="A84" s="3">
         <v>83</v>
       </c>
@@ -10918,7 +10904,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:10" ht="12">
       <c r="A85" s="3">
         <v>84</v>
       </c>
@@ -10950,7 +10936,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10" ht="12">
       <c r="A86" s="3">
         <v>85</v>
       </c>
@@ -10982,7 +10968,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:10" ht="12">
       <c r="A87" s="3">
         <v>86</v>
       </c>
@@ -11014,7 +11000,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:10" ht="12">
       <c r="A88" s="3">
         <v>87</v>
       </c>
@@ -11046,7 +11032,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:10" ht="12">
       <c r="A89" s="3">
         <v>88</v>
       </c>
@@ -11078,7 +11064,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:10" ht="12">
       <c r="A90" s="3">
         <v>89</v>
       </c>
@@ -11110,7 +11096,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:10" ht="12">
       <c r="A91" s="3">
         <v>90</v>
       </c>
@@ -11142,7 +11128,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:10" ht="12">
       <c r="A92" s="3">
         <v>91</v>
       </c>
@@ -11174,7 +11160,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:10" ht="12">
       <c r="A93" s="3">
         <v>92</v>
       </c>
@@ -11206,7 +11192,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:10" ht="12">
       <c r="A94" s="3">
         <v>93</v>
       </c>
@@ -11238,7 +11224,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="95" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:10" ht="12">
       <c r="A95" s="3">
         <v>94</v>
       </c>
@@ -11270,7 +11256,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="96" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:10" ht="12">
       <c r="A96" s="3">
         <v>95</v>
       </c>
@@ -11302,7 +11288,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:10" ht="12">
       <c r="A97" s="3">
         <v>96</v>
       </c>
@@ -11334,7 +11320,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:10" ht="12">
       <c r="A98" s="3">
         <v>97</v>
       </c>
@@ -11366,7 +11352,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="99" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:10" ht="12">
       <c r="A99" s="3">
         <v>98</v>
       </c>
@@ -11398,7 +11384,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:10" ht="12">
       <c r="A100" s="3">
         <v>99</v>
       </c>
@@ -11430,7 +11416,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:10" ht="12">
       <c r="A101" s="3">
         <v>100</v>
       </c>
@@ -11462,7 +11448,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:10" ht="12">
       <c r="A102" s="3">
         <v>101</v>
       </c>
@@ -11491,7 +11477,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="103" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:10" ht="12">
       <c r="A103" s="3">
         <v>102</v>
       </c>
@@ -11520,7 +11506,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="104" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:10" ht="12">
       <c r="A104" s="3">
         <v>103</v>
       </c>
@@ -11552,7 +11538,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="105" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:10" ht="12">
       <c r="A105" s="3">
         <v>104</v>
       </c>
@@ -11584,7 +11570,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="106" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:10" ht="12">
       <c r="A106" s="3">
         <v>105</v>
       </c>
@@ -11616,7 +11602,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:10" ht="12">
       <c r="A107" s="3">
         <v>106</v>
       </c>
@@ -11648,7 +11634,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="108" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:10" ht="12">
       <c r="A108" s="3">
         <v>107</v>
       </c>
@@ -11680,7 +11666,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="109" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:10" ht="12">
       <c r="A109" s="3">
         <v>108</v>
       </c>
@@ -11712,7 +11698,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="110" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:10" ht="12">
       <c r="A110" s="3">
         <v>109</v>
       </c>
@@ -11744,7 +11730,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="111" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:10" ht="12">
       <c r="A111" s="3">
         <v>110</v>
       </c>
@@ -11776,7 +11762,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:10" ht="12">
       <c r="A112" s="3">
         <v>111</v>
       </c>
@@ -11805,7 +11791,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="113" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:10" ht="12">
       <c r="A113" s="3">
         <v>112</v>
       </c>
@@ -11837,7 +11823,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="114" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:10" ht="12">
       <c r="A114" s="3">
         <v>113</v>
       </c>
@@ -11869,298 +11855,298 @@
         <v>872</v>
       </c>
     </row>
-    <row r="115" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:10" ht="12">
       <c r="J115" s="15"/>
     </row>
-    <row r="116" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:10" ht="12">
       <c r="J116" s="15"/>
     </row>
-    <row r="117" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:10" ht="12">
       <c r="J117" s="15"/>
     </row>
-    <row r="118" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:10" ht="12">
       <c r="J118" s="15"/>
     </row>
-    <row r="119" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:10" ht="12">
       <c r="J119" s="15"/>
     </row>
-    <row r="120" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:10" ht="12">
       <c r="J120" s="15"/>
     </row>
-    <row r="121" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:10" ht="12">
       <c r="J121" s="15"/>
     </row>
-    <row r="122" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:10" ht="12">
       <c r="J122" s="15"/>
     </row>
-    <row r="123" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:10" ht="12">
       <c r="J123" s="15"/>
     </row>
-    <row r="124" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:10" ht="12">
       <c r="J124" s="15"/>
     </row>
-    <row r="125" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:10" ht="12">
       <c r="J125" s="15"/>
     </row>
-    <row r="126" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:10" ht="12">
       <c r="J126" s="15"/>
     </row>
-    <row r="127" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:10" ht="12">
       <c r="J127" s="15"/>
     </row>
-    <row r="128" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:10" ht="12">
       <c r="J128" s="15"/>
     </row>
-    <row r="129" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="129" spans="10:10" ht="12">
       <c r="J129" s="15"/>
     </row>
-    <row r="130" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="130" spans="10:10" ht="12">
       <c r="J130" s="15"/>
     </row>
-    <row r="131" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="131" spans="10:10" ht="12">
       <c r="J131" s="15"/>
     </row>
-    <row r="132" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="132" spans="10:10" ht="12">
       <c r="J132" s="15"/>
     </row>
-    <row r="133" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="133" spans="10:10" ht="12">
       <c r="J133" s="15"/>
     </row>
-    <row r="134" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="134" spans="10:10" ht="12">
       <c r="J134" s="15"/>
     </row>
-    <row r="135" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="135" spans="10:10" ht="12">
       <c r="J135" s="15"/>
     </row>
-    <row r="136" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="136" spans="10:10" ht="12">
       <c r="J136" s="15"/>
     </row>
-    <row r="137" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="137" spans="10:10" ht="12">
       <c r="J137" s="15"/>
     </row>
-    <row r="138" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="138" spans="10:10" ht="12">
       <c r="J138" s="15"/>
     </row>
-    <row r="139" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="139" spans="10:10" ht="12">
       <c r="J139" s="15"/>
     </row>
-    <row r="140" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="140" spans="10:10" ht="12">
       <c r="J140" s="15"/>
     </row>
-    <row r="141" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="141" spans="10:10" ht="12">
       <c r="J141" s="15"/>
     </row>
-    <row r="142" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="142" spans="10:10" ht="12">
       <c r="J142" s="15"/>
     </row>
-    <row r="143" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="143" spans="10:10" ht="12">
       <c r="J143" s="15"/>
     </row>
-    <row r="144" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="144" spans="10:10" ht="12">
       <c r="J144" s="15"/>
     </row>
-    <row r="145" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="145" spans="10:10" ht="12">
       <c r="J145" s="15"/>
     </row>
-    <row r="146" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="146" spans="10:10" ht="12">
       <c r="J146" s="15"/>
     </row>
-    <row r="147" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="147" spans="10:10" ht="12">
       <c r="J147" s="15"/>
     </row>
-    <row r="148" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="148" spans="10:10" ht="12">
       <c r="J148" s="15"/>
     </row>
-    <row r="149" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="149" spans="10:10" ht="12">
       <c r="J149" s="15"/>
     </row>
-    <row r="150" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="150" spans="10:10" ht="12">
       <c r="J150" s="15"/>
     </row>
-    <row r="151" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="151" spans="10:10" ht="12">
       <c r="J151" s="15"/>
     </row>
-    <row r="152" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="152" spans="10:10" ht="12">
       <c r="J152" s="15"/>
     </row>
-    <row r="153" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="153" spans="10:10" ht="12">
       <c r="J153" s="15"/>
     </row>
-    <row r="154" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="154" spans="10:10" ht="12">
       <c r="J154" s="15"/>
     </row>
-    <row r="155" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="155" spans="10:10" ht="12">
       <c r="J155" s="15"/>
     </row>
-    <row r="156" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="156" spans="10:10" ht="12">
       <c r="J156" s="15"/>
     </row>
-    <row r="157" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="157" spans="10:10" ht="12">
       <c r="J157" s="15"/>
     </row>
-    <row r="158" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="158" spans="10:10" ht="12">
       <c r="J158" s="15"/>
     </row>
-    <row r="159" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="159" spans="10:10" ht="12">
       <c r="J159" s="15"/>
     </row>
-    <row r="160" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="160" spans="10:10" ht="12">
       <c r="J160" s="15"/>
     </row>
-    <row r="161" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="161" spans="10:10" ht="12">
       <c r="J161" s="15"/>
     </row>
-    <row r="162" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="162" spans="10:10" ht="12">
       <c r="J162" s="15"/>
     </row>
-    <row r="163" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="163" spans="10:10" ht="12">
       <c r="J163" s="15"/>
     </row>
-    <row r="164" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="164" spans="10:10" ht="12">
       <c r="J164" s="15"/>
     </row>
-    <row r="165" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="165" spans="10:10" ht="12">
       <c r="J165" s="15"/>
     </row>
-    <row r="166" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="166" spans="10:10" ht="12">
       <c r="J166" s="15"/>
     </row>
-    <row r="167" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="167" spans="10:10" ht="12">
       <c r="J167" s="15"/>
     </row>
-    <row r="168" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="168" spans="10:10" ht="12">
       <c r="J168" s="15"/>
     </row>
-    <row r="169" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="169" spans="10:10" ht="12">
       <c r="J169" s="15"/>
     </row>
-    <row r="170" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="170" spans="10:10" ht="12">
       <c r="J170" s="15"/>
     </row>
-    <row r="171" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="171" spans="10:10" ht="12">
       <c r="J171" s="15"/>
     </row>
-    <row r="172" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="172" spans="10:10" ht="12">
       <c r="J172" s="15"/>
     </row>
-    <row r="173" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="173" spans="10:10" ht="12">
       <c r="J173" s="15"/>
     </row>
-    <row r="174" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="174" spans="10:10" ht="12">
       <c r="J174" s="15"/>
     </row>
-    <row r="175" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="175" spans="10:10" ht="12">
       <c r="J175" s="15"/>
     </row>
-    <row r="176" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="176" spans="10:10" ht="12">
       <c r="J176" s="15"/>
     </row>
-    <row r="177" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="177" spans="10:10" ht="12">
       <c r="J177" s="15"/>
     </row>
-    <row r="178" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="178" spans="10:10" ht="12">
       <c r="J178" s="15"/>
     </row>
-    <row r="179" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="179" spans="10:10" ht="12">
       <c r="J179" s="15"/>
     </row>
-    <row r="180" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="180" spans="10:10" ht="12">
       <c r="J180" s="15"/>
     </row>
-    <row r="181" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="181" spans="10:10" ht="12">
       <c r="J181" s="15"/>
     </row>
-    <row r="182" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="182" spans="10:10" ht="12">
       <c r="J182" s="15"/>
     </row>
-    <row r="183" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="183" spans="10:10" ht="12">
       <c r="J183" s="15"/>
     </row>
-    <row r="184" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="184" spans="10:10" ht="12">
       <c r="J184" s="15"/>
     </row>
-    <row r="185" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="185" spans="10:10" ht="12">
       <c r="J185" s="15"/>
     </row>
-    <row r="186" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="186" spans="10:10" ht="12">
       <c r="J186" s="15"/>
     </row>
-    <row r="187" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="187" spans="10:10" ht="12">
       <c r="J187" s="15"/>
     </row>
-    <row r="188" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="188" spans="10:10" ht="12">
       <c r="J188" s="15"/>
     </row>
-    <row r="189" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="189" spans="10:10" ht="12">
       <c r="J189" s="15"/>
     </row>
-    <row r="190" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="190" spans="10:10" ht="12">
       <c r="J190" s="15"/>
     </row>
-    <row r="191" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="191" spans="10:10" ht="12">
       <c r="J191" s="15"/>
     </row>
-    <row r="192" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="192" spans="10:10" ht="12">
       <c r="J192" s="15"/>
     </row>
-    <row r="193" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="193" spans="10:10" ht="12">
       <c r="J193" s="15"/>
     </row>
-    <row r="194" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="194" spans="10:10" ht="12">
       <c r="J194" s="15"/>
     </row>
-    <row r="195" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="195" spans="10:10" ht="12">
       <c r="J195" s="15"/>
     </row>
-    <row r="196" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="196" spans="10:10" ht="12">
       <c r="J196" s="15"/>
     </row>
-    <row r="197" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="197" spans="10:10" ht="12">
       <c r="J197" s="15"/>
     </row>
-    <row r="198" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="198" spans="10:10" ht="12">
       <c r="J198" s="15"/>
     </row>
-    <row r="199" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="199" spans="10:10" ht="12">
       <c r="J199" s="15"/>
     </row>
-    <row r="200" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="200" spans="10:10" ht="12">
       <c r="J200" s="15"/>
     </row>
-    <row r="201" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="201" spans="10:10" ht="12">
       <c r="J201" s="15"/>
     </row>
-    <row r="202" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="202" spans="10:10" ht="12">
       <c r="J202" s="15"/>
     </row>
-    <row r="203" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="203" spans="10:10" ht="12">
       <c r="J203" s="15"/>
     </row>
-    <row r="204" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="204" spans="10:10" ht="12">
       <c r="J204" s="15"/>
     </row>
-    <row r="205" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="205" spans="10:10" ht="12">
       <c r="J205" s="15"/>
     </row>
-    <row r="206" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="206" spans="10:10" ht="12">
       <c r="J206" s="15"/>
     </row>
-    <row r="207" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="207" spans="10:10" ht="12">
       <c r="J207" s="15"/>
     </row>
-    <row r="208" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="208" spans="10:10" ht="12">
       <c r="J208" s="15"/>
     </row>
-    <row r="209" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="209" spans="10:10" ht="12">
       <c r="J209" s="15"/>
     </row>
-    <row r="210" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="210" spans="10:10" ht="12">
       <c r="J210" s="15"/>
     </row>
-    <row r="211" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="211" spans="10:10" ht="12">
       <c r="J211" s="15"/>
     </row>
-    <row r="212" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="212" spans="10:10" ht="12">
       <c r="J212" s="15"/>
     </row>
   </sheetData>
@@ -12170,119 +12156,119 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="J3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="J4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="J5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="J6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="J7" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="J8" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="J9" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
-    <hyperlink ref="J10" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="J11" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
-    <hyperlink ref="J12" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
-    <hyperlink ref="J13" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
-    <hyperlink ref="J14" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
-    <hyperlink ref="J15" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
-    <hyperlink ref="J16" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
-    <hyperlink ref="J17" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
-    <hyperlink ref="J18" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
-    <hyperlink ref="J19" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
-    <hyperlink ref="J20" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
-    <hyperlink ref="J21" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
-    <hyperlink ref="J22" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
-    <hyperlink ref="J23" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
-    <hyperlink ref="J24" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
-    <hyperlink ref="J25" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
-    <hyperlink ref="J26" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
-    <hyperlink ref="J27" r:id="rId26" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
-    <hyperlink ref="J28" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
-    <hyperlink ref="J29" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
-    <hyperlink ref="J30" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
-    <hyperlink ref="J31" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
-    <hyperlink ref="J32" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
-    <hyperlink ref="J33" r:id="rId32" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
-    <hyperlink ref="J34" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
-    <hyperlink ref="J35" r:id="rId34" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
-    <hyperlink ref="J36" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
-    <hyperlink ref="J37" r:id="rId36" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
-    <hyperlink ref="J38" r:id="rId37" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
-    <hyperlink ref="J39" r:id="rId38" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
-    <hyperlink ref="J40" r:id="rId39" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
-    <hyperlink ref="J41" r:id="rId40" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
-    <hyperlink ref="J42" r:id="rId41" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
-    <hyperlink ref="J43" r:id="rId42" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
-    <hyperlink ref="J44" r:id="rId43" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
-    <hyperlink ref="J45" r:id="rId44" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
-    <hyperlink ref="J46" r:id="rId45" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
-    <hyperlink ref="J47" r:id="rId46" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
-    <hyperlink ref="J48" r:id="rId47" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
-    <hyperlink ref="J49" r:id="rId48" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
-    <hyperlink ref="J50" r:id="rId49" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
-    <hyperlink ref="J51" r:id="rId50" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
-    <hyperlink ref="J52" r:id="rId51" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
-    <hyperlink ref="J53" r:id="rId52" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
-    <hyperlink ref="J54" r:id="rId53" xr:uid="{00000000-0004-0000-0100-000034000000}"/>
-    <hyperlink ref="J55" r:id="rId54" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
-    <hyperlink ref="J56" r:id="rId55" xr:uid="{00000000-0004-0000-0100-000036000000}"/>
-    <hyperlink ref="J57" r:id="rId56" xr:uid="{00000000-0004-0000-0100-000037000000}"/>
-    <hyperlink ref="J58" r:id="rId57" xr:uid="{00000000-0004-0000-0100-000038000000}"/>
-    <hyperlink ref="J59" r:id="rId58" xr:uid="{00000000-0004-0000-0100-000039000000}"/>
-    <hyperlink ref="J60" r:id="rId59" xr:uid="{00000000-0004-0000-0100-00003A000000}"/>
-    <hyperlink ref="J61" r:id="rId60" xr:uid="{00000000-0004-0000-0100-00003B000000}"/>
-    <hyperlink ref="J62" r:id="rId61" xr:uid="{00000000-0004-0000-0100-00003C000000}"/>
-    <hyperlink ref="J63" r:id="rId62" xr:uid="{00000000-0004-0000-0100-00003D000000}"/>
-    <hyperlink ref="J64" r:id="rId63" xr:uid="{00000000-0004-0000-0100-00003E000000}"/>
-    <hyperlink ref="J65" r:id="rId64" xr:uid="{00000000-0004-0000-0100-00003F000000}"/>
-    <hyperlink ref="J66" r:id="rId65" xr:uid="{00000000-0004-0000-0100-000040000000}"/>
-    <hyperlink ref="J67" r:id="rId66" xr:uid="{00000000-0004-0000-0100-000041000000}"/>
-    <hyperlink ref="J68" r:id="rId67" xr:uid="{00000000-0004-0000-0100-000042000000}"/>
-    <hyperlink ref="J69" r:id="rId68" xr:uid="{00000000-0004-0000-0100-000043000000}"/>
-    <hyperlink ref="J70" r:id="rId69" xr:uid="{00000000-0004-0000-0100-000044000000}"/>
-    <hyperlink ref="J71" r:id="rId70" xr:uid="{00000000-0004-0000-0100-000045000000}"/>
-    <hyperlink ref="J72" r:id="rId71" xr:uid="{00000000-0004-0000-0100-000046000000}"/>
-    <hyperlink ref="J73" r:id="rId72" xr:uid="{00000000-0004-0000-0100-000047000000}"/>
-    <hyperlink ref="J74" r:id="rId73" xr:uid="{00000000-0004-0000-0100-000048000000}"/>
-    <hyperlink ref="J75" r:id="rId74" xr:uid="{00000000-0004-0000-0100-000049000000}"/>
-    <hyperlink ref="J76" r:id="rId75" xr:uid="{00000000-0004-0000-0100-00004A000000}"/>
-    <hyperlink ref="J77" r:id="rId76" xr:uid="{00000000-0004-0000-0100-00004B000000}"/>
-    <hyperlink ref="J78" r:id="rId77" xr:uid="{00000000-0004-0000-0100-00004C000000}"/>
-    <hyperlink ref="J79" r:id="rId78" xr:uid="{00000000-0004-0000-0100-00004D000000}"/>
-    <hyperlink ref="J80" r:id="rId79" xr:uid="{00000000-0004-0000-0100-00004E000000}"/>
-    <hyperlink ref="J81" r:id="rId80" xr:uid="{00000000-0004-0000-0100-00004F000000}"/>
-    <hyperlink ref="J82" r:id="rId81" xr:uid="{00000000-0004-0000-0100-000050000000}"/>
-    <hyperlink ref="J83" r:id="rId82" xr:uid="{00000000-0004-0000-0100-000051000000}"/>
-    <hyperlink ref="J84" r:id="rId83" xr:uid="{00000000-0004-0000-0100-000052000000}"/>
-    <hyperlink ref="J85" r:id="rId84" xr:uid="{00000000-0004-0000-0100-000053000000}"/>
-    <hyperlink ref="J86" r:id="rId85" xr:uid="{00000000-0004-0000-0100-000054000000}"/>
-    <hyperlink ref="J87" r:id="rId86" xr:uid="{00000000-0004-0000-0100-000055000000}"/>
-    <hyperlink ref="J88" r:id="rId87" xr:uid="{00000000-0004-0000-0100-000056000000}"/>
-    <hyperlink ref="J89" r:id="rId88" xr:uid="{00000000-0004-0000-0100-000057000000}"/>
-    <hyperlink ref="J90" r:id="rId89" xr:uid="{00000000-0004-0000-0100-000058000000}"/>
-    <hyperlink ref="J91" r:id="rId90" xr:uid="{00000000-0004-0000-0100-000059000000}"/>
-    <hyperlink ref="J92" r:id="rId91" xr:uid="{00000000-0004-0000-0100-00005A000000}"/>
-    <hyperlink ref="J93" r:id="rId92" xr:uid="{00000000-0004-0000-0100-00005B000000}"/>
-    <hyperlink ref="J94" r:id="rId93" xr:uid="{00000000-0004-0000-0100-00005C000000}"/>
-    <hyperlink ref="J95" r:id="rId94" xr:uid="{00000000-0004-0000-0100-00005D000000}"/>
-    <hyperlink ref="J96" r:id="rId95" xr:uid="{00000000-0004-0000-0100-00005E000000}"/>
-    <hyperlink ref="J97" r:id="rId96" xr:uid="{00000000-0004-0000-0100-00005F000000}"/>
-    <hyperlink ref="J98" r:id="rId97" xr:uid="{00000000-0004-0000-0100-000060000000}"/>
-    <hyperlink ref="J99" r:id="rId98" xr:uid="{00000000-0004-0000-0100-000061000000}"/>
-    <hyperlink ref="J100" r:id="rId99" xr:uid="{00000000-0004-0000-0100-000062000000}"/>
-    <hyperlink ref="J101" r:id="rId100" xr:uid="{00000000-0004-0000-0100-000063000000}"/>
-    <hyperlink ref="J102" r:id="rId101" xr:uid="{00000000-0004-0000-0100-000064000000}"/>
-    <hyperlink ref="J103" r:id="rId102" xr:uid="{00000000-0004-0000-0100-000065000000}"/>
-    <hyperlink ref="J104" r:id="rId103" xr:uid="{00000000-0004-0000-0100-000066000000}"/>
-    <hyperlink ref="J105" r:id="rId104" xr:uid="{00000000-0004-0000-0100-000067000000}"/>
-    <hyperlink ref="J106" r:id="rId105" xr:uid="{00000000-0004-0000-0100-000068000000}"/>
-    <hyperlink ref="J107" r:id="rId106" xr:uid="{00000000-0004-0000-0100-000069000000}"/>
-    <hyperlink ref="J108" r:id="rId107" xr:uid="{00000000-0004-0000-0100-00006A000000}"/>
-    <hyperlink ref="J109" r:id="rId108" xr:uid="{00000000-0004-0000-0100-00006B000000}"/>
-    <hyperlink ref="J110" r:id="rId109" xr:uid="{00000000-0004-0000-0100-00006C000000}"/>
-    <hyperlink ref="J111" r:id="rId110" xr:uid="{00000000-0004-0000-0100-00006D000000}"/>
-    <hyperlink ref="J112" r:id="rId111" xr:uid="{00000000-0004-0000-0100-00006E000000}"/>
-    <hyperlink ref="J113" r:id="rId112" xr:uid="{00000000-0004-0000-0100-00006F000000}"/>
-    <hyperlink ref="J114" r:id="rId113" xr:uid="{00000000-0004-0000-0100-000070000000}"/>
+    <hyperlink ref="J2" r:id="rId1"/>
+    <hyperlink ref="J3" r:id="rId2"/>
+    <hyperlink ref="J4" r:id="rId3"/>
+    <hyperlink ref="J5" r:id="rId4"/>
+    <hyperlink ref="J6" r:id="rId5"/>
+    <hyperlink ref="J7" r:id="rId6"/>
+    <hyperlink ref="J8" r:id="rId7"/>
+    <hyperlink ref="J9" r:id="rId8"/>
+    <hyperlink ref="J10" r:id="rId9"/>
+    <hyperlink ref="J11" r:id="rId10"/>
+    <hyperlink ref="J12" r:id="rId11"/>
+    <hyperlink ref="J13" r:id="rId12"/>
+    <hyperlink ref="J14" r:id="rId13"/>
+    <hyperlink ref="J15" r:id="rId14"/>
+    <hyperlink ref="J16" r:id="rId15"/>
+    <hyperlink ref="J17" r:id="rId16"/>
+    <hyperlink ref="J18" r:id="rId17"/>
+    <hyperlink ref="J19" r:id="rId18"/>
+    <hyperlink ref="J20" r:id="rId19"/>
+    <hyperlink ref="J21" r:id="rId20"/>
+    <hyperlink ref="J22" r:id="rId21"/>
+    <hyperlink ref="J23" r:id="rId22"/>
+    <hyperlink ref="J24" r:id="rId23"/>
+    <hyperlink ref="J25" r:id="rId24"/>
+    <hyperlink ref="J26" r:id="rId25"/>
+    <hyperlink ref="J27" r:id="rId26"/>
+    <hyperlink ref="J28" r:id="rId27"/>
+    <hyperlink ref="J29" r:id="rId28"/>
+    <hyperlink ref="J30" r:id="rId29"/>
+    <hyperlink ref="J31" r:id="rId30"/>
+    <hyperlink ref="J32" r:id="rId31"/>
+    <hyperlink ref="J33" r:id="rId32"/>
+    <hyperlink ref="J34" r:id="rId33"/>
+    <hyperlink ref="J35" r:id="rId34"/>
+    <hyperlink ref="J36" r:id="rId35"/>
+    <hyperlink ref="J37" r:id="rId36"/>
+    <hyperlink ref="J38" r:id="rId37"/>
+    <hyperlink ref="J39" r:id="rId38"/>
+    <hyperlink ref="J40" r:id="rId39"/>
+    <hyperlink ref="J41" r:id="rId40"/>
+    <hyperlink ref="J42" r:id="rId41"/>
+    <hyperlink ref="J43" r:id="rId42"/>
+    <hyperlink ref="J44" r:id="rId43"/>
+    <hyperlink ref="J45" r:id="rId44"/>
+    <hyperlink ref="J46" r:id="rId45"/>
+    <hyperlink ref="J47" r:id="rId46"/>
+    <hyperlink ref="J48" r:id="rId47"/>
+    <hyperlink ref="J49" r:id="rId48"/>
+    <hyperlink ref="J50" r:id="rId49"/>
+    <hyperlink ref="J51" r:id="rId50"/>
+    <hyperlink ref="J52" r:id="rId51"/>
+    <hyperlink ref="J53" r:id="rId52"/>
+    <hyperlink ref="J54" r:id="rId53"/>
+    <hyperlink ref="J55" r:id="rId54"/>
+    <hyperlink ref="J56" r:id="rId55"/>
+    <hyperlink ref="J57" r:id="rId56"/>
+    <hyperlink ref="J58" r:id="rId57"/>
+    <hyperlink ref="J59" r:id="rId58"/>
+    <hyperlink ref="J60" r:id="rId59"/>
+    <hyperlink ref="J61" r:id="rId60"/>
+    <hyperlink ref="J62" r:id="rId61"/>
+    <hyperlink ref="J63" r:id="rId62"/>
+    <hyperlink ref="J64" r:id="rId63"/>
+    <hyperlink ref="J65" r:id="rId64"/>
+    <hyperlink ref="J66" r:id="rId65"/>
+    <hyperlink ref="J67" r:id="rId66"/>
+    <hyperlink ref="J68" r:id="rId67"/>
+    <hyperlink ref="J69" r:id="rId68"/>
+    <hyperlink ref="J70" r:id="rId69"/>
+    <hyperlink ref="J71" r:id="rId70"/>
+    <hyperlink ref="J72" r:id="rId71"/>
+    <hyperlink ref="J73" r:id="rId72"/>
+    <hyperlink ref="J74" r:id="rId73"/>
+    <hyperlink ref="J75" r:id="rId74"/>
+    <hyperlink ref="J76" r:id="rId75"/>
+    <hyperlink ref="J77" r:id="rId76"/>
+    <hyperlink ref="J78" r:id="rId77"/>
+    <hyperlink ref="J79" r:id="rId78"/>
+    <hyperlink ref="J80" r:id="rId79"/>
+    <hyperlink ref="J81" r:id="rId80"/>
+    <hyperlink ref="J82" r:id="rId81"/>
+    <hyperlink ref="J83" r:id="rId82"/>
+    <hyperlink ref="J84" r:id="rId83"/>
+    <hyperlink ref="J85" r:id="rId84"/>
+    <hyperlink ref="J86" r:id="rId85"/>
+    <hyperlink ref="J87" r:id="rId86"/>
+    <hyperlink ref="J88" r:id="rId87"/>
+    <hyperlink ref="J89" r:id="rId88"/>
+    <hyperlink ref="J90" r:id="rId89"/>
+    <hyperlink ref="J91" r:id="rId90"/>
+    <hyperlink ref="J92" r:id="rId91"/>
+    <hyperlink ref="J93" r:id="rId92"/>
+    <hyperlink ref="J94" r:id="rId93"/>
+    <hyperlink ref="J95" r:id="rId94"/>
+    <hyperlink ref="J96" r:id="rId95"/>
+    <hyperlink ref="J97" r:id="rId96"/>
+    <hyperlink ref="J98" r:id="rId97"/>
+    <hyperlink ref="J99" r:id="rId98"/>
+    <hyperlink ref="J100" r:id="rId99"/>
+    <hyperlink ref="J101" r:id="rId100"/>
+    <hyperlink ref="J102" r:id="rId101"/>
+    <hyperlink ref="J103" r:id="rId102"/>
+    <hyperlink ref="J104" r:id="rId103"/>
+    <hyperlink ref="J105" r:id="rId104"/>
+    <hyperlink ref="J106" r:id="rId105"/>
+    <hyperlink ref="J107" r:id="rId106"/>
+    <hyperlink ref="J108" r:id="rId107"/>
+    <hyperlink ref="J109" r:id="rId108"/>
+    <hyperlink ref="J110" r:id="rId109"/>
+    <hyperlink ref="J111" r:id="rId110"/>
+    <hyperlink ref="J112" r:id="rId111"/>
+    <hyperlink ref="J113" r:id="rId112"/>
+    <hyperlink ref="J114" r:id="rId113"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -12296,8 +12282,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -12308,22 +12294,22 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="25.5" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="33.140625" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" customWidth="1"/>
-    <col min="10" max="10" width="33.140625" customWidth="1"/>
-    <col min="11" max="16" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="33.1640625" customWidth="1"/>
+    <col min="8" max="8" width="9.5" customWidth="1"/>
+    <col min="9" max="9" width="17.5" customWidth="1"/>
+    <col min="10" max="10" width="33.1640625" customWidth="1"/>
+    <col min="11" max="16" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="39.75" customHeight="1">
       <c r="A1" s="11" t="s">
         <v>850</v>
       </c>
@@ -12361,7 +12347,7 @@
       <c r="O1" s="12"/>
       <c r="P1" s="12"/>
     </row>
-    <row r="2" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="12">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -12393,7 +12379,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="12">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -12425,7 +12411,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="12">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -12457,7 +12443,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" ht="12">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -12489,7 +12475,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" ht="12">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -12521,7 +12507,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="12">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -12553,7 +12539,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="12">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -12585,7 +12571,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="12">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -12617,7 +12603,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="12">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -12649,7 +12635,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" ht="12">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -12681,7 +12667,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" ht="12">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -12713,7 +12699,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" ht="12">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -12745,7 +12731,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" ht="12">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -12777,7 +12763,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" ht="12">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -12809,7 +12795,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" ht="12">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -12841,7 +12827,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="12">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -12873,7 +12859,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="36">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -12905,7 +12891,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="12">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -12937,7 +12923,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="12">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -12969,7 +12955,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="12">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -13001,7 +12987,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="12">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -13033,7 +13019,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="12">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -13065,7 +13051,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="12">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -13097,7 +13083,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="12">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -13129,7 +13115,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="12">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -13161,7 +13147,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="12">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -13193,7 +13179,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="12">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -13225,7 +13211,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="12">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -13257,7 +13243,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" ht="12">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -13289,7 +13275,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="12">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -13321,7 +13307,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="12">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -13353,7 +13339,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" ht="12">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -13385,7 +13371,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" ht="12">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -13417,7 +13403,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="12">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -13449,7 +13435,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" ht="12">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -13481,7 +13467,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" ht="12">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -13513,7 +13499,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" ht="12">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -13545,7 +13531,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" ht="12">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -13577,7 +13563,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" ht="12">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -13609,7 +13595,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" ht="12">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -13641,7 +13627,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" ht="12">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -13673,7 +13659,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" ht="12">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -13705,7 +13691,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" ht="12">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -13737,7 +13723,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" ht="12">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -13769,7 +13755,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" ht="12">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -13801,7 +13787,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" ht="12">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -13833,7 +13819,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" ht="12">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -13865,7 +13851,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" ht="12">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -13897,7 +13883,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" ht="12">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -13929,7 +13915,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" ht="12">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -13961,7 +13947,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" ht="12">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -13993,7 +13979,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" ht="12">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -14025,7 +14011,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" ht="12">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -14057,7 +14043,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" ht="12">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -14089,7 +14075,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" ht="12">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -14121,7 +14107,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" ht="12">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -14153,7 +14139,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" ht="12">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -14185,7 +14171,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" ht="12">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -14217,7 +14203,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" ht="12">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -14249,7 +14235,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" ht="12">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -14281,7 +14267,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" ht="12">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -14313,7 +14299,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" ht="12">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -14345,7 +14331,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" ht="24">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -14377,7 +14363,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" ht="12">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -14409,7 +14395,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" ht="12">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -14441,7 +14427,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" ht="12">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -14473,7 +14459,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" ht="12">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -14505,7 +14491,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" ht="12">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -14537,7 +14523,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10" ht="12">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -14569,7 +14555,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10" ht="12">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -14601,7 +14587,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10" ht="12">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -14633,7 +14619,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10" ht="12">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -14665,7 +14651,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10" ht="12">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -14697,7 +14683,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10" ht="12">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -14729,7 +14715,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10" ht="12">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -14761,7 +14747,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10" ht="12">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -14793,7 +14779,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10" ht="12">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -14825,7 +14811,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10" ht="12">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -14857,7 +14843,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10" ht="12">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -14889,7 +14875,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" ht="12">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -14921,7 +14907,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10" ht="12">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -14953,7 +14939,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10" ht="12">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -14985,7 +14971,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10" ht="12">
       <c r="A84" s="3">
         <v>83</v>
       </c>
@@ -15017,7 +15003,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:10" ht="12">
       <c r="A85" s="3">
         <v>84</v>
       </c>
@@ -15049,7 +15035,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10" ht="12">
       <c r="A86" s="3">
         <v>85</v>
       </c>
@@ -15081,7 +15067,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:10" ht="12">
       <c r="A87" s="3">
         <v>86</v>
       </c>
@@ -15113,7 +15099,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:10" ht="12">
       <c r="A88" s="3">
         <v>87</v>
       </c>
@@ -15142,7 +15128,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:10" ht="12">
       <c r="A89" s="3">
         <v>88</v>
       </c>
@@ -15171,7 +15157,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:10" ht="12">
       <c r="A90" s="3">
         <v>89</v>
       </c>
@@ -15203,7 +15189,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:10" ht="12">
       <c r="A91" s="3">
         <v>90</v>
       </c>
@@ -15235,7 +15221,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:10" ht="12">
       <c r="A92" s="3">
         <v>91</v>
       </c>
@@ -15267,7 +15253,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:10" ht="12">
       <c r="A93" s="3">
         <v>92</v>
       </c>
@@ -15299,7 +15285,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:10" ht="12">
       <c r="A94" s="3">
         <v>93</v>
       </c>
@@ -15331,7 +15317,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="95" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:10" ht="12">
       <c r="A95" s="3">
         <v>94</v>
       </c>
@@ -15363,7 +15349,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="96" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:10" ht="12">
       <c r="A96" s="3">
         <v>95</v>
       </c>
@@ -15395,7 +15381,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:10" ht="12">
       <c r="A97" s="3">
         <v>96</v>
       </c>
@@ -15427,7 +15413,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:10" ht="12">
       <c r="A98" s="3">
         <v>97</v>
       </c>
@@ -15456,7 +15442,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="99" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:10" ht="12">
       <c r="A99" s="3">
         <v>98</v>
       </c>
@@ -15488,7 +15474,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:10" ht="12">
       <c r="A100" s="3">
         <v>99</v>
       </c>
@@ -15520,7 +15506,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:10" ht="12">
       <c r="A101" s="3">
         <v>100</v>
       </c>
@@ -15552,7 +15538,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:10" ht="12">
       <c r="A102" s="3">
         <v>101</v>
       </c>
@@ -15584,7 +15570,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="103" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:10" ht="12">
       <c r="A103" s="3">
         <v>102</v>
       </c>
@@ -15616,7 +15602,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="104" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:10" ht="12">
       <c r="A104" s="3">
         <v>103</v>
       </c>
@@ -15648,7 +15634,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="105" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:10" ht="12">
       <c r="A105" s="3">
         <v>104</v>
       </c>
@@ -15680,7 +15666,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="106" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:10" ht="12">
       <c r="A106" s="3">
         <v>105</v>
       </c>
@@ -15712,7 +15698,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:10" ht="12">
       <c r="A107" s="3">
         <v>106</v>
       </c>
@@ -15744,7 +15730,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="108" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:10" ht="12">
       <c r="A108" s="3">
         <v>107</v>
       </c>
@@ -15776,7 +15762,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="109" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:10" ht="12">
       <c r="A109" s="3">
         <v>108</v>
       </c>
@@ -15808,271 +15794,271 @@
         <v>849</v>
       </c>
     </row>
-    <row r="110" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:10" ht="12">
       <c r="J110" s="15"/>
     </row>
-    <row r="111" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:10" ht="12">
       <c r="J111" s="15"/>
     </row>
-    <row r="112" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:10" ht="12">
       <c r="J112" s="15"/>
     </row>
-    <row r="113" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="113" spans="10:10" ht="12">
       <c r="J113" s="15"/>
     </row>
-    <row r="114" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="114" spans="10:10" ht="12">
       <c r="J114" s="15"/>
     </row>
-    <row r="115" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="115" spans="10:10" ht="12">
       <c r="J115" s="15"/>
     </row>
-    <row r="116" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="116" spans="10:10" ht="12">
       <c r="J116" s="15"/>
     </row>
-    <row r="117" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="117" spans="10:10" ht="12">
       <c r="J117" s="15"/>
     </row>
-    <row r="118" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="118" spans="10:10" ht="12">
       <c r="J118" s="15"/>
     </row>
-    <row r="119" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="119" spans="10:10" ht="12">
       <c r="J119" s="15"/>
     </row>
-    <row r="120" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="120" spans="10:10" ht="12">
       <c r="J120" s="15"/>
     </row>
-    <row r="121" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="121" spans="10:10" ht="12">
       <c r="J121" s="15"/>
     </row>
-    <row r="122" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="122" spans="10:10" ht="12">
       <c r="J122" s="15"/>
     </row>
-    <row r="123" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="123" spans="10:10" ht="12">
       <c r="J123" s="15"/>
     </row>
-    <row r="124" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="124" spans="10:10" ht="12">
       <c r="J124" s="15"/>
     </row>
-    <row r="125" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="125" spans="10:10" ht="12">
       <c r="J125" s="15"/>
     </row>
-    <row r="126" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="126" spans="10:10" ht="12">
       <c r="J126" s="15"/>
     </row>
-    <row r="127" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="127" spans="10:10" ht="12">
       <c r="J127" s="15"/>
     </row>
-    <row r="128" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="128" spans="10:10" ht="12">
       <c r="J128" s="15"/>
     </row>
-    <row r="129" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="129" spans="10:10" ht="12">
       <c r="J129" s="15"/>
     </row>
-    <row r="130" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="130" spans="10:10" ht="12">
       <c r="J130" s="15"/>
     </row>
-    <row r="131" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="131" spans="10:10" ht="12">
       <c r="J131" s="15"/>
     </row>
-    <row r="132" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="132" spans="10:10" ht="12">
       <c r="J132" s="15"/>
     </row>
-    <row r="133" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="133" spans="10:10" ht="12">
       <c r="J133" s="15"/>
     </row>
-    <row r="134" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="134" spans="10:10" ht="12">
       <c r="J134" s="15"/>
     </row>
-    <row r="135" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="135" spans="10:10" ht="12">
       <c r="J135" s="15"/>
     </row>
-    <row r="136" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="136" spans="10:10" ht="12">
       <c r="J136" s="15"/>
     </row>
-    <row r="137" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="137" spans="10:10" ht="12">
       <c r="J137" s="15"/>
     </row>
-    <row r="138" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="138" spans="10:10" ht="12">
       <c r="J138" s="15"/>
     </row>
-    <row r="139" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="139" spans="10:10" ht="12">
       <c r="J139" s="15"/>
     </row>
-    <row r="140" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="140" spans="10:10" ht="12">
       <c r="J140" s="15"/>
     </row>
-    <row r="141" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="141" spans="10:10" ht="12">
       <c r="J141" s="15"/>
     </row>
-    <row r="142" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="142" spans="10:10" ht="12">
       <c r="J142" s="15"/>
     </row>
-    <row r="143" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="143" spans="10:10" ht="12">
       <c r="J143" s="15"/>
     </row>
-    <row r="144" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="144" spans="10:10" ht="12">
       <c r="J144" s="15"/>
     </row>
-    <row r="145" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="145" spans="10:10" ht="12">
       <c r="J145" s="15"/>
     </row>
-    <row r="146" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="146" spans="10:10" ht="12">
       <c r="J146" s="15"/>
     </row>
-    <row r="147" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="147" spans="10:10" ht="12">
       <c r="J147" s="15"/>
     </row>
-    <row r="148" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="148" spans="10:10" ht="12">
       <c r="J148" s="15"/>
     </row>
-    <row r="149" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="149" spans="10:10" ht="12">
       <c r="J149" s="15"/>
     </row>
-    <row r="150" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="150" spans="10:10" ht="12">
       <c r="J150" s="15"/>
     </row>
-    <row r="151" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="151" spans="10:10" ht="12">
       <c r="J151" s="15"/>
     </row>
-    <row r="152" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="152" spans="10:10" ht="12">
       <c r="J152" s="15"/>
     </row>
-    <row r="153" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="153" spans="10:10" ht="12">
       <c r="J153" s="15"/>
     </row>
-    <row r="154" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="154" spans="10:10" ht="12">
       <c r="J154" s="15"/>
     </row>
-    <row r="155" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="155" spans="10:10" ht="12">
       <c r="J155" s="15"/>
     </row>
-    <row r="156" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="156" spans="10:10" ht="12">
       <c r="J156" s="15"/>
     </row>
-    <row r="157" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="157" spans="10:10" ht="12">
       <c r="J157" s="15"/>
     </row>
-    <row r="158" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="158" spans="10:10" ht="12">
       <c r="J158" s="15"/>
     </row>
-    <row r="159" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="159" spans="10:10" ht="12">
       <c r="J159" s="15"/>
     </row>
-    <row r="160" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="160" spans="10:10" ht="12">
       <c r="J160" s="15"/>
     </row>
-    <row r="161" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="161" spans="10:10" ht="12">
       <c r="J161" s="15"/>
     </row>
-    <row r="162" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="162" spans="10:10" ht="12">
       <c r="J162" s="15"/>
     </row>
-    <row r="163" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="163" spans="10:10" ht="12">
       <c r="J163" s="15"/>
     </row>
-    <row r="164" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="164" spans="10:10" ht="12">
       <c r="J164" s="15"/>
     </row>
-    <row r="165" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="165" spans="10:10" ht="12">
       <c r="J165" s="15"/>
     </row>
-    <row r="166" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="166" spans="10:10" ht="12">
       <c r="J166" s="15"/>
     </row>
-    <row r="167" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="167" spans="10:10" ht="12">
       <c r="J167" s="15"/>
     </row>
-    <row r="168" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="168" spans="10:10" ht="12">
       <c r="J168" s="15"/>
     </row>
-    <row r="169" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="169" spans="10:10" ht="12">
       <c r="J169" s="15"/>
     </row>
-    <row r="170" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="170" spans="10:10" ht="12">
       <c r="J170" s="15"/>
     </row>
-    <row r="171" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="171" spans="10:10" ht="12">
       <c r="J171" s="15"/>
     </row>
-    <row r="172" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="172" spans="10:10" ht="12">
       <c r="J172" s="15"/>
     </row>
-    <row r="173" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="173" spans="10:10" ht="12">
       <c r="J173" s="15"/>
     </row>
-    <row r="174" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="174" spans="10:10" ht="12">
       <c r="J174" s="15"/>
     </row>
-    <row r="175" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="175" spans="10:10" ht="12">
       <c r="J175" s="15"/>
     </row>
-    <row r="176" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="176" spans="10:10" ht="12">
       <c r="J176" s="15"/>
     </row>
-    <row r="177" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="177" spans="10:10" ht="12">
       <c r="J177" s="15"/>
     </row>
-    <row r="178" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="178" spans="10:10" ht="12">
       <c r="J178" s="15"/>
     </row>
-    <row r="179" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="179" spans="10:10" ht="12">
       <c r="J179" s="15"/>
     </row>
-    <row r="180" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="180" spans="10:10" ht="12">
       <c r="J180" s="15"/>
     </row>
-    <row r="181" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="181" spans="10:10" ht="12">
       <c r="J181" s="15"/>
     </row>
-    <row r="182" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="182" spans="10:10" ht="12">
       <c r="J182" s="15"/>
     </row>
-    <row r="183" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="183" spans="10:10" ht="12">
       <c r="J183" s="15"/>
     </row>
-    <row r="184" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="184" spans="10:10" ht="12">
       <c r="J184" s="15"/>
     </row>
-    <row r="185" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="185" spans="10:10" ht="12">
       <c r="J185" s="15"/>
     </row>
-    <row r="186" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="186" spans="10:10" ht="12">
       <c r="J186" s="15"/>
     </row>
-    <row r="187" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="187" spans="10:10" ht="12">
       <c r="J187" s="15"/>
     </row>
-    <row r="188" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="188" spans="10:10" ht="12">
       <c r="J188" s="15"/>
     </row>
-    <row r="189" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="189" spans="10:10" ht="12">
       <c r="J189" s="15"/>
     </row>
-    <row r="190" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="190" spans="10:10" ht="12">
       <c r="J190" s="15"/>
     </row>
-    <row r="191" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="191" spans="10:10" ht="12">
       <c r="J191" s="15"/>
     </row>
-    <row r="192" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="192" spans="10:10" ht="12">
       <c r="J192" s="15"/>
     </row>
-    <row r="193" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="193" spans="10:10" ht="12">
       <c r="J193" s="15"/>
     </row>
-    <row r="194" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="194" spans="10:10" ht="12">
       <c r="J194" s="15"/>
     </row>
-    <row r="195" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="195" spans="10:10" ht="12">
       <c r="J195" s="15"/>
     </row>
-    <row r="196" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="196" spans="10:10" ht="12">
       <c r="J196" s="15"/>
     </row>
-    <row r="197" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="197" spans="10:10" ht="12">
       <c r="J197" s="15"/>
     </row>
-    <row r="198" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="198" spans="10:10" ht="12">
       <c r="J198" s="15"/>
     </row>
   </sheetData>
@@ -16082,114 +16068,114 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="J3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="J4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="J5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="J6" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
-    <hyperlink ref="J7" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
-    <hyperlink ref="J8" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
-    <hyperlink ref="J9" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
-    <hyperlink ref="J10" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
-    <hyperlink ref="J11" r:id="rId10" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
-    <hyperlink ref="J12" r:id="rId11" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
-    <hyperlink ref="J13" r:id="rId12" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
-    <hyperlink ref="J14" r:id="rId13" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
-    <hyperlink ref="J15" r:id="rId14" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
-    <hyperlink ref="J16" r:id="rId15" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
-    <hyperlink ref="J17" r:id="rId16" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
-    <hyperlink ref="J18" r:id="rId17" xr:uid="{00000000-0004-0000-0200-000010000000}"/>
-    <hyperlink ref="J19" r:id="rId18" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
-    <hyperlink ref="J20" r:id="rId19" xr:uid="{00000000-0004-0000-0200-000012000000}"/>
-    <hyperlink ref="J21" r:id="rId20" xr:uid="{00000000-0004-0000-0200-000013000000}"/>
-    <hyperlink ref="J22" r:id="rId21" xr:uid="{00000000-0004-0000-0200-000014000000}"/>
-    <hyperlink ref="J23" r:id="rId22" xr:uid="{00000000-0004-0000-0200-000015000000}"/>
-    <hyperlink ref="J24" r:id="rId23" xr:uid="{00000000-0004-0000-0200-000016000000}"/>
-    <hyperlink ref="J25" r:id="rId24" xr:uid="{00000000-0004-0000-0200-000017000000}"/>
-    <hyperlink ref="J26" r:id="rId25" xr:uid="{00000000-0004-0000-0200-000018000000}"/>
-    <hyperlink ref="J27" r:id="rId26" xr:uid="{00000000-0004-0000-0200-000019000000}"/>
-    <hyperlink ref="J28" r:id="rId27" xr:uid="{00000000-0004-0000-0200-00001A000000}"/>
-    <hyperlink ref="J29" r:id="rId28" xr:uid="{00000000-0004-0000-0200-00001B000000}"/>
-    <hyperlink ref="J30" r:id="rId29" xr:uid="{00000000-0004-0000-0200-00001C000000}"/>
-    <hyperlink ref="J31" r:id="rId30" xr:uid="{00000000-0004-0000-0200-00001D000000}"/>
-    <hyperlink ref="J32" r:id="rId31" xr:uid="{00000000-0004-0000-0200-00001E000000}"/>
-    <hyperlink ref="J33" r:id="rId32" xr:uid="{00000000-0004-0000-0200-00001F000000}"/>
-    <hyperlink ref="J34" r:id="rId33" xr:uid="{00000000-0004-0000-0200-000020000000}"/>
-    <hyperlink ref="J35" r:id="rId34" xr:uid="{00000000-0004-0000-0200-000021000000}"/>
-    <hyperlink ref="J36" r:id="rId35" xr:uid="{00000000-0004-0000-0200-000022000000}"/>
-    <hyperlink ref="J37" r:id="rId36" xr:uid="{00000000-0004-0000-0200-000023000000}"/>
-    <hyperlink ref="J38" r:id="rId37" xr:uid="{00000000-0004-0000-0200-000024000000}"/>
-    <hyperlink ref="J39" r:id="rId38" xr:uid="{00000000-0004-0000-0200-000025000000}"/>
-    <hyperlink ref="J40" r:id="rId39" xr:uid="{00000000-0004-0000-0200-000026000000}"/>
-    <hyperlink ref="J41" r:id="rId40" xr:uid="{00000000-0004-0000-0200-000027000000}"/>
-    <hyperlink ref="J42" r:id="rId41" xr:uid="{00000000-0004-0000-0200-000028000000}"/>
-    <hyperlink ref="J43" r:id="rId42" xr:uid="{00000000-0004-0000-0200-000029000000}"/>
-    <hyperlink ref="J44" r:id="rId43" xr:uid="{00000000-0004-0000-0200-00002A000000}"/>
-    <hyperlink ref="J45" r:id="rId44" xr:uid="{00000000-0004-0000-0200-00002B000000}"/>
-    <hyperlink ref="J46" r:id="rId45" xr:uid="{00000000-0004-0000-0200-00002C000000}"/>
-    <hyperlink ref="J47" r:id="rId46" xr:uid="{00000000-0004-0000-0200-00002D000000}"/>
-    <hyperlink ref="J48" r:id="rId47" xr:uid="{00000000-0004-0000-0200-00002E000000}"/>
-    <hyperlink ref="J49" r:id="rId48" xr:uid="{00000000-0004-0000-0200-00002F000000}"/>
-    <hyperlink ref="J50" r:id="rId49" xr:uid="{00000000-0004-0000-0200-000030000000}"/>
-    <hyperlink ref="J51" r:id="rId50" xr:uid="{00000000-0004-0000-0200-000031000000}"/>
-    <hyperlink ref="J52" r:id="rId51" xr:uid="{00000000-0004-0000-0200-000032000000}"/>
-    <hyperlink ref="J53" r:id="rId52" xr:uid="{00000000-0004-0000-0200-000033000000}"/>
-    <hyperlink ref="J54" r:id="rId53" xr:uid="{00000000-0004-0000-0200-000034000000}"/>
-    <hyperlink ref="J55" r:id="rId54" xr:uid="{00000000-0004-0000-0200-000035000000}"/>
-    <hyperlink ref="J56" r:id="rId55" xr:uid="{00000000-0004-0000-0200-000036000000}"/>
-    <hyperlink ref="J57" r:id="rId56" xr:uid="{00000000-0004-0000-0200-000037000000}"/>
-    <hyperlink ref="J58" r:id="rId57" xr:uid="{00000000-0004-0000-0200-000038000000}"/>
-    <hyperlink ref="J59" r:id="rId58" xr:uid="{00000000-0004-0000-0200-000039000000}"/>
-    <hyperlink ref="J60" r:id="rId59" xr:uid="{00000000-0004-0000-0200-00003A000000}"/>
-    <hyperlink ref="J61" r:id="rId60" xr:uid="{00000000-0004-0000-0200-00003B000000}"/>
-    <hyperlink ref="J62" r:id="rId61" xr:uid="{00000000-0004-0000-0200-00003C000000}"/>
-    <hyperlink ref="J63" r:id="rId62" xr:uid="{00000000-0004-0000-0200-00003D000000}"/>
-    <hyperlink ref="J64" r:id="rId63" xr:uid="{00000000-0004-0000-0200-00003E000000}"/>
-    <hyperlink ref="J65" r:id="rId64" xr:uid="{00000000-0004-0000-0200-00003F000000}"/>
-    <hyperlink ref="J66" r:id="rId65" xr:uid="{00000000-0004-0000-0200-000040000000}"/>
-    <hyperlink ref="J67" r:id="rId66" xr:uid="{00000000-0004-0000-0200-000041000000}"/>
-    <hyperlink ref="J68" r:id="rId67" xr:uid="{00000000-0004-0000-0200-000042000000}"/>
-    <hyperlink ref="J69" r:id="rId68" xr:uid="{00000000-0004-0000-0200-000043000000}"/>
-    <hyperlink ref="J70" r:id="rId69" xr:uid="{00000000-0004-0000-0200-000044000000}"/>
-    <hyperlink ref="J71" r:id="rId70" xr:uid="{00000000-0004-0000-0200-000045000000}"/>
-    <hyperlink ref="J72" r:id="rId71" xr:uid="{00000000-0004-0000-0200-000046000000}"/>
-    <hyperlink ref="J73" r:id="rId72" xr:uid="{00000000-0004-0000-0200-000047000000}"/>
-    <hyperlink ref="J74" r:id="rId73" xr:uid="{00000000-0004-0000-0200-000048000000}"/>
-    <hyperlink ref="J75" r:id="rId74" xr:uid="{00000000-0004-0000-0200-000049000000}"/>
-    <hyperlink ref="J76" r:id="rId75" xr:uid="{00000000-0004-0000-0200-00004A000000}"/>
-    <hyperlink ref="J77" r:id="rId76" xr:uid="{00000000-0004-0000-0200-00004B000000}"/>
-    <hyperlink ref="J78" r:id="rId77" xr:uid="{00000000-0004-0000-0200-00004C000000}"/>
-    <hyperlink ref="J79" r:id="rId78" xr:uid="{00000000-0004-0000-0200-00004D000000}"/>
-    <hyperlink ref="J80" r:id="rId79" xr:uid="{00000000-0004-0000-0200-00004E000000}"/>
-    <hyperlink ref="J81" r:id="rId80" xr:uid="{00000000-0004-0000-0200-00004F000000}"/>
-    <hyperlink ref="J82" r:id="rId81" xr:uid="{00000000-0004-0000-0200-000050000000}"/>
-    <hyperlink ref="J83" r:id="rId82" xr:uid="{00000000-0004-0000-0200-000051000000}"/>
-    <hyperlink ref="J84" r:id="rId83" xr:uid="{00000000-0004-0000-0200-000052000000}"/>
-    <hyperlink ref="J85" r:id="rId84" xr:uid="{00000000-0004-0000-0200-000053000000}"/>
-    <hyperlink ref="J86" r:id="rId85" xr:uid="{00000000-0004-0000-0200-000054000000}"/>
-    <hyperlink ref="J87" r:id="rId86" xr:uid="{00000000-0004-0000-0200-000055000000}"/>
-    <hyperlink ref="J88" r:id="rId87" xr:uid="{00000000-0004-0000-0200-000056000000}"/>
-    <hyperlink ref="J89" r:id="rId88" xr:uid="{00000000-0004-0000-0200-000057000000}"/>
-    <hyperlink ref="J90" r:id="rId89" xr:uid="{00000000-0004-0000-0200-000058000000}"/>
-    <hyperlink ref="J91" r:id="rId90" xr:uid="{00000000-0004-0000-0200-000059000000}"/>
-    <hyperlink ref="J92" r:id="rId91" xr:uid="{00000000-0004-0000-0200-00005A000000}"/>
-    <hyperlink ref="J93" r:id="rId92" xr:uid="{00000000-0004-0000-0200-00005B000000}"/>
-    <hyperlink ref="J94" r:id="rId93" xr:uid="{00000000-0004-0000-0200-00005C000000}"/>
-    <hyperlink ref="J95" r:id="rId94" xr:uid="{00000000-0004-0000-0200-00005D000000}"/>
-    <hyperlink ref="J96" r:id="rId95" xr:uid="{00000000-0004-0000-0200-00005E000000}"/>
-    <hyperlink ref="J97" r:id="rId96" xr:uid="{00000000-0004-0000-0200-00005F000000}"/>
-    <hyperlink ref="J98" r:id="rId97" xr:uid="{00000000-0004-0000-0200-000060000000}"/>
-    <hyperlink ref="J99" r:id="rId98" xr:uid="{00000000-0004-0000-0200-000061000000}"/>
-    <hyperlink ref="J100" r:id="rId99" xr:uid="{00000000-0004-0000-0200-000062000000}"/>
-    <hyperlink ref="J101" r:id="rId100" xr:uid="{00000000-0004-0000-0200-000063000000}"/>
-    <hyperlink ref="J102" r:id="rId101" xr:uid="{00000000-0004-0000-0200-000064000000}"/>
-    <hyperlink ref="J103" r:id="rId102" xr:uid="{00000000-0004-0000-0200-000065000000}"/>
-    <hyperlink ref="J104" r:id="rId103" xr:uid="{00000000-0004-0000-0200-000066000000}"/>
-    <hyperlink ref="J105" r:id="rId104" xr:uid="{00000000-0004-0000-0200-000067000000}"/>
-    <hyperlink ref="J106" r:id="rId105" xr:uid="{00000000-0004-0000-0200-000068000000}"/>
-    <hyperlink ref="J107" r:id="rId106" xr:uid="{00000000-0004-0000-0200-000069000000}"/>
-    <hyperlink ref="J108" r:id="rId107" xr:uid="{00000000-0004-0000-0200-00006A000000}"/>
-    <hyperlink ref="J109" r:id="rId108" xr:uid="{00000000-0004-0000-0200-00006B000000}"/>
+    <hyperlink ref="J2" r:id="rId1"/>
+    <hyperlink ref="J3" r:id="rId2"/>
+    <hyperlink ref="J4" r:id="rId3"/>
+    <hyperlink ref="J5" r:id="rId4"/>
+    <hyperlink ref="J6" r:id="rId5"/>
+    <hyperlink ref="J7" r:id="rId6"/>
+    <hyperlink ref="J8" r:id="rId7"/>
+    <hyperlink ref="J9" r:id="rId8"/>
+    <hyperlink ref="J10" r:id="rId9"/>
+    <hyperlink ref="J11" r:id="rId10"/>
+    <hyperlink ref="J12" r:id="rId11"/>
+    <hyperlink ref="J13" r:id="rId12"/>
+    <hyperlink ref="J14" r:id="rId13"/>
+    <hyperlink ref="J15" r:id="rId14"/>
+    <hyperlink ref="J16" r:id="rId15"/>
+    <hyperlink ref="J17" r:id="rId16"/>
+    <hyperlink ref="J18" r:id="rId17"/>
+    <hyperlink ref="J19" r:id="rId18"/>
+    <hyperlink ref="J20" r:id="rId19"/>
+    <hyperlink ref="J21" r:id="rId20"/>
+    <hyperlink ref="J22" r:id="rId21"/>
+    <hyperlink ref="J23" r:id="rId22"/>
+    <hyperlink ref="J24" r:id="rId23"/>
+    <hyperlink ref="J25" r:id="rId24"/>
+    <hyperlink ref="J26" r:id="rId25"/>
+    <hyperlink ref="J27" r:id="rId26"/>
+    <hyperlink ref="J28" r:id="rId27"/>
+    <hyperlink ref="J29" r:id="rId28"/>
+    <hyperlink ref="J30" r:id="rId29"/>
+    <hyperlink ref="J31" r:id="rId30"/>
+    <hyperlink ref="J32" r:id="rId31"/>
+    <hyperlink ref="J33" r:id="rId32"/>
+    <hyperlink ref="J34" r:id="rId33"/>
+    <hyperlink ref="J35" r:id="rId34"/>
+    <hyperlink ref="J36" r:id="rId35"/>
+    <hyperlink ref="J37" r:id="rId36"/>
+    <hyperlink ref="J38" r:id="rId37"/>
+    <hyperlink ref="J39" r:id="rId38"/>
+    <hyperlink ref="J40" r:id="rId39"/>
+    <hyperlink ref="J41" r:id="rId40"/>
+    <hyperlink ref="J42" r:id="rId41"/>
+    <hyperlink ref="J43" r:id="rId42"/>
+    <hyperlink ref="J44" r:id="rId43"/>
+    <hyperlink ref="J45" r:id="rId44"/>
+    <hyperlink ref="J46" r:id="rId45"/>
+    <hyperlink ref="J47" r:id="rId46"/>
+    <hyperlink ref="J48" r:id="rId47"/>
+    <hyperlink ref="J49" r:id="rId48"/>
+    <hyperlink ref="J50" r:id="rId49"/>
+    <hyperlink ref="J51" r:id="rId50"/>
+    <hyperlink ref="J52" r:id="rId51"/>
+    <hyperlink ref="J53" r:id="rId52"/>
+    <hyperlink ref="J54" r:id="rId53"/>
+    <hyperlink ref="J55" r:id="rId54"/>
+    <hyperlink ref="J56" r:id="rId55"/>
+    <hyperlink ref="J57" r:id="rId56"/>
+    <hyperlink ref="J58" r:id="rId57"/>
+    <hyperlink ref="J59" r:id="rId58"/>
+    <hyperlink ref="J60" r:id="rId59"/>
+    <hyperlink ref="J61" r:id="rId60"/>
+    <hyperlink ref="J62" r:id="rId61"/>
+    <hyperlink ref="J63" r:id="rId62"/>
+    <hyperlink ref="J64" r:id="rId63"/>
+    <hyperlink ref="J65" r:id="rId64"/>
+    <hyperlink ref="J66" r:id="rId65"/>
+    <hyperlink ref="J67" r:id="rId66"/>
+    <hyperlink ref="J68" r:id="rId67"/>
+    <hyperlink ref="J69" r:id="rId68"/>
+    <hyperlink ref="J70" r:id="rId69"/>
+    <hyperlink ref="J71" r:id="rId70"/>
+    <hyperlink ref="J72" r:id="rId71"/>
+    <hyperlink ref="J73" r:id="rId72"/>
+    <hyperlink ref="J74" r:id="rId73"/>
+    <hyperlink ref="J75" r:id="rId74"/>
+    <hyperlink ref="J76" r:id="rId75"/>
+    <hyperlink ref="J77" r:id="rId76"/>
+    <hyperlink ref="J78" r:id="rId77"/>
+    <hyperlink ref="J79" r:id="rId78"/>
+    <hyperlink ref="J80" r:id="rId79"/>
+    <hyperlink ref="J81" r:id="rId80"/>
+    <hyperlink ref="J82" r:id="rId81"/>
+    <hyperlink ref="J83" r:id="rId82"/>
+    <hyperlink ref="J84" r:id="rId83"/>
+    <hyperlink ref="J85" r:id="rId84"/>
+    <hyperlink ref="J86" r:id="rId85"/>
+    <hyperlink ref="J87" r:id="rId86"/>
+    <hyperlink ref="J88" r:id="rId87"/>
+    <hyperlink ref="J89" r:id="rId88"/>
+    <hyperlink ref="J90" r:id="rId89"/>
+    <hyperlink ref="J91" r:id="rId90"/>
+    <hyperlink ref="J92" r:id="rId91"/>
+    <hyperlink ref="J93" r:id="rId92"/>
+    <hyperlink ref="J94" r:id="rId93"/>
+    <hyperlink ref="J95" r:id="rId94"/>
+    <hyperlink ref="J96" r:id="rId95"/>
+    <hyperlink ref="J97" r:id="rId96"/>
+    <hyperlink ref="J98" r:id="rId97"/>
+    <hyperlink ref="J99" r:id="rId98"/>
+    <hyperlink ref="J100" r:id="rId99"/>
+    <hyperlink ref="J101" r:id="rId100"/>
+    <hyperlink ref="J102" r:id="rId101"/>
+    <hyperlink ref="J103" r:id="rId102"/>
+    <hyperlink ref="J104" r:id="rId103"/>
+    <hyperlink ref="J105" r:id="rId104"/>
+    <hyperlink ref="J106" r:id="rId105"/>
+    <hyperlink ref="J107" r:id="rId106"/>
+    <hyperlink ref="J108" r:id="rId107"/>
+    <hyperlink ref="J109" r:id="rId108"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>